<commit_message>
Update date and version.
</commit_message>
<xml_diff>
--- a/ExchangeWebServices/Docs/MS-OXWSSYNC/MS-OXWSSYNC_RequirementSpecification.xlsx
+++ b/ExchangeWebServices/Docs/MS-OXWSSYNC/MS-OXWSSYNC_RequirementSpecification.xlsx
@@ -4382,127 +4382,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="61">
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
+  <dxfs count="37">
     <dxf>
       <font>
         <b val="0"/>
@@ -5055,34 +4935,34 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Requirement" displayName="Requirement" ref="A19:I384" tableType="xml" totalsRowShown="0" headerRowDxfId="40" dataDxfId="39" connectionId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Requirement" displayName="Requirement" ref="A19:I384" tableType="xml" totalsRowShown="0" headerRowDxfId="16" dataDxfId="15" connectionId="1">
   <autoFilter ref="A19:I384"/>
   <tableColumns count="9">
-    <tableColumn id="1" uniqueName="ns1:REQ_ID" name="Req ID" dataDxfId="38">
+    <tableColumn id="1" uniqueName="ns1:REQ_ID" name="Req ID" dataDxfId="14">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:REQ_ID" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="2" uniqueName="ns1:Doc_Sect" name="Doc Sect" dataDxfId="37">
+    <tableColumn id="2" uniqueName="ns1:Doc_Sect" name="Doc Sect" dataDxfId="13">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Doc_Sect" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="3" uniqueName="ns1:Description" name="Description" dataDxfId="36">
+    <tableColumn id="3" uniqueName="ns1:Description" name="Description" dataDxfId="12">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Description" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="18" uniqueName="ns1:Derived" name="Derived" dataDxfId="35">
+    <tableColumn id="18" uniqueName="ns1:Derived" name="Derived" dataDxfId="11">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Derived" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="6" uniqueName="ns1:Behavior" name="Behavior" dataDxfId="34">
+    <tableColumn id="6" uniqueName="ns1:Behavior" name="Behavior" dataDxfId="10">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Behavior" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="7" uniqueName="ns1:Scope" name="Scope" dataDxfId="33">
+    <tableColumn id="7" uniqueName="ns1:Scope" name="Scope" dataDxfId="9">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Scope" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="9" uniqueName="ns1:IsNormative" name="Informative_x000a_/Normative" dataDxfId="32">
+    <tableColumn id="9" uniqueName="ns1:IsNormative" name="Informative_x000a_/Normative" dataDxfId="8">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:IsNormative" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="10" uniqueName="ns1:Verification" name="Verification" dataDxfId="31">
+    <tableColumn id="10" uniqueName="ns1:Verification" name="Verification" dataDxfId="7">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Verification" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="8" uniqueName="ns1:VerificationComment" name="Verification Comment" dataDxfId="30">
+    <tableColumn id="8" uniqueName="ns1:VerificationComment" name="Verification Comment" dataDxfId="6">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:VerificationComment" xmlDataType="string"/>
     </tableColumn>
   </tableColumns>
@@ -5091,12 +4971,12 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Scope" displayName="Scope" ref="A12:C15" totalsRowShown="0" headerRowBorderDxfId="29" tableBorderDxfId="28" totalsRowBorderDxfId="27">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Scope" displayName="Scope" ref="A12:C15" totalsRowShown="0" headerRowBorderDxfId="5" tableBorderDxfId="4" totalsRowBorderDxfId="3">
   <autoFilter ref="A12:C15"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="Scope" dataDxfId="26"/>
-    <tableColumn id="2" name="Test" dataDxfId="25"/>
-    <tableColumn id="3" name="Description" dataDxfId="24"/>
+    <tableColumn id="1" name="Scope" dataDxfId="2"/>
+    <tableColumn id="2" name="Test" dataDxfId="1"/>
+    <tableColumn id="3" name="Description" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5392,8 +5272,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:M386"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A346" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D346" sqref="A346:XFD346"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9:I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -5443,14 +5323,14 @@
         <v>25</v>
       </c>
       <c r="C3" s="36">
-        <v>5</v>
+        <v>7.1</v>
       </c>
       <c r="D3" s="4"/>
       <c r="E3" s="35" t="s">
         <v>26</v>
       </c>
       <c r="F3" s="37">
-        <v>41185</v>
+        <v>42261</v>
       </c>
       <c r="G3" s="38"/>
       <c r="H3" s="4"/>
@@ -15045,76 +14925,76 @@
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="A365:B365 A368:B368 A366:I367 D365:I365 A369:I384 D368:I368 I357:I384 A20:I364">
-    <cfRule type="expression" dxfId="60" priority="77">
+    <cfRule type="expression" dxfId="36" priority="77">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="59" priority="78">
+    <cfRule type="expression" dxfId="35" priority="78">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="58" priority="85">
+    <cfRule type="expression" dxfId="34" priority="85">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A365:B365 A368:B368 A366:I367 D365:I365 A369:I384 D368:I368 I357:I384 A20:I364">
-    <cfRule type="expression" dxfId="57" priority="31">
+    <cfRule type="expression" dxfId="33" priority="31">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="56" priority="32">
+    <cfRule type="expression" dxfId="32" priority="32">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="55" priority="33">
+    <cfRule type="expression" dxfId="31" priority="33">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F20:F384">
-    <cfRule type="expression" dxfId="54" priority="37">
+    <cfRule type="expression" dxfId="30" priority="37">
       <formula>NOT(VLOOKUP(F20,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="53" priority="38">
+    <cfRule type="expression" dxfId="29" priority="38">
       <formula>(VLOOKUP(F20,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C368">
-    <cfRule type="expression" dxfId="52" priority="10">
+    <cfRule type="expression" dxfId="28" priority="10">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="51" priority="11">
+    <cfRule type="expression" dxfId="27" priority="11">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="50" priority="12">
+    <cfRule type="expression" dxfId="26" priority="12">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C368">
-    <cfRule type="expression" dxfId="49" priority="7">
+    <cfRule type="expression" dxfId="25" priority="7">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="48" priority="8">
+    <cfRule type="expression" dxfId="24" priority="8">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="47" priority="9">
+    <cfRule type="expression" dxfId="23" priority="9">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C365">
-    <cfRule type="expression" dxfId="46" priority="4">
+    <cfRule type="expression" dxfId="22" priority="4">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="45" priority="5">
+    <cfRule type="expression" dxfId="21" priority="5">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="44" priority="6">
+    <cfRule type="expression" dxfId="20" priority="6">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C365">
-    <cfRule type="expression" dxfId="43" priority="1">
+    <cfRule type="expression" dxfId="19" priority="1">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="42" priority="2">
+    <cfRule type="expression" dxfId="18" priority="2">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="41" priority="3">
+    <cfRule type="expression" dxfId="17" priority="3">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
@@ -15142,7 +15022,7 @@
     <oddFooter>&amp;F&amp;RPage &amp;P</oddFooter>
   </headerFooter>
   <ignoredErrors>
-    <ignoredError sqref="B1:B9 C3 B10:B46 B108:B109 B47:B103 B178:B211 B361:B386 B340:B352" numberStoredAsText="1"/>
+    <ignoredError sqref="B1:B9 B10:B46 B108:B109 B47:B103 B178:B211 B361:B386 B340:B352" numberStoredAsText="1"/>
   </ignoredErrors>
   <tableParts count="2">
     <tablePart r:id="rId2"/>
@@ -15152,21 +15032,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F2EA47BB262D974097182E2CA8AB13E1" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="74597e8d9e42e7e4fc8eda6d37675aa2">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4aeb20c0e3442673af7ee10786458764">
     <xsd:element name="properties">
@@ -15215,10 +15080,32 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6D33261-F3C6-4621-88F1-D76E5ABE1865}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EDB2DE12-5EF6-4CF2-820D-5F9FE329E08E}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/internal/2005/internalDocumentation"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -15238,16 +15125,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EDB2DE12-5EF6-4CF2-820D-5F9FE329E08E}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6D33261-F3C6-4621-88F1-D76E5ABE1865}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/internal/2005/internalDocumentation"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Update capture code and test case.
</commit_message>
<xml_diff>
--- a/ExchangeWebServices/Docs/MS-OXWSSYNC/MS-OXWSSYNC_RequirementSpecification.xlsx
+++ b/ExchangeWebServices/Docs/MS-OXWSSYNC/MS-OXWSSYNC_RequirementSpecification.xlsx
@@ -5272,8 +5272,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:M386"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9:I9"/>
+    <sheetView tabSelected="1" topLeftCell="A354" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C361" sqref="C361"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -11186,7 +11186,7 @@
       <c r="I240" s="27"/>
     </row>
     <row r="241" spans="1:9" ht="30">
-      <c r="A241" s="25" t="s">
+      <c r="A241" s="18" t="s">
         <v>139</v>
       </c>
       <c r="B241" s="20" t="s">
@@ -11211,7 +11211,7 @@
       <c r="I241" s="27"/>
     </row>
     <row r="242" spans="1:9" ht="30">
-      <c r="A242" s="25" t="s">
+      <c r="A242" s="18" t="s">
         <v>140</v>
       </c>
       <c r="B242" s="20" t="s">
@@ -11783,7 +11783,7 @@
         <v>15</v>
       </c>
       <c r="H264" s="46" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I264" s="48"/>
     </row>
@@ -11833,7 +11833,7 @@
         <v>15</v>
       </c>
       <c r="H266" s="46" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I266" s="48"/>
     </row>
@@ -11883,7 +11883,7 @@
         <v>15</v>
       </c>
       <c r="H268" s="46" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I268" s="48"/>
     </row>
@@ -11935,7 +11935,7 @@
         <v>15</v>
       </c>
       <c r="H270" s="46" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I270" s="48"/>
     </row>
@@ -13871,7 +13871,7 @@
       <c r="I345" s="27"/>
     </row>
     <row r="346" spans="1:9" ht="45">
-      <c r="A346" s="25" t="s">
+      <c r="A346" s="18" t="s">
         <v>358</v>
       </c>
       <c r="B346" s="26" t="s">
@@ -15032,6 +15032,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F2EA47BB262D974097182E2CA8AB13E1" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="74597e8d9e42e7e4fc8eda6d37675aa2">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4aeb20c0e3442673af7ee10786458764">
     <xsd:element name="properties">
@@ -15080,32 +15095,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EDB2DE12-5EF6-4CF2-820D-5F9FE329E08E}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6D33261-F3C6-4621-88F1-D76E5ABE1865}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/internal/2005/internalDocumentation"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -15125,9 +15118,16 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6D33261-F3C6-4621-88F1-D76E5ABE1865}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EDB2DE12-5EF6-4CF2-820D-5F9FE329E08E}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/internal/2005/internalDocumentation"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Add cmd file and update code to fix failed test suite.
</commit_message>
<xml_diff>
--- a/ExchangeWebServices/Docs/MS-OXWSSYNC/MS-OXWSSYNC_RequirementSpecification.xlsx
+++ b/ExchangeWebServices/Docs/MS-OXWSSYNC/MS-OXWSSYNC_RequirementSpecification.xlsx
@@ -10,7 +10,7 @@
     <sheet name="Requirements" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Requirements!$A$19:$G$384</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Requirements!$A$19:$G$388</definedName>
     <definedName name="ExtensionList">Requirements!#REF!</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">Requirements!$A:$A,Requirements!$19:$19</definedName>
     <definedName name="ScopeList">Requirements!#REF!</definedName>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2675" uniqueCount="887">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2711" uniqueCount="899">
   <si>
     <t>Req ID</t>
   </si>
@@ -3951,6 +3951,42 @@
   <si>
     <t>[In Appendix C: Product Behavior] Implementation does include Delete element. (Exchange 2010 and above follow this behavior.)</t>
   </si>
+  <si>
+    <t>[In Appendix C: Product Behavior] Implementation does not support the RoleMember element. (&lt;3&gt; Section 3.1.4.2.3.3:  Exchange 2007, Exchange 2010, and Exchange 2013 do not support the RoleMember element.)</t>
+  </si>
+  <si>
+    <t>[In Appendix C: Product Behavior] Implementation does support the RoleMember element. (Exchange 2016 follow this behavior.)</t>
+  </si>
+  <si>
+    <t>[In Appendix C: Product Behavior] Implementation does not support the Network element. (&lt;4&gt; Section 3.1.4.2.3.3:  Exchange 2007, Exchange 2010, and Exchange 2013 do not support the Network element.)</t>
+  </si>
+  <si>
+    <t>[In Appendix C: Product Behavior] Implementation does support the Network element. (Exchange 2016 follow this behavior.)</t>
+  </si>
+  <si>
+    <t>MS-OXWSSYNC_R37811009</t>
+  </si>
+  <si>
+    <t>MS-OXWSSYNC_R37811010</t>
+  </si>
+  <si>
+    <t>MS-OXWSSYNC_R37811011</t>
+  </si>
+  <si>
+    <t>MS-OXWSSYNC_R37811012</t>
+  </si>
+  <si>
+    <t>Verified by derived requirement: MS-OXWSSYNC_R37811010.</t>
+  </si>
+  <si>
+    <t>MS-OXWSSYNC_R1752001:i</t>
+  </si>
+  <si>
+    <t>MS-OXWSSYNC_R1752003:i</t>
+  </si>
+  <si>
+    <t>Verified by derived requirement: MS-OXWSSYNC_R37811012.</t>
+  </si>
 </sst>
 </file>
 
@@ -4382,7 +4418,515 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="37">
+  <dxfs count="117">
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -4702,110 +5246,6 @@
         <scheme val="none"/>
       </font>
     </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -4935,34 +5375,34 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Requirement" displayName="Requirement" ref="A19:I384" tableType="xml" totalsRowShown="0" headerRowDxfId="16" dataDxfId="15" connectionId="1">
-  <autoFilter ref="A19:I384"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Requirement" displayName="Requirement" ref="A19:I388" tableType="xml" totalsRowShown="0" headerRowDxfId="116" dataDxfId="115" connectionId="1">
+  <autoFilter ref="A19:I388"/>
   <tableColumns count="9">
-    <tableColumn id="1" uniqueName="ns1:REQ_ID" name="Req ID" dataDxfId="14">
+    <tableColumn id="1" uniqueName="ns1:REQ_ID" name="Req ID" dataDxfId="114">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:REQ_ID" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="2" uniqueName="ns1:Doc_Sect" name="Doc Sect" dataDxfId="13">
+    <tableColumn id="2" uniqueName="ns1:Doc_Sect" name="Doc Sect" dataDxfId="113">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Doc_Sect" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="3" uniqueName="ns1:Description" name="Description" dataDxfId="12">
+    <tableColumn id="3" uniqueName="ns1:Description" name="Description" dataDxfId="112">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Description" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="18" uniqueName="ns1:Derived" name="Derived" dataDxfId="11">
+    <tableColumn id="18" uniqueName="ns1:Derived" name="Derived" dataDxfId="111">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Derived" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="6" uniqueName="ns1:Behavior" name="Behavior" dataDxfId="10">
+    <tableColumn id="6" uniqueName="ns1:Behavior" name="Behavior" dataDxfId="110">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Behavior" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="7" uniqueName="ns1:Scope" name="Scope" dataDxfId="9">
+    <tableColumn id="7" uniqueName="ns1:Scope" name="Scope" dataDxfId="109">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Scope" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="9" uniqueName="ns1:IsNormative" name="Informative_x000a_/Normative" dataDxfId="8">
+    <tableColumn id="9" uniqueName="ns1:IsNormative" name="Informative_x000a_/Normative" dataDxfId="108">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:IsNormative" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="10" uniqueName="ns1:Verification" name="Verification" dataDxfId="7">
+    <tableColumn id="10" uniqueName="ns1:Verification" name="Verification" dataDxfId="107">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Verification" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="8" uniqueName="ns1:VerificationComment" name="Verification Comment" dataDxfId="6">
+    <tableColumn id="8" uniqueName="ns1:VerificationComment" name="Verification Comment" dataDxfId="106">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:VerificationComment" xmlDataType="string"/>
     </tableColumn>
   </tableColumns>
@@ -4971,12 +5411,12 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Scope" displayName="Scope" ref="A12:C15" totalsRowShown="0" headerRowBorderDxfId="5" tableBorderDxfId="4" totalsRowBorderDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Scope" displayName="Scope" ref="A12:C15" totalsRowShown="0" headerRowBorderDxfId="105" tableBorderDxfId="104" totalsRowBorderDxfId="103">
   <autoFilter ref="A12:C15"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="Scope" dataDxfId="2"/>
-    <tableColumn id="2" name="Test" dataDxfId="1"/>
-    <tableColumn id="3" name="Description" dataDxfId="0"/>
+    <tableColumn id="1" name="Scope" dataDxfId="102"/>
+    <tableColumn id="2" name="Test" dataDxfId="101"/>
+    <tableColumn id="3" name="Description" dataDxfId="100"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5270,10 +5710,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:M386"/>
+  <dimension ref="A1:M390"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A350" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C354" sqref="C354"/>
+    <sheetView tabSelected="1" topLeftCell="D265" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I266" sqref="I266"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -11762,7 +12202,7 @@
       </c>
       <c r="I263" s="27"/>
     </row>
-    <row r="264" spans="1:9" ht="30">
+    <row r="264" spans="1:9" ht="45">
       <c r="A264" s="18" t="s">
         <v>817</v>
       </c>
@@ -11783,9 +12223,11 @@
         <v>15</v>
       </c>
       <c r="H264" s="46" t="s">
-        <v>18</v>
-      </c>
-      <c r="I264" s="48"/>
+        <v>17</v>
+      </c>
+      <c r="I264" s="48" t="s">
+        <v>895</v>
+      </c>
     </row>
     <row r="265" spans="1:9" ht="30">
       <c r="A265" s="18" t="s">
@@ -11812,7 +12254,7 @@
       </c>
       <c r="I265" s="48"/>
     </row>
-    <row r="266" spans="1:9" ht="30">
+    <row r="266" spans="1:9" ht="45">
       <c r="A266" s="18" t="s">
         <v>819</v>
       </c>
@@ -11833,9 +12275,11 @@
         <v>15</v>
       </c>
       <c r="H266" s="46" t="s">
-        <v>18</v>
-      </c>
-      <c r="I266" s="48"/>
+        <v>17</v>
+      </c>
+      <c r="I266" s="48" t="s">
+        <v>898</v>
+      </c>
     </row>
     <row r="267" spans="1:9" ht="30">
       <c r="A267" s="18" t="s">
@@ -14173,16 +14617,16 @@
     </row>
     <row r="357" spans="1:9" ht="45">
       <c r="A357" s="18" t="s">
-        <v>857</v>
+        <v>891</v>
       </c>
       <c r="B357" s="47" t="s">
         <v>428</v>
       </c>
       <c r="C357" s="48" t="s">
-        <v>882</v>
+        <v>887</v>
       </c>
       <c r="D357" s="46" t="s">
-        <v>864</v>
+        <v>896</v>
       </c>
       <c r="E357" s="25" t="s">
         <v>22</v>
@@ -14200,16 +14644,16 @@
     </row>
     <row r="358" spans="1:9" ht="45">
       <c r="A358" s="18" t="s">
-        <v>858</v>
+        <v>892</v>
       </c>
       <c r="B358" s="47" t="s">
         <v>428</v>
       </c>
       <c r="C358" s="48" t="s">
-        <v>883</v>
+        <v>888</v>
       </c>
       <c r="D358" s="46" t="s">
-        <v>864</v>
+        <v>896</v>
       </c>
       <c r="E358" s="25" t="s">
         <v>22</v>
@@ -14227,24 +14671,24 @@
         <v>690</v>
       </c>
     </row>
-    <row r="359" spans="1:9" ht="30">
+    <row r="359" spans="1:9" ht="45">
       <c r="A359" s="18" t="s">
-        <v>859</v>
+        <v>893</v>
       </c>
       <c r="B359" s="47" t="s">
         <v>428</v>
       </c>
       <c r="C359" s="48" t="s">
-        <v>884</v>
+        <v>889</v>
       </c>
       <c r="D359" s="46" t="s">
-        <v>865</v>
+        <v>897</v>
       </c>
       <c r="E359" s="25" t="s">
         <v>22</v>
       </c>
       <c r="F359" s="46" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="G359" s="46" t="s">
         <v>15</v>
@@ -14256,22 +14700,22 @@
     </row>
     <row r="360" spans="1:9" ht="45">
       <c r="A360" s="18" t="s">
-        <v>860</v>
+        <v>894</v>
       </c>
       <c r="B360" s="47" t="s">
         <v>428</v>
       </c>
       <c r="C360" s="48" t="s">
-        <v>885</v>
+        <v>890</v>
       </c>
       <c r="D360" s="46" t="s">
-        <v>865</v>
+        <v>897</v>
       </c>
       <c r="E360" s="25" t="s">
         <v>22</v>
       </c>
       <c r="F360" s="46" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="G360" s="46" t="s">
         <v>15</v>
@@ -14283,125 +14727,131 @@
         <v>690</v>
       </c>
     </row>
-    <row r="361" spans="1:9" ht="75">
-      <c r="A361" s="25" t="s">
-        <v>365</v>
-      </c>
-      <c r="B361" s="26" t="s">
-        <v>429</v>
-      </c>
-      <c r="C361" s="27" t="s">
-        <v>642</v>
-      </c>
-      <c r="D361" s="25"/>
+    <row r="361" spans="1:9" ht="45">
+      <c r="A361" s="18" t="s">
+        <v>857</v>
+      </c>
+      <c r="B361" s="47" t="s">
+        <v>428</v>
+      </c>
+      <c r="C361" s="48" t="s">
+        <v>882</v>
+      </c>
+      <c r="D361" s="46" t="s">
+        <v>864</v>
+      </c>
       <c r="E361" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="F361" s="25" t="s">
-        <v>6</v>
-      </c>
-      <c r="G361" s="25" t="s">
-        <v>15</v>
-      </c>
-      <c r="H361" s="25" t="s">
-        <v>17</v>
-      </c>
-      <c r="I361" s="27" t="s">
-        <v>688</v>
-      </c>
+      <c r="F361" s="46" t="s">
+        <v>6</v>
+      </c>
+      <c r="G361" s="46" t="s">
+        <v>15</v>
+      </c>
+      <c r="H361" s="46" t="s">
+        <v>18</v>
+      </c>
+      <c r="I361" s="48"/>
     </row>
     <row r="362" spans="1:9" ht="45">
-      <c r="A362" s="25" t="s">
-        <v>366</v>
-      </c>
-      <c r="B362" s="26" t="s">
-        <v>430</v>
-      </c>
-      <c r="C362" s="16" t="s">
-        <v>876</v>
-      </c>
-      <c r="D362" s="25"/>
+      <c r="A362" s="18" t="s">
+        <v>858</v>
+      </c>
+      <c r="B362" s="47" t="s">
+        <v>428</v>
+      </c>
+      <c r="C362" s="48" t="s">
+        <v>883</v>
+      </c>
+      <c r="D362" s="46" t="s">
+        <v>864</v>
+      </c>
       <c r="E362" s="25" t="s">
-        <v>19</v>
-      </c>
-      <c r="F362" s="25" t="s">
+        <v>22</v>
+      </c>
+      <c r="F362" s="46" t="s">
+        <v>6</v>
+      </c>
+      <c r="G362" s="46" t="s">
+        <v>15</v>
+      </c>
+      <c r="H362" s="46" t="s">
+        <v>20</v>
+      </c>
+      <c r="I362" s="27" t="s">
+        <v>690</v>
+      </c>
+    </row>
+    <row r="363" spans="1:9" ht="30">
+      <c r="A363" s="18" t="s">
+        <v>859</v>
+      </c>
+      <c r="B363" s="47" t="s">
+        <v>428</v>
+      </c>
+      <c r="C363" s="48" t="s">
+        <v>884</v>
+      </c>
+      <c r="D363" s="46" t="s">
+        <v>865</v>
+      </c>
+      <c r="E363" s="25" t="s">
+        <v>22</v>
+      </c>
+      <c r="F363" s="46" t="s">
         <v>3</v>
       </c>
-      <c r="G362" s="25" t="s">
-        <v>15</v>
-      </c>
-      <c r="H362" s="25" t="s">
-        <v>17</v>
-      </c>
-      <c r="I362" s="27" t="s">
-        <v>691</v>
-      </c>
-    </row>
-    <row r="363" spans="1:9" ht="30">
-      <c r="A363" s="25" t="s">
-        <v>367</v>
-      </c>
-      <c r="B363" s="26" t="s">
-        <v>430</v>
-      </c>
-      <c r="C363" s="27" t="s">
-        <v>643</v>
-      </c>
-      <c r="D363" s="25"/>
-      <c r="E363" s="25" t="s">
-        <v>19</v>
-      </c>
-      <c r="F363" s="25" t="s">
+      <c r="G363" s="46" t="s">
+        <v>15</v>
+      </c>
+      <c r="H363" s="46" t="s">
+        <v>18</v>
+      </c>
+      <c r="I363" s="48"/>
+    </row>
+    <row r="364" spans="1:9" ht="45">
+      <c r="A364" s="18" t="s">
+        <v>860</v>
+      </c>
+      <c r="B364" s="47" t="s">
+        <v>428</v>
+      </c>
+      <c r="C364" s="48" t="s">
+        <v>885</v>
+      </c>
+      <c r="D364" s="46" t="s">
+        <v>865</v>
+      </c>
+      <c r="E364" s="25" t="s">
+        <v>22</v>
+      </c>
+      <c r="F364" s="46" t="s">
         <v>3</v>
       </c>
-      <c r="G363" s="25" t="s">
-        <v>15</v>
-      </c>
-      <c r="H363" s="25" t="s">
-        <v>17</v>
-      </c>
-      <c r="I363" s="27"/>
-    </row>
-    <row r="364" spans="1:9" ht="60">
-      <c r="A364" s="25" t="s">
-        <v>368</v>
-      </c>
-      <c r="B364" s="26" t="s">
-        <v>430</v>
-      </c>
-      <c r="C364" s="27" t="s">
-        <v>644</v>
-      </c>
-      <c r="D364" s="25"/>
-      <c r="E364" s="25" t="s">
-        <v>19</v>
-      </c>
-      <c r="F364" s="25" t="s">
-        <v>3</v>
-      </c>
-      <c r="G364" s="25" t="s">
-        <v>15</v>
-      </c>
-      <c r="H364" s="25" t="s">
-        <v>17</v>
+      <c r="G364" s="46" t="s">
+        <v>15</v>
+      </c>
+      <c r="H364" s="46" t="s">
+        <v>20</v>
       </c>
       <c r="I364" s="27" t="s">
-        <v>692</v>
-      </c>
-    </row>
-    <row r="365" spans="1:9" ht="409.5">
+        <v>690</v>
+      </c>
+    </row>
+    <row r="365" spans="1:9" ht="75">
       <c r="A365" s="25" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
       <c r="B365" s="26" t="s">
-        <v>431</v>
-      </c>
-      <c r="C365" s="28" t="s">
-        <v>701</v>
+        <v>429</v>
+      </c>
+      <c r="C365" s="27" t="s">
+        <v>642</v>
       </c>
       <c r="D365" s="25"/>
       <c r="E365" s="25" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="F365" s="25" t="s">
         <v>6</v>
@@ -14410,19 +14860,21 @@
         <v>15</v>
       </c>
       <c r="H365" s="25" t="s">
-        <v>21</v>
-      </c>
-      <c r="I365" s="27"/>
-    </row>
-    <row r="366" spans="1:9" ht="30">
+        <v>17</v>
+      </c>
+      <c r="I365" s="27" t="s">
+        <v>688</v>
+      </c>
+    </row>
+    <row r="366" spans="1:9" ht="45">
       <c r="A366" s="25" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
       <c r="B366" s="26" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="C366" s="16" t="s">
-        <v>699</v>
+        <v>876</v>
       </c>
       <c r="D366" s="25"/>
       <c r="E366" s="25" t="s">
@@ -14435,19 +14887,21 @@
         <v>15</v>
       </c>
       <c r="H366" s="25" t="s">
-        <v>20</v>
-      </c>
-      <c r="I366" s="27"/>
+        <v>17</v>
+      </c>
+      <c r="I366" s="27" t="s">
+        <v>691</v>
+      </c>
     </row>
     <row r="367" spans="1:9" ht="30">
       <c r="A367" s="25" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
       <c r="B367" s="26" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="C367" s="27" t="s">
-        <v>645</v>
+        <v>643</v>
       </c>
       <c r="D367" s="25"/>
       <c r="E367" s="25" t="s">
@@ -14460,44 +14914,46 @@
         <v>15</v>
       </c>
       <c r="H367" s="25" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="I367" s="27"/>
     </row>
-    <row r="368" spans="1:9" ht="409.5">
+    <row r="368" spans="1:9" ht="60">
       <c r="A368" s="25" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
       <c r="B368" s="26" t="s">
-        <v>432</v>
-      </c>
-      <c r="C368" s="28" t="s">
-        <v>700</v>
+        <v>430</v>
+      </c>
+      <c r="C368" s="27" t="s">
+        <v>644</v>
       </c>
       <c r="D368" s="25"/>
       <c r="E368" s="25" t="s">
         <v>19</v>
       </c>
       <c r="F368" s="25" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="G368" s="25" t="s">
         <v>15</v>
       </c>
       <c r="H368" s="25" t="s">
-        <v>21</v>
-      </c>
-      <c r="I368" s="27"/>
-    </row>
-    <row r="369" spans="1:9" ht="30">
+        <v>17</v>
+      </c>
+      <c r="I368" s="27" t="s">
+        <v>692</v>
+      </c>
+    </row>
+    <row r="369" spans="1:9" ht="409.5">
       <c r="A369" s="25" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="B369" s="26" t="s">
-        <v>433</v>
-      </c>
-      <c r="C369" s="27" t="s">
-        <v>646</v>
+        <v>431</v>
+      </c>
+      <c r="C369" s="28" t="s">
+        <v>701</v>
       </c>
       <c r="D369" s="25"/>
       <c r="E369" s="25" t="s">
@@ -14514,65 +14970,65 @@
       </c>
       <c r="I369" s="27"/>
     </row>
-    <row r="370" spans="1:9" ht="135">
+    <row r="370" spans="1:9" ht="30">
       <c r="A370" s="25" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="B370" s="26" t="s">
-        <v>433</v>
-      </c>
-      <c r="C370" s="27" t="s">
-        <v>647</v>
+        <v>431</v>
+      </c>
+      <c r="C370" s="16" t="s">
+        <v>699</v>
       </c>
       <c r="D370" s="25"/>
       <c r="E370" s="25" t="s">
         <v>19</v>
       </c>
       <c r="F370" s="25" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="G370" s="25" t="s">
         <v>15</v>
       </c>
       <c r="H370" s="25" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I370" s="27"/>
     </row>
     <row r="371" spans="1:9" ht="30">
       <c r="A371" s="25" t="s">
-        <v>375</v>
+        <v>371</v>
       </c>
       <c r="B371" s="26" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="C371" s="27" t="s">
-        <v>648</v>
+        <v>645</v>
       </c>
       <c r="D371" s="25"/>
       <c r="E371" s="25" t="s">
         <v>19</v>
       </c>
       <c r="F371" s="25" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="G371" s="25" t="s">
         <v>15</v>
       </c>
       <c r="H371" s="25" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I371" s="27"/>
     </row>
-    <row r="372" spans="1:9" ht="255">
+    <row r="372" spans="1:9" ht="409.5">
       <c r="A372" s="25" t="s">
-        <v>376</v>
+        <v>372</v>
       </c>
       <c r="B372" s="26" t="s">
-        <v>434</v>
-      </c>
-      <c r="C372" s="27" t="s">
-        <v>649</v>
+        <v>432</v>
+      </c>
+      <c r="C372" s="28" t="s">
+        <v>700</v>
       </c>
       <c r="D372" s="25"/>
       <c r="E372" s="25" t="s">
@@ -14589,69 +15045,65 @@
       </c>
       <c r="I372" s="27"/>
     </row>
-    <row r="373" spans="1:9" ht="45">
+    <row r="373" spans="1:9" ht="30">
       <c r="A373" s="25" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
       <c r="B373" s="26" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="C373" s="27" t="s">
-        <v>650</v>
+        <v>646</v>
       </c>
       <c r="D373" s="25"/>
       <c r="E373" s="25" t="s">
         <v>19</v>
       </c>
       <c r="F373" s="25" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="G373" s="25" t="s">
         <v>15</v>
       </c>
       <c r="H373" s="25" t="s">
-        <v>17</v>
-      </c>
-      <c r="I373" s="27" t="s">
-        <v>693</v>
-      </c>
-    </row>
-    <row r="374" spans="1:9" ht="45">
+        <v>21</v>
+      </c>
+      <c r="I373" s="27"/>
+    </row>
+    <row r="374" spans="1:9" ht="135">
       <c r="A374" s="25" t="s">
-        <v>378</v>
+        <v>374</v>
       </c>
       <c r="B374" s="26" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="C374" s="27" t="s">
-        <v>651</v>
+        <v>647</v>
       </c>
       <c r="D374" s="25"/>
       <c r="E374" s="25" t="s">
         <v>19</v>
       </c>
       <c r="F374" s="25" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="G374" s="25" t="s">
         <v>15</v>
       </c>
       <c r="H374" s="25" t="s">
-        <v>17</v>
-      </c>
-      <c r="I374" s="16" t="s">
-        <v>702</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="I374" s="27"/>
     </row>
     <row r="375" spans="1:9" ht="30">
       <c r="A375" s="25" t="s">
-        <v>379</v>
+        <v>375</v>
       </c>
       <c r="B375" s="26" t="s">
-        <v>436</v>
-      </c>
-      <c r="C375" s="16" t="s">
-        <v>877</v>
+        <v>433</v>
+      </c>
+      <c r="C375" s="27" t="s">
+        <v>648</v>
       </c>
       <c r="D375" s="25"/>
       <c r="E375" s="25" t="s">
@@ -14664,44 +15116,44 @@
         <v>15</v>
       </c>
       <c r="H375" s="25" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="I375" s="27"/>
     </row>
-    <row r="376" spans="1:9" ht="45">
+    <row r="376" spans="1:9" ht="255">
       <c r="A376" s="25" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
       <c r="B376" s="26" t="s">
-        <v>436</v>
-      </c>
-      <c r="C376" s="16" t="s">
-        <v>652</v>
+        <v>434</v>
+      </c>
+      <c r="C376" s="27" t="s">
+        <v>649</v>
       </c>
       <c r="D376" s="25"/>
       <c r="E376" s="25" t="s">
         <v>19</v>
       </c>
       <c r="F376" s="25" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="G376" s="25" t="s">
         <v>15</v>
       </c>
       <c r="H376" s="25" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="I376" s="27"/>
     </row>
     <row r="377" spans="1:9" ht="45">
       <c r="A377" s="25" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
       <c r="B377" s="26" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="C377" s="27" t="s">
-        <v>653</v>
+        <v>650</v>
       </c>
       <c r="D377" s="25"/>
       <c r="E377" s="25" t="s">
@@ -14717,18 +15169,18 @@
         <v>17</v>
       </c>
       <c r="I377" s="27" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
     </row>
     <row r="378" spans="1:9" ht="45">
       <c r="A378" s="25" t="s">
-        <v>382</v>
+        <v>378</v>
       </c>
       <c r="B378" s="26" t="s">
         <v>436</v>
       </c>
       <c r="C378" s="27" t="s">
-        <v>654</v>
+        <v>651</v>
       </c>
       <c r="D378" s="25"/>
       <c r="E378" s="25" t="s">
@@ -14743,26 +15195,26 @@
       <c r="H378" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="I378" s="27" t="s">
-        <v>695</v>
-      </c>
-    </row>
-    <row r="379" spans="1:9" ht="60">
+      <c r="I378" s="16" t="s">
+        <v>702</v>
+      </c>
+    </row>
+    <row r="379" spans="1:9" ht="30">
       <c r="A379" s="25" t="s">
-        <v>383</v>
+        <v>379</v>
       </c>
       <c r="B379" s="26" t="s">
-        <v>437</v>
-      </c>
-      <c r="C379" s="27" t="s">
-        <v>655</v>
+        <v>436</v>
+      </c>
+      <c r="C379" s="16" t="s">
+        <v>877</v>
       </c>
       <c r="D379" s="25"/>
       <c r="E379" s="25" t="s">
         <v>19</v>
       </c>
       <c r="F379" s="25" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="G379" s="25" t="s">
         <v>15</v>
@@ -14770,144 +15222,248 @@
       <c r="H379" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="I379" s="27" t="s">
-        <v>696</v>
-      </c>
-    </row>
-    <row r="380" spans="1:9" ht="30">
+      <c r="I379" s="27"/>
+    </row>
+    <row r="380" spans="1:9" ht="45">
       <c r="A380" s="25" t="s">
-        <v>384</v>
+        <v>380</v>
       </c>
       <c r="B380" s="26" t="s">
-        <v>438</v>
-      </c>
-      <c r="C380" s="27" t="s">
-        <v>656</v>
+        <v>436</v>
+      </c>
+      <c r="C380" s="16" t="s">
+        <v>652</v>
       </c>
       <c r="D380" s="25"/>
       <c r="E380" s="25" t="s">
         <v>19</v>
       </c>
       <c r="F380" s="25" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="G380" s="25" t="s">
         <v>15</v>
       </c>
       <c r="H380" s="25" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="I380" s="27"/>
     </row>
-    <row r="381" spans="1:9" ht="409.5">
+    <row r="381" spans="1:9" ht="45">
       <c r="A381" s="25" t="s">
-        <v>385</v>
+        <v>381</v>
       </c>
       <c r="B381" s="26" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="C381" s="27" t="s">
-        <v>657</v>
+        <v>653</v>
       </c>
       <c r="D381" s="25"/>
       <c r="E381" s="25" t="s">
         <v>19</v>
       </c>
       <c r="F381" s="25" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="G381" s="25" t="s">
         <v>15</v>
       </c>
       <c r="H381" s="25" t="s">
-        <v>21</v>
-      </c>
-      <c r="I381" s="27"/>
-    </row>
-    <row r="382" spans="1:9" ht="60">
+        <v>17</v>
+      </c>
+      <c r="I381" s="27" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="382" spans="1:9" ht="45">
       <c r="A382" s="25" t="s">
-        <v>386</v>
+        <v>382</v>
       </c>
       <c r="B382" s="26" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="C382" s="27" t="s">
-        <v>658</v>
+        <v>654</v>
       </c>
       <c r="D382" s="25"/>
       <c r="E382" s="25" t="s">
         <v>19</v>
       </c>
       <c r="F382" s="25" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="G382" s="25" t="s">
         <v>15</v>
       </c>
       <c r="H382" s="25" t="s">
-        <v>21</v>
-      </c>
-      <c r="I382" s="27"/>
-    </row>
-    <row r="383" spans="1:9" ht="360">
+        <v>17</v>
+      </c>
+      <c r="I382" s="27" t="s">
+        <v>695</v>
+      </c>
+    </row>
+    <row r="383" spans="1:9" ht="60">
       <c r="A383" s="25" t="s">
-        <v>387</v>
+        <v>383</v>
       </c>
       <c r="B383" s="26" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="C383" s="27" t="s">
-        <v>659</v>
+        <v>655</v>
       </c>
       <c r="D383" s="25"/>
       <c r="E383" s="25" t="s">
         <v>19</v>
       </c>
       <c r="F383" s="25" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="G383" s="25" t="s">
         <v>15</v>
       </c>
       <c r="H383" s="25" t="s">
+        <v>17</v>
+      </c>
+      <c r="I383" s="27" t="s">
+        <v>696</v>
+      </c>
+    </row>
+    <row r="384" spans="1:9" ht="30">
+      <c r="A384" s="25" t="s">
+        <v>384</v>
+      </c>
+      <c r="B384" s="26" t="s">
+        <v>438</v>
+      </c>
+      <c r="C384" s="27" t="s">
+        <v>656</v>
+      </c>
+      <c r="D384" s="25"/>
+      <c r="E384" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="F384" s="25" t="s">
+        <v>6</v>
+      </c>
+      <c r="G384" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="H384" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="I383" s="27"/>
-    </row>
-    <row r="384" spans="1:9" ht="45">
-      <c r="A384" s="25" t="s">
+      <c r="I384" s="27"/>
+    </row>
+    <row r="385" spans="1:9" ht="409.5">
+      <c r="A385" s="25" t="s">
+        <v>385</v>
+      </c>
+      <c r="B385" s="26" t="s">
+        <v>438</v>
+      </c>
+      <c r="C385" s="27" t="s">
+        <v>657</v>
+      </c>
+      <c r="D385" s="25"/>
+      <c r="E385" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="F385" s="25" t="s">
+        <v>6</v>
+      </c>
+      <c r="G385" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="H385" s="25" t="s">
+        <v>21</v>
+      </c>
+      <c r="I385" s="27"/>
+    </row>
+    <row r="386" spans="1:9" ht="60">
+      <c r="A386" s="25" t="s">
+        <v>386</v>
+      </c>
+      <c r="B386" s="26" t="s">
+        <v>438</v>
+      </c>
+      <c r="C386" s="27" t="s">
+        <v>658</v>
+      </c>
+      <c r="D386" s="25"/>
+      <c r="E386" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="F386" s="25" t="s">
+        <v>6</v>
+      </c>
+      <c r="G386" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="H386" s="25" t="s">
+        <v>21</v>
+      </c>
+      <c r="I386" s="27"/>
+    </row>
+    <row r="387" spans="1:9" ht="360">
+      <c r="A387" s="25" t="s">
+        <v>387</v>
+      </c>
+      <c r="B387" s="26" t="s">
+        <v>439</v>
+      </c>
+      <c r="C387" s="27" t="s">
+        <v>659</v>
+      </c>
+      <c r="D387" s="25"/>
+      <c r="E387" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="F387" s="25" t="s">
+        <v>6</v>
+      </c>
+      <c r="G387" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="H387" s="25" t="s">
+        <v>21</v>
+      </c>
+      <c r="I387" s="27"/>
+    </row>
+    <row r="388" spans="1:9" ht="45">
+      <c r="A388" s="25" t="s">
         <v>388</v>
       </c>
-      <c r="B384" s="26" t="s">
+      <c r="B388" s="26" t="s">
         <v>428</v>
       </c>
-      <c r="C384" s="27" t="s">
+      <c r="C388" s="27" t="s">
         <v>660</v>
       </c>
-      <c r="D384" s="25" t="s">
+      <c r="D388" s="25" t="s">
         <v>686</v>
       </c>
-      <c r="E384" s="25" t="s">
+      <c r="E388" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="F384" s="25" t="s">
-        <v>6</v>
-      </c>
-      <c r="G384" s="25" t="s">
-        <v>15</v>
-      </c>
-      <c r="H384" s="25" t="s">
-        <v>18</v>
-      </c>
-      <c r="I384" s="27"/>
-    </row>
-    <row r="385" spans="1:2">
-      <c r="A385" s="3"/>
-      <c r="B385" s="9"/>
-    </row>
-    <row r="386" spans="1:2">
-      <c r="A386" s="3"/>
-      <c r="B386" s="9"/>
+      <c r="F388" s="25" t="s">
+        <v>6</v>
+      </c>
+      <c r="G388" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="H388" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="I388" s="27"/>
+    </row>
+    <row r="389" spans="1:9">
+      <c r="A389" s="3"/>
+      <c r="B389" s="9"/>
+    </row>
+    <row r="390" spans="1:9">
+      <c r="A390" s="3"/>
+      <c r="B390" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="11">
@@ -14924,95 +15480,95 @@
     <mergeCell ref="B17:I17"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="A365:B365 A368:B368 A366:I367 D365:I365 A369:I384 D368:I368 I357:I384 A20:I364">
-    <cfRule type="expression" dxfId="36" priority="77">
+  <conditionalFormatting sqref="A369:B369 A372:B372 A370:I371 D369:I369 A373:I388 D372:I372 I361:I388 A20:I368">
+    <cfRule type="expression" dxfId="99" priority="77">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="35" priority="78">
+    <cfRule type="expression" dxfId="98" priority="78">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="34" priority="85">
+    <cfRule type="expression" dxfId="97" priority="85">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A365:B365 A368:B368 A366:I367 D365:I365 A369:I384 D368:I368 I357:I384 A20:I364">
-    <cfRule type="expression" dxfId="33" priority="31">
+  <conditionalFormatting sqref="A369:B369 A372:B372 A370:I371 D369:I369 A373:I388 D372:I372 I361:I388 A20:I368">
+    <cfRule type="expression" dxfId="96" priority="31">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="32" priority="32">
+    <cfRule type="expression" dxfId="95" priority="32">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="31" priority="33">
+    <cfRule type="expression" dxfId="94" priority="33">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F20:F384">
-    <cfRule type="expression" dxfId="30" priority="37">
+  <conditionalFormatting sqref="F20:F388">
+    <cfRule type="expression" dxfId="93" priority="37">
       <formula>NOT(VLOOKUP(F20,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="29" priority="38">
+    <cfRule type="expression" dxfId="92" priority="38">
       <formula>(VLOOKUP(F20,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C368">
-    <cfRule type="expression" dxfId="28" priority="10">
+  <conditionalFormatting sqref="C372">
+    <cfRule type="expression" dxfId="91" priority="10">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="27" priority="11">
+    <cfRule type="expression" dxfId="90" priority="11">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="26" priority="12">
+    <cfRule type="expression" dxfId="89" priority="12">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C368">
-    <cfRule type="expression" dxfId="25" priority="7">
+  <conditionalFormatting sqref="C372">
+    <cfRule type="expression" dxfId="88" priority="7">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="24" priority="8">
+    <cfRule type="expression" dxfId="87" priority="8">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="23" priority="9">
+    <cfRule type="expression" dxfId="86" priority="9">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C365">
-    <cfRule type="expression" dxfId="22" priority="4">
+  <conditionalFormatting sqref="C369">
+    <cfRule type="expression" dxfId="85" priority="4">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="21" priority="5">
+    <cfRule type="expression" dxfId="84" priority="5">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="20" priority="6">
+    <cfRule type="expression" dxfId="83" priority="6">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C365">
-    <cfRule type="expression" dxfId="19" priority="1">
+  <conditionalFormatting sqref="C369">
+    <cfRule type="expression" dxfId="82" priority="1">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="18" priority="2">
+    <cfRule type="expression" dxfId="81" priority="2">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="17" priority="3">
+    <cfRule type="expression" dxfId="80" priority="3">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="6">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G4 F20:F384">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G4 F20:F388">
       <formula1>$A$13:$A$15</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F4 E20:E384">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F4 E20:E388">
       <formula1>"Protocol,Product"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H4 G20:G384">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H4 G20:G388">
       <formula1>"Informative,Normative"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B13:B15">
       <formula1>"In, Out"</formula1>
     </dataValidation>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H20:H384">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H20:H388">
       <formula1>"Non-testable, Unverified, Adapter, Test Case"</formula1>
     </dataValidation>
   </dataValidations>
@@ -15022,7 +15578,7 @@
     <oddFooter>&amp;F&amp;RPage &amp;P</oddFooter>
   </headerFooter>
   <ignoredErrors>
-    <ignoredError sqref="B1:B9 B10:B46 B108:B109 B47:B103 B178:B211 B361:B386 B340:B352" numberStoredAsText="1"/>
+    <ignoredError sqref="B1:B9 B10:B46 B108:B109 B47:B103 B178:B211 B365:B390 B340:B352" numberStoredAsText="1"/>
   </ignoredErrors>
   <tableParts count="2">
     <tablePart r:id="rId2"/>
@@ -15032,6 +15588,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F2EA47BB262D974097182E2CA8AB13E1" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="74597e8d9e42e7e4fc8eda6d37675aa2">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4aeb20c0e3442673af7ee10786458764">
     <xsd:element name="properties">
@@ -15080,32 +15651,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EDB2DE12-5EF6-4CF2-820D-5F9FE329E08E}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6D33261-F3C6-4621-88F1-D76E5ABE1865}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/internal/2005/internalDocumentation"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -15125,9 +15674,16 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6D33261-F3C6-4621-88F1-D76E5ABE1865}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EDB2DE12-5EF6-4CF2-820D-5F9FE329E08E}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/internal/2005/internalDocumentation"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Fix watchman issues for MS-OXWSSYNC.
</commit_message>
<xml_diff>
--- a/ExchangeWebServices/Docs/MS-OXWSSYNC/MS-OXWSSYNC_RequirementSpecification.xlsx
+++ b/ExchangeWebServices/Docs/MS-OXWSSYNC/MS-OXWSSYNC_RequirementSpecification.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="-15" yWindow="180" windowWidth="15405" windowHeight="6780" tabRatio="570"/>
@@ -15,7 +15,7 @@
     <definedName name="_xlnm.Print_Titles" localSheetId="0">Requirements!$A:$A,Requirements!$19:$19</definedName>
     <definedName name="ScopeList">Requirements!#REF!</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2711" uniqueCount="899">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2709" uniqueCount="898">
   <si>
     <t>Req ID</t>
   </si>
@@ -2671,9 +2671,6 @@
   </si>
   <si>
     <t>This requirement can be enabled/disabled in the deployment.ptfconfig file.</t>
-  </si>
-  <si>
-    <t>Verified by requirements: MS-OXWSSYNC_R2571, MS-OXWSSYNC_R3781.</t>
   </si>
   <si>
     <t>Verified by derived requirements: MS-OXWSSYNC_R2573, MS-OXWSSYNC_R3783.</t>
@@ -3503,12 +3500,6 @@
     <t xml:space="preserve">[In m:SyncFolderHierarchyResponseMessageType Complex Type] This element [IncludesLastFolderInRange] is optional. </t>
   </si>
   <si>
-    <t>Verified by derived requirements: MS-OXWSSYNC_R2601, MS-OXWSSYNC_R2602.</t>
-  </si>
-  <si>
-    <t>Verified by derived requirements: MS-OXWSSYNC_R2631, MS-OXWSSYNC_R2632.</t>
-  </si>
-  <si>
     <t>[In m:SyncFolderHierarchyResponseMessageType Complex Type] This element [Changes] is optional.</t>
   </si>
   <si>
@@ -3886,9 +3877,6 @@
     <t>MS-OXWSSYNC_R1752006:i</t>
   </si>
   <si>
-    <t>MS-OXWSSYNC_R39223:i, MS-OXWSSYNC_R39223:i</t>
-  </si>
-  <si>
     <t>Verified by derived requirements:MS-OXWSSYNC_R39223, MS-OXWSSYNC_R39224.</t>
   </si>
   <si>
@@ -3904,12 +3892,6 @@
     <t>Verified by derived requirement: MS-OXWSSYNC_R37811006.</t>
   </si>
   <si>
-    <t>Verified by derived requirements: MS-OXWSSYNC_R3861, MS-OXWSSYNC_R3862.</t>
-  </si>
-  <si>
-    <t>Verified by derived requirements: MS-OXWSSYNC_R3831, MS-OXWSSYNC_R3832.</t>
-  </si>
-  <si>
     <t>[In m:SyncFolderHierarchyType Complex Type] FolderShape element BaseShape, value=AllProperties, specifies all the properties that are defined for the item or folder.</t>
   </si>
   <si>
@@ -3986,12 +3968,27 @@
   </si>
   <si>
     <t>Verified by derived requirement: MS-OXWSSYNC_R37811012.</t>
+  </si>
+  <si>
+    <t>MS-OXWSSYNC_R39223:i, MS-OXWSSYNC_R39224:i</t>
+  </si>
+  <si>
+    <t>Verified by derived requirements: MS-OXWSSYNC_R2571, MS-OXWSSYNC_R3781.</t>
+  </si>
+  <si>
+    <t>Verified by derived requirements: MS-OXWSSYNC_R2572, MS-OXWSSYNC_R3782.</t>
+  </si>
+  <si>
+    <t>Verified by derived requirement: MS-OXWSSYNC_R3787.</t>
+  </si>
+  <si>
+    <t>Verified by derived requirement: MS-OXWSSYNC_R37801.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
     <numFmt numFmtId="165" formatCode="0.0.0"/>
@@ -4418,515 +4415,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="117">
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
+  <dxfs count="37">
     <dxf>
       <font>
         <b val="0"/>
@@ -5246,6 +4735,110 @@
         <scheme val="none"/>
       </font>
     </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -5375,34 +4968,34 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Requirement" displayName="Requirement" ref="A19:I388" tableType="xml" totalsRowShown="0" headerRowDxfId="116" dataDxfId="115" connectionId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Requirement" displayName="Requirement" ref="A19:I388" tableType="xml" totalsRowShown="0" headerRowDxfId="16" dataDxfId="15" connectionId="1">
   <autoFilter ref="A19:I388"/>
   <tableColumns count="9">
-    <tableColumn id="1" uniqueName="ns1:REQ_ID" name="Req ID" dataDxfId="114">
+    <tableColumn id="1" uniqueName="ns1:REQ_ID" name="Req ID" dataDxfId="14">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:REQ_ID" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="2" uniqueName="ns1:Doc_Sect" name="Doc Sect" dataDxfId="113">
+    <tableColumn id="2" uniqueName="ns1:Doc_Sect" name="Doc Sect" dataDxfId="13">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Doc_Sect" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="3" uniqueName="ns1:Description" name="Description" dataDxfId="112">
+    <tableColumn id="3" uniqueName="ns1:Description" name="Description" dataDxfId="12">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Description" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="18" uniqueName="ns1:Derived" name="Derived" dataDxfId="111">
+    <tableColumn id="18" uniqueName="ns1:Derived" name="Derived" dataDxfId="11">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Derived" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="6" uniqueName="ns1:Behavior" name="Behavior" dataDxfId="110">
+    <tableColumn id="6" uniqueName="ns1:Behavior" name="Behavior" dataDxfId="10">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Behavior" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="7" uniqueName="ns1:Scope" name="Scope" dataDxfId="109">
+    <tableColumn id="7" uniqueName="ns1:Scope" name="Scope" dataDxfId="9">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Scope" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="9" uniqueName="ns1:IsNormative" name="Informative_x000a_/Normative" dataDxfId="108">
+    <tableColumn id="9" uniqueName="ns1:IsNormative" name="Informative_x000a_/Normative" dataDxfId="8">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:IsNormative" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="10" uniqueName="ns1:Verification" name="Verification" dataDxfId="107">
+    <tableColumn id="10" uniqueName="ns1:Verification" name="Verification" dataDxfId="7">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Verification" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="8" uniqueName="ns1:VerificationComment" name="Verification Comment" dataDxfId="106">
+    <tableColumn id="8" uniqueName="ns1:VerificationComment" name="Verification Comment" dataDxfId="6">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:VerificationComment" xmlDataType="string"/>
     </tableColumn>
   </tableColumns>
@@ -5411,12 +5004,12 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Scope" displayName="Scope" ref="A12:C15" totalsRowShown="0" headerRowBorderDxfId="105" tableBorderDxfId="104" totalsRowBorderDxfId="103">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Scope" displayName="Scope" ref="A12:C15" totalsRowShown="0" headerRowBorderDxfId="5" tableBorderDxfId="4" totalsRowBorderDxfId="3">
   <autoFilter ref="A12:C15"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="Scope" dataDxfId="102"/>
-    <tableColumn id="2" name="Test" dataDxfId="101"/>
-    <tableColumn id="3" name="Description" dataDxfId="100"/>
+    <tableColumn id="1" name="Scope" dataDxfId="2"/>
+    <tableColumn id="2" name="Test" dataDxfId="1"/>
+    <tableColumn id="3" name="Description" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5465,7 +5058,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -5498,9 +5091,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -5533,6 +5143,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -5712,16 +5339,14 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:M390"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D265" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I266" sqref="I266"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="24.28515625" style="10" customWidth="1"/>
+    <col min="1" max="1" width="12.42578125" style="10" customWidth="1"/>
     <col min="2" max="2" width="13" style="3" customWidth="1"/>
     <col min="3" max="3" width="85" style="3" customWidth="1"/>
-    <col min="4" max="4" width="22" style="3" customWidth="1"/>
+    <col min="4" max="4" width="28.5703125" style="3" customWidth="1"/>
     <col min="5" max="5" width="12.42578125" style="3" customWidth="1"/>
     <col min="6" max="6" width="12.140625" style="3" customWidth="1"/>
     <col min="7" max="7" width="13.42578125" style="3" customWidth="1"/>
@@ -5733,7 +5358,7 @@
   <sheetData>
     <row r="1" spans="1:11">
       <c r="A1" s="1" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>27</v>
@@ -5745,7 +5370,7 @@
     </row>
     <row r="2" spans="1:11">
       <c r="A2" s="5" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="B2" s="6"/>
       <c r="C2" s="6"/>
@@ -5849,7 +5474,7 @@
         <v>1</v>
       </c>
       <c r="B8" s="57" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="C8" s="58"/>
       <c r="D8" s="58"/>
@@ -5900,7 +5525,7 @@
         <v>8</v>
       </c>
       <c r="B11" s="63" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="C11" s="64"/>
       <c r="D11" s="50"/>
@@ -6027,7 +5652,7 @@
         <v>5</v>
       </c>
       <c r="B18" s="49" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="C18" s="50"/>
       <c r="D18" s="50"/>
@@ -7105,7 +6730,7 @@
         <v>404</v>
       </c>
       <c r="C61" s="16" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="D61" s="25"/>
       <c r="E61" s="25" t="s">
@@ -7130,7 +6755,7 @@
         <v>404</v>
       </c>
       <c r="C62" s="16" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="D62" s="25"/>
       <c r="E62" s="25" t="s">
@@ -7180,7 +6805,7 @@
         <v>404</v>
       </c>
       <c r="C64" s="16" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="D64" s="25"/>
       <c r="E64" s="25" t="s">
@@ -7430,7 +7055,7 @@
         <v>31</v>
       </c>
       <c r="C74" s="16" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="D74" s="25"/>
       <c r="E74" s="25" t="s">
@@ -7455,7 +7080,7 @@
         <v>31</v>
       </c>
       <c r="C75" s="16" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="D75" s="25"/>
       <c r="E75" s="25" t="s">
@@ -7680,7 +7305,7 @@
         <v>407</v>
       </c>
       <c r="C84" s="16" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="D84" s="25"/>
       <c r="E84" s="25" t="s">
@@ -7730,7 +7355,7 @@
         <v>407</v>
       </c>
       <c r="C86" s="16" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
       <c r="D86" s="25"/>
       <c r="E86" s="25" t="s">
@@ -7805,7 +7430,7 @@
         <v>407</v>
       </c>
       <c r="C89" s="16" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
       <c r="D89" s="25"/>
       <c r="E89" s="25" t="s">
@@ -7980,7 +7605,7 @@
         <v>408</v>
       </c>
       <c r="C96" s="16" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="D96" s="25"/>
       <c r="E96" s="25" t="s">
@@ -8155,7 +7780,7 @@
         <v>412</v>
       </c>
       <c r="C103" s="16" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="D103" s="25"/>
       <c r="E103" s="25" t="s">
@@ -8255,7 +7880,7 @@
         <v>412</v>
       </c>
       <c r="C107" s="16" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
       <c r="D107" s="25"/>
       <c r="E107" s="25" t="s">
@@ -8305,7 +7930,7 @@
         <v>412</v>
       </c>
       <c r="C109" s="16" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
       <c r="D109" s="25"/>
       <c r="E109" s="25" t="s">
@@ -8355,7 +7980,7 @@
         <v>413</v>
       </c>
       <c r="C111" s="16" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="D111" s="25"/>
       <c r="E111" s="25" t="s">
@@ -8380,7 +8005,7 @@
         <v>413</v>
       </c>
       <c r="C112" s="16" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="D112" s="25"/>
       <c r="E112" s="25" t="s">
@@ -8480,7 +8105,7 @@
         <v>413</v>
       </c>
       <c r="C116" s="16" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="D116" s="25"/>
       <c r="E116" s="25" t="s">
@@ -8505,7 +8130,7 @@
         <v>413</v>
       </c>
       <c r="C117" s="16" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="D117" s="25"/>
       <c r="E117" s="25" t="s">
@@ -8521,7 +8146,7 @@
         <v>17</v>
       </c>
       <c r="I117" s="16" t="s">
-        <v>868</v>
+        <v>864</v>
       </c>
     </row>
     <row r="118" spans="1:9" ht="330">
@@ -8557,7 +8182,7 @@
         <v>414</v>
       </c>
       <c r="C119" s="16" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
       <c r="D119" s="25"/>
       <c r="E119" s="25" t="s">
@@ -8582,7 +8207,7 @@
         <v>414</v>
       </c>
       <c r="C120" s="16" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="D120" s="25"/>
       <c r="E120" s="25" t="s">
@@ -8607,7 +8232,7 @@
         <v>414</v>
       </c>
       <c r="C121" s="16" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="D121" s="25"/>
       <c r="E121" s="25" t="s">
@@ -8632,7 +8257,7 @@
         <v>414</v>
       </c>
       <c r="C122" s="16" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="D122" s="25"/>
       <c r="E122" s="25" t="s">
@@ -8657,7 +8282,7 @@
         <v>414</v>
       </c>
       <c r="C123" s="16" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="D123" s="25"/>
       <c r="E123" s="25" t="s">
@@ -8682,7 +8307,7 @@
         <v>414</v>
       </c>
       <c r="C124" s="16" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="D124" s="25"/>
       <c r="E124" s="25" t="s">
@@ -8707,7 +8332,7 @@
         <v>414</v>
       </c>
       <c r="C125" s="16" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="D125" s="25"/>
       <c r="E125" s="25" t="s">
@@ -8732,7 +8357,7 @@
         <v>414</v>
       </c>
       <c r="C126" s="16" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="D126" s="25"/>
       <c r="E126" s="25" t="s">
@@ -8757,7 +8382,7 @@
         <v>414</v>
       </c>
       <c r="C127" s="16" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="D127" s="25"/>
       <c r="E127" s="25" t="s">
@@ -8782,7 +8407,7 @@
         <v>414</v>
       </c>
       <c r="C128" s="16" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="D128" s="25"/>
       <c r="E128" s="25" t="s">
@@ -8807,7 +8432,7 @@
         <v>414</v>
       </c>
       <c r="C129" s="16" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="D129" s="25"/>
       <c r="E129" s="25" t="s">
@@ -8832,7 +8457,7 @@
         <v>414</v>
       </c>
       <c r="C130" s="16" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="D130" s="25"/>
       <c r="E130" s="25" t="s">
@@ -8857,7 +8482,7 @@
         <v>414</v>
       </c>
       <c r="C131" s="16" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="D131" s="25"/>
       <c r="E131" s="25" t="s">
@@ -8882,7 +8507,7 @@
         <v>414</v>
       </c>
       <c r="C132" s="16" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="D132" s="25"/>
       <c r="E132" s="25" t="s">
@@ -8907,7 +8532,7 @@
         <v>414</v>
       </c>
       <c r="C133" s="16" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="D133" s="25"/>
       <c r="E133" s="25" t="s">
@@ -8932,7 +8557,7 @@
         <v>414</v>
       </c>
       <c r="C134" s="16" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="D134" s="25"/>
       <c r="E134" s="25" t="s">
@@ -8954,7 +8579,7 @@
         <v>101</v>
       </c>
       <c r="B135" s="26" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="C135" s="16" t="s">
         <v>477</v>
@@ -8979,10 +8604,10 @@
         <v>102</v>
       </c>
       <c r="B136" s="20" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="C136" s="16" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="D136" s="25"/>
       <c r="E136" s="25" t="s">
@@ -9004,10 +8629,10 @@
         <v>103</v>
       </c>
       <c r="B137" s="26" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="C137" s="16" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="D137" s="25"/>
       <c r="E137" s="25" t="s">
@@ -9029,10 +8654,10 @@
         <v>104</v>
       </c>
       <c r="B138" s="20" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="C138" s="16" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="D138" s="25"/>
       <c r="E138" s="25" t="s">
@@ -9054,7 +8679,7 @@
         <v>105</v>
       </c>
       <c r="B139" s="20" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="C139" s="16" t="s">
         <v>478</v>
@@ -9079,10 +8704,10 @@
         <v>106</v>
       </c>
       <c r="B140" s="20" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="C140" s="16" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="D140" s="25"/>
       <c r="E140" s="25" t="s">
@@ -9104,7 +8729,7 @@
         <v>107</v>
       </c>
       <c r="B141" s="20" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="C141" s="16" t="s">
         <v>479</v>
@@ -9129,10 +8754,10 @@
         <v>108</v>
       </c>
       <c r="B142" s="20" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="C142" s="16" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="D142" s="25"/>
       <c r="E142" s="25" t="s">
@@ -9154,7 +8779,7 @@
         <v>109</v>
       </c>
       <c r="B143" s="20" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="C143" s="16" t="s">
         <v>480</v>
@@ -9179,7 +8804,7 @@
         <v>110</v>
       </c>
       <c r="B144" s="20" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="C144" s="16" t="s">
         <v>481</v>
@@ -9204,10 +8829,10 @@
         <v>111</v>
       </c>
       <c r="B145" s="20" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="C145" s="16" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="D145" s="25"/>
       <c r="E145" s="25" t="s">
@@ -9229,7 +8854,7 @@
         <v>112</v>
       </c>
       <c r="B146" s="20" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="C146" s="27" t="s">
         <v>482</v>
@@ -9254,7 +8879,7 @@
         <v>113</v>
       </c>
       <c r="B147" s="20" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="C147" s="16" t="s">
         <v>483</v>
@@ -9279,10 +8904,10 @@
         <v>114</v>
       </c>
       <c r="B148" s="20" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="C148" s="16" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="D148" s="25"/>
       <c r="E148" s="25" t="s">
@@ -9304,10 +8929,10 @@
         <v>115</v>
       </c>
       <c r="B149" s="20" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="C149" s="16" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
       <c r="D149" s="25"/>
       <c r="E149" s="25" t="s">
@@ -9329,10 +8954,10 @@
         <v>116</v>
       </c>
       <c r="B150" s="20" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="C150" s="16" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="D150" s="25"/>
       <c r="E150" s="25" t="s">
@@ -9354,7 +8979,7 @@
         <v>117</v>
       </c>
       <c r="B151" s="20" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="C151" s="27" t="s">
         <v>484</v>
@@ -9379,10 +9004,10 @@
         <v>118</v>
       </c>
       <c r="B152" s="20" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="C152" s="16" t="s">
-        <v>761</v>
+        <v>758</v>
       </c>
       <c r="D152" s="25"/>
       <c r="E152" s="25" t="s">
@@ -9404,7 +9029,7 @@
         <v>270</v>
       </c>
       <c r="B153" s="20" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
       <c r="C153" s="27" t="s">
         <v>571</v>
@@ -9429,10 +9054,10 @@
         <v>271</v>
       </c>
       <c r="B154" s="20" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
       <c r="C154" s="16" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="D154" s="25"/>
       <c r="E154" s="25" t="s">
@@ -9454,7 +9079,7 @@
         <v>272</v>
       </c>
       <c r="B155" s="20" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
       <c r="C155" s="27" t="s">
         <v>572</v>
@@ -9479,7 +9104,7 @@
         <v>248</v>
       </c>
       <c r="B156" s="20" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="C156" s="16" t="s">
         <v>557</v>
@@ -9504,10 +9129,10 @@
         <v>249</v>
       </c>
       <c r="B157" s="20" t="s">
+        <v>749</v>
+      </c>
+      <c r="C157" s="16" t="s">
         <v>750</v>
-      </c>
-      <c r="C157" s="16" t="s">
-        <v>751</v>
       </c>
       <c r="D157" s="25"/>
       <c r="E157" s="25" t="s">
@@ -9529,7 +9154,7 @@
         <v>250</v>
       </c>
       <c r="B158" s="20" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="C158" s="16" t="s">
         <v>558</v>
@@ -9554,10 +9179,10 @@
         <v>251</v>
       </c>
       <c r="B159" s="20" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="C159" s="16" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
       <c r="D159" s="25"/>
       <c r="E159" s="25" t="s">
@@ -9579,10 +9204,10 @@
         <v>252</v>
       </c>
       <c r="B160" s="20" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="C160" s="16" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
       <c r="D160" s="25"/>
       <c r="E160" s="25" t="s">
@@ -9604,7 +9229,7 @@
         <v>253</v>
       </c>
       <c r="B161" s="20" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="C161" s="27" t="s">
         <v>559</v>
@@ -9623,7 +9248,7 @@
         <v>17</v>
       </c>
       <c r="I161" s="16" t="s">
-        <v>874</v>
+        <v>868</v>
       </c>
     </row>
     <row r="162" spans="1:9" ht="30">
@@ -9631,12 +9256,12 @@
         <v>254</v>
       </c>
       <c r="B162" s="20" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="C162" s="16" t="s">
-        <v>873</v>
-      </c>
-      <c r="D162" s="25" t="s">
+        <v>867</v>
+      </c>
+      <c r="D162" s="18" t="s">
         <v>663</v>
       </c>
       <c r="E162" s="25" t="s">
@@ -9658,7 +9283,7 @@
         <v>255</v>
       </c>
       <c r="B163" s="20" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="C163" s="16" t="s">
         <v>560</v>
@@ -9685,7 +9310,7 @@
         <v>256</v>
       </c>
       <c r="B164" s="20" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="C164" s="27" t="s">
         <v>561</v>
@@ -9712,7 +9337,7 @@
         <v>257</v>
       </c>
       <c r="B165" s="20" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="C165" s="27" t="s">
         <v>562</v>
@@ -9739,7 +9364,7 @@
         <v>258</v>
       </c>
       <c r="B166" s="20" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="C166" s="27" t="s">
         <v>563</v>
@@ -9766,10 +9391,10 @@
         <v>259</v>
       </c>
       <c r="B167" s="20" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="C167" s="16" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="D167" s="25"/>
       <c r="E167" s="25" t="s">
@@ -9791,7 +9416,7 @@
         <v>260</v>
       </c>
       <c r="B168" s="20" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="C168" s="27" t="s">
         <v>564</v>
@@ -9811,15 +9436,15 @@
       </c>
       <c r="I168" s="27"/>
     </row>
-    <row r="169" spans="1:9" ht="60">
+    <row r="169" spans="1:9">
       <c r="A169" s="25" t="s">
         <v>261</v>
       </c>
       <c r="B169" s="20" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="C169" s="16" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="D169" s="25"/>
       <c r="E169" s="25" t="s">
@@ -9832,18 +9457,16 @@
         <v>15</v>
       </c>
       <c r="H169" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="I169" s="16" t="s">
-        <v>759</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="I169" s="16"/>
     </row>
     <row r="170" spans="1:9" ht="30">
       <c r="A170" s="18" t="s">
         <v>262</v>
       </c>
       <c r="B170" s="20" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="C170" s="27" t="s">
         <v>565</v>
@@ -9870,7 +9493,7 @@
         <v>263</v>
       </c>
       <c r="B171" s="20" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="C171" s="27" t="s">
         <v>566</v>
@@ -9897,7 +9520,7 @@
         <v>264</v>
       </c>
       <c r="B172" s="20" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="C172" s="27" t="s">
         <v>567</v>
@@ -9922,7 +9545,7 @@
         <v>265</v>
       </c>
       <c r="B173" s="20" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="C173" s="27" t="s">
         <v>568</v>
@@ -9947,10 +9570,10 @@
         <v>266</v>
       </c>
       <c r="B174" s="20" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="C174" s="16" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="D174" s="25"/>
       <c r="E174" s="25" t="s">
@@ -9967,15 +9590,15 @@
       </c>
       <c r="I174" s="27"/>
     </row>
-    <row r="175" spans="1:9" ht="60">
+    <row r="175" spans="1:9">
       <c r="A175" s="25" t="s">
         <v>267</v>
       </c>
       <c r="B175" s="20" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="C175" s="16" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
       <c r="D175" s="25"/>
       <c r="E175" s="25" t="s">
@@ -9988,18 +9611,16 @@
         <v>15</v>
       </c>
       <c r="H175" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="I175" s="16" t="s">
-        <v>760</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="I175" s="16"/>
     </row>
     <row r="176" spans="1:9" ht="30">
       <c r="A176" s="18" t="s">
         <v>268</v>
       </c>
       <c r="B176" s="20" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="C176" s="27" t="s">
         <v>569</v>
@@ -10026,7 +9647,7 @@
         <v>269</v>
       </c>
       <c r="B177" s="20" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="C177" s="27" t="s">
         <v>570</v>
@@ -10331,7 +9952,7 @@
         <v>416</v>
       </c>
       <c r="C189" s="16" t="s">
-        <v>762</v>
+        <v>759</v>
       </c>
       <c r="D189" s="25"/>
       <c r="E189" s="25" t="s">
@@ -10381,7 +10002,7 @@
         <v>416</v>
       </c>
       <c r="C191" s="16" t="s">
-        <v>763</v>
+        <v>760</v>
       </c>
       <c r="D191" s="25"/>
       <c r="E191" s="25" t="s">
@@ -10456,7 +10077,7 @@
         <v>416</v>
       </c>
       <c r="C194" s="16" t="s">
-        <v>764</v>
+        <v>761</v>
       </c>
       <c r="D194" s="25"/>
       <c r="E194" s="25" t="s">
@@ -10631,7 +10252,7 @@
         <v>417</v>
       </c>
       <c r="C201" s="16" t="s">
-        <v>765</v>
+        <v>762</v>
       </c>
       <c r="D201" s="25"/>
       <c r="E201" s="25" t="s">
@@ -10806,7 +10427,7 @@
         <v>421</v>
       </c>
       <c r="C208" s="16" t="s">
-        <v>766</v>
+        <v>763</v>
       </c>
       <c r="D208" s="25"/>
       <c r="E208" s="25" t="s">
@@ -10831,7 +10452,7 @@
         <v>421</v>
       </c>
       <c r="C209" s="16" t="s">
-        <v>767</v>
+        <v>764</v>
       </c>
       <c r="D209" s="25"/>
       <c r="E209" s="25" t="s">
@@ -10881,7 +10502,7 @@
         <v>421</v>
       </c>
       <c r="C211" s="16" t="s">
-        <v>768</v>
+        <v>765</v>
       </c>
       <c r="D211" s="25"/>
       <c r="E211" s="25" t="s">
@@ -10931,7 +10552,7 @@
         <v>421</v>
       </c>
       <c r="C213" s="16" t="s">
-        <v>769</v>
+        <v>766</v>
       </c>
       <c r="D213" s="25"/>
       <c r="E213" s="25" t="s">
@@ -10956,7 +10577,7 @@
         <v>421</v>
       </c>
       <c r="C214" s="16" t="s">
-        <v>770</v>
+        <v>767</v>
       </c>
       <c r="D214" s="25"/>
       <c r="E214" s="25" t="s">
@@ -11006,7 +10627,7 @@
         <v>421</v>
       </c>
       <c r="C216" s="16" t="s">
-        <v>774</v>
+        <v>771</v>
       </c>
       <c r="D216" s="25"/>
       <c r="E216" s="25" t="s">
@@ -11031,7 +10652,7 @@
         <v>422</v>
       </c>
       <c r="C217" s="16" t="s">
-        <v>771</v>
+        <v>768</v>
       </c>
       <c r="D217" s="25"/>
       <c r="E217" s="25" t="s">
@@ -11056,7 +10677,7 @@
         <v>422</v>
       </c>
       <c r="C218" s="16" t="s">
-        <v>772</v>
+        <v>769</v>
       </c>
       <c r="D218" s="25"/>
       <c r="E218" s="25" t="s">
@@ -11081,7 +10702,7 @@
         <v>422</v>
       </c>
       <c r="C219" s="16" t="s">
-        <v>773</v>
+        <v>770</v>
       </c>
       <c r="D219" s="25"/>
       <c r="E219" s="25" t="s">
@@ -11156,7 +10777,7 @@
         <v>423</v>
       </c>
       <c r="C222" s="16" t="s">
-        <v>775</v>
+        <v>772</v>
       </c>
       <c r="D222" s="25"/>
       <c r="E222" s="25" t="s">
@@ -11181,7 +10802,7 @@
         <v>423</v>
       </c>
       <c r="C223" s="16" t="s">
-        <v>776</v>
+        <v>773</v>
       </c>
       <c r="D223" s="25"/>
       <c r="E223" s="25" t="s">
@@ -11281,7 +10902,7 @@
         <v>423</v>
       </c>
       <c r="C227" s="16" t="s">
-        <v>777</v>
+        <v>774</v>
       </c>
       <c r="D227" s="25"/>
       <c r="E227" s="25" t="s">
@@ -11331,7 +10952,7 @@
         <v>423</v>
       </c>
       <c r="C229" s="16" t="s">
-        <v>778</v>
+        <v>775</v>
       </c>
       <c r="D229" s="25"/>
       <c r="E229" s="25" t="s">
@@ -11381,7 +11002,7 @@
         <v>424</v>
       </c>
       <c r="C231" s="16" t="s">
-        <v>779</v>
+        <v>776</v>
       </c>
       <c r="D231" s="25"/>
       <c r="E231" s="25" t="s">
@@ -11406,7 +11027,7 @@
         <v>424</v>
       </c>
       <c r="C232" s="16" t="s">
-        <v>780</v>
+        <v>777</v>
       </c>
       <c r="D232" s="25"/>
       <c r="E232" s="25" t="s">
@@ -11431,7 +11052,7 @@
         <v>424</v>
       </c>
       <c r="C233" s="16" t="s">
-        <v>781</v>
+        <v>778</v>
       </c>
       <c r="D233" s="25"/>
       <c r="E233" s="25" t="s">
@@ -11456,7 +11077,7 @@
         <v>424</v>
       </c>
       <c r="C234" s="16" t="s">
-        <v>862</v>
+        <v>859</v>
       </c>
       <c r="D234" s="25"/>
       <c r="E234" s="25" t="s">
@@ -11472,7 +11093,7 @@
         <v>17</v>
       </c>
       <c r="I234" s="16" t="s">
-        <v>869</v>
+        <v>865</v>
       </c>
     </row>
     <row r="235" spans="1:9" ht="30">
@@ -11508,7 +11129,7 @@
         <v>424</v>
       </c>
       <c r="C236" s="16" t="s">
-        <v>785</v>
+        <v>782</v>
       </c>
       <c r="D236" s="25"/>
       <c r="E236" s="25" t="s">
@@ -11533,7 +11154,7 @@
         <v>424</v>
       </c>
       <c r="C237" s="16" t="s">
-        <v>784</v>
+        <v>781</v>
       </c>
       <c r="D237" s="25"/>
       <c r="E237" s="25" t="s">
@@ -11558,7 +11179,7 @@
         <v>424</v>
       </c>
       <c r="C238" s="16" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="D238" s="25"/>
       <c r="E238" s="25" t="s">
@@ -11583,7 +11204,7 @@
         <v>424</v>
       </c>
       <c r="C239" s="16" t="s">
-        <v>783</v>
+        <v>780</v>
       </c>
       <c r="D239" s="25"/>
       <c r="E239" s="25" t="s">
@@ -11608,7 +11229,7 @@
         <v>424</v>
       </c>
       <c r="C240" s="16" t="s">
-        <v>786</v>
+        <v>783</v>
       </c>
       <c r="D240" s="25"/>
       <c r="E240" s="25" t="s">
@@ -11633,7 +11254,7 @@
         <v>424</v>
       </c>
       <c r="C241" s="16" t="s">
-        <v>787</v>
+        <v>784</v>
       </c>
       <c r="D241" s="25"/>
       <c r="E241" s="25" t="s">
@@ -11658,7 +11279,7 @@
         <v>424</v>
       </c>
       <c r="C242" s="16" t="s">
-        <v>788</v>
+        <v>785</v>
       </c>
       <c r="D242" s="25"/>
       <c r="E242" s="25" t="s">
@@ -11683,7 +11304,7 @@
         <v>424</v>
       </c>
       <c r="C243" s="16" t="s">
-        <v>789</v>
+        <v>786</v>
       </c>
       <c r="D243" s="25"/>
       <c r="E243" s="25" t="s">
@@ -11708,7 +11329,7 @@
         <v>424</v>
       </c>
       <c r="C244" s="16" t="s">
-        <v>790</v>
+        <v>787</v>
       </c>
       <c r="D244" s="25"/>
       <c r="E244" s="25" t="s">
@@ -11735,7 +11356,7 @@
         <v>424</v>
       </c>
       <c r="C245" s="16" t="s">
-        <v>791</v>
+        <v>788</v>
       </c>
       <c r="D245" s="25"/>
       <c r="E245" s="25" t="s">
@@ -11760,7 +11381,7 @@
         <v>424</v>
       </c>
       <c r="C246" s="16" t="s">
-        <v>792</v>
+        <v>789</v>
       </c>
       <c r="D246" s="25"/>
       <c r="E246" s="25" t="s">
@@ -11785,7 +11406,7 @@
         <v>424</v>
       </c>
       <c r="C247" s="16" t="s">
-        <v>793</v>
+        <v>790</v>
       </c>
       <c r="D247" s="25"/>
       <c r="E247" s="25" t="s">
@@ -11810,7 +11431,7 @@
         <v>424</v>
       </c>
       <c r="C248" s="16" t="s">
-        <v>794</v>
+        <v>791</v>
       </c>
       <c r="D248" s="25"/>
       <c r="E248" s="25" t="s">
@@ -11835,7 +11456,7 @@
         <v>424</v>
       </c>
       <c r="C249" s="16" t="s">
-        <v>795</v>
+        <v>792</v>
       </c>
       <c r="D249" s="25"/>
       <c r="E249" s="25" t="s">
@@ -11860,7 +11481,7 @@
         <v>424</v>
       </c>
       <c r="C250" s="16" t="s">
-        <v>796</v>
+        <v>793</v>
       </c>
       <c r="D250" s="25"/>
       <c r="E250" s="25" t="s">
@@ -11885,7 +11506,7 @@
         <v>424</v>
       </c>
       <c r="C251" s="16" t="s">
-        <v>797</v>
+        <v>794</v>
       </c>
       <c r="D251" s="25"/>
       <c r="E251" s="25" t="s">
@@ -11910,7 +11531,7 @@
         <v>424</v>
       </c>
       <c r="C252" s="16" t="s">
-        <v>798</v>
+        <v>795</v>
       </c>
       <c r="D252" s="25"/>
       <c r="E252" s="25" t="s">
@@ -11935,7 +11556,7 @@
         <v>424</v>
       </c>
       <c r="C253" s="16" t="s">
-        <v>799</v>
+        <v>796</v>
       </c>
       <c r="D253" s="25"/>
       <c r="E253" s="25" t="s">
@@ -11960,7 +11581,7 @@
         <v>424</v>
       </c>
       <c r="C254" s="16" t="s">
-        <v>800</v>
+        <v>797</v>
       </c>
       <c r="D254" s="25"/>
       <c r="E254" s="25" t="s">
@@ -11985,7 +11606,7 @@
         <v>424</v>
       </c>
       <c r="C255" s="16" t="s">
-        <v>801</v>
+        <v>798</v>
       </c>
       <c r="D255" s="25"/>
       <c r="E255" s="25" t="s">
@@ -12010,7 +11631,7 @@
         <v>424</v>
       </c>
       <c r="C256" s="16" t="s">
-        <v>802</v>
+        <v>799</v>
       </c>
       <c r="D256" s="25"/>
       <c r="E256" s="25" t="s">
@@ -12035,7 +11656,7 @@
         <v>424</v>
       </c>
       <c r="C257" s="16" t="s">
-        <v>803</v>
+        <v>800</v>
       </c>
       <c r="D257" s="25"/>
       <c r="E257" s="25" t="s">
@@ -12060,7 +11681,7 @@
         <v>424</v>
       </c>
       <c r="C258" s="16" t="s">
-        <v>804</v>
+        <v>801</v>
       </c>
       <c r="D258" s="25"/>
       <c r="E258" s="25" t="s">
@@ -12085,7 +11706,7 @@
         <v>424</v>
       </c>
       <c r="C259" s="16" t="s">
-        <v>805</v>
+        <v>802</v>
       </c>
       <c r="D259" s="25"/>
       <c r="E259" s="25" t="s">
@@ -12110,7 +11731,7 @@
         <v>424</v>
       </c>
       <c r="C260" s="16" t="s">
-        <v>806</v>
+        <v>803</v>
       </c>
       <c r="D260" s="25"/>
       <c r="E260" s="25" t="s">
@@ -12160,7 +11781,7 @@
         <v>424</v>
       </c>
       <c r="C262" s="16" t="s">
-        <v>807</v>
+        <v>804</v>
       </c>
       <c r="D262" s="25"/>
       <c r="E262" s="25" t="s">
@@ -12185,7 +11806,7 @@
         <v>424</v>
       </c>
       <c r="C263" s="16" t="s">
-        <v>808</v>
+        <v>805</v>
       </c>
       <c r="D263" s="25"/>
       <c r="E263" s="25" t="s">
@@ -12204,13 +11825,13 @@
     </row>
     <row r="264" spans="1:9" ht="45">
       <c r="A264" s="18" t="s">
-        <v>817</v>
+        <v>814</v>
       </c>
       <c r="B264" s="20" t="s">
         <v>424</v>
       </c>
       <c r="C264" s="48" t="s">
-        <v>809</v>
+        <v>806</v>
       </c>
       <c r="D264" s="46"/>
       <c r="E264" s="46" t="s">
@@ -12226,18 +11847,18 @@
         <v>17</v>
       </c>
       <c r="I264" s="48" t="s">
-        <v>895</v>
+        <v>889</v>
       </c>
     </row>
     <row r="265" spans="1:9" ht="30">
       <c r="A265" s="18" t="s">
-        <v>818</v>
+        <v>815</v>
       </c>
       <c r="B265" s="20" t="s">
         <v>424</v>
       </c>
       <c r="C265" s="48" t="s">
-        <v>810</v>
+        <v>807</v>
       </c>
       <c r="D265" s="46"/>
       <c r="E265" s="46" t="s">
@@ -12256,13 +11877,13 @@
     </row>
     <row r="266" spans="1:9" ht="45">
       <c r="A266" s="18" t="s">
-        <v>819</v>
+        <v>816</v>
       </c>
       <c r="B266" s="20" t="s">
         <v>424</v>
       </c>
       <c r="C266" s="48" t="s">
-        <v>811</v>
+        <v>808</v>
       </c>
       <c r="D266" s="46"/>
       <c r="E266" s="46" t="s">
@@ -12278,18 +11899,18 @@
         <v>17</v>
       </c>
       <c r="I266" s="48" t="s">
-        <v>898</v>
+        <v>892</v>
       </c>
     </row>
     <row r="267" spans="1:9" ht="30">
       <c r="A267" s="18" t="s">
-        <v>820</v>
+        <v>817</v>
       </c>
       <c r="B267" s="20" t="s">
         <v>424</v>
       </c>
       <c r="C267" s="48" t="s">
-        <v>812</v>
+        <v>809</v>
       </c>
       <c r="D267" s="46"/>
       <c r="E267" s="46" t="s">
@@ -12308,13 +11929,13 @@
     </row>
     <row r="268" spans="1:9" ht="30">
       <c r="A268" s="18" t="s">
-        <v>821</v>
+        <v>818</v>
       </c>
       <c r="B268" s="20" t="s">
         <v>424</v>
       </c>
       <c r="C268" s="48" t="s">
-        <v>813</v>
+        <v>810</v>
       </c>
       <c r="D268" s="46"/>
       <c r="E268" s="46" t="s">
@@ -12333,13 +11954,13 @@
     </row>
     <row r="269" spans="1:9" ht="45">
       <c r="A269" s="18" t="s">
-        <v>822</v>
+        <v>819</v>
       </c>
       <c r="B269" s="20" t="s">
         <v>424</v>
       </c>
       <c r="C269" s="48" t="s">
-        <v>814</v>
+        <v>811</v>
       </c>
       <c r="D269" s="46"/>
       <c r="E269" s="46" t="s">
@@ -12355,18 +11976,18 @@
         <v>17</v>
       </c>
       <c r="I269" s="48" t="s">
-        <v>870</v>
+        <v>866</v>
       </c>
     </row>
     <row r="270" spans="1:9" ht="30">
       <c r="A270" s="18" t="s">
-        <v>823</v>
+        <v>820</v>
       </c>
       <c r="B270" s="20" t="s">
         <v>424</v>
       </c>
       <c r="C270" s="48" t="s">
-        <v>815</v>
+        <v>812</v>
       </c>
       <c r="D270" s="46"/>
       <c r="E270" s="46" t="s">
@@ -12385,13 +12006,13 @@
     </row>
     <row r="271" spans="1:9" ht="30">
       <c r="A271" s="18" t="s">
-        <v>824</v>
+        <v>821</v>
       </c>
       <c r="B271" s="20" t="s">
         <v>424</v>
       </c>
       <c r="C271" s="48" t="s">
-        <v>816</v>
+        <v>813</v>
       </c>
       <c r="D271" s="46"/>
       <c r="E271" s="46" t="s">
@@ -12413,10 +12034,10 @@
         <v>162</v>
       </c>
       <c r="B272" s="20" t="s">
-        <v>835</v>
+        <v>832</v>
       </c>
       <c r="C272" s="16" t="s">
-        <v>825</v>
+        <v>822</v>
       </c>
       <c r="D272" s="25"/>
       <c r="E272" s="25" t="s">
@@ -12438,10 +12059,10 @@
         <v>163</v>
       </c>
       <c r="B273" s="20" t="s">
-        <v>835</v>
+        <v>832</v>
       </c>
       <c r="C273" s="16" t="s">
-        <v>826</v>
+        <v>823</v>
       </c>
       <c r="D273" s="25"/>
       <c r="E273" s="25" t="s">
@@ -12463,10 +12084,10 @@
         <v>164</v>
       </c>
       <c r="B274" s="20" t="s">
-        <v>835</v>
+        <v>832</v>
       </c>
       <c r="C274" s="16" t="s">
-        <v>827</v>
+        <v>824</v>
       </c>
       <c r="D274" s="25"/>
       <c r="E274" s="25" t="s">
@@ -12488,10 +12109,10 @@
         <v>165</v>
       </c>
       <c r="B275" s="20" t="s">
-        <v>835</v>
+        <v>832</v>
       </c>
       <c r="C275" s="16" t="s">
-        <v>828</v>
+        <v>825</v>
       </c>
       <c r="D275" s="25"/>
       <c r="E275" s="25" t="s">
@@ -12513,7 +12134,7 @@
         <v>166</v>
       </c>
       <c r="B276" s="20" t="s">
-        <v>836</v>
+        <v>833</v>
       </c>
       <c r="C276" s="27" t="s">
         <v>493</v>
@@ -12538,10 +12159,10 @@
         <v>167</v>
       </c>
       <c r="B277" s="20" t="s">
-        <v>836</v>
+        <v>833</v>
       </c>
       <c r="C277" s="16" t="s">
-        <v>829</v>
+        <v>826</v>
       </c>
       <c r="D277" s="25"/>
       <c r="E277" s="25" t="s">
@@ -12563,10 +12184,10 @@
         <v>168</v>
       </c>
       <c r="B278" s="20" t="s">
-        <v>836</v>
+        <v>833</v>
       </c>
       <c r="C278" s="16" t="s">
-        <v>830</v>
+        <v>827</v>
       </c>
       <c r="D278" s="25"/>
       <c r="E278" s="25" t="s">
@@ -12588,7 +12209,7 @@
         <v>169</v>
       </c>
       <c r="B279" s="20" t="s">
-        <v>836</v>
+        <v>833</v>
       </c>
       <c r="C279" s="27" t="s">
         <v>494</v>
@@ -12613,7 +12234,7 @@
         <v>170</v>
       </c>
       <c r="B280" s="20" t="s">
-        <v>836</v>
+        <v>833</v>
       </c>
       <c r="C280" s="27" t="s">
         <v>495</v>
@@ -12638,7 +12259,7 @@
         <v>171</v>
       </c>
       <c r="B281" s="20" t="s">
-        <v>836</v>
+        <v>833</v>
       </c>
       <c r="C281" s="27" t="s">
         <v>496</v>
@@ -12663,7 +12284,7 @@
         <v>172</v>
       </c>
       <c r="B282" s="20" t="s">
-        <v>836</v>
+        <v>833</v>
       </c>
       <c r="C282" s="27" t="s">
         <v>497</v>
@@ -12690,7 +12311,7 @@
         <v>173</v>
       </c>
       <c r="B283" s="20" t="s">
-        <v>836</v>
+        <v>833</v>
       </c>
       <c r="C283" s="27" t="s">
         <v>498</v>
@@ -12717,7 +12338,7 @@
         <v>174</v>
       </c>
       <c r="B284" s="20" t="s">
-        <v>837</v>
+        <v>834</v>
       </c>
       <c r="C284" s="27" t="s">
         <v>499</v>
@@ -12742,10 +12363,10 @@
         <v>175</v>
       </c>
       <c r="B285" s="20" t="s">
-        <v>837</v>
+        <v>834</v>
       </c>
       <c r="C285" s="16" t="s">
-        <v>831</v>
+        <v>828</v>
       </c>
       <c r="D285" s="25"/>
       <c r="E285" s="25" t="s">
@@ -12767,7 +12388,7 @@
         <v>176</v>
       </c>
       <c r="B286" s="20" t="s">
-        <v>837</v>
+        <v>834</v>
       </c>
       <c r="C286" s="27" t="s">
         <v>500</v>
@@ -12792,10 +12413,10 @@
         <v>177</v>
       </c>
       <c r="B287" s="20" t="s">
-        <v>837</v>
+        <v>834</v>
       </c>
       <c r="C287" s="16" t="s">
-        <v>832</v>
+        <v>829</v>
       </c>
       <c r="D287" s="25"/>
       <c r="E287" s="25" t="s">
@@ -12817,7 +12438,7 @@
         <v>178</v>
       </c>
       <c r="B288" s="20" t="s">
-        <v>837</v>
+        <v>834</v>
       </c>
       <c r="C288" s="27" t="s">
         <v>501</v>
@@ -12842,7 +12463,7 @@
         <v>179</v>
       </c>
       <c r="B289" s="20" t="s">
-        <v>837</v>
+        <v>834</v>
       </c>
       <c r="C289" s="27" t="s">
         <v>502</v>
@@ -12867,10 +12488,10 @@
         <v>180</v>
       </c>
       <c r="B290" s="20" t="s">
-        <v>837</v>
+        <v>834</v>
       </c>
       <c r="C290" s="16" t="s">
-        <v>833</v>
+        <v>830</v>
       </c>
       <c r="D290" s="25"/>
       <c r="E290" s="25" t="s">
@@ -12892,7 +12513,7 @@
         <v>181</v>
       </c>
       <c r="B291" s="20" t="s">
-        <v>837</v>
+        <v>834</v>
       </c>
       <c r="C291" s="27" t="s">
         <v>503</v>
@@ -12917,7 +12538,7 @@
         <v>182</v>
       </c>
       <c r="B292" s="20" t="s">
-        <v>837</v>
+        <v>834</v>
       </c>
       <c r="C292" s="27" t="s">
         <v>504</v>
@@ -12942,7 +12563,7 @@
         <v>183</v>
       </c>
       <c r="B293" s="20" t="s">
-        <v>837</v>
+        <v>834</v>
       </c>
       <c r="C293" s="27" t="s">
         <v>505</v>
@@ -12969,7 +12590,7 @@
         <v>184</v>
       </c>
       <c r="B294" s="20" t="s">
-        <v>837</v>
+        <v>834</v>
       </c>
       <c r="C294" s="27" t="s">
         <v>506</v>
@@ -12996,10 +12617,10 @@
         <v>185</v>
       </c>
       <c r="B295" s="20" t="s">
-        <v>837</v>
+        <v>834</v>
       </c>
       <c r="C295" s="16" t="s">
-        <v>838</v>
+        <v>835</v>
       </c>
       <c r="D295" s="25"/>
       <c r="E295" s="25" t="s">
@@ -13021,7 +12642,7 @@
         <v>186</v>
       </c>
       <c r="B296" s="20" t="s">
-        <v>837</v>
+        <v>834</v>
       </c>
       <c r="C296" s="27" t="s">
         <v>507</v>
@@ -13046,7 +12667,7 @@
         <v>187</v>
       </c>
       <c r="B297" s="20" t="s">
-        <v>837</v>
+        <v>834</v>
       </c>
       <c r="C297" s="27" t="s">
         <v>508</v>
@@ -13071,10 +12692,10 @@
         <v>188</v>
       </c>
       <c r="B298" s="20" t="s">
-        <v>837</v>
+        <v>834</v>
       </c>
       <c r="C298" s="16" t="s">
-        <v>834</v>
+        <v>831</v>
       </c>
       <c r="D298" s="25"/>
       <c r="E298" s="25" t="s">
@@ -13096,7 +12717,7 @@
         <v>345</v>
       </c>
       <c r="B299" s="20" t="s">
-        <v>840</v>
+        <v>837</v>
       </c>
       <c r="C299" s="27" t="s">
         <v>626</v>
@@ -13121,10 +12742,10 @@
         <v>346</v>
       </c>
       <c r="B300" s="20" t="s">
-        <v>840</v>
+        <v>837</v>
       </c>
       <c r="C300" s="16" t="s">
-        <v>839</v>
+        <v>836</v>
       </c>
       <c r="D300" s="25"/>
       <c r="E300" s="25" t="s">
@@ -13146,7 +12767,7 @@
         <v>347</v>
       </c>
       <c r="B301" s="20" t="s">
-        <v>840</v>
+        <v>837</v>
       </c>
       <c r="C301" s="27" t="s">
         <v>627</v>
@@ -13171,10 +12792,10 @@
         <v>307</v>
       </c>
       <c r="B302" s="20" t="s">
-        <v>841</v>
+        <v>838</v>
       </c>
       <c r="C302" s="16" t="s">
-        <v>842</v>
+        <v>839</v>
       </c>
       <c r="D302" s="25"/>
       <c r="E302" s="25" t="s">
@@ -13196,10 +12817,10 @@
         <v>308</v>
       </c>
       <c r="B303" s="20" t="s">
-        <v>841</v>
+        <v>838</v>
       </c>
       <c r="C303" s="16" t="s">
-        <v>843</v>
+        <v>840</v>
       </c>
       <c r="D303" s="25"/>
       <c r="E303" s="25" t="s">
@@ -13221,7 +12842,7 @@
         <v>309</v>
       </c>
       <c r="B304" s="20" t="s">
-        <v>841</v>
+        <v>838</v>
       </c>
       <c r="C304" s="16" t="s">
         <v>600</v>
@@ -13246,10 +12867,10 @@
         <v>310</v>
       </c>
       <c r="B305" s="20" t="s">
+        <v>838</v>
+      </c>
+      <c r="C305" s="16" t="s">
         <v>841</v>
-      </c>
-      <c r="C305" s="16" t="s">
-        <v>844</v>
       </c>
       <c r="D305" s="25"/>
       <c r="E305" s="25" t="s">
@@ -13271,10 +12892,10 @@
         <v>311</v>
       </c>
       <c r="B306" s="20" t="s">
-        <v>841</v>
+        <v>838</v>
       </c>
       <c r="C306" s="16" t="s">
-        <v>845</v>
+        <v>842</v>
       </c>
       <c r="D306" s="25"/>
       <c r="E306" s="25" t="s">
@@ -13296,7 +12917,7 @@
         <v>312</v>
       </c>
       <c r="B307" s="20" t="s">
-        <v>841</v>
+        <v>838</v>
       </c>
       <c r="C307" s="16" t="s">
         <v>601</v>
@@ -13315,7 +12936,7 @@
         <v>17</v>
       </c>
       <c r="I307" s="16" t="s">
-        <v>879</v>
+        <v>873</v>
       </c>
     </row>
     <row r="308" spans="1:9" ht="30">
@@ -13323,10 +12944,10 @@
         <v>313</v>
       </c>
       <c r="B308" s="20" t="s">
-        <v>841</v>
+        <v>838</v>
       </c>
       <c r="C308" s="16" t="s">
-        <v>875</v>
+        <v>869</v>
       </c>
       <c r="D308" s="25" t="s">
         <v>670</v>
@@ -13350,7 +12971,7 @@
         <v>314</v>
       </c>
       <c r="B309" s="20" t="s">
-        <v>841</v>
+        <v>838</v>
       </c>
       <c r="C309" s="27" t="s">
         <v>602</v>
@@ -13377,7 +12998,7 @@
         <v>315</v>
       </c>
       <c r="B310" s="20" t="s">
-        <v>841</v>
+        <v>838</v>
       </c>
       <c r="C310" s="27" t="s">
         <v>603</v>
@@ -13404,10 +13025,10 @@
         <v>316</v>
       </c>
       <c r="B311" s="20" t="s">
-        <v>841</v>
+        <v>838</v>
       </c>
       <c r="C311" s="16" t="s">
-        <v>878</v>
+        <v>872</v>
       </c>
       <c r="D311" s="25" t="s">
         <v>673</v>
@@ -13431,7 +13052,7 @@
         <v>317</v>
       </c>
       <c r="B312" s="20" t="s">
-        <v>841</v>
+        <v>838</v>
       </c>
       <c r="C312" s="27" t="s">
         <v>604</v>
@@ -13458,7 +13079,7 @@
         <v>318</v>
       </c>
       <c r="B313" s="20" t="s">
-        <v>841</v>
+        <v>838</v>
       </c>
       <c r="C313" s="27" t="s">
         <v>605</v>
@@ -13485,7 +13106,7 @@
         <v>319</v>
       </c>
       <c r="B314" s="20" t="s">
-        <v>841</v>
+        <v>838</v>
       </c>
       <c r="C314" s="27" t="s">
         <v>606</v>
@@ -13512,7 +13133,7 @@
         <v>320</v>
       </c>
       <c r="B315" s="20" t="s">
-        <v>841</v>
+        <v>838</v>
       </c>
       <c r="C315" s="27" t="s">
         <v>607</v>
@@ -13539,10 +13160,10 @@
         <v>321</v>
       </c>
       <c r="B316" s="20" t="s">
-        <v>841</v>
+        <v>838</v>
       </c>
       <c r="C316" s="16" t="s">
-        <v>846</v>
+        <v>843</v>
       </c>
       <c r="D316" s="25"/>
       <c r="E316" s="25" t="s">
@@ -13564,7 +13185,7 @@
         <v>322</v>
       </c>
       <c r="B317" s="20" t="s">
-        <v>841</v>
+        <v>838</v>
       </c>
       <c r="C317" s="27" t="s">
         <v>608</v>
@@ -13589,7 +13210,7 @@
         <v>323</v>
       </c>
       <c r="B318" s="20" t="s">
-        <v>841</v>
+        <v>838</v>
       </c>
       <c r="C318" s="27" t="s">
         <v>609</v>
@@ -13614,7 +13235,7 @@
         <v>324</v>
       </c>
       <c r="B319" s="20" t="s">
-        <v>841</v>
+        <v>838</v>
       </c>
       <c r="C319" s="27" t="s">
         <v>610</v>
@@ -13639,10 +13260,10 @@
         <v>325</v>
       </c>
       <c r="B320" s="20" t="s">
-        <v>841</v>
+        <v>838</v>
       </c>
       <c r="C320" s="16" t="s">
-        <v>847</v>
+        <v>844</v>
       </c>
       <c r="D320" s="25"/>
       <c r="E320" s="25" t="s">
@@ -13664,10 +13285,10 @@
         <v>326</v>
       </c>
       <c r="B321" s="20" t="s">
-        <v>841</v>
+        <v>838</v>
       </c>
       <c r="C321" s="16" t="s">
-        <v>848</v>
+        <v>845</v>
       </c>
       <c r="D321" s="25"/>
       <c r="E321" s="25" t="s">
@@ -13684,12 +13305,12 @@
       </c>
       <c r="I321" s="27"/>
     </row>
-    <row r="322" spans="1:9" ht="60">
+    <row r="322" spans="1:9" ht="30">
       <c r="A322" s="18" t="s">
         <v>327</v>
       </c>
       <c r="B322" s="20" t="s">
-        <v>841</v>
+        <v>838</v>
       </c>
       <c r="C322" s="27" t="s">
         <v>611</v>
@@ -13707,18 +13328,16 @@
         <v>15</v>
       </c>
       <c r="H322" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="I322" s="16" t="s">
-        <v>872</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="I322" s="16"/>
     </row>
     <row r="323" spans="1:9" ht="30">
       <c r="A323" s="25" t="s">
         <v>328</v>
       </c>
       <c r="B323" s="20" t="s">
-        <v>841</v>
+        <v>838</v>
       </c>
       <c r="C323" s="27" t="s">
         <v>612</v>
@@ -13745,10 +13364,10 @@
         <v>329</v>
       </c>
       <c r="B324" s="20" t="s">
-        <v>841</v>
+        <v>838</v>
       </c>
       <c r="C324" s="16" t="s">
-        <v>849</v>
+        <v>846</v>
       </c>
       <c r="D324" s="25"/>
       <c r="E324" s="25" t="s">
@@ -13770,7 +13389,7 @@
         <v>330</v>
       </c>
       <c r="B325" s="20" t="s">
-        <v>841</v>
+        <v>838</v>
       </c>
       <c r="C325" s="27" t="s">
         <v>613</v>
@@ -13795,7 +13414,7 @@
         <v>331</v>
       </c>
       <c r="B326" s="20" t="s">
-        <v>841</v>
+        <v>838</v>
       </c>
       <c r="C326" s="27" t="s">
         <v>614</v>
@@ -13822,7 +13441,7 @@
         <v>332</v>
       </c>
       <c r="B327" s="20" t="s">
-        <v>841</v>
+        <v>838</v>
       </c>
       <c r="C327" s="27" t="s">
         <v>615</v>
@@ -13844,15 +13463,15 @@
       </c>
       <c r="I327" s="27"/>
     </row>
-    <row r="328" spans="1:9" ht="60">
+    <row r="328" spans="1:9">
       <c r="A328" s="25" t="s">
         <v>333</v>
       </c>
       <c r="B328" s="20" t="s">
-        <v>841</v>
+        <v>838</v>
       </c>
       <c r="C328" s="16" t="s">
-        <v>850</v>
+        <v>847</v>
       </c>
       <c r="D328" s="25"/>
       <c r="E328" s="25" t="s">
@@ -13865,18 +13484,16 @@
         <v>15</v>
       </c>
       <c r="H328" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="I328" s="16" t="s">
-        <v>871</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="I328" s="16"/>
     </row>
     <row r="329" spans="1:9" ht="30">
       <c r="A329" s="18" t="s">
         <v>334</v>
       </c>
       <c r="B329" s="20" t="s">
-        <v>841</v>
+        <v>838</v>
       </c>
       <c r="C329" s="27" t="s">
         <v>616</v>
@@ -13903,7 +13520,7 @@
         <v>335</v>
       </c>
       <c r="B330" s="20" t="s">
-        <v>841</v>
+        <v>838</v>
       </c>
       <c r="C330" s="27" t="s">
         <v>617</v>
@@ -13930,7 +13547,7 @@
         <v>336</v>
       </c>
       <c r="B331" s="20" t="s">
-        <v>841</v>
+        <v>838</v>
       </c>
       <c r="C331" s="27" t="s">
         <v>618</v>
@@ -13955,7 +13572,7 @@
         <v>337</v>
       </c>
       <c r="B332" s="20" t="s">
-        <v>841</v>
+        <v>838</v>
       </c>
       <c r="C332" s="27" t="s">
         <v>619</v>
@@ -13980,7 +13597,7 @@
         <v>338</v>
       </c>
       <c r="B333" s="20" t="s">
-        <v>841</v>
+        <v>838</v>
       </c>
       <c r="C333" s="27" t="s">
         <v>620</v>
@@ -14007,7 +13624,7 @@
         <v>339</v>
       </c>
       <c r="B334" s="20" t="s">
-        <v>841</v>
+        <v>838</v>
       </c>
       <c r="C334" s="27" t="s">
         <v>621</v>
@@ -14034,7 +13651,7 @@
         <v>340</v>
       </c>
       <c r="B335" s="20" t="s">
-        <v>841</v>
+        <v>838</v>
       </c>
       <c r="C335" s="27" t="s">
         <v>622</v>
@@ -14059,7 +13676,7 @@
         <v>341</v>
       </c>
       <c r="B336" s="20" t="s">
-        <v>841</v>
+        <v>838</v>
       </c>
       <c r="C336" s="27" t="s">
         <v>623</v>
@@ -14084,10 +13701,10 @@
         <v>342</v>
       </c>
       <c r="B337" s="20" t="s">
-        <v>841</v>
+        <v>838</v>
       </c>
       <c r="C337" s="16" t="s">
-        <v>851</v>
+        <v>848</v>
       </c>
       <c r="D337" s="25"/>
       <c r="E337" s="25" t="s">
@@ -14103,7 +13720,7 @@
         <v>17</v>
       </c>
       <c r="I337" s="16" t="s">
-        <v>866</v>
+        <v>862</v>
       </c>
     </row>
     <row r="338" spans="1:9" ht="45">
@@ -14111,7 +13728,7 @@
         <v>343</v>
       </c>
       <c r="B338" s="20" t="s">
-        <v>841</v>
+        <v>838</v>
       </c>
       <c r="C338" s="27" t="s">
         <v>624</v>
@@ -14132,7 +13749,7 @@
         <v>17</v>
       </c>
       <c r="I338" s="16" t="s">
-        <v>867</v>
+        <v>863</v>
       </c>
     </row>
     <row r="339" spans="1:9" ht="45">
@@ -14140,7 +13757,7 @@
         <v>344</v>
       </c>
       <c r="B339" s="20" t="s">
-        <v>841</v>
+        <v>838</v>
       </c>
       <c r="C339" s="27" t="s">
         <v>625</v>
@@ -14161,7 +13778,7 @@
         <v>17</v>
       </c>
       <c r="I339" s="16" t="s">
-        <v>867</v>
+        <v>863</v>
       </c>
     </row>
     <row r="340" spans="1:9" ht="45">
@@ -14314,7 +13931,7 @@
       </c>
       <c r="I345" s="27"/>
     </row>
-    <row r="346" spans="1:9" ht="45">
+    <row r="346" spans="1:9" ht="30">
       <c r="A346" s="18" t="s">
         <v>358</v>
       </c>
@@ -14337,9 +13954,7 @@
       <c r="H346" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="I346" s="27" t="s">
-        <v>690</v>
-      </c>
+      <c r="I346" s="27"/>
     </row>
     <row r="347" spans="1:9" ht="30">
       <c r="A347" s="25" t="s">
@@ -14505,16 +14120,16 @@
     </row>
     <row r="353" spans="1:9" ht="45">
       <c r="A353" s="18" t="s">
-        <v>853</v>
+        <v>850</v>
       </c>
       <c r="B353" s="47" t="s">
         <v>428</v>
       </c>
       <c r="C353" s="48" t="s">
-        <v>852</v>
+        <v>849</v>
       </c>
       <c r="D353" s="46" t="s">
-        <v>861</v>
+        <v>858</v>
       </c>
       <c r="E353" s="25" t="s">
         <v>22</v>
@@ -14532,16 +14147,16 @@
     </row>
     <row r="354" spans="1:9" ht="45">
       <c r="A354" s="18" t="s">
-        <v>854</v>
+        <v>851</v>
       </c>
       <c r="B354" s="47" t="s">
         <v>428</v>
       </c>
       <c r="C354" s="48" t="s">
-        <v>886</v>
+        <v>880</v>
       </c>
       <c r="D354" s="46" t="s">
-        <v>861</v>
+        <v>858</v>
       </c>
       <c r="E354" s="25" t="s">
         <v>22</v>
@@ -14561,16 +14176,16 @@
     </row>
     <row r="355" spans="1:9" ht="45">
       <c r="A355" s="18" t="s">
-        <v>855</v>
+        <v>852</v>
       </c>
       <c r="B355" s="47" t="s">
         <v>428</v>
       </c>
       <c r="C355" s="16" t="s">
-        <v>880</v>
+        <v>874</v>
       </c>
       <c r="D355" s="46" t="s">
-        <v>863</v>
+        <v>860</v>
       </c>
       <c r="E355" s="25" t="s">
         <v>22</v>
@@ -14588,16 +14203,16 @@
     </row>
     <row r="356" spans="1:9" ht="45">
       <c r="A356" s="18" t="s">
-        <v>856</v>
+        <v>853</v>
       </c>
       <c r="B356" s="47" t="s">
         <v>428</v>
       </c>
       <c r="C356" s="16" t="s">
-        <v>881</v>
+        <v>875</v>
       </c>
       <c r="D356" s="46" t="s">
-        <v>863</v>
+        <v>860</v>
       </c>
       <c r="E356" s="25" t="s">
         <v>22</v>
@@ -14617,16 +14232,16 @@
     </row>
     <row r="357" spans="1:9" ht="45">
       <c r="A357" s="18" t="s">
-        <v>891</v>
+        <v>885</v>
       </c>
       <c r="B357" s="47" t="s">
         <v>428</v>
       </c>
       <c r="C357" s="48" t="s">
-        <v>887</v>
-      </c>
-      <c r="D357" s="46" t="s">
-        <v>896</v>
+        <v>881</v>
+      </c>
+      <c r="D357" s="18" t="s">
+        <v>890</v>
       </c>
       <c r="E357" s="25" t="s">
         <v>22</v>
@@ -14644,16 +14259,16 @@
     </row>
     <row r="358" spans="1:9" ht="45">
       <c r="A358" s="18" t="s">
-        <v>892</v>
+        <v>886</v>
       </c>
       <c r="B358" s="47" t="s">
         <v>428</v>
       </c>
       <c r="C358" s="48" t="s">
-        <v>888</v>
+        <v>882</v>
       </c>
       <c r="D358" s="46" t="s">
-        <v>896</v>
+        <v>890</v>
       </c>
       <c r="E358" s="25" t="s">
         <v>22</v>
@@ -14673,16 +14288,16 @@
     </row>
     <row r="359" spans="1:9" ht="45">
       <c r="A359" s="18" t="s">
-        <v>893</v>
+        <v>887</v>
       </c>
       <c r="B359" s="47" t="s">
         <v>428</v>
       </c>
       <c r="C359" s="48" t="s">
-        <v>889</v>
+        <v>883</v>
       </c>
       <c r="D359" s="46" t="s">
-        <v>897</v>
+        <v>891</v>
       </c>
       <c r="E359" s="25" t="s">
         <v>22</v>
@@ -14700,16 +14315,16 @@
     </row>
     <row r="360" spans="1:9" ht="45">
       <c r="A360" s="18" t="s">
-        <v>894</v>
+        <v>888</v>
       </c>
       <c r="B360" s="47" t="s">
         <v>428</v>
       </c>
       <c r="C360" s="48" t="s">
-        <v>890</v>
+        <v>884</v>
       </c>
       <c r="D360" s="46" t="s">
-        <v>897</v>
+        <v>891</v>
       </c>
       <c r="E360" s="25" t="s">
         <v>22</v>
@@ -14729,16 +14344,16 @@
     </row>
     <row r="361" spans="1:9" ht="45">
       <c r="A361" s="18" t="s">
-        <v>857</v>
+        <v>854</v>
       </c>
       <c r="B361" s="47" t="s">
         <v>428</v>
       </c>
       <c r="C361" s="48" t="s">
-        <v>882</v>
+        <v>876</v>
       </c>
       <c r="D361" s="46" t="s">
-        <v>864</v>
+        <v>861</v>
       </c>
       <c r="E361" s="25" t="s">
         <v>22</v>
@@ -14756,16 +14371,16 @@
     </row>
     <row r="362" spans="1:9" ht="45">
       <c r="A362" s="18" t="s">
-        <v>858</v>
+        <v>855</v>
       </c>
       <c r="B362" s="47" t="s">
         <v>428</v>
       </c>
       <c r="C362" s="48" t="s">
-        <v>883</v>
+        <v>877</v>
       </c>
       <c r="D362" s="46" t="s">
-        <v>864</v>
+        <v>861</v>
       </c>
       <c r="E362" s="25" t="s">
         <v>22</v>
@@ -14785,16 +14400,16 @@
     </row>
     <row r="363" spans="1:9" ht="30">
       <c r="A363" s="18" t="s">
-        <v>859</v>
+        <v>856</v>
       </c>
       <c r="B363" s="47" t="s">
         <v>428</v>
       </c>
       <c r="C363" s="48" t="s">
-        <v>884</v>
-      </c>
-      <c r="D363" s="46" t="s">
-        <v>865</v>
+        <v>878</v>
+      </c>
+      <c r="D363" s="18" t="s">
+        <v>893</v>
       </c>
       <c r="E363" s="25" t="s">
         <v>22</v>
@@ -14812,16 +14427,16 @@
     </row>
     <row r="364" spans="1:9" ht="45">
       <c r="A364" s="18" t="s">
-        <v>860</v>
+        <v>857</v>
       </c>
       <c r="B364" s="47" t="s">
         <v>428</v>
       </c>
       <c r="C364" s="48" t="s">
-        <v>885</v>
-      </c>
-      <c r="D364" s="46" t="s">
-        <v>865</v>
+        <v>879</v>
+      </c>
+      <c r="D364" s="18" t="s">
+        <v>893</v>
       </c>
       <c r="E364" s="25" t="s">
         <v>22</v>
@@ -14866,7 +14481,7 @@
         <v>688</v>
       </c>
     </row>
-    <row r="366" spans="1:9" ht="45">
+    <row r="366" spans="1:9" ht="60">
       <c r="A366" s="25" t="s">
         <v>366</v>
       </c>
@@ -14874,7 +14489,7 @@
         <v>430</v>
       </c>
       <c r="C366" s="16" t="s">
-        <v>876</v>
+        <v>870</v>
       </c>
       <c r="D366" s="25"/>
       <c r="E366" s="25" t="s">
@@ -14889,11 +14504,11 @@
       <c r="H366" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="I366" s="27" t="s">
-        <v>691</v>
-      </c>
-    </row>
-    <row r="367" spans="1:9" ht="30">
+      <c r="I366" s="16" t="s">
+        <v>894</v>
+      </c>
+    </row>
+    <row r="367" spans="1:9" ht="60">
       <c r="A367" s="25" t="s">
         <v>367</v>
       </c>
@@ -14916,7 +14531,9 @@
       <c r="H367" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="I367" s="27"/>
+      <c r="I367" s="16" t="s">
+        <v>895</v>
+      </c>
     </row>
     <row r="368" spans="1:9" ht="60">
       <c r="A368" s="25" t="s">
@@ -14942,7 +14559,7 @@
         <v>17</v>
       </c>
       <c r="I368" s="27" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
     </row>
     <row r="369" spans="1:9" ht="409.5">
@@ -14953,7 +14570,7 @@
         <v>431</v>
       </c>
       <c r="C369" s="28" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="D369" s="25"/>
       <c r="E369" s="25" t="s">
@@ -14978,7 +14595,7 @@
         <v>431</v>
       </c>
       <c r="C370" s="16" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="D370" s="25"/>
       <c r="E370" s="25" t="s">
@@ -15028,7 +14645,7 @@
         <v>432</v>
       </c>
       <c r="C372" s="28" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="D372" s="25"/>
       <c r="E372" s="25" t="s">
@@ -15169,7 +14786,7 @@
         <v>17</v>
       </c>
       <c r="I377" s="27" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
     </row>
     <row r="378" spans="1:9" ht="45">
@@ -15196,10 +14813,10 @@
         <v>17</v>
       </c>
       <c r="I378" s="16" t="s">
-        <v>702</v>
-      </c>
-    </row>
-    <row r="379" spans="1:9" ht="30">
+        <v>701</v>
+      </c>
+    </row>
+    <row r="379" spans="1:9" ht="45">
       <c r="A379" s="25" t="s">
         <v>379</v>
       </c>
@@ -15207,7 +14824,7 @@
         <v>436</v>
       </c>
       <c r="C379" s="16" t="s">
-        <v>877</v>
+        <v>871</v>
       </c>
       <c r="D379" s="25"/>
       <c r="E379" s="25" t="s">
@@ -15222,7 +14839,9 @@
       <c r="H379" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="I379" s="27"/>
+      <c r="I379" s="16" t="s">
+        <v>896</v>
+      </c>
     </row>
     <row r="380" spans="1:9" ht="45">
       <c r="A380" s="25" t="s">
@@ -15247,7 +14866,9 @@
       <c r="H380" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="I380" s="27"/>
+      <c r="I380" s="16" t="s">
+        <v>897</v>
+      </c>
     </row>
     <row r="381" spans="1:9" ht="45">
       <c r="A381" s="25" t="s">
@@ -15273,7 +14894,7 @@
         <v>17</v>
       </c>
       <c r="I381" s="27" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
     </row>
     <row r="382" spans="1:9" ht="45">
@@ -15300,7 +14921,7 @@
         <v>17</v>
       </c>
       <c r="I382" s="27" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
     </row>
     <row r="383" spans="1:9" ht="60">
@@ -15327,7 +14948,7 @@
         <v>17</v>
       </c>
       <c r="I383" s="27" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
     </row>
     <row r="384" spans="1:9" ht="30">
@@ -15481,76 +15102,76 @@
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="A369:B369 A372:B372 A370:I371 D369:I369 A373:I388 D372:I372 I361:I388 A20:I368">
-    <cfRule type="expression" dxfId="99" priority="77">
+    <cfRule type="expression" dxfId="36" priority="77">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="98" priority="78">
+    <cfRule type="expression" dxfId="35" priority="78">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="97" priority="85">
+    <cfRule type="expression" dxfId="34" priority="85">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A369:B369 A372:B372 A370:I371 D369:I369 A373:I388 D372:I372 I361:I388 A20:I368">
-    <cfRule type="expression" dxfId="96" priority="31">
+    <cfRule type="expression" dxfId="33" priority="31">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="95" priority="32">
+    <cfRule type="expression" dxfId="32" priority="32">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="94" priority="33">
+    <cfRule type="expression" dxfId="31" priority="33">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F20:F388">
-    <cfRule type="expression" dxfId="93" priority="37">
+    <cfRule type="expression" dxfId="30" priority="37">
       <formula>NOT(VLOOKUP(F20,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="92" priority="38">
+    <cfRule type="expression" dxfId="29" priority="38">
       <formula>(VLOOKUP(F20,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C372">
-    <cfRule type="expression" dxfId="91" priority="10">
+    <cfRule type="expression" dxfId="28" priority="10">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="90" priority="11">
+    <cfRule type="expression" dxfId="27" priority="11">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="89" priority="12">
+    <cfRule type="expression" dxfId="26" priority="12">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C372">
-    <cfRule type="expression" dxfId="88" priority="7">
+    <cfRule type="expression" dxfId="25" priority="7">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="87" priority="8">
+    <cfRule type="expression" dxfId="24" priority="8">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="86" priority="9">
+    <cfRule type="expression" dxfId="23" priority="9">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C369">
-    <cfRule type="expression" dxfId="85" priority="4">
+    <cfRule type="expression" dxfId="22" priority="4">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="84" priority="5">
+    <cfRule type="expression" dxfId="21" priority="5">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="83" priority="6">
+    <cfRule type="expression" dxfId="20" priority="6">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C369">
-    <cfRule type="expression" dxfId="82" priority="1">
+    <cfRule type="expression" dxfId="19" priority="1">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="81" priority="2">
+    <cfRule type="expression" dxfId="18" priority="2">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="80" priority="3">
+    <cfRule type="expression" dxfId="17" priority="3">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
@@ -15578,7 +15199,7 @@
     <oddFooter>&amp;F&amp;RPage &amp;P</oddFooter>
   </headerFooter>
   <ignoredErrors>
-    <ignoredError sqref="B1:B9 B10:B46 B108:B109 B47:B103 B178:B211 B365:B390 B340:B352" numberStoredAsText="1"/>
+    <ignoredError sqref="B1:B9 B10:B46 B107:B177 B47:B106 B178:B339 B364:B390 B340:B363 C3" numberStoredAsText="1"/>
   </ignoredErrors>
   <tableParts count="2">
     <tablePart r:id="rId2"/>

</xml_diff>

<commit_message>
Fix MS-OXWSSYNC watchman issues.
</commit_message>
<xml_diff>
--- a/ExchangeWebServices/Docs/MS-OXWSSYNC/MS-OXWSSYNC_RequirementSpecification.xlsx
+++ b/ExchangeWebServices/Docs/MS-OXWSSYNC/MS-OXWSSYNC_RequirementSpecification.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2709" uniqueCount="898">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2708" uniqueCount="897">
   <si>
     <t>Req ID</t>
   </si>
@@ -3875,9 +3875,6 @@
   </si>
   <si>
     <t>MS-OXWSSYNC_R1752006:i</t>
-  </si>
-  <si>
-    <t>Verified by derived requirements:MS-OXWSSYNC_R39223, MS-OXWSSYNC_R39224.</t>
   </si>
   <si>
     <t>Verified by derived requirement: MS-OXWSSYNC_R37811008.</t>
@@ -8146,7 +8143,7 @@
         <v>17</v>
       </c>
       <c r="I117" s="16" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
     </row>
     <row r="118" spans="1:9" ht="330">
@@ -8950,7 +8947,7 @@
       <c r="I149" s="16"/>
     </row>
     <row r="150" spans="1:9" ht="30">
-      <c r="A150" s="25" t="s">
+      <c r="A150" s="18" t="s">
         <v>116</v>
       </c>
       <c r="B150" s="20" t="s">
@@ -9248,7 +9245,7 @@
         <v>17</v>
       </c>
       <c r="I161" s="16" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
     </row>
     <row r="162" spans="1:9" ht="30">
@@ -9259,7 +9256,7 @@
         <v>749</v>
       </c>
       <c r="C162" s="16" t="s">
-        <v>867</v>
+        <v>866</v>
       </c>
       <c r="D162" s="18" t="s">
         <v>663</v>
@@ -11093,7 +11090,7 @@
         <v>17</v>
       </c>
       <c r="I234" s="16" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
     </row>
     <row r="235" spans="1:9" ht="30">
@@ -11847,7 +11844,7 @@
         <v>17</v>
       </c>
       <c r="I264" s="48" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
     </row>
     <row r="265" spans="1:9" ht="30">
@@ -11899,7 +11896,7 @@
         <v>17</v>
       </c>
       <c r="I266" s="48" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
     </row>
     <row r="267" spans="1:9" ht="30">
@@ -11976,7 +11973,7 @@
         <v>17</v>
       </c>
       <c r="I269" s="48" t="s">
-        <v>866</v>
+        <v>865</v>
       </c>
     </row>
     <row r="270" spans="1:9" ht="30">
@@ -12936,7 +12933,7 @@
         <v>17</v>
       </c>
       <c r="I307" s="16" t="s">
-        <v>873</v>
+        <v>872</v>
       </c>
     </row>
     <row r="308" spans="1:9" ht="30">
@@ -12947,7 +12944,7 @@
         <v>838</v>
       </c>
       <c r="C308" s="16" t="s">
-        <v>869</v>
+        <v>868</v>
       </c>
       <c r="D308" s="25" t="s">
         <v>670</v>
@@ -13028,7 +13025,7 @@
         <v>838</v>
       </c>
       <c r="C311" s="16" t="s">
-        <v>872</v>
+        <v>871</v>
       </c>
       <c r="D311" s="25" t="s">
         <v>673</v>
@@ -13696,8 +13693,8 @@
       </c>
       <c r="I336" s="27"/>
     </row>
-    <row r="337" spans="1:9" ht="60">
-      <c r="A337" s="25" t="s">
+    <row r="337" spans="1:9">
+      <c r="A337" s="18" t="s">
         <v>342</v>
       </c>
       <c r="B337" s="20" t="s">
@@ -13719,9 +13716,7 @@
       <c r="H337" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="I337" s="16" t="s">
-        <v>862</v>
-      </c>
+      <c r="I337" s="16"/>
     </row>
     <row r="338" spans="1:9" ht="45">
       <c r="A338" s="18" t="s">
@@ -13749,7 +13744,7 @@
         <v>17</v>
       </c>
       <c r="I338" s="16" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
     </row>
     <row r="339" spans="1:9" ht="45">
@@ -13778,7 +13773,7 @@
         <v>17</v>
       </c>
       <c r="I339" s="16" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
     </row>
     <row r="340" spans="1:9" ht="45">
@@ -14153,7 +14148,7 @@
         <v>428</v>
       </c>
       <c r="C354" s="48" t="s">
-        <v>880</v>
+        <v>879</v>
       </c>
       <c r="D354" s="46" t="s">
         <v>858</v>
@@ -14182,7 +14177,7 @@
         <v>428</v>
       </c>
       <c r="C355" s="16" t="s">
-        <v>874</v>
+        <v>873</v>
       </c>
       <c r="D355" s="46" t="s">
         <v>860</v>
@@ -14209,7 +14204,7 @@
         <v>428</v>
       </c>
       <c r="C356" s="16" t="s">
-        <v>875</v>
+        <v>874</v>
       </c>
       <c r="D356" s="46" t="s">
         <v>860</v>
@@ -14232,16 +14227,16 @@
     </row>
     <row r="357" spans="1:9" ht="45">
       <c r="A357" s="18" t="s">
-        <v>885</v>
+        <v>884</v>
       </c>
       <c r="B357" s="47" t="s">
         <v>428</v>
       </c>
       <c r="C357" s="48" t="s">
-        <v>881</v>
+        <v>880</v>
       </c>
       <c r="D357" s="18" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
       <c r="E357" s="25" t="s">
         <v>22</v>
@@ -14259,16 +14254,16 @@
     </row>
     <row r="358" spans="1:9" ht="45">
       <c r="A358" s="18" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
       <c r="B358" s="47" t="s">
         <v>428</v>
       </c>
       <c r="C358" s="48" t="s">
-        <v>882</v>
+        <v>881</v>
       </c>
       <c r="D358" s="46" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
       <c r="E358" s="25" t="s">
         <v>22</v>
@@ -14288,16 +14283,16 @@
     </row>
     <row r="359" spans="1:9" ht="45">
       <c r="A359" s="18" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
       <c r="B359" s="47" t="s">
         <v>428</v>
       </c>
       <c r="C359" s="48" t="s">
-        <v>883</v>
+        <v>882</v>
       </c>
       <c r="D359" s="46" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
       <c r="E359" s="25" t="s">
         <v>22</v>
@@ -14315,16 +14310,16 @@
     </row>
     <row r="360" spans="1:9" ht="45">
       <c r="A360" s="18" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
       <c r="B360" s="47" t="s">
         <v>428</v>
       </c>
       <c r="C360" s="48" t="s">
-        <v>884</v>
+        <v>883</v>
       </c>
       <c r="D360" s="46" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
       <c r="E360" s="25" t="s">
         <v>22</v>
@@ -14350,7 +14345,7 @@
         <v>428</v>
       </c>
       <c r="C361" s="48" t="s">
-        <v>876</v>
+        <v>875</v>
       </c>
       <c r="D361" s="46" t="s">
         <v>861</v>
@@ -14377,7 +14372,7 @@
         <v>428</v>
       </c>
       <c r="C362" s="48" t="s">
-        <v>877</v>
+        <v>876</v>
       </c>
       <c r="D362" s="46" t="s">
         <v>861</v>
@@ -14406,10 +14401,10 @@
         <v>428</v>
       </c>
       <c r="C363" s="48" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
       <c r="D363" s="18" t="s">
-        <v>893</v>
+        <v>892</v>
       </c>
       <c r="E363" s="25" t="s">
         <v>22</v>
@@ -14433,10 +14428,10 @@
         <v>428</v>
       </c>
       <c r="C364" s="48" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
       <c r="D364" s="18" t="s">
-        <v>893</v>
+        <v>892</v>
       </c>
       <c r="E364" s="25" t="s">
         <v>22</v>
@@ -14489,7 +14484,7 @@
         <v>430</v>
       </c>
       <c r="C366" s="16" t="s">
-        <v>870</v>
+        <v>869</v>
       </c>
       <c r="D366" s="25"/>
       <c r="E366" s="25" t="s">
@@ -14505,7 +14500,7 @@
         <v>17</v>
       </c>
       <c r="I366" s="16" t="s">
-        <v>894</v>
+        <v>893</v>
       </c>
     </row>
     <row r="367" spans="1:9" ht="60">
@@ -14532,7 +14527,7 @@
         <v>17</v>
       </c>
       <c r="I367" s="16" t="s">
-        <v>895</v>
+        <v>894</v>
       </c>
     </row>
     <row r="368" spans="1:9" ht="60">
@@ -14824,7 +14819,7 @@
         <v>436</v>
       </c>
       <c r="C379" s="16" t="s">
-        <v>871</v>
+        <v>870</v>
       </c>
       <c r="D379" s="25"/>
       <c r="E379" s="25" t="s">
@@ -14840,7 +14835,7 @@
         <v>17</v>
       </c>
       <c r="I379" s="16" t="s">
-        <v>896</v>
+        <v>895</v>
       </c>
     </row>
     <row r="380" spans="1:9" ht="45">
@@ -14867,7 +14862,7 @@
         <v>17</v>
       </c>
       <c r="I380" s="16" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
     </row>
     <row r="381" spans="1:9" ht="45">
@@ -15209,21 +15204,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F2EA47BB262D974097182E2CA8AB13E1" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="74597e8d9e42e7e4fc8eda6d37675aa2">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4aeb20c0e3442673af7ee10786458764">
     <xsd:element name="properties">
@@ -15272,10 +15252,32 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6D33261-F3C6-4621-88F1-D76E5ABE1865}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EDB2DE12-5EF6-4CF2-820D-5F9FE329E08E}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/internal/2005/internalDocumentation"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -15295,16 +15297,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EDB2DE12-5EF6-4CF2-820D-5F9FE329E08E}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6D33261-F3C6-4621-88F1-D76E5ABE1865}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/internal/2005/internalDocumentation"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Update RS of MS-OXWSSYNC
</commit_message>
<xml_diff>
--- a/ExchangeWebServices/Docs/MS-OXWSSYNC/MS-OXWSSYNC_RequirementSpecification.xlsx
+++ b/ExchangeWebServices/Docs/MS-OXWSSYNC/MS-OXWSSYNC_RequirementSpecification.xlsx
@@ -3,15 +3,15 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22130"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{905A928C-367A-4A78-B054-981F2ADEF4BC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5F103C7-44C0-4CB6-9E6F-784F48E2F78B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21480" yWindow="-120" windowWidth="19440" windowHeight="15000" tabRatio="570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" tabRatio="570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Requirements!$A$19:$G$390</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Requirements!$A$19:$G$391</definedName>
     <definedName name="ExtensionList">Requirements!#REF!</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">Requirements!$A:$A,Requirements!$19:$19</definedName>
     <definedName name="ScopeList">Requirements!#REF!</definedName>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2722" uniqueCount="901">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2729" uniqueCount="903">
   <si>
     <t>Req ID</t>
   </si>
@@ -3628,9 +3628,6 @@
     <t>[In t:SyncFolderItemsCreateOrUpdateType Complex Type] [The element DistributionList] specifies a distribution list to update in the client message store.</t>
   </si>
   <si>
-    <t>[In t:SyncFolderItemsCreateOrUpdateType Complex Type] [The element MeetingMessage] specifies a meeting message to create or update in the client message store.</t>
-  </si>
-  <si>
     <t>[In t:SyncFolderItemsCreateOrUpdateType Complex Type] [The element MeetingRequest] specifies a meeting request message to create in the client message store.</t>
   </si>
   <si>
@@ -3993,6 +3990,15 @@
   </si>
   <si>
     <t>[In Appendix C: Product Behavior] Implementation does return a MessageType complex type. (If a client creates an item of this type, a MessageType complex type is returned.)(Exchange Server 2007 Service Pack 1 (SP1) and above follow this behavior.)</t>
+  </si>
+  <si>
+    <t>MS-OXWSSYNC_R1651</t>
+  </si>
+  <si>
+    <t>[In t:SyncFolderItemsCreateOrUpdateType Complex Type] [The element MeetingMessage] specifies a meeting message to create in the client message store.</t>
+  </si>
+  <si>
+    <t>[In t:SyncFolderItemsCreateOrUpdateType Complex Type] [The element MeetingMessage] specifies a meeting message to update in the client message store.</t>
   </si>
 </sst>
 </file>
@@ -4978,8 +4984,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Requirement" displayName="Requirement" ref="A19:I390" tableType="xml" totalsRowShown="0" headerRowDxfId="16" dataDxfId="15" connectionId="1">
-  <autoFilter ref="A19:I390" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Requirement" displayName="Requirement" ref="A19:I391" tableType="xml" totalsRowShown="0" headerRowDxfId="16" dataDxfId="15" connectionId="1">
+  <autoFilter ref="A19:I391" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" uniqueName="ns1:REQ_ID" name="Req ID" dataDxfId="14">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:REQ_ID" xmlDataType="string"/>
@@ -5347,10 +5353,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:M392"/>
+  <dimension ref="A1:M393"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A355" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C358" sqref="C358"/>
+    <sheetView tabSelected="1" topLeftCell="A247" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C252" sqref="C252"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -7367,7 +7373,7 @@
         <v>407</v>
       </c>
       <c r="C86" s="16" t="s">
-        <v>880</v>
+        <v>879</v>
       </c>
       <c r="D86" s="25"/>
       <c r="E86" s="25" t="s">
@@ -7442,7 +7448,7 @@
         <v>407</v>
       </c>
       <c r="C89" s="16" t="s">
-        <v>881</v>
+        <v>880</v>
       </c>
       <c r="D89" s="25"/>
       <c r="E89" s="25" t="s">
@@ -7617,7 +7623,7 @@
         <v>408</v>
       </c>
       <c r="C96" s="16" t="s">
-        <v>882</v>
+        <v>881</v>
       </c>
       <c r="D96" s="25"/>
       <c r="E96" s="25" t="s">
@@ -8158,7 +8164,7 @@
         <v>17</v>
       </c>
       <c r="I117" s="16" t="s">
-        <v>848</v>
+        <v>847</v>
       </c>
     </row>
     <row r="118" spans="1:9" ht="330">
@@ -8294,7 +8300,7 @@
         <v>414</v>
       </c>
       <c r="C123" s="16" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
       <c r="D123" s="25"/>
       <c r="E123" s="25" t="s">
@@ -9260,7 +9266,7 @@
         <v>17</v>
       </c>
       <c r="I161" s="16" t="s">
-        <v>852</v>
+        <v>851</v>
       </c>
     </row>
     <row r="162" spans="1:9" ht="30">
@@ -9271,7 +9277,7 @@
         <v>744</v>
       </c>
       <c r="C162" s="16" t="s">
-        <v>851</v>
+        <v>850</v>
       </c>
       <c r="D162" s="18" t="s">
         <v>662</v>
@@ -10014,7 +10020,7 @@
         <v>416</v>
       </c>
       <c r="C191" s="16" t="s">
-        <v>883</v>
+        <v>882</v>
       </c>
       <c r="D191" s="25"/>
       <c r="E191" s="25" t="s">
@@ -10089,7 +10095,7 @@
         <v>416</v>
       </c>
       <c r="C194" s="16" t="s">
-        <v>884</v>
+        <v>883</v>
       </c>
       <c r="D194" s="25"/>
       <c r="E194" s="25" t="s">
@@ -10264,7 +10270,7 @@
         <v>417</v>
       </c>
       <c r="C201" s="16" t="s">
-        <v>885</v>
+        <v>884</v>
       </c>
       <c r="D201" s="25"/>
       <c r="E201" s="25" t="s">
@@ -11089,7 +11095,7 @@
         <v>424</v>
       </c>
       <c r="C234" s="16" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
       <c r="D234" s="25"/>
       <c r="E234" s="25" t="s">
@@ -11108,13 +11114,13 @@
     </row>
     <row r="235" spans="1:9" ht="30">
       <c r="A235" s="18" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
       <c r="B235" s="47" t="s">
         <v>424</v>
       </c>
       <c r="C235" s="16" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
       <c r="D235" s="46"/>
       <c r="E235" s="46" t="s">
@@ -11133,13 +11139,13 @@
     </row>
     <row r="236" spans="1:9" ht="45">
       <c r="A236" s="18" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
       <c r="B236" s="47" t="s">
         <v>424</v>
       </c>
       <c r="C236" s="16" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
       <c r="D236" s="46"/>
       <c r="E236" s="46" t="s">
@@ -11155,7 +11161,7 @@
         <v>17</v>
       </c>
       <c r="I236" s="16" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
     </row>
     <row r="237" spans="1:9" ht="30">
@@ -11166,7 +11172,7 @@
         <v>424</v>
       </c>
       <c r="C237" s="16" t="s">
-        <v>893</v>
+        <v>892</v>
       </c>
       <c r="D237" s="25"/>
       <c r="E237" s="25" t="s">
@@ -11241,7 +11247,7 @@
         <v>424</v>
       </c>
       <c r="C240" s="16" t="s">
-        <v>894</v>
+        <v>893</v>
       </c>
       <c r="D240" s="25"/>
       <c r="E240" s="25" t="s">
@@ -11468,7 +11474,7 @@
         <v>424</v>
       </c>
       <c r="C249" s="16" t="s">
-        <v>895</v>
+        <v>894</v>
       </c>
       <c r="D249" s="25"/>
       <c r="E249" s="25" t="s">
@@ -11486,14 +11492,14 @@
       <c r="I249" s="27"/>
     </row>
     <row r="250" spans="1:9" ht="30">
-      <c r="A250" s="25" t="s">
+      <c r="A250" s="18" t="s">
         <v>146</v>
       </c>
       <c r="B250" s="20" t="s">
         <v>424</v>
       </c>
       <c r="C250" s="16" t="s">
-        <v>781</v>
+        <v>901</v>
       </c>
       <c r="D250" s="25"/>
       <c r="E250" s="25" t="s">
@@ -11511,39 +11517,39 @@
       <c r="I250" s="27"/>
     </row>
     <row r="251" spans="1:9" ht="30">
-      <c r="A251" s="25" t="s">
-        <v>147</v>
-      </c>
-      <c r="B251" s="20" t="s">
+      <c r="A251" s="18" t="s">
+        <v>900</v>
+      </c>
+      <c r="B251" s="47" t="s">
         <v>424</v>
       </c>
       <c r="C251" s="16" t="s">
-        <v>896</v>
-      </c>
-      <c r="D251" s="25"/>
-      <c r="E251" s="25" t="s">
-        <v>19</v>
-      </c>
-      <c r="F251" s="25" t="s">
-        <v>6</v>
-      </c>
-      <c r="G251" s="25" t="s">
-        <v>15</v>
-      </c>
-      <c r="H251" s="25" t="s">
+        <v>902</v>
+      </c>
+      <c r="D251" s="46"/>
+      <c r="E251" s="46" t="s">
+        <v>19</v>
+      </c>
+      <c r="F251" s="46" t="s">
+        <v>6</v>
+      </c>
+      <c r="G251" s="46" t="s">
+        <v>15</v>
+      </c>
+      <c r="H251" s="46" t="s">
         <v>20</v>
       </c>
-      <c r="I251" s="27"/>
+      <c r="I251" s="48"/>
     </row>
     <row r="252" spans="1:9" ht="30">
       <c r="A252" s="25" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B252" s="20" t="s">
         <v>424</v>
       </c>
       <c r="C252" s="16" t="s">
-        <v>782</v>
+        <v>895</v>
       </c>
       <c r="D252" s="25"/>
       <c r="E252" s="25" t="s">
@@ -11562,13 +11568,13 @@
     </row>
     <row r="253" spans="1:9" ht="30">
       <c r="A253" s="25" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B253" s="20" t="s">
         <v>424</v>
       </c>
       <c r="C253" s="16" t="s">
-        <v>783</v>
+        <v>781</v>
       </c>
       <c r="D253" s="25"/>
       <c r="E253" s="25" t="s">
@@ -11587,13 +11593,13 @@
     </row>
     <row r="254" spans="1:9" ht="30">
       <c r="A254" s="25" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B254" s="20" t="s">
         <v>424</v>
       </c>
       <c r="C254" s="16" t="s">
-        <v>897</v>
+        <v>782</v>
       </c>
       <c r="D254" s="25"/>
       <c r="E254" s="25" t="s">
@@ -11612,13 +11618,13 @@
     </row>
     <row r="255" spans="1:9" ht="30">
       <c r="A255" s="25" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B255" s="20" t="s">
         <v>424</v>
       </c>
       <c r="C255" s="16" t="s">
-        <v>784</v>
+        <v>896</v>
       </c>
       <c r="D255" s="25"/>
       <c r="E255" s="25" t="s">
@@ -11637,13 +11643,13 @@
     </row>
     <row r="256" spans="1:9" ht="30">
       <c r="A256" s="25" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B256" s="20" t="s">
         <v>424</v>
       </c>
       <c r="C256" s="16" t="s">
-        <v>785</v>
+        <v>783</v>
       </c>
       <c r="D256" s="25"/>
       <c r="E256" s="25" t="s">
@@ -11662,13 +11668,13 @@
     </row>
     <row r="257" spans="1:9" ht="30">
       <c r="A257" s="25" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B257" s="20" t="s">
         <v>424</v>
       </c>
       <c r="C257" s="16" t="s">
-        <v>898</v>
+        <v>784</v>
       </c>
       <c r="D257" s="25"/>
       <c r="E257" s="25" t="s">
@@ -11685,15 +11691,15 @@
       </c>
       <c r="I257" s="27"/>
     </row>
-    <row r="258" spans="1:9" ht="45">
+    <row r="258" spans="1:9" ht="30">
       <c r="A258" s="25" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B258" s="20" t="s">
         <v>424</v>
       </c>
       <c r="C258" s="16" t="s">
-        <v>786</v>
+        <v>897</v>
       </c>
       <c r="D258" s="25"/>
       <c r="E258" s="25" t="s">
@@ -11712,13 +11718,13 @@
     </row>
     <row r="259" spans="1:9" ht="45">
       <c r="A259" s="25" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B259" s="20" t="s">
         <v>424</v>
       </c>
       <c r="C259" s="16" t="s">
-        <v>787</v>
+        <v>785</v>
       </c>
       <c r="D259" s="25"/>
       <c r="E259" s="25" t="s">
@@ -11735,15 +11741,15 @@
       </c>
       <c r="I259" s="27"/>
     </row>
-    <row r="260" spans="1:9" ht="30">
+    <row r="260" spans="1:9" ht="45">
       <c r="A260" s="25" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B260" s="20" t="s">
         <v>424</v>
       </c>
       <c r="C260" s="16" t="s">
-        <v>788</v>
+        <v>786</v>
       </c>
       <c r="D260" s="25"/>
       <c r="E260" s="25" t="s">
@@ -11762,13 +11768,13 @@
     </row>
     <row r="261" spans="1:9" ht="30">
       <c r="A261" s="25" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B261" s="20" t="s">
         <v>424</v>
       </c>
       <c r="C261" s="16" t="s">
-        <v>789</v>
+        <v>787</v>
       </c>
       <c r="D261" s="25"/>
       <c r="E261" s="25" t="s">
@@ -11787,13 +11793,13 @@
     </row>
     <row r="262" spans="1:9" ht="30">
       <c r="A262" s="25" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B262" s="20" t="s">
         <v>424</v>
       </c>
       <c r="C262" s="16" t="s">
-        <v>790</v>
+        <v>788</v>
       </c>
       <c r="D262" s="25"/>
       <c r="E262" s="25" t="s">
@@ -11812,13 +11818,13 @@
     </row>
     <row r="263" spans="1:9" ht="30">
       <c r="A263" s="25" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B263" s="20" t="s">
         <v>424</v>
       </c>
       <c r="C263" s="16" t="s">
-        <v>491</v>
+        <v>789</v>
       </c>
       <c r="D263" s="25"/>
       <c r="E263" s="25" t="s">
@@ -11837,13 +11843,13 @@
     </row>
     <row r="264" spans="1:9" ht="30">
       <c r="A264" s="25" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B264" s="20" t="s">
         <v>424</v>
       </c>
       <c r="C264" s="16" t="s">
-        <v>791</v>
+        <v>491</v>
       </c>
       <c r="D264" s="25"/>
       <c r="E264" s="25" t="s">
@@ -11862,13 +11868,13 @@
     </row>
     <row r="265" spans="1:9" ht="30">
       <c r="A265" s="25" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B265" s="20" t="s">
         <v>424</v>
       </c>
       <c r="C265" s="16" t="s">
-        <v>792</v>
+        <v>790</v>
       </c>
       <c r="D265" s="25"/>
       <c r="E265" s="25" t="s">
@@ -11885,18 +11891,18 @@
       </c>
       <c r="I265" s="27"/>
     </row>
-    <row r="266" spans="1:9" ht="45">
-      <c r="A266" s="18" t="s">
-        <v>801</v>
+    <row r="266" spans="1:9" ht="30">
+      <c r="A266" s="25" t="s">
+        <v>161</v>
       </c>
       <c r="B266" s="20" t="s">
         <v>424</v>
       </c>
-      <c r="C266" s="48" t="s">
-        <v>793</v>
-      </c>
-      <c r="D266" s="46"/>
-      <c r="E266" s="46" t="s">
+      <c r="C266" s="16" t="s">
+        <v>791</v>
+      </c>
+      <c r="D266" s="25"/>
+      <c r="E266" s="25" t="s">
         <v>19</v>
       </c>
       <c r="F266" s="25" t="s">
@@ -11905,22 +11911,20 @@
       <c r="G266" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="H266" s="46" t="s">
-        <v>17</v>
-      </c>
-      <c r="I266" s="48" t="s">
-        <v>871</v>
-      </c>
-    </row>
-    <row r="267" spans="1:9" ht="30">
+      <c r="H266" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="I266" s="27"/>
+    </row>
+    <row r="267" spans="1:9" ht="45">
       <c r="A267" s="18" t="s">
-        <v>802</v>
+        <v>800</v>
       </c>
       <c r="B267" s="20" t="s">
         <v>424</v>
       </c>
       <c r="C267" s="48" t="s">
-        <v>794</v>
+        <v>792</v>
       </c>
       <c r="D267" s="46"/>
       <c r="E267" s="46" t="s">
@@ -11933,19 +11937,21 @@
         <v>15</v>
       </c>
       <c r="H267" s="46" t="s">
-        <v>18</v>
-      </c>
-      <c r="I267" s="48"/>
-    </row>
-    <row r="268" spans="1:9" ht="45">
+        <v>17</v>
+      </c>
+      <c r="I267" s="48" t="s">
+        <v>870</v>
+      </c>
+    </row>
+    <row r="268" spans="1:9" ht="30">
       <c r="A268" s="18" t="s">
-        <v>803</v>
+        <v>801</v>
       </c>
       <c r="B268" s="20" t="s">
         <v>424</v>
       </c>
       <c r="C268" s="48" t="s">
-        <v>795</v>
+        <v>793</v>
       </c>
       <c r="D268" s="46"/>
       <c r="E268" s="46" t="s">
@@ -11958,21 +11964,19 @@
         <v>15</v>
       </c>
       <c r="H268" s="46" t="s">
-        <v>17</v>
-      </c>
-      <c r="I268" s="48" t="s">
-        <v>874</v>
-      </c>
-    </row>
-    <row r="269" spans="1:9" ht="30">
+        <v>18</v>
+      </c>
+      <c r="I268" s="48"/>
+    </row>
+    <row r="269" spans="1:9" ht="45">
       <c r="A269" s="18" t="s">
-        <v>804</v>
+        <v>802</v>
       </c>
       <c r="B269" s="20" t="s">
         <v>424</v>
       </c>
       <c r="C269" s="48" t="s">
-        <v>796</v>
+        <v>794</v>
       </c>
       <c r="D269" s="46"/>
       <c r="E269" s="46" t="s">
@@ -11985,19 +11989,21 @@
         <v>15</v>
       </c>
       <c r="H269" s="46" t="s">
-        <v>18</v>
-      </c>
-      <c r="I269" s="48"/>
+        <v>17</v>
+      </c>
+      <c r="I269" s="48" t="s">
+        <v>873</v>
+      </c>
     </row>
     <row r="270" spans="1:9" ht="30">
       <c r="A270" s="18" t="s">
-        <v>805</v>
+        <v>803</v>
       </c>
       <c r="B270" s="20" t="s">
         <v>424</v>
       </c>
       <c r="C270" s="48" t="s">
-        <v>797</v>
+        <v>795</v>
       </c>
       <c r="D270" s="46"/>
       <c r="E270" s="46" t="s">
@@ -12010,19 +12016,19 @@
         <v>15</v>
       </c>
       <c r="H270" s="46" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I270" s="48"/>
     </row>
-    <row r="271" spans="1:9" ht="45">
+    <row r="271" spans="1:9" ht="30">
       <c r="A271" s="18" t="s">
-        <v>806</v>
+        <v>804</v>
       </c>
       <c r="B271" s="20" t="s">
         <v>424</v>
       </c>
       <c r="C271" s="48" t="s">
-        <v>798</v>
+        <v>796</v>
       </c>
       <c r="D271" s="46"/>
       <c r="E271" s="46" t="s">
@@ -12035,21 +12041,19 @@
         <v>15</v>
       </c>
       <c r="H271" s="46" t="s">
-        <v>17</v>
-      </c>
-      <c r="I271" s="48" t="s">
-        <v>850</v>
-      </c>
-    </row>
-    <row r="272" spans="1:9" ht="30">
+        <v>20</v>
+      </c>
+      <c r="I271" s="48"/>
+    </row>
+    <row r="272" spans="1:9" ht="45">
       <c r="A272" s="18" t="s">
-        <v>807</v>
+        <v>805</v>
       </c>
       <c r="B272" s="20" t="s">
         <v>424</v>
       </c>
       <c r="C272" s="48" t="s">
-        <v>799</v>
+        <v>797</v>
       </c>
       <c r="D272" s="46"/>
       <c r="E272" s="46" t="s">
@@ -12062,19 +12066,21 @@
         <v>15</v>
       </c>
       <c r="H272" s="46" t="s">
-        <v>18</v>
-      </c>
-      <c r="I272" s="48"/>
+        <v>17</v>
+      </c>
+      <c r="I272" s="48" t="s">
+        <v>849</v>
+      </c>
     </row>
     <row r="273" spans="1:9" ht="30">
       <c r="A273" s="18" t="s">
-        <v>808</v>
+        <v>806</v>
       </c>
       <c r="B273" s="20" t="s">
         <v>424</v>
       </c>
       <c r="C273" s="48" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="D273" s="46"/>
       <c r="E273" s="46" t="s">
@@ -12091,40 +12097,40 @@
       </c>
       <c r="I273" s="48"/>
     </row>
-    <row r="274" spans="1:9" ht="135">
-      <c r="A274" s="25" t="s">
+    <row r="274" spans="1:9" ht="30">
+      <c r="A274" s="18" t="s">
+        <v>807</v>
+      </c>
+      <c r="B274" s="20" t="s">
+        <v>424</v>
+      </c>
+      <c r="C274" s="48" t="s">
+        <v>799</v>
+      </c>
+      <c r="D274" s="46"/>
+      <c r="E274" s="46" t="s">
+        <v>19</v>
+      </c>
+      <c r="F274" s="25" t="s">
+        <v>6</v>
+      </c>
+      <c r="G274" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="H274" s="46" t="s">
+        <v>18</v>
+      </c>
+      <c r="I274" s="48"/>
+    </row>
+    <row r="275" spans="1:9" ht="135">
+      <c r="A275" s="25" t="s">
         <v>162</v>
       </c>
-      <c r="B274" s="20" t="s">
-        <v>819</v>
-      </c>
-      <c r="C274" s="16" t="s">
-        <v>809</v>
-      </c>
-      <c r="D274" s="25"/>
-      <c r="E274" s="25" t="s">
-        <v>19</v>
-      </c>
-      <c r="F274" s="25" t="s">
-        <v>6</v>
-      </c>
-      <c r="G274" s="25" t="s">
-        <v>15</v>
-      </c>
-      <c r="H274" s="25" t="s">
-        <v>21</v>
-      </c>
-      <c r="I274" s="27"/>
-    </row>
-    <row r="275" spans="1:9" ht="30">
-      <c r="A275" s="25" t="s">
-        <v>163</v>
-      </c>
       <c r="B275" s="20" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
       <c r="C275" s="16" t="s">
-        <v>810</v>
+        <v>808</v>
       </c>
       <c r="D275" s="25"/>
       <c r="E275" s="25" t="s">
@@ -12134,22 +12140,22 @@
         <v>6</v>
       </c>
       <c r="G275" s="25" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H275" s="25" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="I275" s="27"/>
     </row>
     <row r="276" spans="1:9" ht="30">
       <c r="A276" s="25" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B276" s="20" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
       <c r="C276" s="16" t="s">
-        <v>811</v>
+        <v>809</v>
       </c>
       <c r="D276" s="25"/>
       <c r="E276" s="25" t="s">
@@ -12159,22 +12165,22 @@
         <v>6</v>
       </c>
       <c r="G276" s="25" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H276" s="25" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I276" s="27"/>
     </row>
     <row r="277" spans="1:9" ht="30">
       <c r="A277" s="25" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B277" s="20" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
       <c r="C277" s="16" t="s">
-        <v>812</v>
+        <v>810</v>
       </c>
       <c r="D277" s="25"/>
       <c r="E277" s="25" t="s">
@@ -12187,19 +12193,19 @@
         <v>15</v>
       </c>
       <c r="H277" s="25" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="I277" s="27"/>
     </row>
-    <row r="278" spans="1:9" ht="180">
+    <row r="278" spans="1:9" ht="30">
       <c r="A278" s="25" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B278" s="20" t="s">
-        <v>820</v>
-      </c>
-      <c r="C278" s="27" t="s">
-        <v>492</v>
+        <v>818</v>
+      </c>
+      <c r="C278" s="16" t="s">
+        <v>811</v>
       </c>
       <c r="D278" s="25"/>
       <c r="E278" s="25" t="s">
@@ -12212,19 +12218,19 @@
         <v>15</v>
       </c>
       <c r="H278" s="25" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I278" s="27"/>
     </row>
-    <row r="279" spans="1:9" ht="30">
+    <row r="279" spans="1:9" ht="180">
       <c r="A279" s="25" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B279" s="20" t="s">
-        <v>820</v>
-      </c>
-      <c r="C279" s="16" t="s">
-        <v>813</v>
+        <v>819</v>
+      </c>
+      <c r="C279" s="27" t="s">
+        <v>492</v>
       </c>
       <c r="D279" s="25"/>
       <c r="E279" s="25" t="s">
@@ -12234,22 +12240,22 @@
         <v>6</v>
       </c>
       <c r="G279" s="25" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H279" s="25" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="I279" s="27"/>
     </row>
     <row r="280" spans="1:9" ht="30">
       <c r="A280" s="25" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B280" s="20" t="s">
-        <v>820</v>
+        <v>819</v>
       </c>
       <c r="C280" s="16" t="s">
-        <v>814</v>
+        <v>812</v>
       </c>
       <c r="D280" s="25"/>
       <c r="E280" s="25" t="s">
@@ -12259,22 +12265,22 @@
         <v>6</v>
       </c>
       <c r="G280" s="25" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H280" s="25" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I280" s="27"/>
     </row>
     <row r="281" spans="1:9" ht="30">
       <c r="A281" s="25" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B281" s="20" t="s">
-        <v>820</v>
-      </c>
-      <c r="C281" s="27" t="s">
-        <v>493</v>
+        <v>819</v>
+      </c>
+      <c r="C281" s="16" t="s">
+        <v>813</v>
       </c>
       <c r="D281" s="25"/>
       <c r="E281" s="25" t="s">
@@ -12287,19 +12293,19 @@
         <v>15</v>
       </c>
       <c r="H281" s="25" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="I281" s="27"/>
     </row>
     <row r="282" spans="1:9" ht="30">
       <c r="A282" s="25" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B282" s="20" t="s">
-        <v>820</v>
+        <v>819</v>
       </c>
       <c r="C282" s="27" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="D282" s="25"/>
       <c r="E282" s="25" t="s">
@@ -12312,19 +12318,19 @@
         <v>15</v>
       </c>
       <c r="H282" s="25" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I282" s="27"/>
     </row>
     <row r="283" spans="1:9" ht="30">
       <c r="A283" s="25" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B283" s="20" t="s">
-        <v>820</v>
+        <v>819</v>
       </c>
       <c r="C283" s="27" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="D283" s="25"/>
       <c r="E283" s="25" t="s">
@@ -12337,23 +12343,21 @@
         <v>15</v>
       </c>
       <c r="H283" s="25" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="I283" s="27"/>
     </row>
     <row r="284" spans="1:9" ht="30">
       <c r="A284" s="25" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B284" s="20" t="s">
-        <v>820</v>
+        <v>819</v>
       </c>
       <c r="C284" s="27" t="s">
-        <v>496</v>
-      </c>
-      <c r="D284" s="25" t="s">
-        <v>660</v>
-      </c>
+        <v>495</v>
+      </c>
+      <c r="D284" s="25"/>
       <c r="E284" s="25" t="s">
         <v>19</v>
       </c>
@@ -12370,13 +12374,13 @@
     </row>
     <row r="285" spans="1:9" ht="30">
       <c r="A285" s="25" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B285" s="20" t="s">
-        <v>820</v>
+        <v>819</v>
       </c>
       <c r="C285" s="27" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="D285" s="25" t="s">
         <v>660</v>
@@ -12395,17 +12399,19 @@
       </c>
       <c r="I285" s="27"/>
     </row>
-    <row r="286" spans="1:9" ht="45">
+    <row r="286" spans="1:9" ht="30">
       <c r="A286" s="25" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B286" s="20" t="s">
-        <v>821</v>
+        <v>819</v>
       </c>
       <c r="C286" s="27" t="s">
-        <v>498</v>
-      </c>
-      <c r="D286" s="25"/>
+        <v>497</v>
+      </c>
+      <c r="D286" s="25" t="s">
+        <v>660</v>
+      </c>
       <c r="E286" s="25" t="s">
         <v>19</v>
       </c>
@@ -12416,19 +12422,19 @@
         <v>15</v>
       </c>
       <c r="H286" s="25" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I286" s="27"/>
     </row>
     <row r="287" spans="1:9" ht="45">
       <c r="A287" s="25" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B287" s="20" t="s">
-        <v>821</v>
-      </c>
-      <c r="C287" s="16" t="s">
-        <v>815</v>
+        <v>820</v>
+      </c>
+      <c r="C287" s="27" t="s">
+        <v>498</v>
       </c>
       <c r="D287" s="25"/>
       <c r="E287" s="25" t="s">
@@ -12441,19 +12447,19 @@
         <v>15</v>
       </c>
       <c r="H287" s="25" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="I287" s="27"/>
     </row>
-    <row r="288" spans="1:9" ht="360">
+    <row r="288" spans="1:9" ht="45">
       <c r="A288" s="25" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B288" s="20" t="s">
-        <v>821</v>
-      </c>
-      <c r="C288" s="27" t="s">
-        <v>499</v>
+        <v>820</v>
+      </c>
+      <c r="C288" s="16" t="s">
+        <v>814</v>
       </c>
       <c r="D288" s="25"/>
       <c r="E288" s="25" t="s">
@@ -12466,19 +12472,19 @@
         <v>15</v>
       </c>
       <c r="H288" s="25" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I288" s="27"/>
     </row>
-    <row r="289" spans="1:9" ht="45">
+    <row r="289" spans="1:9" ht="360">
       <c r="A289" s="25" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B289" s="20" t="s">
-        <v>821</v>
-      </c>
-      <c r="C289" s="16" t="s">
-        <v>816</v>
+        <v>820</v>
+      </c>
+      <c r="C289" s="27" t="s">
+        <v>499</v>
       </c>
       <c r="D289" s="25"/>
       <c r="E289" s="25" t="s">
@@ -12488,22 +12494,22 @@
         <v>6</v>
       </c>
       <c r="G289" s="25" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H289" s="25" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="I289" s="27"/>
     </row>
-    <row r="290" spans="1:9" ht="30">
+    <row r="290" spans="1:9" ht="45">
       <c r="A290" s="25" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B290" s="20" t="s">
-        <v>821</v>
-      </c>
-      <c r="C290" s="27" t="s">
-        <v>500</v>
+        <v>820</v>
+      </c>
+      <c r="C290" s="16" t="s">
+        <v>815</v>
       </c>
       <c r="D290" s="25"/>
       <c r="E290" s="25" t="s">
@@ -12513,22 +12519,22 @@
         <v>6</v>
       </c>
       <c r="G290" s="25" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H290" s="25" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I290" s="27"/>
     </row>
-    <row r="291" spans="1:9" ht="45">
+    <row r="291" spans="1:9" ht="30">
       <c r="A291" s="25" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B291" s="20" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
       <c r="C291" s="27" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="D291" s="25"/>
       <c r="E291" s="25" t="s">
@@ -12541,19 +12547,19 @@
         <v>15</v>
       </c>
       <c r="H291" s="25" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="I291" s="27"/>
     </row>
-    <row r="292" spans="1:9" ht="30">
+    <row r="292" spans="1:9" ht="45">
       <c r="A292" s="25" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B292" s="20" t="s">
-        <v>821</v>
-      </c>
-      <c r="C292" s="16" t="s">
-        <v>817</v>
+        <v>820</v>
+      </c>
+      <c r="C292" s="27" t="s">
+        <v>501</v>
       </c>
       <c r="D292" s="25"/>
       <c r="E292" s="25" t="s">
@@ -12563,22 +12569,22 @@
         <v>6</v>
       </c>
       <c r="G292" s="25" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H292" s="25" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="I292" s="27"/>
     </row>
     <row r="293" spans="1:9" ht="30">
       <c r="A293" s="25" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B293" s="20" t="s">
-        <v>821</v>
-      </c>
-      <c r="C293" s="27" t="s">
-        <v>502</v>
+        <v>820</v>
+      </c>
+      <c r="C293" s="16" t="s">
+        <v>816</v>
       </c>
       <c r="D293" s="25"/>
       <c r="E293" s="25" t="s">
@@ -12588,22 +12594,22 @@
         <v>6</v>
       </c>
       <c r="G293" s="25" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H293" s="25" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I293" s="27"/>
     </row>
-    <row r="294" spans="1:9" ht="45">
+    <row r="294" spans="1:9" ht="30">
       <c r="A294" s="25" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B294" s="20" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
       <c r="C294" s="27" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="D294" s="25"/>
       <c r="E294" s="25" t="s">
@@ -12616,23 +12622,21 @@
         <v>15</v>
       </c>
       <c r="H294" s="25" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="I294" s="27"/>
     </row>
     <row r="295" spans="1:9" ht="45">
       <c r="A295" s="25" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B295" s="20" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
       <c r="C295" s="27" t="s">
-        <v>504</v>
-      </c>
-      <c r="D295" s="25" t="s">
-        <v>661</v>
-      </c>
+        <v>503</v>
+      </c>
+      <c r="D295" s="25"/>
       <c r="E295" s="25" t="s">
         <v>19</v>
       </c>
@@ -12649,13 +12653,13 @@
     </row>
     <row r="296" spans="1:9" ht="45">
       <c r="A296" s="25" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B296" s="20" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
       <c r="C296" s="27" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="D296" s="25" t="s">
         <v>661</v>
@@ -12674,17 +12678,19 @@
       </c>
       <c r="I296" s="27"/>
     </row>
-    <row r="297" spans="1:9" ht="30">
+    <row r="297" spans="1:9" ht="45">
       <c r="A297" s="25" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B297" s="20" t="s">
-        <v>821</v>
-      </c>
-      <c r="C297" s="16" t="s">
-        <v>822</v>
-      </c>
-      <c r="D297" s="25"/>
+        <v>820</v>
+      </c>
+      <c r="C297" s="27" t="s">
+        <v>505</v>
+      </c>
+      <c r="D297" s="25" t="s">
+        <v>661</v>
+      </c>
       <c r="E297" s="25" t="s">
         <v>19</v>
       </c>
@@ -12692,22 +12698,22 @@
         <v>6</v>
       </c>
       <c r="G297" s="25" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H297" s="25" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="I297" s="27"/>
     </row>
     <row r="298" spans="1:9" ht="30">
       <c r="A298" s="25" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B298" s="20" t="s">
+        <v>820</v>
+      </c>
+      <c r="C298" s="16" t="s">
         <v>821</v>
-      </c>
-      <c r="C298" s="27" t="s">
-        <v>506</v>
       </c>
       <c r="D298" s="25"/>
       <c r="E298" s="25" t="s">
@@ -12717,22 +12723,22 @@
         <v>6</v>
       </c>
       <c r="G298" s="25" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H298" s="25" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I298" s="27"/>
     </row>
     <row r="299" spans="1:9" ht="30">
       <c r="A299" s="25" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B299" s="20" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
       <c r="C299" s="27" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="D299" s="25"/>
       <c r="E299" s="25" t="s">
@@ -12745,19 +12751,19 @@
         <v>15</v>
       </c>
       <c r="H299" s="25" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="I299" s="27"/>
     </row>
     <row r="300" spans="1:9" ht="30">
       <c r="A300" s="25" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B300" s="20" t="s">
-        <v>821</v>
-      </c>
-      <c r="C300" s="16" t="s">
-        <v>818</v>
+        <v>820</v>
+      </c>
+      <c r="C300" s="27" t="s">
+        <v>507</v>
       </c>
       <c r="D300" s="25"/>
       <c r="E300" s="25" t="s">
@@ -12767,22 +12773,22 @@
         <v>6</v>
       </c>
       <c r="G300" s="25" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H300" s="25" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="I300" s="27"/>
     </row>
     <row r="301" spans="1:9" ht="30">
       <c r="A301" s="25" t="s">
-        <v>345</v>
+        <v>188</v>
       </c>
       <c r="B301" s="20" t="s">
-        <v>824</v>
-      </c>
-      <c r="C301" s="27" t="s">
-        <v>625</v>
+        <v>820</v>
+      </c>
+      <c r="C301" s="16" t="s">
+        <v>817</v>
       </c>
       <c r="D301" s="25"/>
       <c r="E301" s="25" t="s">
@@ -12799,15 +12805,15 @@
       </c>
       <c r="I301" s="27"/>
     </row>
-    <row r="302" spans="1:9" ht="45">
+    <row r="302" spans="1:9" ht="30">
       <c r="A302" s="25" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="B302" s="20" t="s">
-        <v>824</v>
-      </c>
-      <c r="C302" s="16" t="s">
         <v>823</v>
+      </c>
+      <c r="C302" s="27" t="s">
+        <v>625</v>
       </c>
       <c r="D302" s="25"/>
       <c r="E302" s="25" t="s">
@@ -12817,22 +12823,22 @@
         <v>6</v>
       </c>
       <c r="G302" s="25" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H302" s="25" t="s">
         <v>18</v>
       </c>
       <c r="I302" s="27"/>
     </row>
-    <row r="303" spans="1:9" ht="135">
+    <row r="303" spans="1:9" ht="45">
       <c r="A303" s="25" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B303" s="20" t="s">
-        <v>824</v>
-      </c>
-      <c r="C303" s="27" t="s">
-        <v>626</v>
+        <v>823</v>
+      </c>
+      <c r="C303" s="16" t="s">
+        <v>822</v>
       </c>
       <c r="D303" s="25"/>
       <c r="E303" s="25" t="s">
@@ -12845,44 +12851,44 @@
         <v>15</v>
       </c>
       <c r="H303" s="25" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I303" s="27"/>
     </row>
-    <row r="304" spans="1:9" ht="30">
+    <row r="304" spans="1:9" ht="135">
       <c r="A304" s="25" t="s">
-        <v>307</v>
+        <v>347</v>
       </c>
       <c r="B304" s="20" t="s">
-        <v>825</v>
-      </c>
-      <c r="C304" s="16" t="s">
-        <v>826</v>
+        <v>823</v>
+      </c>
+      <c r="C304" s="27" t="s">
+        <v>626</v>
       </c>
       <c r="D304" s="25"/>
       <c r="E304" s="25" t="s">
         <v>19</v>
       </c>
       <c r="F304" s="25" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G304" s="25" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H304" s="25" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="I304" s="27"/>
     </row>
     <row r="305" spans="1:9" ht="30">
       <c r="A305" s="25" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B305" s="20" t="s">
+        <v>824</v>
+      </c>
+      <c r="C305" s="16" t="s">
         <v>825</v>
-      </c>
-      <c r="C305" s="16" t="s">
-        <v>827</v>
       </c>
       <c r="D305" s="25"/>
       <c r="E305" s="25" t="s">
@@ -12892,22 +12898,22 @@
         <v>7</v>
       </c>
       <c r="G305" s="25" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H305" s="25" t="s">
         <v>18</v>
       </c>
       <c r="I305" s="27"/>
     </row>
-    <row r="306" spans="1:9" ht="409.5">
+    <row r="306" spans="1:9" ht="30">
       <c r="A306" s="25" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B306" s="20" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
       <c r="C306" s="16" t="s">
-        <v>599</v>
+        <v>826</v>
       </c>
       <c r="D306" s="25"/>
       <c r="E306" s="25" t="s">
@@ -12924,15 +12930,15 @@
       </c>
       <c r="I306" s="27"/>
     </row>
-    <row r="307" spans="1:9" ht="45">
+    <row r="307" spans="1:9" ht="409.5">
       <c r="A307" s="25" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B307" s="20" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
       <c r="C307" s="16" t="s">
-        <v>828</v>
+        <v>599</v>
       </c>
       <c r="D307" s="25"/>
       <c r="E307" s="25" t="s">
@@ -12942,22 +12948,22 @@
         <v>7</v>
       </c>
       <c r="G307" s="25" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H307" s="25" t="s">
         <v>18</v>
       </c>
       <c r="I307" s="27"/>
     </row>
-    <row r="308" spans="1:9" ht="30">
+    <row r="308" spans="1:9" ht="45">
       <c r="A308" s="25" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B308" s="20" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
       <c r="C308" s="16" t="s">
-        <v>829</v>
+        <v>827</v>
       </c>
       <c r="D308" s="25"/>
       <c r="E308" s="25" t="s">
@@ -12967,53 +12973,49 @@
         <v>7</v>
       </c>
       <c r="G308" s="25" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H308" s="25" t="s">
         <v>18</v>
       </c>
       <c r="I308" s="27"/>
     </row>
-    <row r="309" spans="1:9" ht="165">
+    <row r="309" spans="1:9" ht="30">
       <c r="A309" s="25" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B309" s="20" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
       <c r="C309" s="16" t="s">
-        <v>600</v>
+        <v>828</v>
       </c>
       <c r="D309" s="25"/>
       <c r="E309" s="25" t="s">
         <v>19</v>
       </c>
       <c r="F309" s="25" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="G309" s="25" t="s">
         <v>15</v>
       </c>
       <c r="H309" s="25" t="s">
-        <v>17</v>
-      </c>
-      <c r="I309" s="16" t="s">
-        <v>857</v>
-      </c>
-    </row>
-    <row r="310" spans="1:9" ht="30">
-      <c r="A310" s="18" t="s">
-        <v>313</v>
+        <v>18</v>
+      </c>
+      <c r="I309" s="27"/>
+    </row>
+    <row r="310" spans="1:9" ht="165">
+      <c r="A310" s="25" t="s">
+        <v>312</v>
       </c>
       <c r="B310" s="20" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
       <c r="C310" s="16" t="s">
-        <v>853</v>
-      </c>
-      <c r="D310" s="25" t="s">
-        <v>669</v>
-      </c>
+        <v>600</v>
+      </c>
+      <c r="D310" s="25"/>
       <c r="E310" s="25" t="s">
         <v>19</v>
       </c>
@@ -13023,23 +13025,25 @@
       <c r="G310" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="H310" s="18" t="s">
-        <v>20</v>
-      </c>
-      <c r="I310" s="27"/>
+      <c r="H310" s="25" t="s">
+        <v>17</v>
+      </c>
+      <c r="I310" s="16" t="s">
+        <v>856</v>
+      </c>
     </row>
     <row r="311" spans="1:9" ht="30">
-      <c r="A311" s="25" t="s">
-        <v>314</v>
+      <c r="A311" s="18" t="s">
+        <v>313</v>
       </c>
       <c r="B311" s="20" t="s">
-        <v>825</v>
-      </c>
-      <c r="C311" s="27" t="s">
-        <v>601</v>
+        <v>824</v>
+      </c>
+      <c r="C311" s="16" t="s">
+        <v>852</v>
       </c>
       <c r="D311" s="25" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="E311" s="25" t="s">
         <v>19</v>
@@ -13057,16 +13061,16 @@
     </row>
     <row r="312" spans="1:9" ht="30">
       <c r="A312" s="25" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B312" s="20" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
       <c r="C312" s="27" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="D312" s="25" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="E312" s="25" t="s">
         <v>19</v>
@@ -13077,23 +13081,23 @@
       <c r="G312" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="H312" s="25" t="s">
+      <c r="H312" s="18" t="s">
         <v>20</v>
       </c>
       <c r="I312" s="27"/>
     </row>
-    <row r="313" spans="1:9" ht="45">
+    <row r="313" spans="1:9" ht="30">
       <c r="A313" s="25" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B313" s="20" t="s">
-        <v>825</v>
-      </c>
-      <c r="C313" s="16" t="s">
-        <v>856</v>
+        <v>824</v>
+      </c>
+      <c r="C313" s="27" t="s">
+        <v>602</v>
       </c>
       <c r="D313" s="25" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="E313" s="25" t="s">
         <v>19</v>
@@ -13104,23 +13108,23 @@
       <c r="G313" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="H313" s="18" t="s">
+      <c r="H313" s="25" t="s">
         <v>20</v>
       </c>
       <c r="I313" s="27"/>
     </row>
     <row r="314" spans="1:9" ht="45">
-      <c r="A314" s="18" t="s">
-        <v>317</v>
+      <c r="A314" s="25" t="s">
+        <v>316</v>
       </c>
       <c r="B314" s="20" t="s">
-        <v>825</v>
-      </c>
-      <c r="C314" s="27" t="s">
-        <v>603</v>
-      </c>
-      <c r="D314" s="18" t="s">
-        <v>673</v>
+        <v>824</v>
+      </c>
+      <c r="C314" s="16" t="s">
+        <v>855</v>
+      </c>
+      <c r="D314" s="25" t="s">
+        <v>672</v>
       </c>
       <c r="E314" s="25" t="s">
         <v>19</v>
@@ -13137,17 +13141,17 @@
       <c r="I314" s="27"/>
     </row>
     <row r="315" spans="1:9" ht="45">
-      <c r="A315" s="25" t="s">
-        <v>318</v>
+      <c r="A315" s="18" t="s">
+        <v>317</v>
       </c>
       <c r="B315" s="20" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
       <c r="C315" s="27" t="s">
-        <v>604</v>
-      </c>
-      <c r="D315" s="25" t="s">
-        <v>674</v>
+        <v>603</v>
+      </c>
+      <c r="D315" s="18" t="s">
+        <v>673</v>
       </c>
       <c r="E315" s="25" t="s">
         <v>19</v>
@@ -13163,18 +13167,18 @@
       </c>
       <c r="I315" s="27"/>
     </row>
-    <row r="316" spans="1:9" ht="30">
+    <row r="316" spans="1:9" ht="45">
       <c r="A316" s="25" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B316" s="20" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
       <c r="C316" s="27" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="D316" s="25" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="E316" s="25" t="s">
         <v>19</v>
@@ -13185,23 +13189,23 @@
       <c r="G316" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="H316" s="25" t="s">
+      <c r="H316" s="18" t="s">
         <v>20</v>
       </c>
       <c r="I316" s="27"/>
     </row>
     <row r="317" spans="1:9" ht="30">
       <c r="A317" s="25" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B317" s="20" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
       <c r="C317" s="27" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="D317" s="25" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="E317" s="25" t="s">
         <v>19</v>
@@ -13219,88 +13223,90 @@
     </row>
     <row r="318" spans="1:9" ht="30">
       <c r="A318" s="25" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B318" s="20" t="s">
-        <v>825</v>
-      </c>
-      <c r="C318" s="16" t="s">
-        <v>830</v>
-      </c>
-      <c r="D318" s="25"/>
+        <v>824</v>
+      </c>
+      <c r="C318" s="27" t="s">
+        <v>606</v>
+      </c>
+      <c r="D318" s="25" t="s">
+        <v>676</v>
+      </c>
       <c r="E318" s="25" t="s">
         <v>19</v>
       </c>
       <c r="F318" s="25" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="G318" s="25" t="s">
         <v>15</v>
       </c>
       <c r="H318" s="25" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="I318" s="27"/>
     </row>
     <row r="319" spans="1:9" ht="30">
       <c r="A319" s="25" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B319" s="20" t="s">
-        <v>825</v>
-      </c>
-      <c r="C319" s="27" t="s">
-        <v>607</v>
+        <v>824</v>
+      </c>
+      <c r="C319" s="16" t="s">
+        <v>829</v>
       </c>
       <c r="D319" s="25"/>
       <c r="E319" s="25" t="s">
         <v>19</v>
       </c>
       <c r="F319" s="25" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="G319" s="25" t="s">
         <v>15</v>
       </c>
       <c r="H319" s="25" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I319" s="27"/>
     </row>
     <row r="320" spans="1:9" ht="30">
       <c r="A320" s="25" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B320" s="20" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
       <c r="C320" s="27" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="D320" s="25"/>
       <c r="E320" s="25" t="s">
         <v>19</v>
       </c>
       <c r="F320" s="25" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="G320" s="25" t="s">
         <v>15</v>
       </c>
       <c r="H320" s="25" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="I320" s="27"/>
     </row>
     <row r="321" spans="1:9" ht="30">
       <c r="A321" s="25" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B321" s="20" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
       <c r="C321" s="27" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="D321" s="25"/>
       <c r="E321" s="25" t="s">
@@ -13317,47 +13323,47 @@
       </c>
       <c r="I321" s="27"/>
     </row>
-    <row r="322" spans="1:9" ht="45">
+    <row r="322" spans="1:9" ht="30">
       <c r="A322" s="25" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B322" s="20" t="s">
-        <v>825</v>
-      </c>
-      <c r="C322" s="16" t="s">
-        <v>831</v>
+        <v>824</v>
+      </c>
+      <c r="C322" s="27" t="s">
+        <v>609</v>
       </c>
       <c r="D322" s="25"/>
       <c r="E322" s="25" t="s">
         <v>19</v>
       </c>
       <c r="F322" s="25" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G322" s="25" t="s">
         <v>15</v>
       </c>
       <c r="H322" s="25" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I322" s="27"/>
     </row>
-    <row r="323" spans="1:9">
+    <row r="323" spans="1:9" ht="45">
       <c r="A323" s="25" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B323" s="20" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
       <c r="C323" s="16" t="s">
-        <v>832</v>
+        <v>830</v>
       </c>
       <c r="D323" s="25"/>
       <c r="E323" s="25" t="s">
         <v>19</v>
       </c>
       <c r="F323" s="25" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="G323" s="25" t="s">
         <v>15</v>
@@ -13367,19 +13373,17 @@
       </c>
       <c r="I323" s="27"/>
     </row>
-    <row r="324" spans="1:9" ht="30">
-      <c r="A324" s="18" t="s">
-        <v>327</v>
+    <row r="324" spans="1:9">
+      <c r="A324" s="25" t="s">
+        <v>326</v>
       </c>
       <c r="B324" s="20" t="s">
-        <v>825</v>
-      </c>
-      <c r="C324" s="27" t="s">
-        <v>610</v>
-      </c>
-      <c r="D324" s="25" t="s">
-        <v>677</v>
-      </c>
+        <v>824</v>
+      </c>
+      <c r="C324" s="16" t="s">
+        <v>831</v>
+      </c>
+      <c r="D324" s="25"/>
       <c r="E324" s="25" t="s">
         <v>19</v>
       </c>
@@ -13389,20 +13393,20 @@
       <c r="G324" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="H324" s="18" t="s">
+      <c r="H324" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="I324" s="16"/>
+      <c r="I324" s="27"/>
     </row>
     <row r="325" spans="1:9" ht="30">
-      <c r="A325" s="25" t="s">
-        <v>328</v>
+      <c r="A325" s="18" t="s">
+        <v>327</v>
       </c>
       <c r="B325" s="20" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
       <c r="C325" s="27" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="D325" s="25" t="s">
         <v>677</v>
@@ -13416,74 +13420,74 @@
       <c r="G325" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="H325" s="25" t="s">
+      <c r="H325" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="I325" s="27"/>
+      <c r="I325" s="16"/>
     </row>
     <row r="326" spans="1:9" ht="30">
       <c r="A326" s="25" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B326" s="20" t="s">
-        <v>825</v>
-      </c>
-      <c r="C326" s="16" t="s">
-        <v>833</v>
-      </c>
-      <c r="D326" s="25"/>
+        <v>824</v>
+      </c>
+      <c r="C326" s="27" t="s">
+        <v>611</v>
+      </c>
+      <c r="D326" s="25" t="s">
+        <v>677</v>
+      </c>
       <c r="E326" s="25" t="s">
         <v>19</v>
       </c>
       <c r="F326" s="25" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="G326" s="25" t="s">
         <v>15</v>
       </c>
       <c r="H326" s="25" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="I326" s="27"/>
     </row>
     <row r="327" spans="1:9" ht="30">
       <c r="A327" s="25" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B327" s="20" t="s">
-        <v>825</v>
-      </c>
-      <c r="C327" s="27" t="s">
-        <v>612</v>
+        <v>824</v>
+      </c>
+      <c r="C327" s="16" t="s">
+        <v>832</v>
       </c>
       <c r="D327" s="25"/>
       <c r="E327" s="25" t="s">
         <v>19</v>
       </c>
       <c r="F327" s="25" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="G327" s="25" t="s">
         <v>15</v>
       </c>
       <c r="H327" s="25" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I327" s="27"/>
     </row>
     <row r="328" spans="1:9" ht="30">
       <c r="A328" s="25" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B328" s="20" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
       <c r="C328" s="27" t="s">
-        <v>613</v>
-      </c>
-      <c r="D328" s="25" t="s">
-        <v>678</v>
-      </c>
+        <v>612</v>
+      </c>
+      <c r="D328" s="25"/>
       <c r="E328" s="25" t="s">
         <v>19</v>
       </c>
@@ -13500,13 +13504,13 @@
     </row>
     <row r="329" spans="1:9" ht="30">
       <c r="A329" s="25" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B329" s="20" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
       <c r="C329" s="27" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="D329" s="25" t="s">
         <v>678</v>
@@ -13525,17 +13529,19 @@
       </c>
       <c r="I329" s="27"/>
     </row>
-    <row r="330" spans="1:9">
+    <row r="330" spans="1:9" ht="30">
       <c r="A330" s="25" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B330" s="20" t="s">
-        <v>825</v>
-      </c>
-      <c r="C330" s="16" t="s">
-        <v>834</v>
-      </c>
-      <c r="D330" s="25"/>
+        <v>824</v>
+      </c>
+      <c r="C330" s="27" t="s">
+        <v>614</v>
+      </c>
+      <c r="D330" s="25" t="s">
+        <v>678</v>
+      </c>
       <c r="E330" s="25" t="s">
         <v>19</v>
       </c>
@@ -13545,24 +13551,22 @@
       <c r="G330" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="H330" s="18" t="s">
+      <c r="H330" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="I330" s="16"/>
-    </row>
-    <row r="331" spans="1:9" ht="30">
-      <c r="A331" s="18" t="s">
-        <v>334</v>
+      <c r="I330" s="27"/>
+    </row>
+    <row r="331" spans="1:9">
+      <c r="A331" s="25" t="s">
+        <v>333</v>
       </c>
       <c r="B331" s="20" t="s">
-        <v>825</v>
-      </c>
-      <c r="C331" s="27" t="s">
-        <v>615</v>
-      </c>
-      <c r="D331" s="25" t="s">
-        <v>679</v>
-      </c>
+        <v>824</v>
+      </c>
+      <c r="C331" s="16" t="s">
+        <v>833</v>
+      </c>
+      <c r="D331" s="25"/>
       <c r="E331" s="25" t="s">
         <v>19</v>
       </c>
@@ -13572,20 +13576,20 @@
       <c r="G331" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="H331" s="25" t="s">
+      <c r="H331" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="I331" s="27"/>
+      <c r="I331" s="16"/>
     </row>
     <row r="332" spans="1:9" ht="30">
-      <c r="A332" s="25" t="s">
-        <v>335</v>
+      <c r="A332" s="18" t="s">
+        <v>334</v>
       </c>
       <c r="B332" s="20" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
       <c r="C332" s="27" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="D332" s="25" t="s">
         <v>679</v>
@@ -13606,63 +13610,65 @@
     </row>
     <row r="333" spans="1:9" ht="30">
       <c r="A333" s="25" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B333" s="20" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
       <c r="C333" s="27" t="s">
-        <v>617</v>
-      </c>
-      <c r="D333" s="25"/>
+        <v>616</v>
+      </c>
+      <c r="D333" s="25" t="s">
+        <v>679</v>
+      </c>
       <c r="E333" s="25" t="s">
         <v>19</v>
       </c>
       <c r="F333" s="25" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="G333" s="25" t="s">
         <v>15</v>
       </c>
       <c r="H333" s="25" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="I333" s="27"/>
     </row>
     <row r="334" spans="1:9" ht="30">
       <c r="A334" s="25" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B334" s="20" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
       <c r="C334" s="27" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="D334" s="25"/>
       <c r="E334" s="25" t="s">
         <v>19</v>
       </c>
       <c r="F334" s="25" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="G334" s="25" t="s">
         <v>15</v>
       </c>
       <c r="H334" s="25" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I334" s="27"/>
     </row>
-    <row r="335" spans="1:9" ht="45">
+    <row r="335" spans="1:9" ht="30">
       <c r="A335" s="25" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B335" s="20" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
       <c r="C335" s="27" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="D335" s="25"/>
       <c r="E335" s="25" t="s">
@@ -13675,25 +13681,21 @@
         <v>15</v>
       </c>
       <c r="H335" s="25" t="s">
-        <v>17</v>
-      </c>
-      <c r="I335" s="16" t="s">
-        <v>688</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="I335" s="27"/>
     </row>
     <row r="336" spans="1:9" ht="45">
       <c r="A336" s="25" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B336" s="20" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
       <c r="C336" s="27" t="s">
-        <v>620</v>
-      </c>
-      <c r="D336" s="25" t="s">
-        <v>680</v>
-      </c>
+        <v>619</v>
+      </c>
+      <c r="D336" s="25"/>
       <c r="E336" s="25" t="s">
         <v>19</v>
       </c>
@@ -13704,44 +13706,48 @@
         <v>15</v>
       </c>
       <c r="H336" s="25" t="s">
+        <v>17</v>
+      </c>
+      <c r="I336" s="16" t="s">
+        <v>688</v>
+      </c>
+    </row>
+    <row r="337" spans="1:9" ht="45">
+      <c r="A337" s="25" t="s">
+        <v>339</v>
+      </c>
+      <c r="B337" s="20" t="s">
+        <v>824</v>
+      </c>
+      <c r="C337" s="27" t="s">
+        <v>620</v>
+      </c>
+      <c r="D337" s="25" t="s">
+        <v>680</v>
+      </c>
+      <c r="E337" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="F337" s="25" t="s">
+        <v>3</v>
+      </c>
+      <c r="G337" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="H337" s="25" t="s">
         <v>20</v>
-      </c>
-      <c r="I336" s="27"/>
-    </row>
-    <row r="337" spans="1:9" ht="30">
-      <c r="A337" s="25" t="s">
-        <v>340</v>
-      </c>
-      <c r="B337" s="20" t="s">
-        <v>825</v>
-      </c>
-      <c r="C337" s="27" t="s">
-        <v>621</v>
-      </c>
-      <c r="D337" s="25"/>
-      <c r="E337" s="25" t="s">
-        <v>19</v>
-      </c>
-      <c r="F337" s="25" t="s">
-        <v>7</v>
-      </c>
-      <c r="G337" s="25" t="s">
-        <v>15</v>
-      </c>
-      <c r="H337" s="25" t="s">
-        <v>18</v>
       </c>
       <c r="I337" s="27"/>
     </row>
     <row r="338" spans="1:9" ht="30">
       <c r="A338" s="25" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B338" s="20" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
       <c r="C338" s="27" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="D338" s="25"/>
       <c r="E338" s="25" t="s">
@@ -13758,44 +13764,42 @@
       </c>
       <c r="I338" s="27"/>
     </row>
-    <row r="339" spans="1:9">
-      <c r="A339" s="18" t="s">
-        <v>342</v>
+    <row r="339" spans="1:9" ht="30">
+      <c r="A339" s="25" t="s">
+        <v>341</v>
       </c>
       <c r="B339" s="20" t="s">
-        <v>825</v>
-      </c>
-      <c r="C339" s="16" t="s">
-        <v>835</v>
+        <v>824</v>
+      </c>
+      <c r="C339" s="27" t="s">
+        <v>622</v>
       </c>
       <c r="D339" s="25"/>
       <c r="E339" s="25" t="s">
         <v>19</v>
       </c>
       <c r="F339" s="25" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="G339" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="H339" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="I339" s="16"/>
-    </row>
-    <row r="340" spans="1:9" ht="45">
+      <c r="H339" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="I339" s="27"/>
+    </row>
+    <row r="340" spans="1:9">
       <c r="A340" s="18" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="B340" s="20" t="s">
-        <v>825</v>
-      </c>
-      <c r="C340" s="27" t="s">
-        <v>623</v>
-      </c>
-      <c r="D340" s="25" t="s">
-        <v>681</v>
-      </c>
+        <v>824</v>
+      </c>
+      <c r="C340" s="16" t="s">
+        <v>834</v>
+      </c>
+      <c r="D340" s="25"/>
       <c r="E340" s="25" t="s">
         <v>19</v>
       </c>
@@ -13808,19 +13812,17 @@
       <c r="H340" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="I340" s="16" t="s">
-        <v>847</v>
-      </c>
+      <c r="I340" s="16"/>
     </row>
     <row r="341" spans="1:9" ht="45">
-      <c r="A341" s="25" t="s">
-        <v>344</v>
+      <c r="A341" s="18" t="s">
+        <v>343</v>
       </c>
       <c r="B341" s="20" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
       <c r="C341" s="27" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="D341" s="25" t="s">
         <v>681</v>
@@ -13838,20 +13840,22 @@
         <v>17</v>
       </c>
       <c r="I341" s="16" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
     </row>
     <row r="342" spans="1:9" ht="45">
       <c r="A342" s="25" t="s">
-        <v>352</v>
-      </c>
-      <c r="B342" s="26" t="s">
-        <v>425</v>
+        <v>344</v>
+      </c>
+      <c r="B342" s="20" t="s">
+        <v>824</v>
       </c>
       <c r="C342" s="27" t="s">
-        <v>628</v>
-      </c>
-      <c r="D342" s="25"/>
+        <v>624</v>
+      </c>
+      <c r="D342" s="25" t="s">
+        <v>681</v>
+      </c>
       <c r="E342" s="25" t="s">
         <v>19</v>
       </c>
@@ -13859,32 +13863,34 @@
         <v>3</v>
       </c>
       <c r="G342" s="25" t="s">
-        <v>16</v>
-      </c>
-      <c r="H342" s="25" t="s">
-        <v>18</v>
-      </c>
-      <c r="I342" s="27"/>
-    </row>
-    <row r="343" spans="1:9" ht="30">
+        <v>15</v>
+      </c>
+      <c r="H342" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="I342" s="16" t="s">
+        <v>846</v>
+      </c>
+    </row>
+    <row r="343" spans="1:9" ht="45">
       <c r="A343" s="25" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="B343" s="26" t="s">
         <v>425</v>
       </c>
       <c r="C343" s="27" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="D343" s="25"/>
       <c r="E343" s="25" t="s">
         <v>19</v>
       </c>
       <c r="F343" s="25" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="G343" s="25" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H343" s="25" t="s">
         <v>18</v>
@@ -13893,13 +13899,13 @@
     </row>
     <row r="344" spans="1:9" ht="30">
       <c r="A344" s="25" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B344" s="26" t="s">
         <v>425</v>
       </c>
-      <c r="C344" s="16" t="s">
-        <v>630</v>
+      <c r="C344" s="27" t="s">
+        <v>629</v>
       </c>
       <c r="D344" s="25"/>
       <c r="E344" s="25" t="s">
@@ -13916,15 +13922,15 @@
       </c>
       <c r="I344" s="27"/>
     </row>
-    <row r="345" spans="1:9" ht="225">
+    <row r="345" spans="1:9" ht="30">
       <c r="A345" s="25" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B345" s="26" t="s">
-        <v>426</v>
-      </c>
-      <c r="C345" s="27" t="s">
-        <v>631</v>
+        <v>425</v>
+      </c>
+      <c r="C345" s="16" t="s">
+        <v>630</v>
       </c>
       <c r="D345" s="25"/>
       <c r="E345" s="25" t="s">
@@ -13941,15 +13947,15 @@
       </c>
       <c r="I345" s="27"/>
     </row>
-    <row r="346" spans="1:9" ht="210">
+    <row r="346" spans="1:9" ht="225">
       <c r="A346" s="25" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B346" s="26" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="C346" s="27" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="D346" s="25"/>
       <c r="E346" s="25" t="s">
@@ -13966,15 +13972,15 @@
       </c>
       <c r="I346" s="27"/>
     </row>
-    <row r="347" spans="1:9" ht="45">
+    <row r="347" spans="1:9" ht="210">
       <c r="A347" s="25" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B347" s="26" t="s">
         <v>427</v>
       </c>
       <c r="C347" s="27" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="D347" s="25"/>
       <c r="E347" s="25" t="s">
@@ -13984,47 +13990,47 @@
         <v>7</v>
       </c>
       <c r="G347" s="25" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H347" s="25" t="s">
         <v>18</v>
       </c>
       <c r="I347" s="27"/>
     </row>
-    <row r="348" spans="1:9" ht="30">
-      <c r="A348" s="18" t="s">
-        <v>358</v>
+    <row r="348" spans="1:9" ht="45">
+      <c r="A348" s="25" t="s">
+        <v>357</v>
       </c>
       <c r="B348" s="26" t="s">
         <v>427</v>
       </c>
       <c r="C348" s="27" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="D348" s="25"/>
       <c r="E348" s="25" t="s">
         <v>19</v>
       </c>
       <c r="F348" s="25" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="G348" s="25" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H348" s="25" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I348" s="27"/>
     </row>
     <row r="349" spans="1:9" ht="30">
-      <c r="A349" s="25" t="s">
-        <v>359</v>
+      <c r="A349" s="18" t="s">
+        <v>358</v>
       </c>
       <c r="B349" s="26" t="s">
         <v>427</v>
       </c>
-      <c r="C349" s="16" t="s">
-        <v>635</v>
+      <c r="C349" s="27" t="s">
+        <v>634</v>
       </c>
       <c r="D349" s="25"/>
       <c r="E349" s="25" t="s">
@@ -14036,45 +14042,45 @@
       <c r="G349" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="H349" s="18" t="s">
+      <c r="H349" s="25" t="s">
         <v>20</v>
       </c>
       <c r="I349" s="27"/>
     </row>
-    <row r="350" spans="1:9" ht="45">
-      <c r="A350" s="18" t="s">
-        <v>360</v>
+    <row r="350" spans="1:9" ht="30">
+      <c r="A350" s="25" t="s">
+        <v>359</v>
       </c>
       <c r="B350" s="26" t="s">
-        <v>428</v>
-      </c>
-      <c r="C350" s="27" t="s">
-        <v>636</v>
+        <v>427</v>
+      </c>
+      <c r="C350" s="16" t="s">
+        <v>635</v>
       </c>
       <c r="D350" s="25"/>
       <c r="E350" s="25" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="F350" s="25" t="s">
         <v>3</v>
       </c>
       <c r="G350" s="25" t="s">
-        <v>16</v>
-      </c>
-      <c r="H350" s="25" t="s">
-        <v>18</v>
+        <v>15</v>
+      </c>
+      <c r="H350" s="18" t="s">
+        <v>20</v>
       </c>
       <c r="I350" s="27"/>
     </row>
-    <row r="351" spans="1:9" ht="30">
-      <c r="A351" s="25" t="s">
-        <v>361</v>
+    <row r="351" spans="1:9" ht="45">
+      <c r="A351" s="18" t="s">
+        <v>360</v>
       </c>
       <c r="B351" s="26" t="s">
         <v>428</v>
       </c>
       <c r="C351" s="27" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="D351" s="25"/>
       <c r="E351" s="25" t="s">
@@ -14091,19 +14097,17 @@
       </c>
       <c r="I351" s="27"/>
     </row>
-    <row r="352" spans="1:9" ht="45">
+    <row r="352" spans="1:9" ht="30">
       <c r="A352" s="25" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B352" s="26" t="s">
         <v>428</v>
       </c>
       <c r="C352" s="27" t="s">
-        <v>638</v>
-      </c>
-      <c r="D352" s="25" t="s">
-        <v>682</v>
-      </c>
+        <v>637</v>
+      </c>
+      <c r="D352" s="25"/>
       <c r="E352" s="25" t="s">
         <v>22</v>
       </c>
@@ -14111,27 +14115,25 @@
         <v>3</v>
       </c>
       <c r="G352" s="25" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H352" s="25" t="s">
-        <v>21</v>
-      </c>
-      <c r="I352" s="27" t="s">
-        <v>689</v>
-      </c>
-    </row>
-    <row r="353" spans="1:9" ht="60">
+        <v>18</v>
+      </c>
+      <c r="I352" s="27"/>
+    </row>
+    <row r="353" spans="1:9" ht="45">
       <c r="A353" s="25" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B353" s="26" t="s">
         <v>428</v>
       </c>
       <c r="C353" s="27" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="D353" s="25" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="E353" s="25" t="s">
         <v>22</v>
@@ -14143,30 +14145,30 @@
         <v>15</v>
       </c>
       <c r="H353" s="25" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="I353" s="27" t="s">
         <v>689</v>
       </c>
     </row>
-    <row r="354" spans="1:9" ht="45">
+    <row r="354" spans="1:9" ht="60">
       <c r="A354" s="25" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="B354" s="26" t="s">
         <v>428</v>
       </c>
-      <c r="C354" s="16" t="s">
-        <v>640</v>
+      <c r="C354" s="27" t="s">
+        <v>639</v>
       </c>
       <c r="D354" s="25" t="s">
-        <v>684</v>
-      </c>
-      <c r="E354" s="18" t="s">
+        <v>683</v>
+      </c>
+      <c r="E354" s="25" t="s">
         <v>22</v>
       </c>
       <c r="F354" s="25" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="G354" s="25" t="s">
         <v>15</v>
@@ -14179,73 +14181,73 @@
       </c>
     </row>
     <row r="355" spans="1:9" ht="45">
-      <c r="A355" s="18" t="s">
-        <v>837</v>
-      </c>
-      <c r="B355" s="47" t="s">
+      <c r="A355" s="25" t="s">
+        <v>364</v>
+      </c>
+      <c r="B355" s="26" t="s">
         <v>428</v>
       </c>
-      <c r="C355" s="48" t="s">
-        <v>836</v>
-      </c>
-      <c r="D355" s="46" t="s">
-        <v>845</v>
-      </c>
-      <c r="E355" s="25" t="s">
+      <c r="C355" s="16" t="s">
+        <v>640</v>
+      </c>
+      <c r="D355" s="25" t="s">
+        <v>684</v>
+      </c>
+      <c r="E355" s="18" t="s">
         <v>22</v>
       </c>
       <c r="F355" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="G355" s="46" t="s">
-        <v>15</v>
-      </c>
-      <c r="H355" s="46" t="s">
-        <v>18</v>
-      </c>
-      <c r="I355" s="48"/>
+      <c r="G355" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="H355" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="I355" s="27" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="356" spans="1:9" ht="45">
       <c r="A356" s="18" t="s">
-        <v>838</v>
+        <v>836</v>
       </c>
       <c r="B356" s="47" t="s">
         <v>428</v>
       </c>
-      <c r="C356" s="16" t="s">
-        <v>862</v>
+      <c r="C356" s="48" t="s">
+        <v>835</v>
       </c>
       <c r="D356" s="46" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
       <c r="E356" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="F356" s="46" t="s">
+      <c r="F356" s="25" t="s">
         <v>6</v>
       </c>
       <c r="G356" s="46" t="s">
         <v>15</v>
       </c>
       <c r="H356" s="46" t="s">
-        <v>20</v>
-      </c>
-      <c r="I356" s="27" t="s">
-        <v>689</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="I356" s="48"/>
     </row>
     <row r="357" spans="1:9" ht="45">
       <c r="A357" s="18" t="s">
-        <v>839</v>
+        <v>837</v>
       </c>
       <c r="B357" s="47" t="s">
         <v>428</v>
       </c>
       <c r="C357" s="16" t="s">
-        <v>899</v>
-      </c>
-      <c r="D357" s="18" t="s">
-        <v>892</v>
+        <v>861</v>
+      </c>
+      <c r="D357" s="46" t="s">
+        <v>844</v>
       </c>
       <c r="E357" s="25" t="s">
         <v>22</v>
@@ -14257,22 +14259,24 @@
         <v>15</v>
       </c>
       <c r="H357" s="46" t="s">
-        <v>18</v>
-      </c>
-      <c r="I357" s="48"/>
+        <v>20</v>
+      </c>
+      <c r="I357" s="27" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="358" spans="1:9" ht="45">
       <c r="A358" s="18" t="s">
-        <v>840</v>
+        <v>838</v>
       </c>
       <c r="B358" s="47" t="s">
         <v>428</v>
       </c>
       <c r="C358" s="16" t="s">
-        <v>900</v>
+        <v>898</v>
       </c>
       <c r="D358" s="18" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
       <c r="E358" s="25" t="s">
         <v>22</v>
@@ -14284,24 +14288,22 @@
         <v>15</v>
       </c>
       <c r="H358" s="46" t="s">
-        <v>20</v>
-      </c>
-      <c r="I358" s="27" t="s">
-        <v>689</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="I358" s="48"/>
     </row>
     <row r="359" spans="1:9" ht="45">
       <c r="A359" s="18" t="s">
-        <v>867</v>
+        <v>839</v>
       </c>
       <c r="B359" s="47" t="s">
         <v>428</v>
       </c>
-      <c r="C359" s="48" t="s">
-        <v>863</v>
+      <c r="C359" s="16" t="s">
+        <v>899</v>
       </c>
       <c r="D359" s="18" t="s">
-        <v>872</v>
+        <v>891</v>
       </c>
       <c r="E359" s="25" t="s">
         <v>22</v>
@@ -14313,22 +14315,24 @@
         <v>15</v>
       </c>
       <c r="H359" s="46" t="s">
-        <v>18</v>
-      </c>
-      <c r="I359" s="48"/>
+        <v>20</v>
+      </c>
+      <c r="I359" s="27" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="360" spans="1:9" ht="45">
       <c r="A360" s="18" t="s">
-        <v>868</v>
+        <v>866</v>
       </c>
       <c r="B360" s="47" t="s">
         <v>428</v>
       </c>
       <c r="C360" s="48" t="s">
-        <v>864</v>
-      </c>
-      <c r="D360" s="46" t="s">
-        <v>872</v>
+        <v>862</v>
+      </c>
+      <c r="D360" s="18" t="s">
+        <v>871</v>
       </c>
       <c r="E360" s="25" t="s">
         <v>22</v>
@@ -14340,24 +14344,22 @@
         <v>15</v>
       </c>
       <c r="H360" s="46" t="s">
-        <v>20</v>
-      </c>
-      <c r="I360" s="27" t="s">
-        <v>689</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="I360" s="48"/>
     </row>
     <row r="361" spans="1:9" ht="45">
       <c r="A361" s="18" t="s">
-        <v>869</v>
+        <v>867</v>
       </c>
       <c r="B361" s="47" t="s">
         <v>428</v>
       </c>
       <c r="C361" s="48" t="s">
-        <v>865</v>
+        <v>863</v>
       </c>
       <c r="D361" s="46" t="s">
-        <v>873</v>
+        <v>871</v>
       </c>
       <c r="E361" s="25" t="s">
         <v>22</v>
@@ -14369,22 +14371,24 @@
         <v>15</v>
       </c>
       <c r="H361" s="46" t="s">
-        <v>18</v>
-      </c>
-      <c r="I361" s="48"/>
+        <v>20</v>
+      </c>
+      <c r="I361" s="27" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="362" spans="1:9" ht="45">
       <c r="A362" s="18" t="s">
-        <v>870</v>
+        <v>868</v>
       </c>
       <c r="B362" s="47" t="s">
         <v>428</v>
       </c>
       <c r="C362" s="48" t="s">
-        <v>866</v>
+        <v>864</v>
       </c>
       <c r="D362" s="46" t="s">
-        <v>873</v>
+        <v>872</v>
       </c>
       <c r="E362" s="25" t="s">
         <v>22</v>
@@ -14396,24 +14400,22 @@
         <v>15</v>
       </c>
       <c r="H362" s="46" t="s">
-        <v>20</v>
-      </c>
-      <c r="I362" s="27" t="s">
-        <v>689</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="I362" s="48"/>
     </row>
     <row r="363" spans="1:9" ht="45">
       <c r="A363" s="18" t="s">
-        <v>841</v>
+        <v>869</v>
       </c>
       <c r="B363" s="47" t="s">
         <v>428</v>
       </c>
       <c r="C363" s="48" t="s">
-        <v>858</v>
+        <v>865</v>
       </c>
       <c r="D363" s="46" t="s">
-        <v>846</v>
+        <v>872</v>
       </c>
       <c r="E363" s="25" t="s">
         <v>22</v>
@@ -14425,22 +14427,24 @@
         <v>15</v>
       </c>
       <c r="H363" s="46" t="s">
-        <v>18</v>
-      </c>
-      <c r="I363" s="48"/>
+        <v>20</v>
+      </c>
+      <c r="I363" s="27" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="364" spans="1:9" ht="45">
       <c r="A364" s="18" t="s">
-        <v>842</v>
+        <v>840</v>
       </c>
       <c r="B364" s="47" t="s">
         <v>428</v>
       </c>
       <c r="C364" s="48" t="s">
-        <v>859</v>
+        <v>857</v>
       </c>
       <c r="D364" s="46" t="s">
-        <v>846</v>
+        <v>845</v>
       </c>
       <c r="E364" s="25" t="s">
         <v>22</v>
@@ -14452,51 +14456,51 @@
         <v>15</v>
       </c>
       <c r="H364" s="46" t="s">
-        <v>20</v>
-      </c>
-      <c r="I364" s="27" t="s">
-        <v>689</v>
-      </c>
-    </row>
-    <row r="365" spans="1:9" ht="30">
+        <v>18</v>
+      </c>
+      <c r="I364" s="48"/>
+    </row>
+    <row r="365" spans="1:9" ht="45">
       <c r="A365" s="18" t="s">
-        <v>843</v>
+        <v>841</v>
       </c>
       <c r="B365" s="47" t="s">
         <v>428</v>
       </c>
       <c r="C365" s="48" t="s">
-        <v>860</v>
-      </c>
-      <c r="D365" s="18" t="s">
-        <v>875</v>
+        <v>858</v>
+      </c>
+      <c r="D365" s="46" t="s">
+        <v>845</v>
       </c>
       <c r="E365" s="25" t="s">
         <v>22</v>
       </c>
       <c r="F365" s="46" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="G365" s="46" t="s">
         <v>15</v>
       </c>
       <c r="H365" s="46" t="s">
-        <v>18</v>
-      </c>
-      <c r="I365" s="48"/>
-    </row>
-    <row r="366" spans="1:9" ht="45">
+        <v>20</v>
+      </c>
+      <c r="I365" s="27" t="s">
+        <v>689</v>
+      </c>
+    </row>
+    <row r="366" spans="1:9" ht="30">
       <c r="A366" s="18" t="s">
-        <v>844</v>
+        <v>842</v>
       </c>
       <c r="B366" s="47" t="s">
         <v>428</v>
       </c>
       <c r="C366" s="48" t="s">
-        <v>861</v>
+        <v>859</v>
       </c>
       <c r="D366" s="18" t="s">
-        <v>875</v>
+        <v>874</v>
       </c>
       <c r="E366" s="25" t="s">
         <v>22</v>
@@ -14508,55 +14512,55 @@
         <v>15</v>
       </c>
       <c r="H366" s="46" t="s">
-        <v>20</v>
-      </c>
-      <c r="I366" s="27" t="s">
-        <v>689</v>
-      </c>
-    </row>
-    <row r="367" spans="1:9" ht="75">
-      <c r="A367" s="25" t="s">
-        <v>365</v>
-      </c>
-      <c r="B367" s="26" t="s">
-        <v>429</v>
-      </c>
-      <c r="C367" s="27" t="s">
-        <v>641</v>
-      </c>
-      <c r="D367" s="25"/>
+        <v>18</v>
+      </c>
+      <c r="I366" s="48"/>
+    </row>
+    <row r="367" spans="1:9" ht="45">
+      <c r="A367" s="18" t="s">
+        <v>843</v>
+      </c>
+      <c r="B367" s="47" t="s">
+        <v>428</v>
+      </c>
+      <c r="C367" s="48" t="s">
+        <v>860</v>
+      </c>
+      <c r="D367" s="18" t="s">
+        <v>874</v>
+      </c>
       <c r="E367" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="F367" s="25" t="s">
-        <v>6</v>
-      </c>
-      <c r="G367" s="25" t="s">
-        <v>15</v>
-      </c>
-      <c r="H367" s="25" t="s">
-        <v>17</v>
+      <c r="F367" s="46" t="s">
+        <v>3</v>
+      </c>
+      <c r="G367" s="46" t="s">
+        <v>15</v>
+      </c>
+      <c r="H367" s="46" t="s">
+        <v>20</v>
       </c>
       <c r="I367" s="27" t="s">
-        <v>687</v>
-      </c>
-    </row>
-    <row r="368" spans="1:9" ht="60">
+        <v>689</v>
+      </c>
+    </row>
+    <row r="368" spans="1:9" ht="75">
       <c r="A368" s="25" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B368" s="26" t="s">
-        <v>430</v>
-      </c>
-      <c r="C368" s="16" t="s">
-        <v>854</v>
+        <v>429</v>
+      </c>
+      <c r="C368" s="27" t="s">
+        <v>641</v>
       </c>
       <c r="D368" s="25"/>
       <c r="E368" s="25" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="F368" s="25" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="G368" s="25" t="s">
         <v>15</v>
@@ -14564,19 +14568,19 @@
       <c r="H368" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="I368" s="16" t="s">
-        <v>876</v>
+      <c r="I368" s="27" t="s">
+        <v>687</v>
       </c>
     </row>
     <row r="369" spans="1:9" ht="60">
       <c r="A369" s="25" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="B369" s="26" t="s">
         <v>430</v>
       </c>
-      <c r="C369" s="27" t="s">
-        <v>642</v>
+      <c r="C369" s="16" t="s">
+        <v>853</v>
       </c>
       <c r="D369" s="25"/>
       <c r="E369" s="25" t="s">
@@ -14592,18 +14596,18 @@
         <v>17</v>
       </c>
       <c r="I369" s="16" t="s">
-        <v>877</v>
+        <v>875</v>
       </c>
     </row>
     <row r="370" spans="1:9" ht="60">
       <c r="A370" s="25" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="B370" s="26" t="s">
         <v>430</v>
       </c>
       <c r="C370" s="27" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="D370" s="25"/>
       <c r="E370" s="25" t="s">
@@ -14618,69 +14622,71 @@
       <c r="H370" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="I370" s="27" t="s">
-        <v>690</v>
-      </c>
-    </row>
-    <row r="371" spans="1:9" ht="409.5">
+      <c r="I370" s="16" t="s">
+        <v>876</v>
+      </c>
+    </row>
+    <row r="371" spans="1:9" ht="60">
       <c r="A371" s="25" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="B371" s="26" t="s">
-        <v>431</v>
-      </c>
-      <c r="C371" s="28" t="s">
-        <v>699</v>
+        <v>430</v>
+      </c>
+      <c r="C371" s="27" t="s">
+        <v>643</v>
       </c>
       <c r="D371" s="25"/>
       <c r="E371" s="25" t="s">
         <v>19</v>
       </c>
       <c r="F371" s="25" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="G371" s="25" t="s">
         <v>15</v>
       </c>
       <c r="H371" s="25" t="s">
-        <v>21</v>
-      </c>
-      <c r="I371" s="27"/>
-    </row>
-    <row r="372" spans="1:9" ht="30">
+        <v>17</v>
+      </c>
+      <c r="I371" s="27" t="s">
+        <v>690</v>
+      </c>
+    </row>
+    <row r="372" spans="1:9" ht="409.5">
       <c r="A372" s="25" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B372" s="26" t="s">
         <v>431</v>
       </c>
-      <c r="C372" s="16" t="s">
-        <v>697</v>
+      <c r="C372" s="28" t="s">
+        <v>699</v>
       </c>
       <c r="D372" s="25"/>
       <c r="E372" s="25" t="s">
         <v>19</v>
       </c>
       <c r="F372" s="25" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="G372" s="25" t="s">
         <v>15</v>
       </c>
       <c r="H372" s="25" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="I372" s="27"/>
     </row>
     <row r="373" spans="1:9" ht="30">
       <c r="A373" s="25" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="B373" s="26" t="s">
         <v>431</v>
       </c>
-      <c r="C373" s="27" t="s">
-        <v>644</v>
+      <c r="C373" s="16" t="s">
+        <v>697</v>
       </c>
       <c r="D373" s="25"/>
       <c r="E373" s="25" t="s">
@@ -14697,40 +14703,40 @@
       </c>
       <c r="I373" s="27"/>
     </row>
-    <row r="374" spans="1:9" ht="409.5">
+    <row r="374" spans="1:9" ht="30">
       <c r="A374" s="25" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B374" s="26" t="s">
-        <v>432</v>
-      </c>
-      <c r="C374" s="28" t="s">
-        <v>698</v>
+        <v>431</v>
+      </c>
+      <c r="C374" s="27" t="s">
+        <v>644</v>
       </c>
       <c r="D374" s="25"/>
       <c r="E374" s="25" t="s">
         <v>19</v>
       </c>
       <c r="F374" s="25" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="G374" s="25" t="s">
         <v>15</v>
       </c>
       <c r="H374" s="25" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I374" s="27"/>
     </row>
-    <row r="375" spans="1:9" ht="30">
+    <row r="375" spans="1:9" ht="409.5">
       <c r="A375" s="25" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B375" s="26" t="s">
-        <v>433</v>
-      </c>
-      <c r="C375" s="27" t="s">
-        <v>645</v>
+        <v>432</v>
+      </c>
+      <c r="C375" s="28" t="s">
+        <v>698</v>
       </c>
       <c r="D375" s="25"/>
       <c r="E375" s="25" t="s">
@@ -14747,15 +14753,15 @@
       </c>
       <c r="I375" s="27"/>
     </row>
-    <row r="376" spans="1:9" ht="135">
+    <row r="376" spans="1:9" ht="30">
       <c r="A376" s="25" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="B376" s="26" t="s">
         <v>433</v>
       </c>
       <c r="C376" s="27" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="D376" s="25"/>
       <c r="E376" s="25" t="s">
@@ -14772,15 +14778,15 @@
       </c>
       <c r="I376" s="27"/>
     </row>
-    <row r="377" spans="1:9" ht="30">
+    <row r="377" spans="1:9" ht="135">
       <c r="A377" s="25" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B377" s="26" t="s">
         <v>433</v>
       </c>
       <c r="C377" s="27" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="D377" s="25"/>
       <c r="E377" s="25" t="s">
@@ -14797,15 +14803,15 @@
       </c>
       <c r="I377" s="27"/>
     </row>
-    <row r="378" spans="1:9" ht="255">
+    <row r="378" spans="1:9" ht="30">
       <c r="A378" s="25" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="B378" s="26" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="C378" s="27" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="D378" s="25"/>
       <c r="E378" s="25" t="s">
@@ -14822,42 +14828,40 @@
       </c>
       <c r="I378" s="27"/>
     </row>
-    <row r="379" spans="1:9" ht="45">
+    <row r="379" spans="1:9" ht="255">
       <c r="A379" s="25" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="B379" s="26" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="C379" s="27" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="D379" s="25"/>
       <c r="E379" s="25" t="s">
         <v>19</v>
       </c>
       <c r="F379" s="25" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="G379" s="25" t="s">
         <v>15</v>
       </c>
       <c r="H379" s="25" t="s">
-        <v>17</v>
-      </c>
-      <c r="I379" s="27" t="s">
-        <v>691</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="I379" s="27"/>
     </row>
     <row r="380" spans="1:9" ht="45">
       <c r="A380" s="25" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B380" s="26" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="C380" s="27" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="D380" s="25"/>
       <c r="E380" s="25" t="s">
@@ -14872,26 +14876,26 @@
       <c r="H380" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="I380" s="16" t="s">
-        <v>700</v>
+      <c r="I380" s="27" t="s">
+        <v>691</v>
       </c>
     </row>
     <row r="381" spans="1:9" ht="45">
       <c r="A381" s="25" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B381" s="26" t="s">
         <v>436</v>
       </c>
-      <c r="C381" s="16" t="s">
-        <v>855</v>
+      <c r="C381" s="27" t="s">
+        <v>650</v>
       </c>
       <c r="D381" s="25"/>
       <c r="E381" s="25" t="s">
         <v>19</v>
       </c>
       <c r="F381" s="25" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="G381" s="25" t="s">
         <v>15</v>
@@ -14900,25 +14904,25 @@
         <v>17</v>
       </c>
       <c r="I381" s="16" t="s">
-        <v>878</v>
+        <v>700</v>
       </c>
     </row>
     <row r="382" spans="1:9" ht="45">
       <c r="A382" s="25" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="B382" s="26" t="s">
         <v>436</v>
       </c>
       <c r="C382" s="16" t="s">
-        <v>651</v>
+        <v>854</v>
       </c>
       <c r="D382" s="25"/>
       <c r="E382" s="25" t="s">
         <v>19</v>
       </c>
       <c r="F382" s="25" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="G382" s="25" t="s">
         <v>15</v>
@@ -14927,18 +14931,18 @@
         <v>17</v>
       </c>
       <c r="I382" s="16" t="s">
-        <v>879</v>
+        <v>877</v>
       </c>
     </row>
     <row r="383" spans="1:9" ht="45">
       <c r="A383" s="25" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="B383" s="26" t="s">
         <v>436</v>
       </c>
-      <c r="C383" s="27" t="s">
-        <v>652</v>
+      <c r="C383" s="16" t="s">
+        <v>651</v>
       </c>
       <c r="D383" s="25"/>
       <c r="E383" s="25" t="s">
@@ -14953,19 +14957,19 @@
       <c r="H383" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="I383" s="27" t="s">
-        <v>692</v>
+      <c r="I383" s="16" t="s">
+        <v>878</v>
       </c>
     </row>
     <row r="384" spans="1:9" ht="45">
       <c r="A384" s="25" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="B384" s="26" t="s">
         <v>436</v>
       </c>
       <c r="C384" s="27" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="D384" s="25"/>
       <c r="E384" s="25" t="s">
@@ -14981,18 +14985,18 @@
         <v>17</v>
       </c>
       <c r="I384" s="27" t="s">
-        <v>693</v>
-      </c>
-    </row>
-    <row r="385" spans="1:9" ht="60">
+        <v>692</v>
+      </c>
+    </row>
+    <row r="385" spans="1:9" ht="45">
       <c r="A385" s="25" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="B385" s="26" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="C385" s="27" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="D385" s="25"/>
       <c r="E385" s="25" t="s">
@@ -15008,43 +15012,45 @@
         <v>17</v>
       </c>
       <c r="I385" s="27" t="s">
-        <v>694</v>
-      </c>
-    </row>
-    <row r="386" spans="1:9" ht="30">
+        <v>693</v>
+      </c>
+    </row>
+    <row r="386" spans="1:9" ht="60">
       <c r="A386" s="25" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="B386" s="26" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="C386" s="27" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="D386" s="25"/>
       <c r="E386" s="25" t="s">
         <v>19</v>
       </c>
       <c r="F386" s="25" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="G386" s="25" t="s">
         <v>15</v>
       </c>
       <c r="H386" s="25" t="s">
-        <v>21</v>
-      </c>
-      <c r="I386" s="27"/>
-    </row>
-    <row r="387" spans="1:9" ht="409.5">
+        <v>17</v>
+      </c>
+      <c r="I386" s="27" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="387" spans="1:9" ht="30">
       <c r="A387" s="25" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="B387" s="26" t="s">
         <v>438</v>
       </c>
       <c r="C387" s="27" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="D387" s="25"/>
       <c r="E387" s="25" t="s">
@@ -15061,15 +15067,15 @@
       </c>
       <c r="I387" s="27"/>
     </row>
-    <row r="388" spans="1:9" ht="60">
+    <row r="388" spans="1:9" ht="409.5">
       <c r="A388" s="25" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="B388" s="26" t="s">
         <v>438</v>
       </c>
       <c r="C388" s="27" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="D388" s="25"/>
       <c r="E388" s="25" t="s">
@@ -15086,15 +15092,15 @@
       </c>
       <c r="I388" s="27"/>
     </row>
-    <row r="389" spans="1:9" ht="360">
+    <row r="389" spans="1:9" ht="60">
       <c r="A389" s="25" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="B389" s="26" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="C389" s="27" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="D389" s="25"/>
       <c r="E389" s="25" t="s">
@@ -15111,40 +15117,65 @@
       </c>
       <c r="I389" s="27"/>
     </row>
-    <row r="390" spans="1:9" ht="45">
+    <row r="390" spans="1:9" ht="360">
       <c r="A390" s="25" t="s">
+        <v>387</v>
+      </c>
+      <c r="B390" s="26" t="s">
+        <v>439</v>
+      </c>
+      <c r="C390" s="27" t="s">
+        <v>658</v>
+      </c>
+      <c r="D390" s="25"/>
+      <c r="E390" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="F390" s="25" t="s">
+        <v>6</v>
+      </c>
+      <c r="G390" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="H390" s="25" t="s">
+        <v>21</v>
+      </c>
+      <c r="I390" s="27"/>
+    </row>
+    <row r="391" spans="1:9" ht="45">
+      <c r="A391" s="25" t="s">
         <v>388</v>
       </c>
-      <c r="B390" s="26" t="s">
+      <c r="B391" s="26" t="s">
         <v>428</v>
       </c>
-      <c r="C390" s="27" t="s">
+      <c r="C391" s="27" t="s">
         <v>659</v>
       </c>
-      <c r="D390" s="25" t="s">
+      <c r="D391" s="25" t="s">
         <v>685</v>
       </c>
-      <c r="E390" s="25" t="s">
+      <c r="E391" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="F390" s="25" t="s">
-        <v>6</v>
-      </c>
-      <c r="G390" s="25" t="s">
-        <v>15</v>
-      </c>
-      <c r="H390" s="25" t="s">
-        <v>18</v>
-      </c>
-      <c r="I390" s="27"/>
-    </row>
-    <row r="391" spans="1:9">
-      <c r="A391" s="3"/>
-      <c r="B391" s="9"/>
+      <c r="F391" s="25" t="s">
+        <v>6</v>
+      </c>
+      <c r="G391" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="H391" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="I391" s="27"/>
     </row>
     <row r="392" spans="1:9">
       <c r="A392" s="3"/>
       <c r="B392" s="9"/>
+    </row>
+    <row r="393" spans="1:9">
+      <c r="A393" s="3"/>
+      <c r="B393" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="11">
@@ -15161,7 +15192,7 @@
     <mergeCell ref="B17:I17"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="A371:B371 A374:B374 A372:I373 D371:I371 A375:I390 D374:I374 I363:I390 A20:I370">
+  <conditionalFormatting sqref="A372:B372 A375:B375 A373:I374 D372:I372 A376:I391 D375:I375 I364:I391 A20:I371">
     <cfRule type="expression" dxfId="36" priority="77">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
@@ -15172,7 +15203,7 @@
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A371:B371 A374:B374 A372:I373 D371:I371 A375:I390 D374:I374 I363:I390 A20:I370">
+  <conditionalFormatting sqref="A372:B372 A375:B375 A373:I374 D372:I372 A376:I391 D375:I375 I364:I391 A20:I371">
     <cfRule type="expression" dxfId="33" priority="31">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
@@ -15183,7 +15214,7 @@
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F20:F390">
+  <conditionalFormatting sqref="F20:F391">
     <cfRule type="expression" dxfId="30" priority="37">
       <formula>NOT(VLOOKUP(F20,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
@@ -15191,7 +15222,7 @@
       <formula>(VLOOKUP(F20,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C374">
+  <conditionalFormatting sqref="C375">
     <cfRule type="expression" dxfId="28" priority="10">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
@@ -15202,7 +15233,7 @@
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C374">
+  <conditionalFormatting sqref="C375">
     <cfRule type="expression" dxfId="25" priority="7">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
@@ -15213,7 +15244,7 @@
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C371">
+  <conditionalFormatting sqref="C372">
     <cfRule type="expression" dxfId="22" priority="4">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
@@ -15224,7 +15255,7 @@
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C371">
+  <conditionalFormatting sqref="C372">
     <cfRule type="expression" dxfId="19" priority="1">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
@@ -15236,20 +15267,20 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="6">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G4 F20:F390" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G4 F20:F391" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>$A$13:$A$15</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F4 E20:E390" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F4 E20:E391" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"Protocol,Product"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H4 G20:G390" xr:uid="{00000000-0002-0000-0000-000002000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H4 G20:G391" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>"Informative,Normative"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B13:B15" xr:uid="{00000000-0002-0000-0000-000003000000}">
       <formula1>"In, Out"</formula1>
     </dataValidation>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3" xr:uid="{00000000-0002-0000-0000-000004000000}"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H20:H390" xr:uid="{00000000-0002-0000-0000-000005000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H20:H391" xr:uid="{00000000-0002-0000-0000-000005000000}">
       <formula1>"Non-testable, Unverified, Adapter, Test Case"</formula1>
     </dataValidation>
   </dataValidations>
@@ -15259,7 +15290,7 @@
     <oddFooter>&amp;F&amp;RPage &amp;P</oddFooter>
   </headerFooter>
   <ignoredErrors>
-    <ignoredError sqref="B1:B9 B10:B46 B237:B392 B47:B233" numberStoredAsText="1"/>
+    <ignoredError sqref="B1:B9 B10:B46 B252:B393 B47:B233 B237:B249" numberStoredAsText="1"/>
   </ignoredErrors>
   <tableParts count="2">
     <tablePart r:id="rId2"/>
@@ -15269,9 +15300,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -15324,24 +15358,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{923F65C5-DEAB-400B-AA1F-124F40EE10AC}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6D33261-F3C6-4621-88F1-D76E5ABE1865}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -15362,9 +15387,15 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6D33261-F3C6-4621-88F1-D76E5ABE1865}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{923F65C5-DEAB-400B-AA1F-124F40EE10AC}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Update RS and md file for MS-OXWSSYNC.
</commit_message>
<xml_diff>
--- a/ExchangeWebServices/Docs/MS-OXWSSYNC/MS-OXWSSYNC_RequirementSpecification.xlsx
+++ b/ExchangeWebServices/Docs/MS-OXWSSYNC/MS-OXWSSYNC_RequirementSpecification.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26731"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{178A1655-8AD7-4207-B17A-21B1CB7D07E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DAC4E32-7FA0-445B-8E4C-2A82151845E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22932" yWindow="-1272" windowWidth="23256" windowHeight="12456" tabRatio="570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements" sheetId="2" r:id="rId1"/>
@@ -2205,13 +2205,6 @@
   </si>
   <si>
     <t>[In tns:SyncFolderItemsSoapIn Message] [The part name RequestVersion] specifies a SOAP header that identifies the schema version for the request.</t>
-  </si>
-  <si>
-    <t>[In tns:SyncFolderItemsSoapOut] The SyncFolderItemsSoapOut WSDL message specifies the response from the SyncFoldersItems operation.
-&lt;wsdl:message name="SyncFolderItemsSoapOut"&gt;
-   &lt;wsdl:part name="SyncFolderItemsResult" element="tns:SyncFolderItemsResponse" /&gt;
-   &lt;wsdl:part name="ServerVersion" element="t:ServerVersionInfo"/&gt;
-&lt;/wsdl:message&gt;</t>
   </si>
   <si>
     <t>[In tns:SyncFolderItemsSoapOut] The SyncFolderItemsSoapOut WSDL message is the output message for the following SOAP action: http://schemas.microsoft.com/exchange/services/2006/messages/SyncFolderItems.</t>
@@ -3404,9 +3397,6 @@
     <t>[In m:SyncFolderHierarchyResponseMessageType Complex Type] The SyncFolderHierarchyResponseMessageType complex type extends the ResponseMessageType complex type ([MS-OXWSCDATA] section 2.2.4.67).</t>
   </si>
   <si>
-    <t>[In m:SyncFolderHierarchyResponseMessageType Complex Type] The following table [in 3.1.4.1.3.4] lists the child elements of the SyncFolderHieracrchyResponseMessageType complex type.</t>
-  </si>
-  <si>
     <t>[In m:SyncFolderHierarchyResponseMessageType Complex Type] [The Element SyncState] This element is optional.</t>
   </si>
   <si>
@@ -4029,6 +4019,16 @@
   </si>
   <si>
     <t>[In m:SyncFolderItemsType Complex Type] This element [MinimumCount] specifies the minimum number of items (from the latest received time) to include in a synchronization response..</t>
+  </si>
+  <si>
+    <t>[In m:SyncFolderHierarchyResponseMessageType Complex Type] The following table [in 3.1.4.1.3.4] lists the child elements of the SyncFolderHierarchyResponseMessageType complex type.</t>
+  </si>
+  <si>
+    <t>[In tns:SyncFolderItemsSoapOut] The SyncFolderItemsSoapOut WSDL message specifies the response from the SyncFolderItems operation.
+&lt;wsdl:message name="SyncFolderItemsSoapOut"&gt;
+   &lt;wsdl:part name="SyncFolderItemsResult" element="tns:SyncFolderItemsResponse" /&gt;
+   &lt;wsdl:part name="ServerVersion" element="t:ServerVersionInfo"/&gt;
+&lt;/wsdl:message&gt;</t>
   </si>
 </sst>
 </file>
@@ -5052,9 +5052,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -5092,9 +5092,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -5127,26 +5127,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -5179,26 +5162,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -5375,8 +5341,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:I396"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A336" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C345" sqref="C345"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7:I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
@@ -5396,7 +5362,7 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" s="1" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>27</v>
@@ -5405,7 +5371,7 @@
     </row>
     <row r="2" spans="1:9">
       <c r="A2" s="4" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
@@ -5426,7 +5392,7 @@
         <v>26</v>
       </c>
       <c r="F3" s="31">
-        <v>44978</v>
+        <v>45153</v>
       </c>
       <c r="G3" s="32"/>
       <c r="I3" s="29"/>
@@ -5494,7 +5460,7 @@
         <v>1</v>
       </c>
       <c r="B8" s="51" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="C8" s="52"/>
       <c r="D8" s="52"/>
@@ -5539,7 +5505,7 @@
         <v>8</v>
       </c>
       <c r="B11" s="57" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="C11" s="58"/>
       <c r="D11" s="44"/>
@@ -5652,7 +5618,7 @@
         <v>5</v>
       </c>
       <c r="B18" s="43" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="C18" s="44"/>
       <c r="D18" s="44"/>
@@ -5990,7 +5956,7 @@
         <v>17</v>
       </c>
       <c r="I31" s="16" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
     </row>
     <row r="32" spans="1:9" s="15" customFormat="1" ht="28.8">
@@ -6726,7 +6692,7 @@
         <v>404</v>
       </c>
       <c r="C61" s="13" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="D61" s="21"/>
       <c r="E61" s="21" t="s">
@@ -6751,7 +6717,7 @@
         <v>404</v>
       </c>
       <c r="C62" s="13" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="D62" s="21"/>
       <c r="E62" s="21" t="s">
@@ -6801,7 +6767,7 @@
         <v>404</v>
       </c>
       <c r="C64" s="13" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="D64" s="21"/>
       <c r="E64" s="21" t="s">
@@ -7051,7 +7017,7 @@
         <v>31</v>
       </c>
       <c r="C74" s="13" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="D74" s="21"/>
       <c r="E74" s="21" t="s">
@@ -7076,7 +7042,7 @@
         <v>31</v>
       </c>
       <c r="C75" s="13" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="D75" s="21"/>
       <c r="E75" s="21" t="s">
@@ -7301,7 +7267,7 @@
         <v>407</v>
       </c>
       <c r="C84" s="13" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="D84" s="21"/>
       <c r="E84" s="21" t="s">
@@ -7351,7 +7317,7 @@
         <v>407</v>
       </c>
       <c r="C86" s="13" t="s">
-        <v>878</v>
+        <v>876</v>
       </c>
       <c r="D86" s="21"/>
       <c r="E86" s="21" t="s">
@@ -7426,7 +7392,7 @@
         <v>407</v>
       </c>
       <c r="C89" s="13" t="s">
-        <v>879</v>
+        <v>877</v>
       </c>
       <c r="D89" s="21"/>
       <c r="E89" s="21" t="s">
@@ -7601,7 +7567,7 @@
         <v>408</v>
       </c>
       <c r="C96" s="13" t="s">
-        <v>880</v>
+        <v>878</v>
       </c>
       <c r="D96" s="21"/>
       <c r="E96" s="21" t="s">
@@ -7776,7 +7742,7 @@
         <v>412</v>
       </c>
       <c r="C103" s="13" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="D103" s="21"/>
       <c r="E103" s="21" t="s">
@@ -7876,7 +7842,7 @@
         <v>412</v>
       </c>
       <c r="C107" s="13" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
       <c r="D107" s="21"/>
       <c r="E107" s="21" t="s">
@@ -7926,7 +7892,7 @@
         <v>412</v>
       </c>
       <c r="C109" s="13" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="D109" s="21"/>
       <c r="E109" s="21" t="s">
@@ -7976,7 +7942,7 @@
         <v>413</v>
       </c>
       <c r="C111" s="13" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="D111" s="21"/>
       <c r="E111" s="21" t="s">
@@ -8001,7 +7967,7 @@
         <v>413</v>
       </c>
       <c r="C112" s="13" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
       <c r="D112" s="21"/>
       <c r="E112" s="21" t="s">
@@ -8101,7 +8067,7 @@
         <v>413</v>
       </c>
       <c r="C116" s="13" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
       <c r="D116" s="21"/>
       <c r="E116" s="21" t="s">
@@ -8126,7 +8092,7 @@
         <v>413</v>
       </c>
       <c r="C117" s="13" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="D117" s="21"/>
       <c r="E117" s="21" t="s">
@@ -8142,7 +8108,7 @@
         <v>17</v>
       </c>
       <c r="I117" s="13" t="s">
-        <v>846</v>
+        <v>844</v>
       </c>
     </row>
     <row r="118" spans="1:9" ht="316.8">
@@ -8178,7 +8144,7 @@
         <v>414</v>
       </c>
       <c r="C119" s="13" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="D119" s="21"/>
       <c r="E119" s="21" t="s">
@@ -8203,7 +8169,7 @@
         <v>414</v>
       </c>
       <c r="C120" s="13" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="D120" s="21"/>
       <c r="E120" s="21" t="s">
@@ -8228,7 +8194,7 @@
         <v>414</v>
       </c>
       <c r="C121" s="13" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="D121" s="21"/>
       <c r="E121" s="21" t="s">
@@ -8253,7 +8219,7 @@
         <v>414</v>
       </c>
       <c r="C122" s="13" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="D122" s="21"/>
       <c r="E122" s="21" t="s">
@@ -8278,7 +8244,7 @@
         <v>414</v>
       </c>
       <c r="C123" s="13" t="s">
-        <v>884</v>
+        <v>882</v>
       </c>
       <c r="D123" s="21"/>
       <c r="E123" s="21" t="s">
@@ -8303,7 +8269,7 @@
         <v>414</v>
       </c>
       <c r="C124" s="13" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
       <c r="D124" s="21"/>
       <c r="E124" s="21" t="s">
@@ -8328,7 +8294,7 @@
         <v>414</v>
       </c>
       <c r="C125" s="13" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
       <c r="D125" s="21"/>
       <c r="E125" s="21" t="s">
@@ -8353,7 +8319,7 @@
         <v>414</v>
       </c>
       <c r="C126" s="13" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="D126" s="21"/>
       <c r="E126" s="21" t="s">
@@ -8378,7 +8344,7 @@
         <v>414</v>
       </c>
       <c r="C127" s="13" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="D127" s="21"/>
       <c r="E127" s="21" t="s">
@@ -8403,7 +8369,7 @@
         <v>414</v>
       </c>
       <c r="C128" s="13" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="D128" s="21"/>
       <c r="E128" s="21" t="s">
@@ -8428,7 +8394,7 @@
         <v>414</v>
       </c>
       <c r="C129" s="13" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="D129" s="21"/>
       <c r="E129" s="21" t="s">
@@ -8453,7 +8419,7 @@
         <v>414</v>
       </c>
       <c r="C130" s="13" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="D130" s="21"/>
       <c r="E130" s="21" t="s">
@@ -8478,7 +8444,7 @@
         <v>414</v>
       </c>
       <c r="C131" s="13" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="D131" s="21"/>
       <c r="E131" s="21" t="s">
@@ -8503,7 +8469,7 @@
         <v>414</v>
       </c>
       <c r="C132" s="13" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="D132" s="21"/>
       <c r="E132" s="21" t="s">
@@ -8528,7 +8494,7 @@
         <v>414</v>
       </c>
       <c r="C133" s="13" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="D133" s="21"/>
       <c r="E133" s="21" t="s">
@@ -8553,7 +8519,7 @@
         <v>414</v>
       </c>
       <c r="C134" s="13" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="D134" s="21"/>
       <c r="E134" s="21" t="s">
@@ -8575,7 +8541,7 @@
         <v>101</v>
       </c>
       <c r="B135" s="22" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="C135" s="13" t="s">
         <v>477</v>
@@ -8600,10 +8566,10 @@
         <v>102</v>
       </c>
       <c r="B136" s="16" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="C136" s="13" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="D136" s="21"/>
       <c r="E136" s="21" t="s">
@@ -8625,10 +8591,10 @@
         <v>103</v>
       </c>
       <c r="B137" s="22" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="C137" s="13" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="D137" s="21"/>
       <c r="E137" s="21" t="s">
@@ -8650,10 +8616,10 @@
         <v>104</v>
       </c>
       <c r="B138" s="16" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="C138" s="13" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="D138" s="21"/>
       <c r="E138" s="21" t="s">
@@ -8675,7 +8641,7 @@
         <v>105</v>
       </c>
       <c r="B139" s="16" t="s">
-        <v>740</v>
+        <v>738</v>
       </c>
       <c r="C139" s="13" t="s">
         <v>478</v>
@@ -8700,10 +8666,10 @@
         <v>106</v>
       </c>
       <c r="B140" s="16" t="s">
-        <v>740</v>
+        <v>738</v>
       </c>
       <c r="C140" s="13" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="D140" s="21"/>
       <c r="E140" s="21" t="s">
@@ -8725,7 +8691,7 @@
         <v>107</v>
       </c>
       <c r="B141" s="16" t="s">
-        <v>740</v>
+        <v>738</v>
       </c>
       <c r="C141" s="13" t="s">
         <v>479</v>
@@ -8750,10 +8716,10 @@
         <v>108</v>
       </c>
       <c r="B142" s="16" t="s">
-        <v>740</v>
+        <v>738</v>
       </c>
       <c r="C142" s="13" t="s">
-        <v>736</v>
+        <v>907</v>
       </c>
       <c r="D142" s="21"/>
       <c r="E142" s="21" t="s">
@@ -8775,7 +8741,7 @@
         <v>109</v>
       </c>
       <c r="B143" s="16" t="s">
-        <v>740</v>
+        <v>738</v>
       </c>
       <c r="C143" s="13" t="s">
         <v>480</v>
@@ -8800,7 +8766,7 @@
         <v>110</v>
       </c>
       <c r="B144" s="16" t="s">
-        <v>740</v>
+        <v>738</v>
       </c>
       <c r="C144" s="13" t="s">
         <v>481</v>
@@ -8825,10 +8791,10 @@
         <v>111</v>
       </c>
       <c r="B145" s="16" t="s">
-        <v>740</v>
+        <v>738</v>
       </c>
       <c r="C145" s="13" t="s">
-        <v>737</v>
+        <v>735</v>
       </c>
       <c r="D145" s="21"/>
       <c r="E145" s="21" t="s">
@@ -8850,7 +8816,7 @@
         <v>112</v>
       </c>
       <c r="B146" s="16" t="s">
-        <v>740</v>
+        <v>738</v>
       </c>
       <c r="C146" s="23" t="s">
         <v>482</v>
@@ -8875,7 +8841,7 @@
         <v>113</v>
       </c>
       <c r="B147" s="16" t="s">
-        <v>740</v>
+        <v>738</v>
       </c>
       <c r="C147" s="13" t="s">
         <v>483</v>
@@ -8900,10 +8866,10 @@
         <v>114</v>
       </c>
       <c r="B148" s="16" t="s">
-        <v>740</v>
+        <v>738</v>
       </c>
       <c r="C148" s="13" t="s">
-        <v>739</v>
+        <v>737</v>
       </c>
       <c r="D148" s="21"/>
       <c r="E148" s="21" t="s">
@@ -8925,10 +8891,10 @@
         <v>115</v>
       </c>
       <c r="B149" s="16" t="s">
-        <v>740</v>
+        <v>738</v>
       </c>
       <c r="C149" s="13" t="s">
-        <v>751</v>
+        <v>749</v>
       </c>
       <c r="D149" s="21"/>
       <c r="E149" s="21" t="s">
@@ -8950,10 +8916,10 @@
         <v>116</v>
       </c>
       <c r="B150" s="16" t="s">
-        <v>740</v>
+        <v>738</v>
       </c>
       <c r="C150" s="13" t="s">
-        <v>738</v>
+        <v>736</v>
       </c>
       <c r="D150" s="21"/>
       <c r="E150" s="21" t="s">
@@ -8975,7 +8941,7 @@
         <v>117</v>
       </c>
       <c r="B151" s="16" t="s">
-        <v>740</v>
+        <v>738</v>
       </c>
       <c r="C151" s="23" t="s">
         <v>484</v>
@@ -9000,10 +8966,10 @@
         <v>118</v>
       </c>
       <c r="B152" s="16" t="s">
-        <v>740</v>
+        <v>738</v>
       </c>
       <c r="C152" s="13" t="s">
-        <v>752</v>
+        <v>750</v>
       </c>
       <c r="D152" s="21"/>
       <c r="E152" s="21" t="s">
@@ -9025,7 +8991,7 @@
         <v>270</v>
       </c>
       <c r="B153" s="16" t="s">
-        <v>742</v>
+        <v>740</v>
       </c>
       <c r="C153" s="23" t="s">
         <v>570</v>
@@ -9050,10 +9016,10 @@
         <v>271</v>
       </c>
       <c r="B154" s="16" t="s">
-        <v>742</v>
+        <v>740</v>
       </c>
       <c r="C154" s="13" t="s">
-        <v>741</v>
+        <v>739</v>
       </c>
       <c r="D154" s="21"/>
       <c r="E154" s="21" t="s">
@@ -9075,7 +9041,7 @@
         <v>272</v>
       </c>
       <c r="B155" s="16" t="s">
-        <v>742</v>
+        <v>740</v>
       </c>
       <c r="C155" s="23" t="s">
         <v>571</v>
@@ -9100,7 +9066,7 @@
         <v>248</v>
       </c>
       <c r="B156" s="16" t="s">
-        <v>743</v>
+        <v>741</v>
       </c>
       <c r="C156" s="13" t="s">
         <v>556</v>
@@ -9125,10 +9091,10 @@
         <v>249</v>
       </c>
       <c r="B157" s="16" t="s">
-        <v>743</v>
+        <v>741</v>
       </c>
       <c r="C157" s="13" t="s">
-        <v>744</v>
+        <v>742</v>
       </c>
       <c r="D157" s="21"/>
       <c r="E157" s="21" t="s">
@@ -9150,7 +9116,7 @@
         <v>250</v>
       </c>
       <c r="B158" s="16" t="s">
-        <v>743</v>
+        <v>741</v>
       </c>
       <c r="C158" s="13" t="s">
         <v>557</v>
@@ -9175,10 +9141,10 @@
         <v>251</v>
       </c>
       <c r="B159" s="16" t="s">
+        <v>741</v>
+      </c>
+      <c r="C159" s="13" t="s">
         <v>743</v>
-      </c>
-      <c r="C159" s="13" t="s">
-        <v>745</v>
       </c>
       <c r="D159" s="21"/>
       <c r="E159" s="21" t="s">
@@ -9200,10 +9166,10 @@
         <v>252</v>
       </c>
       <c r="B160" s="16" t="s">
-        <v>743</v>
+        <v>741</v>
       </c>
       <c r="C160" s="13" t="s">
-        <v>746</v>
+        <v>744</v>
       </c>
       <c r="D160" s="21"/>
       <c r="E160" s="21" t="s">
@@ -9225,7 +9191,7 @@
         <v>253</v>
       </c>
       <c r="B161" s="16" t="s">
-        <v>743</v>
+        <v>741</v>
       </c>
       <c r="C161" s="23" t="s">
         <v>558</v>
@@ -9244,7 +9210,7 @@
         <v>17</v>
       </c>
       <c r="I161" s="13" t="s">
-        <v>850</v>
+        <v>848</v>
       </c>
     </row>
     <row r="162" spans="1:9" ht="28.8">
@@ -9252,13 +9218,13 @@
         <v>254</v>
       </c>
       <c r="B162" s="16" t="s">
-        <v>743</v>
+        <v>741</v>
       </c>
       <c r="C162" s="13" t="s">
-        <v>849</v>
+        <v>847</v>
       </c>
       <c r="D162" s="14" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="E162" s="21" t="s">
         <v>19</v>
@@ -9279,13 +9245,13 @@
         <v>255</v>
       </c>
       <c r="B163" s="16" t="s">
-        <v>743</v>
+        <v>741</v>
       </c>
       <c r="C163" s="13" t="s">
         <v>559</v>
       </c>
       <c r="D163" s="21" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="E163" s="21" t="s">
         <v>19</v>
@@ -9306,13 +9272,13 @@
         <v>256</v>
       </c>
       <c r="B164" s="16" t="s">
-        <v>743</v>
+        <v>741</v>
       </c>
       <c r="C164" s="23" t="s">
         <v>560</v>
       </c>
       <c r="D164" s="21" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="E164" s="21" t="s">
         <v>19</v>
@@ -9333,13 +9299,13 @@
         <v>257</v>
       </c>
       <c r="B165" s="16" t="s">
-        <v>743</v>
+        <v>741</v>
       </c>
       <c r="C165" s="23" t="s">
         <v>561</v>
       </c>
       <c r="D165" s="21" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="E165" s="21" t="s">
         <v>19</v>
@@ -9360,13 +9326,13 @@
         <v>258</v>
       </c>
       <c r="B166" s="16" t="s">
-        <v>743</v>
+        <v>741</v>
       </c>
       <c r="C166" s="23" t="s">
         <v>562</v>
       </c>
       <c r="D166" s="21" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="E166" s="21" t="s">
         <v>19</v>
@@ -9387,10 +9353,10 @@
         <v>259</v>
       </c>
       <c r="B167" s="16" t="s">
-        <v>743</v>
+        <v>741</v>
       </c>
       <c r="C167" s="13" t="s">
-        <v>747</v>
+        <v>745</v>
       </c>
       <c r="D167" s="21"/>
       <c r="E167" s="21" t="s">
@@ -9412,7 +9378,7 @@
         <v>260</v>
       </c>
       <c r="B168" s="16" t="s">
-        <v>743</v>
+        <v>741</v>
       </c>
       <c r="C168" s="23" t="s">
         <v>563</v>
@@ -9437,10 +9403,10 @@
         <v>261</v>
       </c>
       <c r="B169" s="16" t="s">
-        <v>743</v>
+        <v>741</v>
       </c>
       <c r="C169" s="13" t="s">
-        <v>748</v>
+        <v>746</v>
       </c>
       <c r="D169" s="21"/>
       <c r="E169" s="21" t="s">
@@ -9462,13 +9428,13 @@
         <v>262</v>
       </c>
       <c r="B170" s="16" t="s">
-        <v>743</v>
+        <v>741</v>
       </c>
       <c r="C170" s="23" t="s">
         <v>564</v>
       </c>
       <c r="D170" s="21" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="E170" s="21" t="s">
         <v>19</v>
@@ -9489,13 +9455,13 @@
         <v>263</v>
       </c>
       <c r="B171" s="16" t="s">
-        <v>743</v>
+        <v>741</v>
       </c>
       <c r="C171" s="23" t="s">
         <v>565</v>
       </c>
       <c r="D171" s="21" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="E171" s="21" t="s">
         <v>19</v>
@@ -9516,7 +9482,7 @@
         <v>264</v>
       </c>
       <c r="B172" s="16" t="s">
-        <v>743</v>
+        <v>741</v>
       </c>
       <c r="C172" s="23" t="s">
         <v>566</v>
@@ -9541,7 +9507,7 @@
         <v>265</v>
       </c>
       <c r="B173" s="16" t="s">
-        <v>743</v>
+        <v>741</v>
       </c>
       <c r="C173" s="23" t="s">
         <v>567</v>
@@ -9566,10 +9532,10 @@
         <v>266</v>
       </c>
       <c r="B174" s="16" t="s">
-        <v>743</v>
+        <v>741</v>
       </c>
       <c r="C174" s="13" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="D174" s="21"/>
       <c r="E174" s="21" t="s">
@@ -9591,10 +9557,10 @@
         <v>267</v>
       </c>
       <c r="B175" s="16" t="s">
-        <v>743</v>
+        <v>741</v>
       </c>
       <c r="C175" s="13" t="s">
-        <v>750</v>
+        <v>748</v>
       </c>
       <c r="D175" s="21"/>
       <c r="E175" s="21" t="s">
@@ -9616,13 +9582,13 @@
         <v>268</v>
       </c>
       <c r="B176" s="16" t="s">
-        <v>743</v>
+        <v>741</v>
       </c>
       <c r="C176" s="23" t="s">
         <v>568</v>
       </c>
       <c r="D176" s="21" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="E176" s="21" t="s">
         <v>19</v>
@@ -9643,13 +9609,13 @@
         <v>269</v>
       </c>
       <c r="B177" s="16" t="s">
-        <v>743</v>
+        <v>741</v>
       </c>
       <c r="C177" s="23" t="s">
         <v>569</v>
       </c>
       <c r="D177" s="21" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="E177" s="21" t="s">
         <v>19</v>
@@ -9948,7 +9914,7 @@
         <v>416</v>
       </c>
       <c r="C189" s="13" t="s">
-        <v>753</v>
+        <v>751</v>
       </c>
       <c r="D189" s="21"/>
       <c r="E189" s="21" t="s">
@@ -9998,7 +9964,7 @@
         <v>416</v>
       </c>
       <c r="C191" s="13" t="s">
-        <v>881</v>
+        <v>879</v>
       </c>
       <c r="D191" s="21"/>
       <c r="E191" s="21" t="s">
@@ -10073,7 +10039,7 @@
         <v>416</v>
       </c>
       <c r="C194" s="13" t="s">
-        <v>882</v>
+        <v>880</v>
       </c>
       <c r="D194" s="21"/>
       <c r="E194" s="21" t="s">
@@ -10122,8 +10088,8 @@
       <c r="B196" s="22" t="s">
         <v>417</v>
       </c>
-      <c r="C196" s="23" t="s">
-        <v>587</v>
+      <c r="C196" s="13" t="s">
+        <v>908</v>
       </c>
       <c r="D196" s="21"/>
       <c r="E196" s="21" t="s">
@@ -10148,7 +10114,7 @@
         <v>417</v>
       </c>
       <c r="C197" s="23" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="D197" s="21"/>
       <c r="E197" s="21" t="s">
@@ -10173,7 +10139,7 @@
         <v>417</v>
       </c>
       <c r="C198" s="23" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="D198" s="21"/>
       <c r="E198" s="21" t="s">
@@ -10198,7 +10164,7 @@
         <v>417</v>
       </c>
       <c r="C199" s="23" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="D199" s="21"/>
       <c r="E199" s="21" t="s">
@@ -10223,7 +10189,7 @@
         <v>417</v>
       </c>
       <c r="C200" s="23" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="D200" s="21"/>
       <c r="E200" s="21" t="s">
@@ -10248,7 +10214,7 @@
         <v>417</v>
       </c>
       <c r="C201" s="13" t="s">
-        <v>883</v>
+        <v>881</v>
       </c>
       <c r="D201" s="21"/>
       <c r="E201" s="21" t="s">
@@ -10273,7 +10239,7 @@
         <v>417</v>
       </c>
       <c r="C202" s="23" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="D202" s="21"/>
       <c r="E202" s="21" t="s">
@@ -10298,7 +10264,7 @@
         <v>418</v>
       </c>
       <c r="C203" s="23" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="D203" s="21"/>
       <c r="E203" s="21" t="s">
@@ -10323,7 +10289,7 @@
         <v>418</v>
       </c>
       <c r="C204" s="23" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="D204" s="21"/>
       <c r="E204" s="21" t="s">
@@ -10348,7 +10314,7 @@
         <v>418</v>
       </c>
       <c r="C205" s="23" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="D205" s="21"/>
       <c r="E205" s="21" t="s">
@@ -10373,7 +10339,7 @@
         <v>419</v>
       </c>
       <c r="C206" s="23" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="D206" s="21"/>
       <c r="E206" s="21" t="s">
@@ -10398,7 +10364,7 @@
         <v>420</v>
       </c>
       <c r="C207" s="23" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="D207" s="21"/>
       <c r="E207" s="21" t="s">
@@ -10423,7 +10389,7 @@
         <v>421</v>
       </c>
       <c r="C208" s="13" t="s">
-        <v>754</v>
+        <v>752</v>
       </c>
       <c r="D208" s="21"/>
       <c r="E208" s="21" t="s">
@@ -10448,7 +10414,7 @@
         <v>421</v>
       </c>
       <c r="C209" s="13" t="s">
-        <v>755</v>
+        <v>753</v>
       </c>
       <c r="D209" s="21"/>
       <c r="E209" s="21" t="s">
@@ -10473,7 +10439,7 @@
         <v>421</v>
       </c>
       <c r="C210" s="23" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="D210" s="21"/>
       <c r="E210" s="21" t="s">
@@ -10498,7 +10464,7 @@
         <v>421</v>
       </c>
       <c r="C211" s="13" t="s">
-        <v>756</v>
+        <v>754</v>
       </c>
       <c r="D211" s="21"/>
       <c r="E211" s="21" t="s">
@@ -10548,7 +10514,7 @@
         <v>421</v>
       </c>
       <c r="C213" s="13" t="s">
-        <v>757</v>
+        <v>755</v>
       </c>
       <c r="D213" s="21"/>
       <c r="E213" s="21" t="s">
@@ -10573,7 +10539,7 @@
         <v>421</v>
       </c>
       <c r="C214" s="13" t="s">
-        <v>758</v>
+        <v>756</v>
       </c>
       <c r="D214" s="21"/>
       <c r="E214" s="21" t="s">
@@ -10623,7 +10589,7 @@
         <v>421</v>
       </c>
       <c r="C216" s="13" t="s">
-        <v>762</v>
+        <v>760</v>
       </c>
       <c r="D216" s="21"/>
       <c r="E216" s="21" t="s">
@@ -10648,7 +10614,7 @@
         <v>422</v>
       </c>
       <c r="C217" s="13" t="s">
-        <v>759</v>
+        <v>757</v>
       </c>
       <c r="D217" s="21"/>
       <c r="E217" s="21" t="s">
@@ -10673,7 +10639,7 @@
         <v>422</v>
       </c>
       <c r="C218" s="13" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="D218" s="21"/>
       <c r="E218" s="21" t="s">
@@ -10698,7 +10664,7 @@
         <v>422</v>
       </c>
       <c r="C219" s="13" t="s">
-        <v>761</v>
+        <v>759</v>
       </c>
       <c r="D219" s="21"/>
       <c r="E219" s="21" t="s">
@@ -10723,7 +10689,7 @@
         <v>422</v>
       </c>
       <c r="C220" s="23" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="D220" s="21"/>
       <c r="E220" s="21" t="s">
@@ -10773,7 +10739,7 @@
         <v>423</v>
       </c>
       <c r="C222" s="13" t="s">
-        <v>763</v>
+        <v>761</v>
       </c>
       <c r="D222" s="21"/>
       <c r="E222" s="21" t="s">
@@ -10798,7 +10764,7 @@
         <v>423</v>
       </c>
       <c r="C223" s="13" t="s">
-        <v>764</v>
+        <v>762</v>
       </c>
       <c r="D223" s="21"/>
       <c r="E223" s="21" t="s">
@@ -10898,7 +10864,7 @@
         <v>423</v>
       </c>
       <c r="C227" s="13" t="s">
-        <v>765</v>
+        <v>763</v>
       </c>
       <c r="D227" s="21"/>
       <c r="E227" s="21" t="s">
@@ -10948,7 +10914,7 @@
         <v>423</v>
       </c>
       <c r="C229" s="13" t="s">
-        <v>766</v>
+        <v>764</v>
       </c>
       <c r="D229" s="21"/>
       <c r="E229" s="21" t="s">
@@ -10998,7 +10964,7 @@
         <v>424</v>
       </c>
       <c r="C231" s="13" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="D231" s="21"/>
       <c r="E231" s="21" t="s">
@@ -11023,7 +10989,7 @@
         <v>424</v>
       </c>
       <c r="C232" s="13" t="s">
-        <v>768</v>
+        <v>766</v>
       </c>
       <c r="D232" s="21"/>
       <c r="E232" s="21" t="s">
@@ -11048,7 +11014,7 @@
         <v>424</v>
       </c>
       <c r="C233" s="13" t="s">
-        <v>769</v>
+        <v>767</v>
       </c>
       <c r="D233" s="21"/>
       <c r="E233" s="21" t="s">
@@ -11073,7 +11039,7 @@
         <v>424</v>
       </c>
       <c r="C234" s="13" t="s">
-        <v>889</v>
+        <v>887</v>
       </c>
       <c r="D234" s="21"/>
       <c r="E234" s="21" t="s">
@@ -11092,13 +11058,13 @@
     </row>
     <row r="235" spans="1:9" ht="28.8">
       <c r="A235" s="14" t="s">
-        <v>885</v>
+        <v>883</v>
       </c>
       <c r="B235" s="41" t="s">
         <v>424</v>
       </c>
       <c r="C235" s="13" t="s">
-        <v>887</v>
+        <v>885</v>
       </c>
       <c r="D235" s="40"/>
       <c r="E235" s="40" t="s">
@@ -11117,13 +11083,13 @@
     </row>
     <row r="236" spans="1:9" ht="28.8">
       <c r="A236" s="14" t="s">
-        <v>886</v>
+        <v>884</v>
       </c>
       <c r="B236" s="41" t="s">
         <v>424</v>
       </c>
       <c r="C236" s="13" t="s">
-        <v>888</v>
+        <v>886</v>
       </c>
       <c r="D236" s="40"/>
       <c r="E236" s="40" t="s">
@@ -11139,7 +11105,7 @@
         <v>17</v>
       </c>
       <c r="I236" s="13" t="s">
-        <v>847</v>
+        <v>845</v>
       </c>
     </row>
     <row r="237" spans="1:9" ht="28.8">
@@ -11150,7 +11116,7 @@
         <v>424</v>
       </c>
       <c r="C237" s="13" t="s">
-        <v>891</v>
+        <v>889</v>
       </c>
       <c r="D237" s="21"/>
       <c r="E237" s="21" t="s">
@@ -11175,7 +11141,7 @@
         <v>424</v>
       </c>
       <c r="C238" s="13" t="s">
-        <v>772</v>
+        <v>770</v>
       </c>
       <c r="D238" s="21"/>
       <c r="E238" s="21" t="s">
@@ -11200,7 +11166,7 @@
         <v>424</v>
       </c>
       <c r="C239" s="13" t="s">
-        <v>771</v>
+        <v>769</v>
       </c>
       <c r="D239" s="21"/>
       <c r="E239" s="21" t="s">
@@ -11225,7 +11191,7 @@
         <v>424</v>
       </c>
       <c r="C240" s="13" t="s">
-        <v>892</v>
+        <v>890</v>
       </c>
       <c r="D240" s="21"/>
       <c r="E240" s="21" t="s">
@@ -11250,7 +11216,7 @@
         <v>424</v>
       </c>
       <c r="C241" s="13" t="s">
-        <v>770</v>
+        <v>768</v>
       </c>
       <c r="D241" s="21"/>
       <c r="E241" s="21" t="s">
@@ -11275,7 +11241,7 @@
         <v>424</v>
       </c>
       <c r="C242" s="13" t="s">
-        <v>773</v>
+        <v>771</v>
       </c>
       <c r="D242" s="21"/>
       <c r="E242" s="21" t="s">
@@ -11300,7 +11266,7 @@
         <v>424</v>
       </c>
       <c r="C243" s="13" t="s">
-        <v>774</v>
+        <v>772</v>
       </c>
       <c r="D243" s="21"/>
       <c r="E243" s="21" t="s">
@@ -11325,7 +11291,7 @@
         <v>424</v>
       </c>
       <c r="C244" s="13" t="s">
-        <v>775</v>
+        <v>773</v>
       </c>
       <c r="D244" s="21"/>
       <c r="E244" s="21" t="s">
@@ -11350,7 +11316,7 @@
         <v>424</v>
       </c>
       <c r="C245" s="13" t="s">
-        <v>776</v>
+        <v>774</v>
       </c>
       <c r="D245" s="21"/>
       <c r="E245" s="21" t="s">
@@ -11375,7 +11341,7 @@
         <v>424</v>
       </c>
       <c r="C246" s="13" t="s">
-        <v>777</v>
+        <v>775</v>
       </c>
       <c r="D246" s="21"/>
       <c r="E246" s="21" t="s">
@@ -11391,7 +11357,7 @@
         <v>17</v>
       </c>
       <c r="I246" s="13" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
     </row>
     <row r="247" spans="1:9" ht="28.8">
@@ -11402,7 +11368,7 @@
         <v>424</v>
       </c>
       <c r="C247" s="13" t="s">
-        <v>778</v>
+        <v>776</v>
       </c>
       <c r="D247" s="21"/>
       <c r="E247" s="21" t="s">
@@ -11427,7 +11393,7 @@
         <v>424</v>
       </c>
       <c r="C248" s="13" t="s">
-        <v>779</v>
+        <v>777</v>
       </c>
       <c r="D248" s="21"/>
       <c r="E248" s="21" t="s">
@@ -11452,7 +11418,7 @@
         <v>424</v>
       </c>
       <c r="C249" s="13" t="s">
-        <v>893</v>
+        <v>891</v>
       </c>
       <c r="D249" s="21"/>
       <c r="E249" s="21" t="s">
@@ -11477,7 +11443,7 @@
         <v>424</v>
       </c>
       <c r="C250" s="13" t="s">
-        <v>900</v>
+        <v>898</v>
       </c>
       <c r="D250" s="21"/>
       <c r="E250" s="21" t="s">
@@ -11496,13 +11462,13 @@
     </row>
     <row r="251" spans="1:9" ht="28.8">
       <c r="A251" s="14" t="s">
-        <v>899</v>
+        <v>897</v>
       </c>
       <c r="B251" s="41" t="s">
         <v>424</v>
       </c>
       <c r="C251" s="13" t="s">
-        <v>901</v>
+        <v>899</v>
       </c>
       <c r="D251" s="40"/>
       <c r="E251" s="40" t="s">
@@ -11527,7 +11493,7 @@
         <v>424</v>
       </c>
       <c r="C252" s="13" t="s">
-        <v>894</v>
+        <v>892</v>
       </c>
       <c r="D252" s="21"/>
       <c r="E252" s="21" t="s">
@@ -11552,7 +11518,7 @@
         <v>424</v>
       </c>
       <c r="C253" s="13" t="s">
-        <v>780</v>
+        <v>778</v>
       </c>
       <c r="D253" s="21"/>
       <c r="E253" s="21" t="s">
@@ -11577,7 +11543,7 @@
         <v>424</v>
       </c>
       <c r="C254" s="13" t="s">
-        <v>781</v>
+        <v>779</v>
       </c>
       <c r="D254" s="21"/>
       <c r="E254" s="21" t="s">
@@ -11602,7 +11568,7 @@
         <v>424</v>
       </c>
       <c r="C255" s="13" t="s">
-        <v>895</v>
+        <v>893</v>
       </c>
       <c r="D255" s="21"/>
       <c r="E255" s="21" t="s">
@@ -11627,7 +11593,7 @@
         <v>424</v>
       </c>
       <c r="C256" s="13" t="s">
-        <v>782</v>
+        <v>780</v>
       </c>
       <c r="D256" s="21"/>
       <c r="E256" s="21" t="s">
@@ -11652,7 +11618,7 @@
         <v>424</v>
       </c>
       <c r="C257" s="13" t="s">
-        <v>783</v>
+        <v>781</v>
       </c>
       <c r="D257" s="21"/>
       <c r="E257" s="21" t="s">
@@ -11677,7 +11643,7 @@
         <v>424</v>
       </c>
       <c r="C258" s="13" t="s">
-        <v>896</v>
+        <v>894</v>
       </c>
       <c r="D258" s="21"/>
       <c r="E258" s="21" t="s">
@@ -11702,7 +11668,7 @@
         <v>424</v>
       </c>
       <c r="C259" s="13" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="D259" s="21"/>
       <c r="E259" s="21" t="s">
@@ -11727,7 +11693,7 @@
         <v>424</v>
       </c>
       <c r="C260" s="13" t="s">
-        <v>785</v>
+        <v>783</v>
       </c>
       <c r="D260" s="21"/>
       <c r="E260" s="21" t="s">
@@ -11752,7 +11718,7 @@
         <v>424</v>
       </c>
       <c r="C261" s="13" t="s">
-        <v>786</v>
+        <v>784</v>
       </c>
       <c r="D261" s="21"/>
       <c r="E261" s="21" t="s">
@@ -11777,7 +11743,7 @@
         <v>424</v>
       </c>
       <c r="C262" s="13" t="s">
-        <v>787</v>
+        <v>785</v>
       </c>
       <c r="D262" s="21"/>
       <c r="E262" s="21" t="s">
@@ -11802,7 +11768,7 @@
         <v>424</v>
       </c>
       <c r="C263" s="13" t="s">
-        <v>788</v>
+        <v>786</v>
       </c>
       <c r="D263" s="21"/>
       <c r="E263" s="21" t="s">
@@ -11852,7 +11818,7 @@
         <v>424</v>
       </c>
       <c r="C265" s="13" t="s">
-        <v>789</v>
+        <v>787</v>
       </c>
       <c r="D265" s="21"/>
       <c r="E265" s="21" t="s">
@@ -11877,7 +11843,7 @@
         <v>424</v>
       </c>
       <c r="C266" s="13" t="s">
-        <v>790</v>
+        <v>788</v>
       </c>
       <c r="D266" s="21"/>
       <c r="E266" s="21" t="s">
@@ -11896,13 +11862,13 @@
     </row>
     <row r="267" spans="1:9" ht="28.8">
       <c r="A267" s="14" t="s">
-        <v>799</v>
+        <v>797</v>
       </c>
       <c r="B267" s="16" t="s">
         <v>424</v>
       </c>
       <c r="C267" s="42" t="s">
-        <v>791</v>
+        <v>789</v>
       </c>
       <c r="D267" s="40"/>
       <c r="E267" s="40" t="s">
@@ -11918,18 +11884,18 @@
         <v>17</v>
       </c>
       <c r="I267" s="42" t="s">
-        <v>869</v>
+        <v>867</v>
       </c>
     </row>
     <row r="268" spans="1:9" ht="28.8">
       <c r="A268" s="14" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="B268" s="16" t="s">
         <v>424</v>
       </c>
       <c r="C268" s="42" t="s">
-        <v>792</v>
+        <v>790</v>
       </c>
       <c r="D268" s="40"/>
       <c r="E268" s="40" t="s">
@@ -11948,13 +11914,13 @@
     </row>
     <row r="269" spans="1:9" ht="28.8">
       <c r="A269" s="14" t="s">
-        <v>801</v>
+        <v>799</v>
       </c>
       <c r="B269" s="16" t="s">
         <v>424</v>
       </c>
       <c r="C269" s="42" t="s">
-        <v>793</v>
+        <v>791</v>
       </c>
       <c r="D269" s="40"/>
       <c r="E269" s="40" t="s">
@@ -11970,18 +11936,18 @@
         <v>17</v>
       </c>
       <c r="I269" s="42" t="s">
-        <v>872</v>
+        <v>870</v>
       </c>
     </row>
     <row r="270" spans="1:9" ht="28.8">
       <c r="A270" s="14" t="s">
-        <v>802</v>
+        <v>800</v>
       </c>
       <c r="B270" s="16" t="s">
         <v>424</v>
       </c>
       <c r="C270" s="42" t="s">
-        <v>794</v>
+        <v>792</v>
       </c>
       <c r="D270" s="40"/>
       <c r="E270" s="40" t="s">
@@ -12000,13 +11966,13 @@
     </row>
     <row r="271" spans="1:9" ht="28.8">
       <c r="A271" s="14" t="s">
-        <v>803</v>
+        <v>801</v>
       </c>
       <c r="B271" s="16" t="s">
         <v>424</v>
       </c>
       <c r="C271" s="42" t="s">
-        <v>795</v>
+        <v>793</v>
       </c>
       <c r="D271" s="40"/>
       <c r="E271" s="40" t="s">
@@ -12025,13 +11991,13 @@
     </row>
     <row r="272" spans="1:9" ht="28.8">
       <c r="A272" s="14" t="s">
-        <v>804</v>
+        <v>802</v>
       </c>
       <c r="B272" s="16" t="s">
         <v>424</v>
       </c>
       <c r="C272" s="42" t="s">
-        <v>796</v>
+        <v>794</v>
       </c>
       <c r="D272" s="40"/>
       <c r="E272" s="40" t="s">
@@ -12047,18 +12013,18 @@
         <v>17</v>
       </c>
       <c r="I272" s="42" t="s">
-        <v>848</v>
+        <v>846</v>
       </c>
     </row>
     <row r="273" spans="1:9" ht="28.8">
       <c r="A273" s="14" t="s">
-        <v>805</v>
+        <v>803</v>
       </c>
       <c r="B273" s="16" t="s">
         <v>424</v>
       </c>
       <c r="C273" s="42" t="s">
-        <v>797</v>
+        <v>795</v>
       </c>
       <c r="D273" s="40"/>
       <c r="E273" s="40" t="s">
@@ -12077,13 +12043,13 @@
     </row>
     <row r="274" spans="1:9" ht="28.8">
       <c r="A274" s="14" t="s">
-        <v>806</v>
+        <v>804</v>
       </c>
       <c r="B274" s="16" t="s">
         <v>424</v>
       </c>
       <c r="C274" s="42" t="s">
-        <v>798</v>
+        <v>796</v>
       </c>
       <c r="D274" s="40"/>
       <c r="E274" s="40" t="s">
@@ -12105,10 +12071,10 @@
         <v>162</v>
       </c>
       <c r="B275" s="16" t="s">
-        <v>817</v>
+        <v>815</v>
       </c>
       <c r="C275" s="13" t="s">
-        <v>807</v>
+        <v>805</v>
       </c>
       <c r="D275" s="21"/>
       <c r="E275" s="21" t="s">
@@ -12130,10 +12096,10 @@
         <v>163</v>
       </c>
       <c r="B276" s="16" t="s">
-        <v>817</v>
+        <v>815</v>
       </c>
       <c r="C276" s="13" t="s">
-        <v>808</v>
+        <v>806</v>
       </c>
       <c r="D276" s="21"/>
       <c r="E276" s="21" t="s">
@@ -12155,10 +12121,10 @@
         <v>164</v>
       </c>
       <c r="B277" s="16" t="s">
-        <v>817</v>
+        <v>815</v>
       </c>
       <c r="C277" s="13" t="s">
-        <v>809</v>
+        <v>807</v>
       </c>
       <c r="D277" s="21"/>
       <c r="E277" s="21" t="s">
@@ -12180,10 +12146,10 @@
         <v>165</v>
       </c>
       <c r="B278" s="16" t="s">
-        <v>817</v>
+        <v>815</v>
       </c>
       <c r="C278" s="13" t="s">
-        <v>810</v>
+        <v>808</v>
       </c>
       <c r="D278" s="21"/>
       <c r="E278" s="21" t="s">
@@ -12205,7 +12171,7 @@
         <v>166</v>
       </c>
       <c r="B279" s="16" t="s">
-        <v>818</v>
+        <v>816</v>
       </c>
       <c r="C279" s="23" t="s">
         <v>492</v>
@@ -12230,10 +12196,10 @@
         <v>167</v>
       </c>
       <c r="B280" s="16" t="s">
-        <v>818</v>
+        <v>816</v>
       </c>
       <c r="C280" s="13" t="s">
-        <v>811</v>
+        <v>809</v>
       </c>
       <c r="D280" s="21"/>
       <c r="E280" s="21" t="s">
@@ -12255,10 +12221,10 @@
         <v>168</v>
       </c>
       <c r="B281" s="16" t="s">
-        <v>818</v>
+        <v>816</v>
       </c>
       <c r="C281" s="13" t="s">
-        <v>812</v>
+        <v>810</v>
       </c>
       <c r="D281" s="21"/>
       <c r="E281" s="21" t="s">
@@ -12280,7 +12246,7 @@
         <v>169</v>
       </c>
       <c r="B282" s="16" t="s">
-        <v>818</v>
+        <v>816</v>
       </c>
       <c r="C282" s="23" t="s">
         <v>493</v>
@@ -12305,7 +12271,7 @@
         <v>170</v>
       </c>
       <c r="B283" s="16" t="s">
-        <v>818</v>
+        <v>816</v>
       </c>
       <c r="C283" s="23" t="s">
         <v>494</v>
@@ -12330,7 +12296,7 @@
         <v>171</v>
       </c>
       <c r="B284" s="16" t="s">
-        <v>818</v>
+        <v>816</v>
       </c>
       <c r="C284" s="23" t="s">
         <v>495</v>
@@ -12355,13 +12321,13 @@
         <v>172</v>
       </c>
       <c r="B285" s="16" t="s">
-        <v>818</v>
+        <v>816</v>
       </c>
       <c r="C285" s="23" t="s">
         <v>496</v>
       </c>
       <c r="D285" s="21" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="E285" s="21" t="s">
         <v>19</v>
@@ -12382,13 +12348,13 @@
         <v>173</v>
       </c>
       <c r="B286" s="16" t="s">
-        <v>818</v>
+        <v>816</v>
       </c>
       <c r="C286" s="23" t="s">
         <v>497</v>
       </c>
       <c r="D286" s="21" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="E286" s="21" t="s">
         <v>19</v>
@@ -12409,7 +12375,7 @@
         <v>174</v>
       </c>
       <c r="B287" s="16" t="s">
-        <v>819</v>
+        <v>817</v>
       </c>
       <c r="C287" s="23" t="s">
         <v>498</v>
@@ -12434,10 +12400,10 @@
         <v>175</v>
       </c>
       <c r="B288" s="16" t="s">
-        <v>819</v>
+        <v>817</v>
       </c>
       <c r="C288" s="13" t="s">
-        <v>813</v>
+        <v>811</v>
       </c>
       <c r="D288" s="21"/>
       <c r="E288" s="21" t="s">
@@ -12459,7 +12425,7 @@
         <v>176</v>
       </c>
       <c r="B289" s="16" t="s">
-        <v>819</v>
+        <v>817</v>
       </c>
       <c r="C289" s="23" t="s">
         <v>499</v>
@@ -12484,10 +12450,10 @@
         <v>177</v>
       </c>
       <c r="B290" s="16" t="s">
-        <v>819</v>
+        <v>817</v>
       </c>
       <c r="C290" s="13" t="s">
-        <v>814</v>
+        <v>812</v>
       </c>
       <c r="D290" s="21"/>
       <c r="E290" s="21" t="s">
@@ -12509,7 +12475,7 @@
         <v>178</v>
       </c>
       <c r="B291" s="16" t="s">
-        <v>819</v>
+        <v>817</v>
       </c>
       <c r="C291" s="23" t="s">
         <v>500</v>
@@ -12534,7 +12500,7 @@
         <v>179</v>
       </c>
       <c r="B292" s="16" t="s">
-        <v>819</v>
+        <v>817</v>
       </c>
       <c r="C292" s="23" t="s">
         <v>501</v>
@@ -12559,10 +12525,10 @@
         <v>180</v>
       </c>
       <c r="B293" s="16" t="s">
-        <v>819</v>
+        <v>817</v>
       </c>
       <c r="C293" s="13" t="s">
-        <v>815</v>
+        <v>813</v>
       </c>
       <c r="D293" s="21"/>
       <c r="E293" s="21" t="s">
@@ -12584,7 +12550,7 @@
         <v>181</v>
       </c>
       <c r="B294" s="16" t="s">
-        <v>819</v>
+        <v>817</v>
       </c>
       <c r="C294" s="23" t="s">
         <v>502</v>
@@ -12609,7 +12575,7 @@
         <v>182</v>
       </c>
       <c r="B295" s="16" t="s">
-        <v>819</v>
+        <v>817</v>
       </c>
       <c r="C295" s="23" t="s">
         <v>503</v>
@@ -12634,13 +12600,13 @@
         <v>183</v>
       </c>
       <c r="B296" s="16" t="s">
-        <v>819</v>
+        <v>817</v>
       </c>
       <c r="C296" s="23" t="s">
         <v>504</v>
       </c>
       <c r="D296" s="21" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="E296" s="21" t="s">
         <v>19</v>
@@ -12661,13 +12627,13 @@
         <v>184</v>
       </c>
       <c r="B297" s="16" t="s">
-        <v>819</v>
+        <v>817</v>
       </c>
       <c r="C297" s="23" t="s">
         <v>505</v>
       </c>
       <c r="D297" s="21" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="E297" s="21" t="s">
         <v>19</v>
@@ -12688,10 +12654,10 @@
         <v>185</v>
       </c>
       <c r="B298" s="16" t="s">
-        <v>819</v>
+        <v>817</v>
       </c>
       <c r="C298" s="13" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="D298" s="21"/>
       <c r="E298" s="21" t="s">
@@ -12713,7 +12679,7 @@
         <v>186</v>
       </c>
       <c r="B299" s="16" t="s">
-        <v>819</v>
+        <v>817</v>
       </c>
       <c r="C299" s="23" t="s">
         <v>506</v>
@@ -12738,7 +12704,7 @@
         <v>187</v>
       </c>
       <c r="B300" s="16" t="s">
-        <v>819</v>
+        <v>817</v>
       </c>
       <c r="C300" s="23" t="s">
         <v>507</v>
@@ -12763,10 +12729,10 @@
         <v>188</v>
       </c>
       <c r="B301" s="16" t="s">
-        <v>819</v>
+        <v>817</v>
       </c>
       <c r="C301" s="13" t="s">
-        <v>816</v>
+        <v>814</v>
       </c>
       <c r="D301" s="21"/>
       <c r="E301" s="21" t="s">
@@ -12788,10 +12754,10 @@
         <v>345</v>
       </c>
       <c r="B302" s="16" t="s">
-        <v>822</v>
+        <v>820</v>
       </c>
       <c r="C302" s="23" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="D302" s="21"/>
       <c r="E302" s="21" t="s">
@@ -12813,10 +12779,10 @@
         <v>346</v>
       </c>
       <c r="B303" s="16" t="s">
-        <v>822</v>
+        <v>820</v>
       </c>
       <c r="C303" s="13" t="s">
-        <v>821</v>
+        <v>819</v>
       </c>
       <c r="D303" s="21"/>
       <c r="E303" s="21" t="s">
@@ -12838,10 +12804,10 @@
         <v>347</v>
       </c>
       <c r="B304" s="16" t="s">
-        <v>822</v>
+        <v>820</v>
       </c>
       <c r="C304" s="23" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="D304" s="21"/>
       <c r="E304" s="21" t="s">
@@ -12863,10 +12829,10 @@
         <v>307</v>
       </c>
       <c r="B305" s="16" t="s">
-        <v>823</v>
+        <v>821</v>
       </c>
       <c r="C305" s="13" t="s">
-        <v>824</v>
+        <v>822</v>
       </c>
       <c r="D305" s="21"/>
       <c r="E305" s="21" t="s">
@@ -12888,10 +12854,10 @@
         <v>308</v>
       </c>
       <c r="B306" s="16" t="s">
+        <v>821</v>
+      </c>
+      <c r="C306" s="13" t="s">
         <v>823</v>
-      </c>
-      <c r="C306" s="13" t="s">
-        <v>825</v>
       </c>
       <c r="D306" s="21"/>
       <c r="E306" s="21" t="s">
@@ -12913,10 +12879,10 @@
         <v>309</v>
       </c>
       <c r="B307" s="16" t="s">
-        <v>823</v>
+        <v>821</v>
       </c>
       <c r="C307" s="13" t="s">
-        <v>902</v>
+        <v>900</v>
       </c>
       <c r="D307" s="21"/>
       <c r="E307" s="21" t="s">
@@ -12938,10 +12904,10 @@
         <v>310</v>
       </c>
       <c r="B308" s="16" t="s">
-        <v>823</v>
+        <v>821</v>
       </c>
       <c r="C308" s="13" t="s">
-        <v>826</v>
+        <v>824</v>
       </c>
       <c r="D308" s="21"/>
       <c r="E308" s="21" t="s">
@@ -12963,10 +12929,10 @@
         <v>311</v>
       </c>
       <c r="B309" s="16" t="s">
-        <v>823</v>
+        <v>821</v>
       </c>
       <c r="C309" s="13" t="s">
-        <v>827</v>
+        <v>825</v>
       </c>
       <c r="D309" s="21"/>
       <c r="E309" s="21" t="s">
@@ -12988,10 +12954,10 @@
         <v>312</v>
       </c>
       <c r="B310" s="16" t="s">
-        <v>823</v>
+        <v>821</v>
       </c>
       <c r="C310" s="13" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="D310" s="21"/>
       <c r="E310" s="21" t="s">
@@ -13007,7 +12973,7 @@
         <v>17</v>
       </c>
       <c r="I310" s="13" t="s">
-        <v>855</v>
+        <v>853</v>
       </c>
     </row>
     <row r="311" spans="1:9" ht="28.8">
@@ -13015,13 +12981,13 @@
         <v>313</v>
       </c>
       <c r="B311" s="16" t="s">
-        <v>823</v>
+        <v>821</v>
       </c>
       <c r="C311" s="13" t="s">
-        <v>851</v>
+        <v>849</v>
       </c>
       <c r="D311" s="21" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="E311" s="21" t="s">
         <v>19</v>
@@ -13042,13 +13008,13 @@
         <v>314</v>
       </c>
       <c r="B312" s="16" t="s">
-        <v>823</v>
+        <v>821</v>
       </c>
       <c r="C312" s="23" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="D312" s="21" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="E312" s="21" t="s">
         <v>19</v>
@@ -13069,13 +13035,13 @@
         <v>315</v>
       </c>
       <c r="B313" s="16" t="s">
-        <v>823</v>
+        <v>821</v>
       </c>
       <c r="C313" s="23" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="D313" s="21" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="E313" s="21" t="s">
         <v>19</v>
@@ -13096,13 +13062,13 @@
         <v>316</v>
       </c>
       <c r="B314" s="16" t="s">
-        <v>823</v>
+        <v>821</v>
       </c>
       <c r="C314" s="13" t="s">
-        <v>854</v>
+        <v>852</v>
       </c>
       <c r="D314" s="21" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="E314" s="21" t="s">
         <v>19</v>
@@ -13123,13 +13089,13 @@
         <v>317</v>
       </c>
       <c r="B315" s="16" t="s">
-        <v>823</v>
+        <v>821</v>
       </c>
       <c r="C315" s="23" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="D315" s="14" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="E315" s="21" t="s">
         <v>19</v>
@@ -13150,13 +13116,13 @@
         <v>318</v>
       </c>
       <c r="B316" s="16" t="s">
-        <v>823</v>
+        <v>821</v>
       </c>
       <c r="C316" s="23" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="D316" s="21" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="E316" s="21" t="s">
         <v>19</v>
@@ -13177,13 +13143,13 @@
         <v>319</v>
       </c>
       <c r="B317" s="16" t="s">
-        <v>823</v>
+        <v>821</v>
       </c>
       <c r="C317" s="23" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="D317" s="21" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="E317" s="21" t="s">
         <v>19</v>
@@ -13204,13 +13170,13 @@
         <v>320</v>
       </c>
       <c r="B318" s="16" t="s">
-        <v>823</v>
+        <v>821</v>
       </c>
       <c r="C318" s="23" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="D318" s="21" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="E318" s="21" t="s">
         <v>19</v>
@@ -13231,10 +13197,10 @@
         <v>321</v>
       </c>
       <c r="B319" s="16" t="s">
-        <v>823</v>
+        <v>821</v>
       </c>
       <c r="C319" s="13" t="s">
-        <v>828</v>
+        <v>826</v>
       </c>
       <c r="D319" s="21"/>
       <c r="E319" s="21" t="s">
@@ -13256,10 +13222,10 @@
         <v>322</v>
       </c>
       <c r="B320" s="16" t="s">
-        <v>823</v>
+        <v>821</v>
       </c>
       <c r="C320" s="23" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="D320" s="21"/>
       <c r="E320" s="21" t="s">
@@ -13281,10 +13247,10 @@
         <v>323</v>
       </c>
       <c r="B321" s="16" t="s">
-        <v>823</v>
+        <v>821</v>
       </c>
       <c r="C321" s="23" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="D321" s="21"/>
       <c r="E321" s="21" t="s">
@@ -13306,10 +13272,10 @@
         <v>324</v>
       </c>
       <c r="B322" s="16" t="s">
-        <v>823</v>
+        <v>821</v>
       </c>
       <c r="C322" s="23" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="D322" s="21"/>
       <c r="E322" s="21" t="s">
@@ -13331,10 +13297,10 @@
         <v>325</v>
       </c>
       <c r="B323" s="16" t="s">
-        <v>823</v>
+        <v>821</v>
       </c>
       <c r="C323" s="13" t="s">
-        <v>829</v>
+        <v>827</v>
       </c>
       <c r="D323" s="21"/>
       <c r="E323" s="21" t="s">
@@ -13356,10 +13322,10 @@
         <v>326</v>
       </c>
       <c r="B324" s="16" t="s">
-        <v>823</v>
+        <v>821</v>
       </c>
       <c r="C324" s="13" t="s">
-        <v>830</v>
+        <v>828</v>
       </c>
       <c r="D324" s="21"/>
       <c r="E324" s="21" t="s">
@@ -13381,13 +13347,13 @@
         <v>327</v>
       </c>
       <c r="B325" s="16" t="s">
-        <v>823</v>
+        <v>821</v>
       </c>
       <c r="C325" s="23" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="D325" s="21" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="E325" s="21" t="s">
         <v>19</v>
@@ -13408,13 +13374,13 @@
         <v>328</v>
       </c>
       <c r="B326" s="16" t="s">
-        <v>823</v>
+        <v>821</v>
       </c>
       <c r="C326" s="23" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="D326" s="21" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="E326" s="21" t="s">
         <v>19</v>
@@ -13435,10 +13401,10 @@
         <v>329</v>
       </c>
       <c r="B327" s="16" t="s">
-        <v>823</v>
+        <v>821</v>
       </c>
       <c r="C327" s="13" t="s">
-        <v>831</v>
+        <v>829</v>
       </c>
       <c r="D327" s="21"/>
       <c r="E327" s="21" t="s">
@@ -13460,10 +13426,10 @@
         <v>330</v>
       </c>
       <c r="B328" s="16" t="s">
-        <v>823</v>
+        <v>821</v>
       </c>
       <c r="C328" s="23" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="D328" s="21"/>
       <c r="E328" s="21" t="s">
@@ -13485,13 +13451,13 @@
         <v>331</v>
       </c>
       <c r="B329" s="16" t="s">
-        <v>823</v>
+        <v>821</v>
       </c>
       <c r="C329" s="23" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="D329" s="21" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="E329" s="21" t="s">
         <v>19</v>
@@ -13512,13 +13478,13 @@
         <v>332</v>
       </c>
       <c r="B330" s="16" t="s">
-        <v>823</v>
+        <v>821</v>
       </c>
       <c r="C330" s="23" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="D330" s="21" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="E330" s="21" t="s">
         <v>19</v>
@@ -13539,10 +13505,10 @@
         <v>333</v>
       </c>
       <c r="B331" s="16" t="s">
-        <v>823</v>
+        <v>821</v>
       </c>
       <c r="C331" s="13" t="s">
-        <v>832</v>
+        <v>830</v>
       </c>
       <c r="D331" s="21"/>
       <c r="E331" s="21" t="s">
@@ -13564,13 +13530,13 @@
         <v>334</v>
       </c>
       <c r="B332" s="16" t="s">
-        <v>823</v>
+        <v>821</v>
       </c>
       <c r="C332" s="23" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="D332" s="21" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="E332" s="21" t="s">
         <v>19</v>
@@ -13591,13 +13557,13 @@
         <v>335</v>
       </c>
       <c r="B333" s="16" t="s">
-        <v>823</v>
+        <v>821</v>
       </c>
       <c r="C333" s="23" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="D333" s="21" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="E333" s="21" t="s">
         <v>19</v>
@@ -13618,10 +13584,10 @@
         <v>336</v>
       </c>
       <c r="B334" s="16" t="s">
-        <v>823</v>
+        <v>821</v>
       </c>
       <c r="C334" s="23" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="D334" s="21"/>
       <c r="E334" s="21" t="s">
@@ -13643,10 +13609,10 @@
         <v>337</v>
       </c>
       <c r="B335" s="16" t="s">
-        <v>823</v>
+        <v>821</v>
       </c>
       <c r="C335" s="23" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="D335" s="21"/>
       <c r="E335" s="21" t="s">
@@ -13668,10 +13634,10 @@
         <v>338</v>
       </c>
       <c r="B336" s="16" t="s">
-        <v>823</v>
+        <v>821</v>
       </c>
       <c r="C336" s="23" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="D336" s="21"/>
       <c r="E336" s="21" t="s">
@@ -13687,7 +13653,7 @@
         <v>17</v>
       </c>
       <c r="I336" s="13" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
     </row>
     <row r="337" spans="1:9" ht="28.8">
@@ -13695,13 +13661,13 @@
         <v>339</v>
       </c>
       <c r="B337" s="16" t="s">
-        <v>823</v>
+        <v>821</v>
       </c>
       <c r="C337" s="23" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="D337" s="21" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="E337" s="21" t="s">
         <v>19</v>
@@ -13722,10 +13688,10 @@
         <v>340</v>
       </c>
       <c r="B338" s="16" t="s">
-        <v>823</v>
+        <v>821</v>
       </c>
       <c r="C338" s="23" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="D338" s="21"/>
       <c r="E338" s="21" t="s">
@@ -13747,10 +13713,10 @@
         <v>341</v>
       </c>
       <c r="B339" s="16" t="s">
-        <v>823</v>
+        <v>821</v>
       </c>
       <c r="C339" s="23" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="D339" s="21"/>
       <c r="E339" s="21" t="s">
@@ -13772,10 +13738,10 @@
         <v>342</v>
       </c>
       <c r="B340" s="16" t="s">
-        <v>823</v>
+        <v>821</v>
       </c>
       <c r="C340" s="13" t="s">
-        <v>833</v>
+        <v>831</v>
       </c>
       <c r="D340" s="21"/>
       <c r="E340" s="21" t="s">
@@ -13797,13 +13763,13 @@
         <v>343</v>
       </c>
       <c r="B341" s="16" t="s">
-        <v>823</v>
+        <v>821</v>
       </c>
       <c r="C341" s="23" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="D341" s="21" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="E341" s="21" t="s">
         <v>19</v>
@@ -13818,7 +13784,7 @@
         <v>17</v>
       </c>
       <c r="I341" s="13" t="s">
-        <v>845</v>
+        <v>843</v>
       </c>
     </row>
     <row r="342" spans="1:9" ht="28.8">
@@ -13826,13 +13792,13 @@
         <v>344</v>
       </c>
       <c r="B342" s="16" t="s">
-        <v>823</v>
+        <v>821</v>
       </c>
       <c r="C342" s="13" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="D342" s="21" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="E342" s="21" t="s">
         <v>19</v>
@@ -13847,18 +13813,18 @@
         <v>17</v>
       </c>
       <c r="I342" s="13" t="s">
-        <v>845</v>
+        <v>843</v>
       </c>
     </row>
     <row r="343" spans="1:9" ht="28.8">
       <c r="A343" s="14" t="s">
-        <v>903</v>
+        <v>901</v>
       </c>
       <c r="B343" s="16" t="s">
-        <v>823</v>
+        <v>821</v>
       </c>
       <c r="C343" s="13" t="s">
-        <v>906</v>
+        <v>904</v>
       </c>
       <c r="D343" s="40"/>
       <c r="E343" s="40" t="s">
@@ -13877,13 +13843,13 @@
     </row>
     <row r="344" spans="1:9" ht="28.8">
       <c r="A344" s="14" t="s">
-        <v>904</v>
+        <v>902</v>
       </c>
       <c r="B344" s="16" t="s">
-        <v>823</v>
+        <v>821</v>
       </c>
       <c r="C344" s="13" t="s">
-        <v>907</v>
+        <v>905</v>
       </c>
       <c r="D344" s="40"/>
       <c r="E344" s="40" t="s">
@@ -13902,13 +13868,13 @@
     </row>
     <row r="345" spans="1:9" ht="28.8">
       <c r="A345" s="14" t="s">
-        <v>905</v>
+        <v>903</v>
       </c>
       <c r="B345" s="16" t="s">
-        <v>823</v>
+        <v>821</v>
       </c>
       <c r="C345" s="13" t="s">
-        <v>908</v>
+        <v>906</v>
       </c>
       <c r="D345" s="40"/>
       <c r="E345" s="40" t="s">
@@ -13933,7 +13899,7 @@
         <v>425</v>
       </c>
       <c r="C346" s="23" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="D346" s="21"/>
       <c r="E346" s="21" t="s">
@@ -13958,7 +13924,7 @@
         <v>425</v>
       </c>
       <c r="C347" s="23" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="D347" s="21"/>
       <c r="E347" s="21" t="s">
@@ -13983,7 +13949,7 @@
         <v>425</v>
       </c>
       <c r="C348" s="13" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="D348" s="21"/>
       <c r="E348" s="21" t="s">
@@ -14008,7 +13974,7 @@
         <v>426</v>
       </c>
       <c r="C349" s="23" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="D349" s="21"/>
       <c r="E349" s="21" t="s">
@@ -14033,7 +13999,7 @@
         <v>427</v>
       </c>
       <c r="C350" s="23" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="D350" s="21"/>
       <c r="E350" s="21" t="s">
@@ -14058,7 +14024,7 @@
         <v>427</v>
       </c>
       <c r="C351" s="23" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="D351" s="21"/>
       <c r="E351" s="21" t="s">
@@ -14083,7 +14049,7 @@
         <v>427</v>
       </c>
       <c r="C352" s="23" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="D352" s="21"/>
       <c r="E352" s="21" t="s">
@@ -14108,7 +14074,7 @@
         <v>427</v>
       </c>
       <c r="C353" s="13" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="D353" s="21"/>
       <c r="E353" s="21" t="s">
@@ -14133,7 +14099,7 @@
         <v>428</v>
       </c>
       <c r="C354" s="23" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="D354" s="21"/>
       <c r="E354" s="21" t="s">
@@ -14158,7 +14124,7 @@
         <v>428</v>
       </c>
       <c r="C355" s="23" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="D355" s="21"/>
       <c r="E355" s="21" t="s">
@@ -14183,10 +14149,10 @@
         <v>428</v>
       </c>
       <c r="C356" s="23" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="D356" s="21" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="E356" s="21" t="s">
         <v>22</v>
@@ -14201,7 +14167,7 @@
         <v>21</v>
       </c>
       <c r="I356" s="23" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
     </row>
     <row r="357" spans="1:9" ht="43.2">
@@ -14212,10 +14178,10 @@
         <v>428</v>
       </c>
       <c r="C357" s="23" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="D357" s="21" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="E357" s="21" t="s">
         <v>22</v>
@@ -14230,7 +14196,7 @@
         <v>20</v>
       </c>
       <c r="I357" s="23" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
     </row>
     <row r="358" spans="1:9" ht="43.2">
@@ -14241,10 +14207,10 @@
         <v>428</v>
       </c>
       <c r="C358" s="13" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="D358" s="21" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="E358" s="14" t="s">
         <v>22</v>
@@ -14259,21 +14225,21 @@
         <v>20</v>
       </c>
       <c r="I358" s="23" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
     </row>
     <row r="359" spans="1:9" ht="43.2">
       <c r="A359" s="14" t="s">
-        <v>835</v>
+        <v>833</v>
       </c>
       <c r="B359" s="41" t="s">
         <v>428</v>
       </c>
       <c r="C359" s="42" t="s">
-        <v>834</v>
+        <v>832</v>
       </c>
       <c r="D359" s="40" t="s">
-        <v>843</v>
+        <v>841</v>
       </c>
       <c r="E359" s="21" t="s">
         <v>22</v>
@@ -14291,16 +14257,16 @@
     </row>
     <row r="360" spans="1:9" ht="43.2">
       <c r="A360" s="14" t="s">
-        <v>836</v>
+        <v>834</v>
       </c>
       <c r="B360" s="41" t="s">
         <v>428</v>
       </c>
       <c r="C360" s="13" t="s">
-        <v>860</v>
+        <v>858</v>
       </c>
       <c r="D360" s="40" t="s">
-        <v>843</v>
+        <v>841</v>
       </c>
       <c r="E360" s="21" t="s">
         <v>22</v>
@@ -14315,21 +14281,21 @@
         <v>20</v>
       </c>
       <c r="I360" s="23" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
     </row>
     <row r="361" spans="1:9" ht="28.8">
       <c r="A361" s="14" t="s">
-        <v>837</v>
+        <v>835</v>
       </c>
       <c r="B361" s="41" t="s">
         <v>428</v>
       </c>
       <c r="C361" s="13" t="s">
-        <v>897</v>
+        <v>895</v>
       </c>
       <c r="D361" s="14" t="s">
-        <v>890</v>
+        <v>888</v>
       </c>
       <c r="E361" s="21" t="s">
         <v>22</v>
@@ -14347,16 +14313,16 @@
     </row>
     <row r="362" spans="1:9" ht="43.2">
       <c r="A362" s="14" t="s">
-        <v>838</v>
+        <v>836</v>
       </c>
       <c r="B362" s="41" t="s">
         <v>428</v>
       </c>
       <c r="C362" s="13" t="s">
-        <v>898</v>
+        <v>896</v>
       </c>
       <c r="D362" s="14" t="s">
-        <v>890</v>
+        <v>888</v>
       </c>
       <c r="E362" s="21" t="s">
         <v>22</v>
@@ -14371,21 +14337,21 @@
         <v>20</v>
       </c>
       <c r="I362" s="23" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
     </row>
     <row r="363" spans="1:9" ht="43.2">
       <c r="A363" s="14" t="s">
-        <v>865</v>
+        <v>863</v>
       </c>
       <c r="B363" s="41" t="s">
         <v>428</v>
       </c>
       <c r="C363" s="42" t="s">
-        <v>861</v>
+        <v>859</v>
       </c>
       <c r="D363" s="14" t="s">
-        <v>870</v>
+        <v>868</v>
       </c>
       <c r="E363" s="21" t="s">
         <v>22</v>
@@ -14403,16 +14369,16 @@
     </row>
     <row r="364" spans="1:9" ht="43.2">
       <c r="A364" s="14" t="s">
-        <v>866</v>
+        <v>864</v>
       </c>
       <c r="B364" s="41" t="s">
         <v>428</v>
       </c>
       <c r="C364" s="42" t="s">
-        <v>862</v>
+        <v>860</v>
       </c>
       <c r="D364" s="40" t="s">
-        <v>870</v>
+        <v>868</v>
       </c>
       <c r="E364" s="21" t="s">
         <v>22</v>
@@ -14427,21 +14393,21 @@
         <v>20</v>
       </c>
       <c r="I364" s="23" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
     </row>
     <row r="365" spans="1:9" ht="43.2">
       <c r="A365" s="14" t="s">
-        <v>867</v>
+        <v>865</v>
       </c>
       <c r="B365" s="41" t="s">
         <v>428</v>
       </c>
       <c r="C365" s="42" t="s">
-        <v>863</v>
+        <v>861</v>
       </c>
       <c r="D365" s="40" t="s">
-        <v>871</v>
+        <v>869</v>
       </c>
       <c r="E365" s="21" t="s">
         <v>22</v>
@@ -14459,16 +14425,16 @@
     </row>
     <row r="366" spans="1:9" ht="43.2">
       <c r="A366" s="14" t="s">
-        <v>868</v>
+        <v>866</v>
       </c>
       <c r="B366" s="41" t="s">
         <v>428</v>
       </c>
       <c r="C366" s="42" t="s">
-        <v>864</v>
+        <v>862</v>
       </c>
       <c r="D366" s="40" t="s">
-        <v>871</v>
+        <v>869</v>
       </c>
       <c r="E366" s="21" t="s">
         <v>22</v>
@@ -14483,21 +14449,21 @@
         <v>20</v>
       </c>
       <c r="I366" s="23" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
     </row>
     <row r="367" spans="1:9" ht="43.2">
       <c r="A367" s="14" t="s">
-        <v>839</v>
+        <v>837</v>
       </c>
       <c r="B367" s="41" t="s">
         <v>428</v>
       </c>
       <c r="C367" s="42" t="s">
-        <v>856</v>
+        <v>854</v>
       </c>
       <c r="D367" s="40" t="s">
-        <v>844</v>
+        <v>842</v>
       </c>
       <c r="E367" s="21" t="s">
         <v>22</v>
@@ -14515,16 +14481,16 @@
     </row>
     <row r="368" spans="1:9" ht="43.2">
       <c r="A368" s="14" t="s">
-        <v>840</v>
+        <v>838</v>
       </c>
       <c r="B368" s="41" t="s">
         <v>428</v>
       </c>
       <c r="C368" s="42" t="s">
-        <v>857</v>
+        <v>855</v>
       </c>
       <c r="D368" s="40" t="s">
-        <v>844</v>
+        <v>842</v>
       </c>
       <c r="E368" s="21" t="s">
         <v>22</v>
@@ -14539,21 +14505,21 @@
         <v>20</v>
       </c>
       <c r="I368" s="23" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
     </row>
     <row r="369" spans="1:9" ht="28.8">
       <c r="A369" s="14" t="s">
-        <v>841</v>
+        <v>839</v>
       </c>
       <c r="B369" s="41" t="s">
         <v>428</v>
       </c>
       <c r="C369" s="13" t="s">
-        <v>858</v>
+        <v>856</v>
       </c>
       <c r="D369" s="14" t="s">
-        <v>873</v>
+        <v>871</v>
       </c>
       <c r="E369" s="21" t="s">
         <v>22</v>
@@ -14571,16 +14537,16 @@
     </row>
     <row r="370" spans="1:9" ht="43.2">
       <c r="A370" s="14" t="s">
-        <v>842</v>
+        <v>840</v>
       </c>
       <c r="B370" s="41" t="s">
         <v>428</v>
       </c>
       <c r="C370" s="42" t="s">
-        <v>859</v>
+        <v>857</v>
       </c>
       <c r="D370" s="14" t="s">
-        <v>873</v>
+        <v>871</v>
       </c>
       <c r="E370" s="21" t="s">
         <v>22</v>
@@ -14595,7 +14561,7 @@
         <v>20</v>
       </c>
       <c r="I370" s="23" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
     </row>
     <row r="371" spans="1:9" ht="72">
@@ -14606,7 +14572,7 @@
         <v>429</v>
       </c>
       <c r="C371" s="23" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="D371" s="21"/>
       <c r="E371" s="21" t="s">
@@ -14622,7 +14588,7 @@
         <v>17</v>
       </c>
       <c r="I371" s="23" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
     </row>
     <row r="372" spans="1:9" ht="43.2">
@@ -14633,7 +14599,7 @@
         <v>430</v>
       </c>
       <c r="C372" s="13" t="s">
-        <v>852</v>
+        <v>850</v>
       </c>
       <c r="D372" s="21"/>
       <c r="E372" s="21" t="s">
@@ -14649,7 +14615,7 @@
         <v>17</v>
       </c>
       <c r="I372" s="13" t="s">
-        <v>874</v>
+        <v>872</v>
       </c>
     </row>
     <row r="373" spans="1:9" ht="43.2">
@@ -14660,7 +14626,7 @@
         <v>430</v>
       </c>
       <c r="C373" s="23" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="D373" s="21"/>
       <c r="E373" s="21" t="s">
@@ -14676,7 +14642,7 @@
         <v>17</v>
       </c>
       <c r="I373" s="13" t="s">
-        <v>875</v>
+        <v>873</v>
       </c>
     </row>
     <row r="374" spans="1:9" ht="43.2">
@@ -14687,7 +14653,7 @@
         <v>430</v>
       </c>
       <c r="C374" s="23" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="D374" s="21"/>
       <c r="E374" s="21" t="s">
@@ -14703,7 +14669,7 @@
         <v>17</v>
       </c>
       <c r="I374" s="23" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
     </row>
     <row r="375" spans="1:9" ht="409.6">
@@ -14714,7 +14680,7 @@
         <v>431</v>
       </c>
       <c r="C375" s="24" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="D375" s="21"/>
       <c r="E375" s="21" t="s">
@@ -14739,7 +14705,7 @@
         <v>431</v>
       </c>
       <c r="C376" s="13" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="D376" s="21"/>
       <c r="E376" s="21" t="s">
@@ -14764,7 +14730,7 @@
         <v>431</v>
       </c>
       <c r="C377" s="23" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="D377" s="21"/>
       <c r="E377" s="21" t="s">
@@ -14789,7 +14755,7 @@
         <v>432</v>
       </c>
       <c r="C378" s="24" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="D378" s="21"/>
       <c r="E378" s="21" t="s">
@@ -14814,7 +14780,7 @@
         <v>433</v>
       </c>
       <c r="C379" s="23" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="D379" s="21"/>
       <c r="E379" s="21" t="s">
@@ -14839,7 +14805,7 @@
         <v>433</v>
       </c>
       <c r="C380" s="23" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="D380" s="21"/>
       <c r="E380" s="21" t="s">
@@ -14864,7 +14830,7 @@
         <v>433</v>
       </c>
       <c r="C381" s="23" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="D381" s="21"/>
       <c r="E381" s="21" t="s">
@@ -14889,7 +14855,7 @@
         <v>434</v>
       </c>
       <c r="C382" s="23" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="D382" s="21"/>
       <c r="E382" s="21" t="s">
@@ -14914,7 +14880,7 @@
         <v>435</v>
       </c>
       <c r="C383" s="23" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="D383" s="21"/>
       <c r="E383" s="21" t="s">
@@ -14930,7 +14896,7 @@
         <v>17</v>
       </c>
       <c r="I383" s="23" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
     </row>
     <row r="384" spans="1:9" ht="43.2">
@@ -14941,7 +14907,7 @@
         <v>436</v>
       </c>
       <c r="C384" s="23" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="D384" s="21"/>
       <c r="E384" s="21" t="s">
@@ -14957,7 +14923,7 @@
         <v>17</v>
       </c>
       <c r="I384" s="13" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
     </row>
     <row r="385" spans="1:9" ht="28.8">
@@ -14968,7 +14934,7 @@
         <v>436</v>
       </c>
       <c r="C385" s="13" t="s">
-        <v>853</v>
+        <v>851</v>
       </c>
       <c r="D385" s="21"/>
       <c r="E385" s="21" t="s">
@@ -14984,7 +14950,7 @@
         <v>17</v>
       </c>
       <c r="I385" s="13" t="s">
-        <v>876</v>
+        <v>874</v>
       </c>
     </row>
     <row r="386" spans="1:9" ht="28.8">
@@ -14995,7 +14961,7 @@
         <v>436</v>
       </c>
       <c r="C386" s="13" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="D386" s="21"/>
       <c r="E386" s="21" t="s">
@@ -15011,7 +14977,7 @@
         <v>17</v>
       </c>
       <c r="I386" s="13" t="s">
-        <v>877</v>
+        <v>875</v>
       </c>
     </row>
     <row r="387" spans="1:9" ht="28.8">
@@ -15022,7 +14988,7 @@
         <v>436</v>
       </c>
       <c r="C387" s="23" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="D387" s="21"/>
       <c r="E387" s="21" t="s">
@@ -15038,7 +15004,7 @@
         <v>17</v>
       </c>
       <c r="I387" s="23" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
     </row>
     <row r="388" spans="1:9" ht="43.2">
@@ -15049,7 +15015,7 @@
         <v>436</v>
       </c>
       <c r="C388" s="23" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="D388" s="21"/>
       <c r="E388" s="21" t="s">
@@ -15065,7 +15031,7 @@
         <v>17</v>
       </c>
       <c r="I388" s="23" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
     </row>
     <row r="389" spans="1:9" ht="43.2">
@@ -15076,7 +15042,7 @@
         <v>437</v>
       </c>
       <c r="C389" s="23" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="D389" s="21"/>
       <c r="E389" s="21" t="s">
@@ -15092,7 +15058,7 @@
         <v>17</v>
       </c>
       <c r="I389" s="23" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
     </row>
     <row r="390" spans="1:9">
@@ -15103,7 +15069,7 @@
         <v>438</v>
       </c>
       <c r="C390" s="23" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="D390" s="21"/>
       <c r="E390" s="21" t="s">
@@ -15128,7 +15094,7 @@
         <v>438</v>
       </c>
       <c r="C391" s="23" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="D391" s="21"/>
       <c r="E391" s="21" t="s">
@@ -15153,7 +15119,7 @@
         <v>438</v>
       </c>
       <c r="C392" s="23" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="D392" s="21"/>
       <c r="E392" s="21" t="s">
@@ -15178,7 +15144,7 @@
         <v>439</v>
       </c>
       <c r="C393" s="23" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="D393" s="21"/>
       <c r="E393" s="21" t="s">
@@ -15203,10 +15169,10 @@
         <v>428</v>
       </c>
       <c r="C394" s="23" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="D394" s="21" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="E394" s="21" t="s">
         <v>22</v>
@@ -15360,6 +15326,12 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F2EA47BB262D974097182E2CA8AB13E1" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="74597e8d9e42e7e4fc8eda6d37675aa2">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4aeb20c0e3442673af7ee10786458764">
     <xsd:element name="properties">
@@ -15408,12 +15380,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6D33261-F3C6-4621-88F1-D76E5ABE1865}">
   <ds:schemaRefs>
@@ -15423,6 +15389,20 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{923F65C5-DEAB-400B-AA1F-124F40EE10AC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EDB2DE12-5EF6-4CF2-820D-5F9FE329E08E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -15437,20 +15417,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{923F65C5-DEAB-400B-AA1F-124F40EE10AC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{f42aa342-8706-4288-bd11-ebb85995028c}" enabled="1" method="Privileged" siteId="{72f988bf-86f1-41af-91ab-2d7cd011db47}" removed="0"/>

</xml_diff>

<commit_message>
Updated md and RS version numbers for MS-OXWSSYNC on release 20250218.
</commit_message>
<xml_diff>
--- a/ExchangeWebServices/Docs/MS-OXWSSYNC/MS-OXWSSYNC_RequirementSpecification.xlsx
+++ b/ExchangeWebServices/Docs/MS-OXWSSYNC/MS-OXWSSYNC_RequirementSpecification.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28623"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C7DEEC3-0512-49ED-8BF5-28612D044567}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5AD963D-F716-4B61-9984-3F718C2AD7D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4451,7 +4451,81 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="37">
+  <dxfs count="31">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -4771,110 +4845,6 @@
         <scheme val="none"/>
       </font>
     </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -5004,7 +4974,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Requirement" displayName="Requirement" ref="A19:I394" tableType="xml" totalsRowShown="0" headerRowDxfId="16" dataDxfId="15" connectionId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Requirement" displayName="Requirement" ref="A19:I394" tableType="xml" totalsRowShown="0" headerRowDxfId="30" dataDxfId="29" connectionId="1">
   <autoFilter ref="A19:I394" xr:uid="{00000000-0009-0000-0100-000001000000}">
     <filterColumn colId="1">
       <filters>
@@ -5013,31 +4983,31 @@
     </filterColumn>
   </autoFilter>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" uniqueName="ns1:REQ_ID" name="Req ID" dataDxfId="14">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" uniqueName="ns1:REQ_ID" name="Req ID" dataDxfId="28">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:REQ_ID" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" uniqueName="ns1:Doc_Sect" name="Doc Sect" dataDxfId="13">
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" uniqueName="ns1:Doc_Sect" name="Doc Sect" dataDxfId="27">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Doc_Sect" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" uniqueName="ns1:Description" name="Description" dataDxfId="12">
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" uniqueName="ns1:Description" name="Description" dataDxfId="26">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Description" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" uniqueName="ns1:Derived" name="Derived" dataDxfId="11">
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" uniqueName="ns1:Derived" name="Derived" dataDxfId="25">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Derived" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" uniqueName="ns1:Behavior" name="Behavior" dataDxfId="10">
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" uniqueName="ns1:Behavior" name="Behavior" dataDxfId="24">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Behavior" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" uniqueName="ns1:Scope" name="Scope" dataDxfId="9">
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" uniqueName="ns1:Scope" name="Scope" dataDxfId="23">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Scope" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" uniqueName="ns1:IsNormative" name="Informative_x000a_/Normative" dataDxfId="8">
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" uniqueName="ns1:IsNormative" name="Informative_x000a_/Normative" dataDxfId="22">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:IsNormative" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" uniqueName="ns1:Verification" name="Verification" dataDxfId="7">
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" uniqueName="ns1:Verification" name="Verification" dataDxfId="21">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Verification" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" uniqueName="ns1:VerificationComment" name="Verification Comment" dataDxfId="6">
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" uniqueName="ns1:VerificationComment" name="Verification Comment" dataDxfId="20">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:VerificationComment" xmlDataType="string"/>
     </tableColumn>
   </tableColumns>
@@ -5046,12 +5016,12 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Scope" displayName="Scope" ref="A12:C15" totalsRowShown="0" headerRowBorderDxfId="5" tableBorderDxfId="4" totalsRowBorderDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Scope" displayName="Scope" ref="A12:C15" totalsRowShown="0" headerRowBorderDxfId="19" tableBorderDxfId="18" totalsRowBorderDxfId="17">
   <autoFilter ref="A12:C15" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Scope" dataDxfId="2"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Test" dataDxfId="1"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Description" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Scope" dataDxfId="16"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Test" dataDxfId="15"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Description" dataDxfId="14"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5347,8 +5317,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:I396"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C149" sqref="C149"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
@@ -5398,7 +5368,7 @@
         <v>26</v>
       </c>
       <c r="F3" s="31">
-        <v>45243</v>
+        <v>45706</v>
       </c>
       <c r="G3" s="32"/>
       <c r="I3" s="29"/>
@@ -15215,78 +15185,54 @@
     <mergeCell ref="B17:I17"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="A375:B375 A378:B378 A376:I377 D375:I375 A379:I394 D378:I378 I367:I394 A20:I374">
-    <cfRule type="expression" dxfId="36" priority="77">
+  <conditionalFormatting sqref="A20:I374 I367:I394 A375:B375 D375:I375 A376:I377 A378:B378 D378:I378 A379:I394">
+    <cfRule type="expression" dxfId="13" priority="31">
+      <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="12" priority="32">
+      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="11" priority="33">
+      <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="10" priority="77">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="35" priority="78">
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C375">
+    <cfRule type="expression" dxfId="9" priority="1">
+      <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="8" priority="2">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="34" priority="85">
+    <cfRule type="expression" dxfId="7" priority="3">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
+    <cfRule type="expression" dxfId="6" priority="4">
+      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
+    </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A375:B375 A378:B378 A376:I377 D375:I375 A379:I394 D378:I378 I367:I394 A20:I374">
-    <cfRule type="expression" dxfId="33" priority="31">
+  <conditionalFormatting sqref="C378">
+    <cfRule type="expression" dxfId="5" priority="7">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="32" priority="32">
+    <cfRule type="expression" dxfId="4" priority="8">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="31" priority="33">
+    <cfRule type="expression" dxfId="3" priority="9">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="2" priority="10">
+      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F20:F394">
-    <cfRule type="expression" dxfId="30" priority="37">
+    <cfRule type="expression" dxfId="1" priority="37">
       <formula>NOT(VLOOKUP(F20,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="29" priority="38">
+    <cfRule type="expression" dxfId="0" priority="38">
       <formula>(VLOOKUP(F20,$A$12:$C$15,2,FALSE)="In")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C378">
-    <cfRule type="expression" dxfId="28" priority="10">
-      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="27" priority="11">
-      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="26" priority="12">
-      <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C378">
-    <cfRule type="expression" dxfId="25" priority="7">
-      <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="24" priority="8">
-      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="23" priority="9">
-      <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C375">
-    <cfRule type="expression" dxfId="22" priority="4">
-      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="21" priority="5">
-      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="20" priority="6">
-      <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C375">
-    <cfRule type="expression" dxfId="19" priority="1">
-      <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="18" priority="2">
-      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="17" priority="3">
-      <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="6">
@@ -15323,21 +15269,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F2EA47BB262D974097182E2CA8AB13E1" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="74597e8d9e42e7e4fc8eda6d37675aa2">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4aeb20c0e3442673af7ee10786458764">
     <xsd:element name="properties">
@@ -15386,29 +15317,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{923F65C5-DEAB-400B-AA1F-124F40EE10AC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6D33261-F3C6-4621-88F1-D76E5ABE1865}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EDB2DE12-5EF6-4CF2-820D-5F9FE329E08E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -15423,6 +15347,28 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6D33261-F3C6-4621-88F1-D76E5ABE1865}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{923F65C5-DEAB-400B-AA1F-124F40EE10AC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{f42aa342-8706-4288-bd11-ebb85995028c}" enabled="1" method="Privileged" siteId="{72f988bf-86f1-41af-91ab-2d7cd011db47}" removed="0"/>

</xml_diff>

<commit_message>
Update RS and code for MS-OXWSSYNC release 20250520
</commit_message>
<xml_diff>
--- a/ExchangeWebServices/Docs/MS-OXWSSYNC/MS-OXWSSYNC_RequirementSpecification.xlsx
+++ b/ExchangeWebServices/Docs/MS-OXWSSYNC/MS-OXWSSYNC_RequirementSpecification.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28827"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5AD963D-F716-4B61-9984-3F718C2AD7D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09A7CD55-F123-41CD-AA45-42EAFF994E9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements" sheetId="2" r:id="rId1"/>
@@ -4036,14 +4036,14 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
-    <numFmt numFmtId="165" formatCode="0.0.0"/>
+    <numFmt numFmtId="176" formatCode="yyyy\-mm\-dd"/>
+    <numFmt numFmtId="177" formatCode="0.0.0"/>
   </numFmts>
   <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -4290,7 +4290,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -4320,7 +4320,7 @@
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="177" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -4358,8 +4358,8 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4449,7 +4449,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="31">
     <dxf>
@@ -5318,20 +5318,20 @@
   <dimension ref="A1:I396"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="B9" sqref="B9:I9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12.453125" style="3" customWidth="1"/>
+    <col min="1" max="1" width="12.5" style="3" customWidth="1"/>
     <col min="2" max="2" width="13" style="3" customWidth="1"/>
     <col min="3" max="3" width="85" style="3" customWidth="1"/>
-    <col min="4" max="4" width="28.54296875" style="3" customWidth="1"/>
-    <col min="5" max="5" width="12.453125" style="3" customWidth="1"/>
-    <col min="6" max="6" width="12.08984375" style="3" customWidth="1"/>
-    <col min="7" max="7" width="13.453125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="28.5" style="3" customWidth="1"/>
+    <col min="5" max="5" width="12.5" style="3" customWidth="1"/>
+    <col min="6" max="6" width="12.125" style="3" customWidth="1"/>
+    <col min="7" max="7" width="13.5" style="3" customWidth="1"/>
     <col min="8" max="8" width="23" style="3" customWidth="1"/>
-    <col min="9" max="9" width="28.6328125" style="3" customWidth="1"/>
+    <col min="9" max="9" width="28.625" style="3" customWidth="1"/>
     <col min="10" max="10" width="9" style="3" customWidth="1"/>
     <col min="11" max="16384" width="9" style="3"/>
   </cols>
@@ -5362,13 +5362,13 @@
         <v>25</v>
       </c>
       <c r="C3" s="30">
-        <v>9.1999999999999993</v>
+        <v>10</v>
       </c>
       <c r="E3" s="6" t="s">
         <v>26</v>
       </c>
       <c r="F3" s="31">
-        <v>45706</v>
+        <v>45797</v>
       </c>
       <c r="G3" s="32"/>
       <c r="I3" s="29"/>
@@ -5604,7 +5604,7 @@
       <c r="H18" s="44"/>
       <c r="I18" s="45"/>
     </row>
-    <row r="19" spans="1:9" ht="29">
+    <row r="19" spans="1:9" ht="30">
       <c r="A19" s="3" t="s">
         <v>0</v>
       </c>
@@ -5633,7 +5633,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:9" s="15" customFormat="1" ht="58" hidden="1">
+    <row r="20" spans="1:9" s="15" customFormat="1" ht="60" hidden="1">
       <c r="A20" s="14" t="s">
         <v>40</v>
       </c>
@@ -5658,7 +5658,7 @@
       </c>
       <c r="I20" s="16"/>
     </row>
-    <row r="21" spans="1:9" s="15" customFormat="1" ht="29" hidden="1">
+    <row r="21" spans="1:9" s="15" customFormat="1" ht="30" hidden="1">
       <c r="A21" s="14" t="s">
         <v>41</v>
       </c>
@@ -5683,7 +5683,7 @@
       </c>
       <c r="I21" s="16"/>
     </row>
-    <row r="22" spans="1:9" s="15" customFormat="1" ht="29" hidden="1">
+    <row r="22" spans="1:9" s="15" customFormat="1" ht="30" hidden="1">
       <c r="A22" s="14" t="s">
         <v>42</v>
       </c>
@@ -5708,7 +5708,7 @@
       </c>
       <c r="I22" s="16"/>
     </row>
-    <row r="23" spans="1:9" s="15" customFormat="1" ht="29" hidden="1">
+    <row r="23" spans="1:9" s="15" customFormat="1" hidden="1">
       <c r="A23" s="14" t="s">
         <v>43</v>
       </c>
@@ -5758,7 +5758,7 @@
       </c>
       <c r="I24" s="16"/>
     </row>
-    <row r="25" spans="1:9" s="15" customFormat="1" ht="29" hidden="1">
+    <row r="25" spans="1:9" s="15" customFormat="1" ht="30" hidden="1">
       <c r="A25" s="14" t="s">
         <v>45</v>
       </c>
@@ -5783,7 +5783,7 @@
       </c>
       <c r="I25" s="16"/>
     </row>
-    <row r="26" spans="1:9" s="15" customFormat="1" ht="43.5" hidden="1">
+    <row r="26" spans="1:9" s="15" customFormat="1" ht="45" hidden="1">
       <c r="A26" s="14" t="s">
         <v>46</v>
       </c>
@@ -5858,7 +5858,7 @@
       </c>
       <c r="I28" s="16"/>
     </row>
-    <row r="29" spans="1:9" s="15" customFormat="1" ht="29" hidden="1">
+    <row r="29" spans="1:9" s="15" customFormat="1" hidden="1">
       <c r="A29" s="14" t="s">
         <v>49</v>
       </c>
@@ -5908,7 +5908,7 @@
       </c>
       <c r="I30" s="16"/>
     </row>
-    <row r="31" spans="1:9" s="15" customFormat="1" ht="29" hidden="1">
+    <row r="31" spans="1:9" s="15" customFormat="1" ht="30" hidden="1">
       <c r="A31" s="14" t="s">
         <v>51</v>
       </c>
@@ -5935,7 +5935,7 @@
         <v>684</v>
       </c>
     </row>
-    <row r="32" spans="1:9" s="15" customFormat="1" ht="29" hidden="1">
+    <row r="32" spans="1:9" s="15" customFormat="1" ht="30" hidden="1">
       <c r="A32" s="14" t="s">
         <v>52</v>
       </c>
@@ -5960,7 +5960,7 @@
       </c>
       <c r="I32" s="16"/>
     </row>
-    <row r="33" spans="1:9" s="15" customFormat="1" ht="43.5" hidden="1">
+    <row r="33" spans="1:9" s="15" customFormat="1" ht="30" hidden="1">
       <c r="A33" s="14" t="s">
         <v>53</v>
       </c>
@@ -5985,7 +5985,7 @@
       </c>
       <c r="I33" s="16"/>
     </row>
-    <row r="34" spans="1:9" ht="43.5" hidden="1">
+    <row r="34" spans="1:9" ht="30" hidden="1">
       <c r="A34" s="21" t="s">
         <v>54</v>
       </c>
@@ -6010,7 +6010,7 @@
       </c>
       <c r="I34" s="23"/>
     </row>
-    <row r="35" spans="1:9" ht="58" hidden="1">
+    <row r="35" spans="1:9" ht="45" hidden="1">
       <c r="A35" s="21" t="s">
         <v>55</v>
       </c>
@@ -6035,7 +6035,7 @@
       </c>
       <c r="I35" s="23"/>
     </row>
-    <row r="36" spans="1:9" ht="29" hidden="1">
+    <row r="36" spans="1:9" ht="30" hidden="1">
       <c r="A36" s="21" t="s">
         <v>56</v>
       </c>
@@ -6060,7 +6060,7 @@
       </c>
       <c r="I36" s="23"/>
     </row>
-    <row r="37" spans="1:9" ht="29" hidden="1">
+    <row r="37" spans="1:9" ht="30" hidden="1">
       <c r="A37" s="21" t="s">
         <v>57</v>
       </c>
@@ -6085,7 +6085,7 @@
       </c>
       <c r="I37" s="23"/>
     </row>
-    <row r="38" spans="1:9" ht="29" hidden="1">
+    <row r="38" spans="1:9" ht="30" hidden="1">
       <c r="A38" s="21" t="s">
         <v>58</v>
       </c>
@@ -6110,7 +6110,7 @@
       </c>
       <c r="I38" s="23"/>
     </row>
-    <row r="39" spans="1:9" ht="29" hidden="1">
+    <row r="39" spans="1:9" ht="30" hidden="1">
       <c r="A39" s="21" t="s">
         <v>59</v>
       </c>
@@ -6135,7 +6135,7 @@
       </c>
       <c r="I39" s="23"/>
     </row>
-    <row r="40" spans="1:9" ht="29" hidden="1">
+    <row r="40" spans="1:9" ht="30" hidden="1">
       <c r="A40" s="21" t="s">
         <v>60</v>
       </c>
@@ -6160,7 +6160,7 @@
       </c>
       <c r="I40" s="23"/>
     </row>
-    <row r="41" spans="1:9" ht="29" hidden="1">
+    <row r="41" spans="1:9" ht="30" hidden="1">
       <c r="A41" s="21" t="s">
         <v>61</v>
       </c>
@@ -6185,7 +6185,7 @@
       </c>
       <c r="I41" s="23"/>
     </row>
-    <row r="42" spans="1:9" ht="29" hidden="1">
+    <row r="42" spans="1:9" ht="30" hidden="1">
       <c r="A42" s="21" t="s">
         <v>62</v>
       </c>
@@ -6210,7 +6210,7 @@
       </c>
       <c r="I42" s="23"/>
     </row>
-    <row r="43" spans="1:9" ht="29" hidden="1">
+    <row r="43" spans="1:9" ht="30" hidden="1">
       <c r="A43" s="21" t="s">
         <v>63</v>
       </c>
@@ -6235,7 +6235,7 @@
       </c>
       <c r="I43" s="23"/>
     </row>
-    <row r="44" spans="1:9" ht="29" hidden="1">
+    <row r="44" spans="1:9" ht="30" hidden="1">
       <c r="A44" s="21" t="s">
         <v>64</v>
       </c>
@@ -6260,7 +6260,7 @@
       </c>
       <c r="I44" s="23"/>
     </row>
-    <row r="45" spans="1:9" ht="43.5" hidden="1">
+    <row r="45" spans="1:9" ht="45" hidden="1">
       <c r="A45" s="21" t="s">
         <v>65</v>
       </c>
@@ -6285,7 +6285,7 @@
       </c>
       <c r="I45" s="23"/>
     </row>
-    <row r="46" spans="1:9" ht="29" hidden="1">
+    <row r="46" spans="1:9" ht="30" hidden="1">
       <c r="A46" s="21" t="s">
         <v>66</v>
       </c>
@@ -6310,7 +6310,7 @@
       </c>
       <c r="I46" s="23"/>
     </row>
-    <row r="47" spans="1:9" ht="29" hidden="1">
+    <row r="47" spans="1:9" ht="30" hidden="1">
       <c r="A47" s="21" t="s">
         <v>189</v>
       </c>
@@ -6335,7 +6335,7 @@
       </c>
       <c r="I47" s="23"/>
     </row>
-    <row r="48" spans="1:9" ht="29" hidden="1">
+    <row r="48" spans="1:9" ht="30" hidden="1">
       <c r="A48" s="21" t="s">
         <v>190</v>
       </c>
@@ -6360,7 +6360,7 @@
       </c>
       <c r="I48" s="23"/>
     </row>
-    <row r="49" spans="1:9" ht="29" hidden="1">
+    <row r="49" spans="1:9" ht="30" hidden="1">
       <c r="A49" s="21" t="s">
         <v>191</v>
       </c>
@@ -6385,7 +6385,7 @@
       </c>
       <c r="I49" s="23"/>
     </row>
-    <row r="50" spans="1:9" ht="29" hidden="1">
+    <row r="50" spans="1:9" ht="30" hidden="1">
       <c r="A50" s="21" t="s">
         <v>192</v>
       </c>
@@ -6410,7 +6410,7 @@
       </c>
       <c r="I50" s="23"/>
     </row>
-    <row r="51" spans="1:9" ht="29" hidden="1">
+    <row r="51" spans="1:9" ht="30" hidden="1">
       <c r="A51" s="21" t="s">
         <v>193</v>
       </c>
@@ -6460,7 +6460,7 @@
       </c>
       <c r="I52" s="23"/>
     </row>
-    <row r="53" spans="1:9" ht="29" hidden="1">
+    <row r="53" spans="1:9" ht="30" hidden="1">
       <c r="A53" s="21" t="s">
         <v>195</v>
       </c>
@@ -6485,7 +6485,7 @@
       </c>
       <c r="I53" s="23"/>
     </row>
-    <row r="54" spans="1:9" ht="43.5" hidden="1">
+    <row r="54" spans="1:9" ht="45" hidden="1">
       <c r="A54" s="21" t="s">
         <v>196</v>
       </c>
@@ -6510,7 +6510,7 @@
       </c>
       <c r="I54" s="23"/>
     </row>
-    <row r="55" spans="1:9" ht="29" hidden="1">
+    <row r="55" spans="1:9" ht="30" hidden="1">
       <c r="A55" s="21" t="s">
         <v>197</v>
       </c>
@@ -6535,7 +6535,7 @@
       </c>
       <c r="I55" s="23"/>
     </row>
-    <row r="56" spans="1:9" ht="43.5" hidden="1">
+    <row r="56" spans="1:9" ht="45" hidden="1">
       <c r="A56" s="21" t="s">
         <v>198</v>
       </c>
@@ -6560,7 +6560,7 @@
       </c>
       <c r="I56" s="23"/>
     </row>
-    <row r="57" spans="1:9" ht="43.5" hidden="1">
+    <row r="57" spans="1:9" ht="30" hidden="1">
       <c r="A57" s="21" t="s">
         <v>199</v>
       </c>
@@ -6585,7 +6585,7 @@
       </c>
       <c r="I57" s="23"/>
     </row>
-    <row r="58" spans="1:9" ht="43.5" hidden="1">
+    <row r="58" spans="1:9" ht="45" hidden="1">
       <c r="A58" s="21" t="s">
         <v>200</v>
       </c>
@@ -6610,7 +6610,7 @@
       </c>
       <c r="I58" s="23"/>
     </row>
-    <row r="59" spans="1:9" ht="58" hidden="1">
+    <row r="59" spans="1:9" ht="60" hidden="1">
       <c r="A59" s="21" t="s">
         <v>201</v>
       </c>
@@ -6635,7 +6635,7 @@
       </c>
       <c r="I59" s="23"/>
     </row>
-    <row r="60" spans="1:9" ht="43.5" hidden="1">
+    <row r="60" spans="1:9" ht="45" hidden="1">
       <c r="A60" s="21" t="s">
         <v>202</v>
       </c>
@@ -6660,7 +6660,7 @@
       </c>
       <c r="I60" s="23"/>
     </row>
-    <row r="61" spans="1:9" ht="58" hidden="1">
+    <row r="61" spans="1:9" ht="45" hidden="1">
       <c r="A61" s="21" t="s">
         <v>203</v>
       </c>
@@ -6685,7 +6685,7 @@
       </c>
       <c r="I61" s="23"/>
     </row>
-    <row r="62" spans="1:9" ht="43.5" hidden="1">
+    <row r="62" spans="1:9" ht="45" hidden="1">
       <c r="A62" s="21" t="s">
         <v>204</v>
       </c>
@@ -6710,7 +6710,7 @@
       </c>
       <c r="I62" s="23"/>
     </row>
-    <row r="63" spans="1:9" ht="29" hidden="1">
+    <row r="63" spans="1:9" hidden="1">
       <c r="A63" s="21" t="s">
         <v>205</v>
       </c>
@@ -6735,7 +6735,7 @@
       </c>
       <c r="I63" s="23"/>
     </row>
-    <row r="64" spans="1:9" ht="58" hidden="1">
+    <row r="64" spans="1:9" ht="60" hidden="1">
       <c r="A64" s="21" t="s">
         <v>206</v>
       </c>
@@ -6760,7 +6760,7 @@
       </c>
       <c r="I64" s="23"/>
     </row>
-    <row r="65" spans="1:9" ht="43.5" hidden="1">
+    <row r="65" spans="1:9" ht="45" hidden="1">
       <c r="A65" s="21" t="s">
         <v>207</v>
       </c>
@@ -6785,7 +6785,7 @@
       </c>
       <c r="I65" s="23"/>
     </row>
-    <row r="66" spans="1:9" ht="43.5" hidden="1">
+    <row r="66" spans="1:9" ht="45" hidden="1">
       <c r="A66" s="21" t="s">
         <v>208</v>
       </c>
@@ -6810,7 +6810,7 @@
       </c>
       <c r="I66" s="23"/>
     </row>
-    <row r="67" spans="1:9" ht="43.5" hidden="1">
+    <row r="67" spans="1:9" ht="30" hidden="1">
       <c r="A67" s="21" t="s">
         <v>209</v>
       </c>
@@ -6835,7 +6835,7 @@
       </c>
       <c r="I67" s="23"/>
     </row>
-    <row r="68" spans="1:9" ht="29" hidden="1">
+    <row r="68" spans="1:9" ht="30" hidden="1">
       <c r="A68" s="21" t="s">
         <v>210</v>
       </c>
@@ -6860,7 +6860,7 @@
       </c>
       <c r="I68" s="23"/>
     </row>
-    <row r="69" spans="1:9" ht="29" hidden="1">
+    <row r="69" spans="1:9" ht="30" hidden="1">
       <c r="A69" s="21" t="s">
         <v>211</v>
       </c>
@@ -6885,7 +6885,7 @@
       </c>
       <c r="I69" s="23"/>
     </row>
-    <row r="70" spans="1:9" ht="29" hidden="1">
+    <row r="70" spans="1:9" ht="30" hidden="1">
       <c r="A70" s="21" t="s">
         <v>212</v>
       </c>
@@ -6910,7 +6910,7 @@
       </c>
       <c r="I70" s="23"/>
     </row>
-    <row r="71" spans="1:9" ht="87" hidden="1">
+    <row r="71" spans="1:9" ht="90" hidden="1">
       <c r="A71" s="21" t="s">
         <v>213</v>
       </c>
@@ -6935,7 +6935,7 @@
       </c>
       <c r="I71" s="23"/>
     </row>
-    <row r="72" spans="1:9" ht="261" hidden="1">
+    <row r="72" spans="1:9" ht="255" hidden="1">
       <c r="A72" s="21" t="s">
         <v>214</v>
       </c>
@@ -6960,7 +6960,7 @@
       </c>
       <c r="I72" s="23"/>
     </row>
-    <row r="73" spans="1:9" ht="43.5" hidden="1">
+    <row r="73" spans="1:9" ht="45" hidden="1">
       <c r="A73" s="21" t="s">
         <v>215</v>
       </c>
@@ -6985,7 +6985,7 @@
       </c>
       <c r="I73" s="23"/>
     </row>
-    <row r="74" spans="1:9" ht="29" hidden="1">
+    <row r="74" spans="1:9" ht="30" hidden="1">
       <c r="A74" s="21" t="s">
         <v>216</v>
       </c>
@@ -7010,7 +7010,7 @@
       </c>
       <c r="I74" s="23"/>
     </row>
-    <row r="75" spans="1:9" ht="29" hidden="1">
+    <row r="75" spans="1:9" ht="30" hidden="1">
       <c r="A75" s="21" t="s">
         <v>217</v>
       </c>
@@ -7035,7 +7035,7 @@
       </c>
       <c r="I75" s="23"/>
     </row>
-    <row r="76" spans="1:9" ht="43.5" hidden="1">
+    <row r="76" spans="1:9" ht="30" hidden="1">
       <c r="A76" s="21" t="s">
         <v>218</v>
       </c>
@@ -7060,7 +7060,7 @@
       </c>
       <c r="I76" s="23"/>
     </row>
-    <row r="77" spans="1:9" ht="29" hidden="1">
+    <row r="77" spans="1:9" ht="30" hidden="1">
       <c r="A77" s="21" t="s">
         <v>219</v>
       </c>
@@ -7085,7 +7085,7 @@
       </c>
       <c r="I77" s="23"/>
     </row>
-    <row r="78" spans="1:9" ht="29" hidden="1">
+    <row r="78" spans="1:9" ht="30" hidden="1">
       <c r="A78" s="21" t="s">
         <v>220</v>
       </c>
@@ -7110,7 +7110,7 @@
       </c>
       <c r="I78" s="23"/>
     </row>
-    <row r="79" spans="1:9" ht="116" hidden="1">
+    <row r="79" spans="1:9" ht="120" hidden="1">
       <c r="A79" s="21" t="s">
         <v>221</v>
       </c>
@@ -7135,7 +7135,7 @@
       </c>
       <c r="I79" s="23"/>
     </row>
-    <row r="80" spans="1:9" ht="43.5" hidden="1">
+    <row r="80" spans="1:9" ht="45" hidden="1">
       <c r="A80" s="21" t="s">
         <v>222</v>
       </c>
@@ -7160,7 +7160,7 @@
       </c>
       <c r="I80" s="23"/>
     </row>
-    <row r="81" spans="1:9" ht="43.5" hidden="1">
+    <row r="81" spans="1:9" ht="45" hidden="1">
       <c r="A81" s="21" t="s">
         <v>223</v>
       </c>
@@ -7185,7 +7185,7 @@
       </c>
       <c r="I81" s="23"/>
     </row>
-    <row r="82" spans="1:9" ht="29" hidden="1">
+    <row r="82" spans="1:9" ht="30" hidden="1">
       <c r="A82" s="21" t="s">
         <v>224</v>
       </c>
@@ -7210,7 +7210,7 @@
       </c>
       <c r="I82" s="23"/>
     </row>
-    <row r="83" spans="1:9" ht="29" hidden="1">
+    <row r="83" spans="1:9" ht="30" hidden="1">
       <c r="A83" s="21" t="s">
         <v>225</v>
       </c>
@@ -7235,7 +7235,7 @@
       </c>
       <c r="I83" s="23"/>
     </row>
-    <row r="84" spans="1:9" ht="29" hidden="1">
+    <row r="84" spans="1:9" ht="30" hidden="1">
       <c r="A84" s="21" t="s">
         <v>226</v>
       </c>
@@ -7260,7 +7260,7 @@
       </c>
       <c r="I84" s="23"/>
     </row>
-    <row r="85" spans="1:9" ht="29" hidden="1">
+    <row r="85" spans="1:9" ht="30" hidden="1">
       <c r="A85" s="21" t="s">
         <v>227</v>
       </c>
@@ -7285,7 +7285,7 @@
       </c>
       <c r="I85" s="23"/>
     </row>
-    <row r="86" spans="1:9" ht="29" hidden="1">
+    <row r="86" spans="1:9" ht="30" hidden="1">
       <c r="A86" s="21" t="s">
         <v>228</v>
       </c>
@@ -7310,7 +7310,7 @@
       </c>
       <c r="I86" s="23"/>
     </row>
-    <row r="87" spans="1:9" ht="29" hidden="1">
+    <row r="87" spans="1:9" ht="30" hidden="1">
       <c r="A87" s="21" t="s">
         <v>229</v>
       </c>
@@ -7335,7 +7335,7 @@
       </c>
       <c r="I87" s="23"/>
     </row>
-    <row r="88" spans="1:9" ht="29" hidden="1">
+    <row r="88" spans="1:9" hidden="1">
       <c r="A88" s="21" t="s">
         <v>230</v>
       </c>
@@ -7360,7 +7360,7 @@
       </c>
       <c r="I88" s="23"/>
     </row>
-    <row r="89" spans="1:9" ht="29" hidden="1">
+    <row r="89" spans="1:9" ht="30" hidden="1">
       <c r="A89" s="21" t="s">
         <v>231</v>
       </c>
@@ -7385,7 +7385,7 @@
       </c>
       <c r="I89" s="23"/>
     </row>
-    <row r="90" spans="1:9" ht="29" hidden="1">
+    <row r="90" spans="1:9" ht="30" hidden="1">
       <c r="A90" s="21" t="s">
         <v>232</v>
       </c>
@@ -7410,7 +7410,7 @@
       </c>
       <c r="I90" s="23"/>
     </row>
-    <row r="91" spans="1:9" ht="101.5" hidden="1">
+    <row r="91" spans="1:9" ht="90" hidden="1">
       <c r="A91" s="21" t="s">
         <v>233</v>
       </c>
@@ -7435,7 +7435,7 @@
       </c>
       <c r="I91" s="23"/>
     </row>
-    <row r="92" spans="1:9" ht="43.5" hidden="1">
+    <row r="92" spans="1:9" ht="45" hidden="1">
       <c r="A92" s="21" t="s">
         <v>234</v>
       </c>
@@ -7460,7 +7460,7 @@
       </c>
       <c r="I92" s="23"/>
     </row>
-    <row r="93" spans="1:9" ht="43.5" hidden="1">
+    <row r="93" spans="1:9" ht="45" hidden="1">
       <c r="A93" s="21" t="s">
         <v>235</v>
       </c>
@@ -7485,7 +7485,7 @@
       </c>
       <c r="I93" s="23"/>
     </row>
-    <row r="94" spans="1:9" ht="29" hidden="1">
+    <row r="94" spans="1:9" ht="30" hidden="1">
       <c r="A94" s="21" t="s">
         <v>236</v>
       </c>
@@ -7510,7 +7510,7 @@
       </c>
       <c r="I94" s="23"/>
     </row>
-    <row r="95" spans="1:9" ht="29" hidden="1">
+    <row r="95" spans="1:9" ht="30" hidden="1">
       <c r="A95" s="21" t="s">
         <v>237</v>
       </c>
@@ -7535,7 +7535,7 @@
       </c>
       <c r="I95" s="23"/>
     </row>
-    <row r="96" spans="1:9" ht="29" hidden="1">
+    <row r="96" spans="1:9" ht="30" hidden="1">
       <c r="A96" s="21" t="s">
         <v>238</v>
       </c>
@@ -7560,7 +7560,7 @@
       </c>
       <c r="I96" s="23"/>
     </row>
-    <row r="97" spans="1:9" ht="29" hidden="1">
+    <row r="97" spans="1:9" ht="30" hidden="1">
       <c r="A97" s="21" t="s">
         <v>239</v>
       </c>
@@ -7585,7 +7585,7 @@
       </c>
       <c r="I97" s="23"/>
     </row>
-    <row r="98" spans="1:9" ht="43.5" hidden="1">
+    <row r="98" spans="1:9" ht="30" hidden="1">
       <c r="A98" s="21" t="s">
         <v>240</v>
       </c>
@@ -7610,7 +7610,7 @@
       </c>
       <c r="I98" s="23"/>
     </row>
-    <row r="99" spans="1:9" ht="29" hidden="1">
+    <row r="99" spans="1:9" ht="30" hidden="1">
       <c r="A99" s="21" t="s">
         <v>241</v>
       </c>
@@ -7635,7 +7635,7 @@
       </c>
       <c r="I99" s="23"/>
     </row>
-    <row r="100" spans="1:9" ht="29" hidden="1">
+    <row r="100" spans="1:9" ht="30" hidden="1">
       <c r="A100" s="21" t="s">
         <v>242</v>
       </c>
@@ -7660,7 +7660,7 @@
       </c>
       <c r="I100" s="23"/>
     </row>
-    <row r="101" spans="1:9" ht="58" hidden="1">
+    <row r="101" spans="1:9" ht="60" hidden="1">
       <c r="A101" s="21" t="s">
         <v>243</v>
       </c>
@@ -7685,7 +7685,7 @@
       </c>
       <c r="I101" s="23"/>
     </row>
-    <row r="102" spans="1:9" ht="72.5" hidden="1">
+    <row r="102" spans="1:9" ht="75" hidden="1">
       <c r="A102" s="21" t="s">
         <v>244</v>
       </c>
@@ -7710,7 +7710,7 @@
       </c>
       <c r="I102" s="23"/>
     </row>
-    <row r="103" spans="1:9" ht="72.5" hidden="1">
+    <row r="103" spans="1:9" ht="60" hidden="1">
       <c r="A103" s="21" t="s">
         <v>245</v>
       </c>
@@ -7735,7 +7735,7 @@
       </c>
       <c r="I103" s="23"/>
     </row>
-    <row r="104" spans="1:9" ht="43.5" hidden="1">
+    <row r="104" spans="1:9" ht="30" hidden="1">
       <c r="A104" s="21" t="s">
         <v>67</v>
       </c>
@@ -7760,7 +7760,7 @@
       </c>
       <c r="I104" s="23"/>
     </row>
-    <row r="105" spans="1:9" ht="29" hidden="1">
+    <row r="105" spans="1:9" ht="30" hidden="1">
       <c r="A105" s="21" t="s">
         <v>68</v>
       </c>
@@ -7785,7 +7785,7 @@
       </c>
       <c r="I105" s="23"/>
     </row>
-    <row r="106" spans="1:9" ht="29" hidden="1">
+    <row r="106" spans="1:9" ht="30" hidden="1">
       <c r="A106" s="21" t="s">
         <v>69</v>
       </c>
@@ -7810,7 +7810,7 @@
       </c>
       <c r="I106" s="23"/>
     </row>
-    <row r="107" spans="1:9" ht="29" hidden="1">
+    <row r="107" spans="1:9" ht="30" hidden="1">
       <c r="A107" s="21" t="s">
         <v>70</v>
       </c>
@@ -7835,7 +7835,7 @@
       </c>
       <c r="I107" s="23"/>
     </row>
-    <row r="108" spans="1:9" ht="29" hidden="1">
+    <row r="108" spans="1:9" ht="30" hidden="1">
       <c r="A108" s="21" t="s">
         <v>246</v>
       </c>
@@ -7860,7 +7860,7 @@
       </c>
       <c r="I108" s="23"/>
     </row>
-    <row r="109" spans="1:9" ht="29" hidden="1">
+    <row r="109" spans="1:9" ht="30" hidden="1">
       <c r="A109" s="21" t="s">
         <v>247</v>
       </c>
@@ -7885,7 +7885,7 @@
       </c>
       <c r="I109" s="23"/>
     </row>
-    <row r="110" spans="1:9" ht="304.5" hidden="1">
+    <row r="110" spans="1:9" ht="315" hidden="1">
       <c r="A110" s="21" t="s">
         <v>76</v>
       </c>
@@ -7910,7 +7910,7 @@
       </c>
       <c r="I110" s="23"/>
     </row>
-    <row r="111" spans="1:9" ht="29" hidden="1">
+    <row r="111" spans="1:9" ht="30" hidden="1">
       <c r="A111" s="21" t="s">
         <v>77</v>
       </c>
@@ -7935,7 +7935,7 @@
       </c>
       <c r="I111" s="23"/>
     </row>
-    <row r="112" spans="1:9" ht="29" hidden="1">
+    <row r="112" spans="1:9" ht="30" hidden="1">
       <c r="A112" s="21" t="s">
         <v>78</v>
       </c>
@@ -7960,7 +7960,7 @@
       </c>
       <c r="I112" s="23"/>
     </row>
-    <row r="113" spans="1:9" ht="29" hidden="1">
+    <row r="113" spans="1:9" ht="30" hidden="1">
       <c r="A113" s="21" t="s">
         <v>79</v>
       </c>
@@ -7985,7 +7985,7 @@
       </c>
       <c r="I113" s="23"/>
     </row>
-    <row r="114" spans="1:9" ht="29" hidden="1">
+    <row r="114" spans="1:9" ht="30" hidden="1">
       <c r="A114" s="21" t="s">
         <v>80</v>
       </c>
@@ -8010,7 +8010,7 @@
       </c>
       <c r="I114" s="23"/>
     </row>
-    <row r="115" spans="1:9" ht="29" hidden="1">
+    <row r="115" spans="1:9" ht="30" hidden="1">
       <c r="A115" s="21" t="s">
         <v>81</v>
       </c>
@@ -8035,7 +8035,7 @@
       </c>
       <c r="I115" s="23"/>
     </row>
-    <row r="116" spans="1:9" ht="29" hidden="1">
+    <row r="116" spans="1:9" ht="30" hidden="1">
       <c r="A116" s="21" t="s">
         <v>82</v>
       </c>
@@ -8060,7 +8060,7 @@
       </c>
       <c r="I116" s="23"/>
     </row>
-    <row r="117" spans="1:9" ht="29" hidden="1">
+    <row r="117" spans="1:9" ht="30" hidden="1">
       <c r="A117" s="14" t="s">
         <v>83</v>
       </c>
@@ -8087,7 +8087,7 @@
         <v>843</v>
       </c>
     </row>
-    <row r="118" spans="1:9" ht="319" hidden="1">
+    <row r="118" spans="1:9" ht="315" hidden="1">
       <c r="A118" s="21" t="s">
         <v>84</v>
       </c>
@@ -8112,7 +8112,7 @@
       </c>
       <c r="I118" s="23"/>
     </row>
-    <row r="119" spans="1:9" ht="43.5" hidden="1">
+    <row r="119" spans="1:9" ht="45" hidden="1">
       <c r="A119" s="21" t="s">
         <v>85</v>
       </c>
@@ -8137,7 +8137,7 @@
       </c>
       <c r="I119" s="23"/>
     </row>
-    <row r="120" spans="1:9" ht="29" hidden="1">
+    <row r="120" spans="1:9" ht="30" hidden="1">
       <c r="A120" s="21" t="s">
         <v>86</v>
       </c>
@@ -8162,7 +8162,7 @@
       </c>
       <c r="I120" s="23"/>
     </row>
-    <row r="121" spans="1:9" ht="29" hidden="1">
+    <row r="121" spans="1:9" ht="30" hidden="1">
       <c r="A121" s="21" t="s">
         <v>87</v>
       </c>
@@ -8187,7 +8187,7 @@
       </c>
       <c r="I121" s="23"/>
     </row>
-    <row r="122" spans="1:9" ht="29" hidden="1">
+    <row r="122" spans="1:9" ht="30" hidden="1">
       <c r="A122" s="21" t="s">
         <v>88</v>
       </c>
@@ -8212,7 +8212,7 @@
       </c>
       <c r="I122" s="23"/>
     </row>
-    <row r="123" spans="1:9" ht="29" hidden="1">
+    <row r="123" spans="1:9" ht="30" hidden="1">
       <c r="A123" s="21" t="s">
         <v>89</v>
       </c>
@@ -8237,7 +8237,7 @@
       </c>
       <c r="I123" s="23"/>
     </row>
-    <row r="124" spans="1:9" ht="29" hidden="1">
+    <row r="124" spans="1:9" ht="30" hidden="1">
       <c r="A124" s="21" t="s">
         <v>90</v>
       </c>
@@ -8262,7 +8262,7 @@
       </c>
       <c r="I124" s="23"/>
     </row>
-    <row r="125" spans="1:9" ht="29" hidden="1">
+    <row r="125" spans="1:9" ht="30" hidden="1">
       <c r="A125" s="21" t="s">
         <v>91</v>
       </c>
@@ -8287,7 +8287,7 @@
       </c>
       <c r="I125" s="23"/>
     </row>
-    <row r="126" spans="1:9" ht="29" hidden="1">
+    <row r="126" spans="1:9" ht="30" hidden="1">
       <c r="A126" s="21" t="s">
         <v>92</v>
       </c>
@@ -8312,7 +8312,7 @@
       </c>
       <c r="I126" s="23"/>
     </row>
-    <row r="127" spans="1:9" ht="29" hidden="1">
+    <row r="127" spans="1:9" ht="30" hidden="1">
       <c r="A127" s="21" t="s">
         <v>93</v>
       </c>
@@ -8337,7 +8337,7 @@
       </c>
       <c r="I127" s="23"/>
     </row>
-    <row r="128" spans="1:9" ht="29" hidden="1">
+    <row r="128" spans="1:9" ht="30" hidden="1">
       <c r="A128" s="21" t="s">
         <v>94</v>
       </c>
@@ -8362,7 +8362,7 @@
       </c>
       <c r="I128" s="23"/>
     </row>
-    <row r="129" spans="1:9" ht="29" hidden="1">
+    <row r="129" spans="1:9" ht="30" hidden="1">
       <c r="A129" s="21" t="s">
         <v>95</v>
       </c>
@@ -8387,7 +8387,7 @@
       </c>
       <c r="I129" s="23"/>
     </row>
-    <row r="130" spans="1:9" ht="29" hidden="1">
+    <row r="130" spans="1:9" ht="30" hidden="1">
       <c r="A130" s="21" t="s">
         <v>96</v>
       </c>
@@ -8412,7 +8412,7 @@
       </c>
       <c r="I130" s="23"/>
     </row>
-    <row r="131" spans="1:9" ht="29" hidden="1">
+    <row r="131" spans="1:9" ht="30" hidden="1">
       <c r="A131" s="21" t="s">
         <v>97</v>
       </c>
@@ -8437,7 +8437,7 @@
       </c>
       <c r="I131" s="23"/>
     </row>
-    <row r="132" spans="1:9" ht="29" hidden="1">
+    <row r="132" spans="1:9" ht="30" hidden="1">
       <c r="A132" s="21" t="s">
         <v>98</v>
       </c>
@@ -8462,7 +8462,7 @@
       </c>
       <c r="I132" s="23"/>
     </row>
-    <row r="133" spans="1:9" ht="29" hidden="1">
+    <row r="133" spans="1:9" ht="30" hidden="1">
       <c r="A133" s="21" t="s">
         <v>99</v>
       </c>
@@ -8487,7 +8487,7 @@
       </c>
       <c r="I133" s="23"/>
     </row>
-    <row r="134" spans="1:9" ht="29" hidden="1">
+    <row r="134" spans="1:9" ht="30" hidden="1">
       <c r="A134" s="21" t="s">
         <v>100</v>
       </c>
@@ -8512,7 +8512,7 @@
       </c>
       <c r="I134" s="23"/>
     </row>
-    <row r="135" spans="1:9" ht="130.5" hidden="1">
+    <row r="135" spans="1:9" ht="135" hidden="1">
       <c r="A135" s="21" t="s">
         <v>101</v>
       </c>
@@ -8537,7 +8537,7 @@
       </c>
       <c r="I135" s="23"/>
     </row>
-    <row r="136" spans="1:9" ht="29" hidden="1">
+    <row r="136" spans="1:9" ht="30" hidden="1">
       <c r="A136" s="21" t="s">
         <v>102</v>
       </c>
@@ -8562,7 +8562,7 @@
       </c>
       <c r="I136" s="23"/>
     </row>
-    <row r="137" spans="1:9" ht="29" hidden="1">
+    <row r="137" spans="1:9" ht="30" hidden="1">
       <c r="A137" s="21" t="s">
         <v>103</v>
       </c>
@@ -8587,7 +8587,7 @@
       </c>
       <c r="I137" s="23"/>
     </row>
-    <row r="138" spans="1:9" ht="29" hidden="1">
+    <row r="138" spans="1:9" ht="30" hidden="1">
       <c r="A138" s="21" t="s">
         <v>104</v>
       </c>
@@ -8612,7 +8612,7 @@
       </c>
       <c r="I138" s="23"/>
     </row>
-    <row r="139" spans="1:9" ht="43.5">
+    <row r="139" spans="1:9" ht="45">
       <c r="A139" s="21" t="s">
         <v>105</v>
       </c>
@@ -8637,7 +8637,7 @@
       </c>
       <c r="I139" s="23"/>
     </row>
-    <row r="140" spans="1:9" ht="43.5">
+    <row r="140" spans="1:9" ht="45">
       <c r="A140" s="21" t="s">
         <v>106</v>
       </c>
@@ -8662,7 +8662,7 @@
       </c>
       <c r="I140" s="23"/>
     </row>
-    <row r="141" spans="1:9" ht="348">
+    <row r="141" spans="1:9" ht="360">
       <c r="A141" s="21" t="s">
         <v>107</v>
       </c>
@@ -8687,7 +8687,7 @@
       </c>
       <c r="I141" s="23"/>
     </row>
-    <row r="142" spans="1:9" ht="43.5">
+    <row r="142" spans="1:9" ht="30">
       <c r="A142" s="21" t="s">
         <v>108</v>
       </c>
@@ -8712,7 +8712,7 @@
       </c>
       <c r="I142" s="23"/>
     </row>
-    <row r="143" spans="1:9" ht="29">
+    <row r="143" spans="1:9" ht="30">
       <c r="A143" s="21" t="s">
         <v>109</v>
       </c>
@@ -8737,7 +8737,7 @@
       </c>
       <c r="I143" s="23"/>
     </row>
-    <row r="144" spans="1:9" ht="43.5">
+    <row r="144" spans="1:9" ht="45">
       <c r="A144" s="21" t="s">
         <v>110</v>
       </c>
@@ -8762,7 +8762,7 @@
       </c>
       <c r="I144" s="23"/>
     </row>
-    <row r="145" spans="1:9" ht="29">
+    <row r="145" spans="1:9" ht="30">
       <c r="A145" s="21" t="s">
         <v>111</v>
       </c>
@@ -8787,7 +8787,7 @@
       </c>
       <c r="I145" s="13"/>
     </row>
-    <row r="146" spans="1:9" ht="29">
+    <row r="146" spans="1:9" ht="30">
       <c r="A146" s="21" t="s">
         <v>112</v>
       </c>
@@ -8812,7 +8812,7 @@
       </c>
       <c r="I146" s="23"/>
     </row>
-    <row r="147" spans="1:9" ht="43.5">
+    <row r="147" spans="1:9" ht="30">
       <c r="A147" s="14" t="s">
         <v>113</v>
       </c>
@@ -8837,7 +8837,7 @@
       </c>
       <c r="I147" s="23"/>
     </row>
-    <row r="148" spans="1:9" ht="29">
+    <row r="148" spans="1:9" ht="30">
       <c r="A148" s="21" t="s">
         <v>114</v>
       </c>
@@ -8862,7 +8862,7 @@
       </c>
       <c r="I148" s="23"/>
     </row>
-    <row r="149" spans="1:9" ht="29">
+    <row r="149" spans="1:9" ht="30">
       <c r="A149" s="14" t="s">
         <v>115</v>
       </c>
@@ -8887,7 +8887,7 @@
       </c>
       <c r="I149" s="13"/>
     </row>
-    <row r="150" spans="1:9" ht="29">
+    <row r="150" spans="1:9" ht="30">
       <c r="A150" s="14" t="s">
         <v>116</v>
       </c>
@@ -8912,7 +8912,7 @@
       </c>
       <c r="I150" s="23"/>
     </row>
-    <row r="151" spans="1:9" ht="29">
+    <row r="151" spans="1:9" ht="30">
       <c r="A151" s="21" t="s">
         <v>117</v>
       </c>
@@ -8937,7 +8937,7 @@
       </c>
       <c r="I151" s="23"/>
     </row>
-    <row r="152" spans="1:9" ht="29">
+    <row r="152" spans="1:9">
       <c r="A152" s="14" t="s">
         <v>118</v>
       </c>
@@ -8962,7 +8962,7 @@
       </c>
       <c r="I152" s="13"/>
     </row>
-    <row r="153" spans="1:9" ht="29" hidden="1">
+    <row r="153" spans="1:9" ht="30" hidden="1">
       <c r="A153" s="21" t="s">
         <v>270</v>
       </c>
@@ -8987,7 +8987,7 @@
       </c>
       <c r="I153" s="23"/>
     </row>
-    <row r="154" spans="1:9" ht="43.5" hidden="1">
+    <row r="154" spans="1:9" ht="30" hidden="1">
       <c r="A154" s="21" t="s">
         <v>271</v>
       </c>
@@ -9012,7 +9012,7 @@
       </c>
       <c r="I154" s="23"/>
     </row>
-    <row r="155" spans="1:9" ht="130.5" hidden="1">
+    <row r="155" spans="1:9" ht="135" hidden="1">
       <c r="A155" s="21" t="s">
         <v>272</v>
       </c>
@@ -9037,7 +9037,7 @@
       </c>
       <c r="I155" s="23"/>
     </row>
-    <row r="156" spans="1:9" ht="29" hidden="1">
+    <row r="156" spans="1:9" ht="30" hidden="1">
       <c r="A156" s="21" t="s">
         <v>248</v>
       </c>
@@ -9062,7 +9062,7 @@
       </c>
       <c r="I156" s="23"/>
     </row>
-    <row r="157" spans="1:9" ht="29" hidden="1">
+    <row r="157" spans="1:9" ht="30" hidden="1">
       <c r="A157" s="21" t="s">
         <v>249</v>
       </c>
@@ -9087,7 +9087,7 @@
       </c>
       <c r="I157" s="23"/>
     </row>
-    <row r="158" spans="1:9" ht="319" hidden="1">
+    <row r="158" spans="1:9" ht="330" hidden="1">
       <c r="A158" s="21" t="s">
         <v>250</v>
       </c>
@@ -9112,7 +9112,7 @@
       </c>
       <c r="I158" s="23"/>
     </row>
-    <row r="159" spans="1:9" ht="29" hidden="1">
+    <row r="159" spans="1:9" ht="30" hidden="1">
       <c r="A159" s="21" t="s">
         <v>251</v>
       </c>
@@ -9137,7 +9137,7 @@
       </c>
       <c r="I159" s="23"/>
     </row>
-    <row r="160" spans="1:9" ht="29" hidden="1">
+    <row r="160" spans="1:9" ht="30" hidden="1">
       <c r="A160" s="21" t="s">
         <v>252</v>
       </c>
@@ -9162,7 +9162,7 @@
       </c>
       <c r="I160" s="23"/>
     </row>
-    <row r="161" spans="1:9" ht="101.5" hidden="1">
+    <row r="161" spans="1:9" ht="90" hidden="1">
       <c r="A161" s="21" t="s">
         <v>253</v>
       </c>
@@ -9189,7 +9189,7 @@
         <v>847</v>
       </c>
     </row>
-    <row r="162" spans="1:9" ht="29" hidden="1">
+    <row r="162" spans="1:9" ht="30" hidden="1">
       <c r="A162" s="21" t="s">
         <v>254</v>
       </c>
@@ -9216,7 +9216,7 @@
       </c>
       <c r="I162" s="23"/>
     </row>
-    <row r="163" spans="1:9" ht="29" hidden="1">
+    <row r="163" spans="1:9" ht="30" hidden="1">
       <c r="A163" s="21" t="s">
         <v>255</v>
       </c>
@@ -9243,7 +9243,7 @@
       </c>
       <c r="I163" s="23"/>
     </row>
-    <row r="164" spans="1:9" ht="29" hidden="1">
+    <row r="164" spans="1:9" ht="30" hidden="1">
       <c r="A164" s="21" t="s">
         <v>256</v>
       </c>
@@ -9270,7 +9270,7 @@
       </c>
       <c r="I164" s="23"/>
     </row>
-    <row r="165" spans="1:9" ht="29" hidden="1">
+    <row r="165" spans="1:9" ht="30" hidden="1">
       <c r="A165" s="21" t="s">
         <v>257</v>
       </c>
@@ -9297,7 +9297,7 @@
       </c>
       <c r="I165" s="23"/>
     </row>
-    <row r="166" spans="1:9" ht="29" hidden="1">
+    <row r="166" spans="1:9" ht="30" hidden="1">
       <c r="A166" s="21" t="s">
         <v>258</v>
       </c>
@@ -9324,7 +9324,7 @@
       </c>
       <c r="I166" s="23"/>
     </row>
-    <row r="167" spans="1:9" ht="29" hidden="1">
+    <row r="167" spans="1:9" ht="30" hidden="1">
       <c r="A167" s="21" t="s">
         <v>259</v>
       </c>
@@ -9349,7 +9349,7 @@
       </c>
       <c r="I167" s="23"/>
     </row>
-    <row r="168" spans="1:9" ht="29" hidden="1">
+    <row r="168" spans="1:9" ht="30" hidden="1">
       <c r="A168" s="21" t="s">
         <v>260</v>
       </c>
@@ -9399,7 +9399,7 @@
       </c>
       <c r="I169" s="13"/>
     </row>
-    <row r="170" spans="1:9" ht="29" hidden="1">
+    <row r="170" spans="1:9" ht="30" hidden="1">
       <c r="A170" s="14" t="s">
         <v>262</v>
       </c>
@@ -9426,7 +9426,7 @@
       </c>
       <c r="I170" s="23"/>
     </row>
-    <row r="171" spans="1:9" ht="29" hidden="1">
+    <row r="171" spans="1:9" ht="30" hidden="1">
       <c r="A171" s="21" t="s">
         <v>263</v>
       </c>
@@ -9478,7 +9478,7 @@
       </c>
       <c r="I172" s="23"/>
     </row>
-    <row r="173" spans="1:9" ht="29" hidden="1">
+    <row r="173" spans="1:9" ht="30" hidden="1">
       <c r="A173" s="21" t="s">
         <v>265</v>
       </c>
@@ -9503,7 +9503,7 @@
       </c>
       <c r="I173" s="23"/>
     </row>
-    <row r="174" spans="1:9" ht="29" hidden="1">
+    <row r="174" spans="1:9" ht="30" hidden="1">
       <c r="A174" s="21" t="s">
         <v>266</v>
       </c>
@@ -9553,7 +9553,7 @@
       </c>
       <c r="I175" s="13"/>
     </row>
-    <row r="176" spans="1:9" ht="29" hidden="1">
+    <row r="176" spans="1:9" ht="30" hidden="1">
       <c r="A176" s="14" t="s">
         <v>268</v>
       </c>
@@ -9580,7 +9580,7 @@
       </c>
       <c r="I176" s="23"/>
     </row>
-    <row r="177" spans="1:9" ht="29" hidden="1">
+    <row r="177" spans="1:9" ht="30" hidden="1">
       <c r="A177" s="21" t="s">
         <v>269</v>
       </c>
@@ -9607,7 +9607,7 @@
       </c>
       <c r="I177" s="23"/>
     </row>
-    <row r="178" spans="1:9" ht="29" hidden="1">
+    <row r="178" spans="1:9" ht="30" hidden="1">
       <c r="A178" s="21" t="s">
         <v>273</v>
       </c>
@@ -9632,7 +9632,7 @@
       </c>
       <c r="I178" s="23"/>
     </row>
-    <row r="179" spans="1:9" ht="87" hidden="1">
+    <row r="179" spans="1:9" ht="75" hidden="1">
       <c r="A179" s="21" t="s">
         <v>274</v>
       </c>
@@ -9657,7 +9657,7 @@
       </c>
       <c r="I179" s="23"/>
     </row>
-    <row r="180" spans="1:9" ht="261" hidden="1">
+    <row r="180" spans="1:9" ht="225" hidden="1">
       <c r="A180" s="21" t="s">
         <v>275</v>
       </c>
@@ -9682,7 +9682,7 @@
       </c>
       <c r="I180" s="23"/>
     </row>
-    <row r="181" spans="1:9" ht="29" hidden="1">
+    <row r="181" spans="1:9" ht="30" hidden="1">
       <c r="A181" s="21" t="s">
         <v>276</v>
       </c>
@@ -9707,7 +9707,7 @@
       </c>
       <c r="I181" s="23"/>
     </row>
-    <row r="182" spans="1:9" ht="29" hidden="1">
+    <row r="182" spans="1:9" ht="30" hidden="1">
       <c r="A182" s="21" t="s">
         <v>277</v>
       </c>
@@ -9732,7 +9732,7 @@
       </c>
       <c r="I182" s="23"/>
     </row>
-    <row r="183" spans="1:9" ht="29" hidden="1">
+    <row r="183" spans="1:9" ht="30" hidden="1">
       <c r="A183" s="21" t="s">
         <v>278</v>
       </c>
@@ -9757,7 +9757,7 @@
       </c>
       <c r="I183" s="23"/>
     </row>
-    <row r="184" spans="1:9" ht="116" hidden="1">
+    <row r="184" spans="1:9" ht="120" hidden="1">
       <c r="A184" s="21" t="s">
         <v>279</v>
       </c>
@@ -9782,7 +9782,7 @@
       </c>
       <c r="I184" s="23"/>
     </row>
-    <row r="185" spans="1:9" ht="29" hidden="1">
+    <row r="185" spans="1:9" ht="30" hidden="1">
       <c r="A185" s="21" t="s">
         <v>280</v>
       </c>
@@ -9807,7 +9807,7 @@
       </c>
       <c r="I185" s="23"/>
     </row>
-    <row r="186" spans="1:9" ht="43.5" hidden="1">
+    <row r="186" spans="1:9" ht="45" hidden="1">
       <c r="A186" s="21" t="s">
         <v>281</v>
       </c>
@@ -9832,7 +9832,7 @@
       </c>
       <c r="I186" s="23"/>
     </row>
-    <row r="187" spans="1:9" ht="29" hidden="1">
+    <row r="187" spans="1:9" ht="30" hidden="1">
       <c r="A187" s="21" t="s">
         <v>282</v>
       </c>
@@ -9857,7 +9857,7 @@
       </c>
       <c r="I187" s="23"/>
     </row>
-    <row r="188" spans="1:9" ht="29" hidden="1">
+    <row r="188" spans="1:9" ht="30" hidden="1">
       <c r="A188" s="21" t="s">
         <v>283</v>
       </c>
@@ -9882,7 +9882,7 @@
       </c>
       <c r="I188" s="23"/>
     </row>
-    <row r="189" spans="1:9" ht="29" hidden="1">
+    <row r="189" spans="1:9" ht="30" hidden="1">
       <c r="A189" s="21" t="s">
         <v>284</v>
       </c>
@@ -9907,7 +9907,7 @@
       </c>
       <c r="I189" s="23"/>
     </row>
-    <row r="190" spans="1:9" ht="29" hidden="1">
+    <row r="190" spans="1:9" ht="30" hidden="1">
       <c r="A190" s="21" t="s">
         <v>285</v>
       </c>
@@ -9932,7 +9932,7 @@
       </c>
       <c r="I190" s="23"/>
     </row>
-    <row r="191" spans="1:9" ht="29" hidden="1">
+    <row r="191" spans="1:9" ht="30" hidden="1">
       <c r="A191" s="21" t="s">
         <v>286</v>
       </c>
@@ -9957,7 +9957,7 @@
       </c>
       <c r="I191" s="23"/>
     </row>
-    <row r="192" spans="1:9" ht="29" hidden="1">
+    <row r="192" spans="1:9" ht="30" hidden="1">
       <c r="A192" s="21" t="s">
         <v>287</v>
       </c>
@@ -10007,7 +10007,7 @@
       </c>
       <c r="I193" s="23"/>
     </row>
-    <row r="194" spans="1:9" ht="29" hidden="1">
+    <row r="194" spans="1:9" ht="30" hidden="1">
       <c r="A194" s="21" t="s">
         <v>289</v>
       </c>
@@ -10032,7 +10032,7 @@
       </c>
       <c r="I194" s="23"/>
     </row>
-    <row r="195" spans="1:9" ht="29" hidden="1">
+    <row r="195" spans="1:9" ht="30" hidden="1">
       <c r="A195" s="21" t="s">
         <v>290</v>
       </c>
@@ -10057,7 +10057,7 @@
       </c>
       <c r="I195" s="23"/>
     </row>
-    <row r="196" spans="1:9" ht="87" hidden="1">
+    <row r="196" spans="1:9" ht="90" hidden="1">
       <c r="A196" s="21" t="s">
         <v>291</v>
       </c>
@@ -10082,7 +10082,7 @@
       </c>
       <c r="I196" s="23"/>
     </row>
-    <row r="197" spans="1:9" ht="43.5" hidden="1">
+    <row r="197" spans="1:9" ht="30" hidden="1">
       <c r="A197" s="21" t="s">
         <v>292</v>
       </c>
@@ -10107,7 +10107,7 @@
       </c>
       <c r="I197" s="23"/>
     </row>
-    <row r="198" spans="1:9" ht="29" hidden="1">
+    <row r="198" spans="1:9" ht="30" hidden="1">
       <c r="A198" s="21" t="s">
         <v>293</v>
       </c>
@@ -10132,7 +10132,7 @@
       </c>
       <c r="I198" s="23"/>
     </row>
-    <row r="199" spans="1:9" ht="29" hidden="1">
+    <row r="199" spans="1:9" ht="30" hidden="1">
       <c r="A199" s="21" t="s">
         <v>294</v>
       </c>
@@ -10157,7 +10157,7 @@
       </c>
       <c r="I199" s="23"/>
     </row>
-    <row r="200" spans="1:9" ht="29" hidden="1">
+    <row r="200" spans="1:9" ht="30" hidden="1">
       <c r="A200" s="21" t="s">
         <v>295</v>
       </c>
@@ -10182,7 +10182,7 @@
       </c>
       <c r="I200" s="23"/>
     </row>
-    <row r="201" spans="1:9" ht="29" hidden="1">
+    <row r="201" spans="1:9" ht="30" hidden="1">
       <c r="A201" s="21" t="s">
         <v>296</v>
       </c>
@@ -10207,7 +10207,7 @@
       </c>
       <c r="I201" s="23"/>
     </row>
-    <row r="202" spans="1:9" ht="29" hidden="1">
+    <row r="202" spans="1:9" ht="30" hidden="1">
       <c r="A202" s="21" t="s">
         <v>297</v>
       </c>
@@ -10232,7 +10232,7 @@
       </c>
       <c r="I202" s="23"/>
     </row>
-    <row r="203" spans="1:9" ht="43.5" hidden="1">
+    <row r="203" spans="1:9" ht="30" hidden="1">
       <c r="A203" s="21" t="s">
         <v>298</v>
       </c>
@@ -10257,7 +10257,7 @@
       </c>
       <c r="I203" s="23"/>
     </row>
-    <row r="204" spans="1:9" ht="29" hidden="1">
+    <row r="204" spans="1:9" ht="30" hidden="1">
       <c r="A204" s="21" t="s">
         <v>299</v>
       </c>
@@ -10282,7 +10282,7 @@
       </c>
       <c r="I204" s="23"/>
     </row>
-    <row r="205" spans="1:9" ht="29" hidden="1">
+    <row r="205" spans="1:9" ht="30" hidden="1">
       <c r="A205" s="21" t="s">
         <v>300</v>
       </c>
@@ -10307,7 +10307,7 @@
       </c>
       <c r="I205" s="23"/>
     </row>
-    <row r="206" spans="1:9" ht="72.5" hidden="1">
+    <row r="206" spans="1:9" ht="75" hidden="1">
       <c r="A206" s="21" t="s">
         <v>301</v>
       </c>
@@ -10332,7 +10332,7 @@
       </c>
       <c r="I206" s="23"/>
     </row>
-    <row r="207" spans="1:9" ht="72.5" hidden="1">
+    <row r="207" spans="1:9" ht="60" hidden="1">
       <c r="A207" s="21" t="s">
         <v>302</v>
       </c>
@@ -10357,7 +10357,7 @@
       </c>
       <c r="I207" s="23"/>
     </row>
-    <row r="208" spans="1:9" ht="72.5" hidden="1">
+    <row r="208" spans="1:9" ht="60" hidden="1">
       <c r="A208" s="21" t="s">
         <v>303</v>
       </c>
@@ -10382,7 +10382,7 @@
       </c>
       <c r="I208" s="23"/>
     </row>
-    <row r="209" spans="1:9" ht="29" hidden="1">
+    <row r="209" spans="1:9" ht="30" hidden="1">
       <c r="A209" s="21" t="s">
         <v>304</v>
       </c>
@@ -10407,7 +10407,7 @@
       </c>
       <c r="I209" s="23"/>
     </row>
-    <row r="210" spans="1:9" ht="29" hidden="1">
+    <row r="210" spans="1:9" ht="30" hidden="1">
       <c r="A210" s="21" t="s">
         <v>305</v>
       </c>
@@ -10432,7 +10432,7 @@
       </c>
       <c r="I210" s="23"/>
     </row>
-    <row r="211" spans="1:9" ht="29" hidden="1">
+    <row r="211" spans="1:9" hidden="1">
       <c r="A211" s="21" t="s">
         <v>306</v>
       </c>
@@ -10457,7 +10457,7 @@
       </c>
       <c r="I211" s="23"/>
     </row>
-    <row r="212" spans="1:9" ht="43.5" hidden="1">
+    <row r="212" spans="1:9" ht="30" hidden="1">
       <c r="A212" s="21" t="s">
         <v>71</v>
       </c>
@@ -10482,7 +10482,7 @@
       </c>
       <c r="I212" s="23"/>
     </row>
-    <row r="213" spans="1:9" ht="29" hidden="1">
+    <row r="213" spans="1:9" ht="30" hidden="1">
       <c r="A213" s="21" t="s">
         <v>72</v>
       </c>
@@ -10507,7 +10507,7 @@
       </c>
       <c r="I213" s="23"/>
     </row>
-    <row r="214" spans="1:9" ht="29" hidden="1">
+    <row r="214" spans="1:9" ht="30" hidden="1">
       <c r="A214" s="21" t="s">
         <v>73</v>
       </c>
@@ -10532,7 +10532,7 @@
       </c>
       <c r="I214" s="23"/>
     </row>
-    <row r="215" spans="1:9" ht="29" hidden="1">
+    <row r="215" spans="1:9" ht="30" hidden="1">
       <c r="A215" s="21" t="s">
         <v>74</v>
       </c>
@@ -10557,7 +10557,7 @@
       </c>
       <c r="I215" s="23"/>
     </row>
-    <row r="216" spans="1:9" ht="29" hidden="1">
+    <row r="216" spans="1:9" ht="30" hidden="1">
       <c r="A216" s="21" t="s">
         <v>75</v>
       </c>
@@ -10582,7 +10582,7 @@
       </c>
       <c r="I216" s="23"/>
     </row>
-    <row r="217" spans="1:9" ht="174" hidden="1">
+    <row r="217" spans="1:9" ht="180" hidden="1">
       <c r="A217" s="21" t="s">
         <v>348</v>
       </c>
@@ -10607,7 +10607,7 @@
       </c>
       <c r="I217" s="23"/>
     </row>
-    <row r="218" spans="1:9" ht="29" hidden="1">
+    <row r="218" spans="1:9" ht="30" hidden="1">
       <c r="A218" s="21" t="s">
         <v>349</v>
       </c>
@@ -10632,7 +10632,7 @@
       </c>
       <c r="I218" s="23"/>
     </row>
-    <row r="219" spans="1:9" ht="29" hidden="1">
+    <row r="219" spans="1:9" ht="30" hidden="1">
       <c r="A219" s="21" t="s">
         <v>350</v>
       </c>
@@ -10657,7 +10657,7 @@
       </c>
       <c r="I219" s="23"/>
     </row>
-    <row r="220" spans="1:9" ht="29" hidden="1">
+    <row r="220" spans="1:9" ht="30" hidden="1">
       <c r="A220" s="21" t="s">
         <v>351</v>
       </c>
@@ -10682,7 +10682,7 @@
       </c>
       <c r="I220" s="23"/>
     </row>
-    <row r="221" spans="1:9" ht="348" hidden="1">
+    <row r="221" spans="1:9" ht="360" hidden="1">
       <c r="A221" s="21" t="s">
         <v>119</v>
       </c>
@@ -10707,7 +10707,7 @@
       </c>
       <c r="I221" s="23"/>
     </row>
-    <row r="222" spans="1:9" ht="43.5" hidden="1">
+    <row r="222" spans="1:9" ht="30" hidden="1">
       <c r="A222" s="21" t="s">
         <v>120</v>
       </c>
@@ -10732,7 +10732,7 @@
       </c>
       <c r="I222" s="23"/>
     </row>
-    <row r="223" spans="1:9" ht="29" hidden="1">
+    <row r="223" spans="1:9" ht="30" hidden="1">
       <c r="A223" s="21" t="s">
         <v>121</v>
       </c>
@@ -10757,7 +10757,7 @@
       </c>
       <c r="I223" s="23"/>
     </row>
-    <row r="224" spans="1:9" ht="29" hidden="1">
+    <row r="224" spans="1:9" ht="30" hidden="1">
       <c r="A224" s="21" t="s">
         <v>122</v>
       </c>
@@ -10782,7 +10782,7 @@
       </c>
       <c r="I224" s="23"/>
     </row>
-    <row r="225" spans="1:9" ht="29" hidden="1">
+    <row r="225" spans="1:9" ht="30" hidden="1">
       <c r="A225" s="21" t="s">
         <v>123</v>
       </c>
@@ -10807,7 +10807,7 @@
       </c>
       <c r="I225" s="23"/>
     </row>
-    <row r="226" spans="1:9" ht="29" hidden="1">
+    <row r="226" spans="1:9" ht="30" hidden="1">
       <c r="A226" s="21" t="s">
         <v>124</v>
       </c>
@@ -10832,7 +10832,7 @@
       </c>
       <c r="I226" s="23"/>
     </row>
-    <row r="227" spans="1:9" ht="29" hidden="1">
+    <row r="227" spans="1:9" ht="30" hidden="1">
       <c r="A227" s="21" t="s">
         <v>125</v>
       </c>
@@ -10857,7 +10857,7 @@
       </c>
       <c r="I227" s="23"/>
     </row>
-    <row r="228" spans="1:9" ht="29" hidden="1">
+    <row r="228" spans="1:9" ht="30" hidden="1">
       <c r="A228" s="21" t="s">
         <v>126</v>
       </c>
@@ -10882,7 +10882,7 @@
       </c>
       <c r="I228" s="23"/>
     </row>
-    <row r="229" spans="1:9" ht="29" hidden="1">
+    <row r="229" spans="1:9" ht="30" hidden="1">
       <c r="A229" s="21" t="s">
         <v>127</v>
       </c>
@@ -10907,7 +10907,7 @@
       </c>
       <c r="I229" s="23"/>
     </row>
-    <row r="230" spans="1:9" ht="29" hidden="1">
+    <row r="230" spans="1:9" ht="30" hidden="1">
       <c r="A230" s="21" t="s">
         <v>128</v>
       </c>
@@ -10957,7 +10957,7 @@
       </c>
       <c r="I231" s="23"/>
     </row>
-    <row r="232" spans="1:9" ht="72.5" hidden="1">
+    <row r="232" spans="1:9" ht="60" hidden="1">
       <c r="A232" s="21" t="s">
         <v>130</v>
       </c>
@@ -10982,7 +10982,7 @@
       </c>
       <c r="I232" s="23"/>
     </row>
-    <row r="233" spans="1:9" ht="29" hidden="1">
+    <row r="233" spans="1:9" ht="30" hidden="1">
       <c r="A233" s="21" t="s">
         <v>131</v>
       </c>
@@ -11007,7 +11007,7 @@
       </c>
       <c r="I233" s="23"/>
     </row>
-    <row r="234" spans="1:9" ht="29" hidden="1">
+    <row r="234" spans="1:9" ht="30" hidden="1">
       <c r="A234" s="14" t="s">
         <v>132</v>
       </c>
@@ -11032,7 +11032,7 @@
       </c>
       <c r="I234" s="13"/>
     </row>
-    <row r="235" spans="1:9" ht="29" hidden="1">
+    <row r="235" spans="1:9" ht="30" hidden="1">
       <c r="A235" s="14" t="s">
         <v>882</v>
       </c>
@@ -11057,7 +11057,7 @@
       </c>
       <c r="I235" s="42"/>
     </row>
-    <row r="236" spans="1:9" ht="29" hidden="1">
+    <row r="236" spans="1:9" ht="30" hidden="1">
       <c r="A236" s="14" t="s">
         <v>883</v>
       </c>
@@ -11084,7 +11084,7 @@
         <v>844</v>
       </c>
     </row>
-    <row r="237" spans="1:9" ht="29" hidden="1">
+    <row r="237" spans="1:9" ht="30" hidden="1">
       <c r="A237" s="21" t="s">
         <v>133</v>
       </c>
@@ -11109,7 +11109,7 @@
       </c>
       <c r="I237" s="23"/>
     </row>
-    <row r="238" spans="1:9" ht="29" hidden="1">
+    <row r="238" spans="1:9" ht="30" hidden="1">
       <c r="A238" s="21" t="s">
         <v>134</v>
       </c>
@@ -11134,7 +11134,7 @@
       </c>
       <c r="I238" s="23"/>
     </row>
-    <row r="239" spans="1:9" ht="29" hidden="1">
+    <row r="239" spans="1:9" ht="30" hidden="1">
       <c r="A239" s="21" t="s">
         <v>135</v>
       </c>
@@ -11159,7 +11159,7 @@
       </c>
       <c r="I239" s="23"/>
     </row>
-    <row r="240" spans="1:9" ht="29" hidden="1">
+    <row r="240" spans="1:9" ht="30" hidden="1">
       <c r="A240" s="21" t="s">
         <v>136</v>
       </c>
@@ -11184,7 +11184,7 @@
       </c>
       <c r="I240" s="23"/>
     </row>
-    <row r="241" spans="1:9" ht="29" hidden="1">
+    <row r="241" spans="1:9" ht="30" hidden="1">
       <c r="A241" s="21" t="s">
         <v>137</v>
       </c>
@@ -11209,7 +11209,7 @@
       </c>
       <c r="I241" s="23"/>
     </row>
-    <row r="242" spans="1:9" ht="29" hidden="1">
+    <row r="242" spans="1:9" ht="30" hidden="1">
       <c r="A242" s="21" t="s">
         <v>138</v>
       </c>
@@ -11234,7 +11234,7 @@
       </c>
       <c r="I242" s="23"/>
     </row>
-    <row r="243" spans="1:9" ht="29" hidden="1">
+    <row r="243" spans="1:9" ht="30" hidden="1">
       <c r="A243" s="14" t="s">
         <v>139</v>
       </c>
@@ -11259,7 +11259,7 @@
       </c>
       <c r="I243" s="23"/>
     </row>
-    <row r="244" spans="1:9" ht="29" hidden="1">
+    <row r="244" spans="1:9" ht="30" hidden="1">
       <c r="A244" s="14" t="s">
         <v>140</v>
       </c>
@@ -11284,7 +11284,7 @@
       </c>
       <c r="I244" s="23"/>
     </row>
-    <row r="245" spans="1:9" ht="29" hidden="1">
+    <row r="245" spans="1:9" ht="30" hidden="1">
       <c r="A245" s="21" t="s">
         <v>141</v>
       </c>
@@ -11309,7 +11309,7 @@
       </c>
       <c r="I245" s="23"/>
     </row>
-    <row r="246" spans="1:9" ht="29" hidden="1">
+    <row r="246" spans="1:9" ht="30" hidden="1">
       <c r="A246" s="21" t="s">
         <v>142</v>
       </c>
@@ -11336,7 +11336,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="247" spans="1:9" ht="29" hidden="1">
+    <row r="247" spans="1:9" ht="30" hidden="1">
       <c r="A247" s="21" t="s">
         <v>143</v>
       </c>
@@ -11361,7 +11361,7 @@
       </c>
       <c r="I247" s="23"/>
     </row>
-    <row r="248" spans="1:9" ht="29" hidden="1">
+    <row r="248" spans="1:9" ht="30" hidden="1">
       <c r="A248" s="21" t="s">
         <v>144</v>
       </c>
@@ -11386,7 +11386,7 @@
       </c>
       <c r="I248" s="23"/>
     </row>
-    <row r="249" spans="1:9" ht="29" hidden="1">
+    <row r="249" spans="1:9" ht="30" hidden="1">
       <c r="A249" s="14" t="s">
         <v>145</v>
       </c>
@@ -11411,7 +11411,7 @@
       </c>
       <c r="I249" s="23"/>
     </row>
-    <row r="250" spans="1:9" ht="29" hidden="1">
+    <row r="250" spans="1:9" ht="30" hidden="1">
       <c r="A250" s="14" t="s">
         <v>146</v>
       </c>
@@ -11436,7 +11436,7 @@
       </c>
       <c r="I250" s="23"/>
     </row>
-    <row r="251" spans="1:9" ht="29" hidden="1">
+    <row r="251" spans="1:9" ht="30" hidden="1">
       <c r="A251" s="14" t="s">
         <v>896</v>
       </c>
@@ -11461,7 +11461,7 @@
       </c>
       <c r="I251" s="42"/>
     </row>
-    <row r="252" spans="1:9" ht="29" hidden="1">
+    <row r="252" spans="1:9" ht="30" hidden="1">
       <c r="A252" s="21" t="s">
         <v>147</v>
       </c>
@@ -11486,7 +11486,7 @@
       </c>
       <c r="I252" s="23"/>
     </row>
-    <row r="253" spans="1:9" ht="29" hidden="1">
+    <row r="253" spans="1:9" ht="30" hidden="1">
       <c r="A253" s="21" t="s">
         <v>148</v>
       </c>
@@ -11511,7 +11511,7 @@
       </c>
       <c r="I253" s="23"/>
     </row>
-    <row r="254" spans="1:9" ht="29" hidden="1">
+    <row r="254" spans="1:9" ht="30" hidden="1">
       <c r="A254" s="21" t="s">
         <v>149</v>
       </c>
@@ -11536,7 +11536,7 @@
       </c>
       <c r="I254" s="23"/>
     </row>
-    <row r="255" spans="1:9" ht="29" hidden="1">
+    <row r="255" spans="1:9" ht="30" hidden="1">
       <c r="A255" s="21" t="s">
         <v>150</v>
       </c>
@@ -11561,7 +11561,7 @@
       </c>
       <c r="I255" s="23"/>
     </row>
-    <row r="256" spans="1:9" ht="29" hidden="1">
+    <row r="256" spans="1:9" ht="30" hidden="1">
       <c r="A256" s="21" t="s">
         <v>151</v>
       </c>
@@ -11586,7 +11586,7 @@
       </c>
       <c r="I256" s="23"/>
     </row>
-    <row r="257" spans="1:9" ht="29" hidden="1">
+    <row r="257" spans="1:9" ht="30" hidden="1">
       <c r="A257" s="21" t="s">
         <v>152</v>
       </c>
@@ -11611,7 +11611,7 @@
       </c>
       <c r="I257" s="23"/>
     </row>
-    <row r="258" spans="1:9" ht="29" hidden="1">
+    <row r="258" spans="1:9" ht="30" hidden="1">
       <c r="A258" s="21" t="s">
         <v>153</v>
       </c>
@@ -11636,7 +11636,7 @@
       </c>
       <c r="I258" s="23"/>
     </row>
-    <row r="259" spans="1:9" ht="29" hidden="1">
+    <row r="259" spans="1:9" ht="30" hidden="1">
       <c r="A259" s="21" t="s">
         <v>154</v>
       </c>
@@ -11661,7 +11661,7 @@
       </c>
       <c r="I259" s="23"/>
     </row>
-    <row r="260" spans="1:9" ht="29" hidden="1">
+    <row r="260" spans="1:9" ht="30" hidden="1">
       <c r="A260" s="21" t="s">
         <v>155</v>
       </c>
@@ -11686,7 +11686,7 @@
       </c>
       <c r="I260" s="23"/>
     </row>
-    <row r="261" spans="1:9" ht="29" hidden="1">
+    <row r="261" spans="1:9" ht="30" hidden="1">
       <c r="A261" s="21" t="s">
         <v>156</v>
       </c>
@@ -11711,7 +11711,7 @@
       </c>
       <c r="I261" s="23"/>
     </row>
-    <row r="262" spans="1:9" ht="29" hidden="1">
+    <row r="262" spans="1:9" ht="30" hidden="1">
       <c r="A262" s="21" t="s">
         <v>157</v>
       </c>
@@ -11736,7 +11736,7 @@
       </c>
       <c r="I262" s="23"/>
     </row>
-    <row r="263" spans="1:9" ht="29" hidden="1">
+    <row r="263" spans="1:9" ht="30" hidden="1">
       <c r="A263" s="21" t="s">
         <v>158</v>
       </c>
@@ -11761,7 +11761,7 @@
       </c>
       <c r="I263" s="23"/>
     </row>
-    <row r="264" spans="1:9" ht="29" hidden="1">
+    <row r="264" spans="1:9" ht="30" hidden="1">
       <c r="A264" s="21" t="s">
         <v>159</v>
       </c>
@@ -11786,7 +11786,7 @@
       </c>
       <c r="I264" s="23"/>
     </row>
-    <row r="265" spans="1:9" ht="29" hidden="1">
+    <row r="265" spans="1:9" ht="30" hidden="1">
       <c r="A265" s="21" t="s">
         <v>160</v>
       </c>
@@ -11811,7 +11811,7 @@
       </c>
       <c r="I265" s="23"/>
     </row>
-    <row r="266" spans="1:9" ht="29" hidden="1">
+    <row r="266" spans="1:9" ht="30" hidden="1">
       <c r="A266" s="21" t="s">
         <v>161</v>
       </c>
@@ -11836,7 +11836,7 @@
       </c>
       <c r="I266" s="23"/>
     </row>
-    <row r="267" spans="1:9" ht="29" hidden="1">
+    <row r="267" spans="1:9" ht="30" hidden="1">
       <c r="A267" s="14" t="s">
         <v>796</v>
       </c>
@@ -11863,7 +11863,7 @@
         <v>866</v>
       </c>
     </row>
-    <row r="268" spans="1:9" ht="29" hidden="1">
+    <row r="268" spans="1:9" ht="30" hidden="1">
       <c r="A268" s="14" t="s">
         <v>797</v>
       </c>
@@ -11888,7 +11888,7 @@
       </c>
       <c r="I268" s="42"/>
     </row>
-    <row r="269" spans="1:9" ht="29" hidden="1">
+    <row r="269" spans="1:9" ht="30" hidden="1">
       <c r="A269" s="14" t="s">
         <v>798</v>
       </c>
@@ -11915,7 +11915,7 @@
         <v>869</v>
       </c>
     </row>
-    <row r="270" spans="1:9" ht="29" hidden="1">
+    <row r="270" spans="1:9" hidden="1">
       <c r="A270" s="14" t="s">
         <v>799</v>
       </c>
@@ -11940,7 +11940,7 @@
       </c>
       <c r="I270" s="42"/>
     </row>
-    <row r="271" spans="1:9" ht="29" hidden="1">
+    <row r="271" spans="1:9" ht="30" hidden="1">
       <c r="A271" s="14" t="s">
         <v>800</v>
       </c>
@@ -11965,7 +11965,7 @@
       </c>
       <c r="I271" s="42"/>
     </row>
-    <row r="272" spans="1:9" ht="29" hidden="1">
+    <row r="272" spans="1:9" ht="30" hidden="1">
       <c r="A272" s="14" t="s">
         <v>801</v>
       </c>
@@ -11992,7 +11992,7 @@
         <v>845</v>
       </c>
     </row>
-    <row r="273" spans="1:9" ht="29" hidden="1">
+    <row r="273" spans="1:9" ht="30" hidden="1">
       <c r="A273" s="14" t="s">
         <v>802</v>
       </c>
@@ -12017,7 +12017,7 @@
       </c>
       <c r="I273" s="42"/>
     </row>
-    <row r="274" spans="1:9" ht="29" hidden="1">
+    <row r="274" spans="1:9" hidden="1">
       <c r="A274" s="14" t="s">
         <v>803</v>
       </c>
@@ -12042,7 +12042,7 @@
       </c>
       <c r="I274" s="42"/>
     </row>
-    <row r="275" spans="1:9" ht="130.5" hidden="1">
+    <row r="275" spans="1:9" ht="135" hidden="1">
       <c r="A275" s="21" t="s">
         <v>162</v>
       </c>
@@ -12067,7 +12067,7 @@
       </c>
       <c r="I275" s="23"/>
     </row>
-    <row r="276" spans="1:9" ht="29" hidden="1">
+    <row r="276" spans="1:9" ht="30" hidden="1">
       <c r="A276" s="21" t="s">
         <v>163</v>
       </c>
@@ -12092,7 +12092,7 @@
       </c>
       <c r="I276" s="23"/>
     </row>
-    <row r="277" spans="1:9" ht="29" hidden="1">
+    <row r="277" spans="1:9" ht="30" hidden="1">
       <c r="A277" s="21" t="s">
         <v>164</v>
       </c>
@@ -12117,7 +12117,7 @@
       </c>
       <c r="I277" s="23"/>
     </row>
-    <row r="278" spans="1:9" ht="29" hidden="1">
+    <row r="278" spans="1:9" ht="30" hidden="1">
       <c r="A278" s="21" t="s">
         <v>165</v>
       </c>
@@ -12142,7 +12142,7 @@
       </c>
       <c r="I278" s="23"/>
     </row>
-    <row r="279" spans="1:9" ht="174" hidden="1">
+    <row r="279" spans="1:9" ht="180" hidden="1">
       <c r="A279" s="21" t="s">
         <v>166</v>
       </c>
@@ -12167,7 +12167,7 @@
       </c>
       <c r="I279" s="23"/>
     </row>
-    <row r="280" spans="1:9" ht="29" hidden="1">
+    <row r="280" spans="1:9" ht="30" hidden="1">
       <c r="A280" s="21" t="s">
         <v>167</v>
       </c>
@@ -12192,7 +12192,7 @@
       </c>
       <c r="I280" s="23"/>
     </row>
-    <row r="281" spans="1:9" ht="29" hidden="1">
+    <row r="281" spans="1:9" ht="30" hidden="1">
       <c r="A281" s="21" t="s">
         <v>168</v>
       </c>
@@ -12217,7 +12217,7 @@
       </c>
       <c r="I281" s="23"/>
     </row>
-    <row r="282" spans="1:9" ht="29" hidden="1">
+    <row r="282" spans="1:9" ht="30" hidden="1">
       <c r="A282" s="21" t="s">
         <v>169</v>
       </c>
@@ -12242,7 +12242,7 @@
       </c>
       <c r="I282" s="23"/>
     </row>
-    <row r="283" spans="1:9" ht="29" hidden="1">
+    <row r="283" spans="1:9" hidden="1">
       <c r="A283" s="21" t="s">
         <v>170</v>
       </c>
@@ -12267,7 +12267,7 @@
       </c>
       <c r="I283" s="23"/>
     </row>
-    <row r="284" spans="1:9" ht="29" hidden="1">
+    <row r="284" spans="1:9" ht="30" hidden="1">
       <c r="A284" s="21" t="s">
         <v>171</v>
       </c>
@@ -12292,7 +12292,7 @@
       </c>
       <c r="I284" s="23"/>
     </row>
-    <row r="285" spans="1:9" ht="29" hidden="1">
+    <row r="285" spans="1:9" hidden="1">
       <c r="A285" s="21" t="s">
         <v>172</v>
       </c>
@@ -12319,7 +12319,7 @@
       </c>
       <c r="I285" s="23"/>
     </row>
-    <row r="286" spans="1:9" ht="29" hidden="1">
+    <row r="286" spans="1:9" hidden="1">
       <c r="A286" s="21" t="s">
         <v>173</v>
       </c>
@@ -12346,7 +12346,7 @@
       </c>
       <c r="I286" s="23"/>
     </row>
-    <row r="287" spans="1:9" ht="43.5" hidden="1">
+    <row r="287" spans="1:9" ht="45" hidden="1">
       <c r="A287" s="21" t="s">
         <v>174</v>
       </c>
@@ -12371,7 +12371,7 @@
       </c>
       <c r="I287" s="23"/>
     </row>
-    <row r="288" spans="1:9" ht="43.5" hidden="1">
+    <row r="288" spans="1:9" ht="30" hidden="1">
       <c r="A288" s="21" t="s">
         <v>175</v>
       </c>
@@ -12396,7 +12396,7 @@
       </c>
       <c r="I288" s="23"/>
     </row>
-    <row r="289" spans="1:9" ht="348" hidden="1">
+    <row r="289" spans="1:9" ht="360" hidden="1">
       <c r="A289" s="21" t="s">
         <v>176</v>
       </c>
@@ -12421,7 +12421,7 @@
       </c>
       <c r="I289" s="23"/>
     </row>
-    <row r="290" spans="1:9" ht="43.5" hidden="1">
+    <row r="290" spans="1:9" ht="45" hidden="1">
       <c r="A290" s="21" t="s">
         <v>177</v>
       </c>
@@ -12446,7 +12446,7 @@
       </c>
       <c r="I290" s="23"/>
     </row>
-    <row r="291" spans="1:9" ht="29" hidden="1">
+    <row r="291" spans="1:9" ht="30" hidden="1">
       <c r="A291" s="21" t="s">
         <v>178</v>
       </c>
@@ -12471,7 +12471,7 @@
       </c>
       <c r="I291" s="23"/>
     </row>
-    <row r="292" spans="1:9" ht="43.5" hidden="1">
+    <row r="292" spans="1:9" ht="45" hidden="1">
       <c r="A292" s="21" t="s">
         <v>179</v>
       </c>
@@ -12521,7 +12521,7 @@
       </c>
       <c r="I293" s="23"/>
     </row>
-    <row r="294" spans="1:9" ht="29" hidden="1">
+    <row r="294" spans="1:9" ht="30" hidden="1">
       <c r="A294" s="21" t="s">
         <v>181</v>
       </c>
@@ -12546,7 +12546,7 @@
       </c>
       <c r="I294" s="23"/>
     </row>
-    <row r="295" spans="1:9" ht="43.5" hidden="1">
+    <row r="295" spans="1:9" ht="30" hidden="1">
       <c r="A295" s="21" t="s">
         <v>182</v>
       </c>
@@ -12571,7 +12571,7 @@
       </c>
       <c r="I295" s="23"/>
     </row>
-    <row r="296" spans="1:9" ht="29" hidden="1">
+    <row r="296" spans="1:9" ht="30" hidden="1">
       <c r="A296" s="21" t="s">
         <v>183</v>
       </c>
@@ -12598,7 +12598,7 @@
       </c>
       <c r="I296" s="23"/>
     </row>
-    <row r="297" spans="1:9" ht="43.5" hidden="1">
+    <row r="297" spans="1:9" ht="30" hidden="1">
       <c r="A297" s="21" t="s">
         <v>184</v>
       </c>
@@ -12625,7 +12625,7 @@
       </c>
       <c r="I297" s="23"/>
     </row>
-    <row r="298" spans="1:9" ht="29" hidden="1">
+    <row r="298" spans="1:9" ht="30" hidden="1">
       <c r="A298" s="21" t="s">
         <v>185</v>
       </c>
@@ -12650,7 +12650,7 @@
       </c>
       <c r="I298" s="23"/>
     </row>
-    <row r="299" spans="1:9" ht="29" hidden="1">
+    <row r="299" spans="1:9" ht="30" hidden="1">
       <c r="A299" s="21" t="s">
         <v>186</v>
       </c>
@@ -12675,7 +12675,7 @@
       </c>
       <c r="I299" s="23"/>
     </row>
-    <row r="300" spans="1:9" ht="29" hidden="1">
+    <row r="300" spans="1:9" ht="30" hidden="1">
       <c r="A300" s="21" t="s">
         <v>187</v>
       </c>
@@ -12725,7 +12725,7 @@
       </c>
       <c r="I301" s="23"/>
     </row>
-    <row r="302" spans="1:9" ht="29" hidden="1">
+    <row r="302" spans="1:9" ht="30" hidden="1">
       <c r="A302" s="21" t="s">
         <v>345</v>
       </c>
@@ -12750,7 +12750,7 @@
       </c>
       <c r="I302" s="23"/>
     </row>
-    <row r="303" spans="1:9" ht="29" hidden="1">
+    <row r="303" spans="1:9" ht="30" hidden="1">
       <c r="A303" s="21" t="s">
         <v>346</v>
       </c>
@@ -12775,7 +12775,7 @@
       </c>
       <c r="I303" s="23"/>
     </row>
-    <row r="304" spans="1:9" ht="130.5" hidden="1">
+    <row r="304" spans="1:9" ht="120" hidden="1">
       <c r="A304" s="21" t="s">
         <v>347</v>
       </c>
@@ -12800,7 +12800,7 @@
       </c>
       <c r="I304" s="23"/>
     </row>
-    <row r="305" spans="1:9" ht="29" hidden="1">
+    <row r="305" spans="1:9" ht="30" hidden="1">
       <c r="A305" s="21" t="s">
         <v>307</v>
       </c>
@@ -12825,7 +12825,7 @@
       </c>
       <c r="I305" s="23"/>
     </row>
-    <row r="306" spans="1:9" ht="29" hidden="1">
+    <row r="306" spans="1:9" ht="30" hidden="1">
       <c r="A306" s="21" t="s">
         <v>308</v>
       </c>
@@ -12875,7 +12875,7 @@
       </c>
       <c r="I307" s="23"/>
     </row>
-    <row r="308" spans="1:9" ht="43.5" hidden="1">
+    <row r="308" spans="1:9" ht="45" hidden="1">
       <c r="A308" s="21" t="s">
         <v>310</v>
       </c>
@@ -12900,7 +12900,7 @@
       </c>
       <c r="I308" s="23"/>
     </row>
-    <row r="309" spans="1:9" ht="29" hidden="1">
+    <row r="309" spans="1:9" ht="30" hidden="1">
       <c r="A309" s="21" t="s">
         <v>311</v>
       </c>
@@ -12925,7 +12925,7 @@
       </c>
       <c r="I309" s="23"/>
     </row>
-    <row r="310" spans="1:9" ht="159.5" hidden="1">
+    <row r="310" spans="1:9" ht="150" hidden="1">
       <c r="A310" s="21" t="s">
         <v>312</v>
       </c>
@@ -12952,7 +12952,7 @@
         <v>852</v>
       </c>
     </row>
-    <row r="311" spans="1:9" ht="29" hidden="1">
+    <row r="311" spans="1:9" ht="30" hidden="1">
       <c r="A311" s="14" t="s">
         <v>313</v>
       </c>
@@ -12979,7 +12979,7 @@
       </c>
       <c r="I311" s="23"/>
     </row>
-    <row r="312" spans="1:9" ht="29" hidden="1">
+    <row r="312" spans="1:9" ht="30" hidden="1">
       <c r="A312" s="21" t="s">
         <v>314</v>
       </c>
@@ -13006,7 +13006,7 @@
       </c>
       <c r="I312" s="23"/>
     </row>
-    <row r="313" spans="1:9" ht="29" hidden="1">
+    <row r="313" spans="1:9" ht="30" hidden="1">
       <c r="A313" s="21" t="s">
         <v>315</v>
       </c>
@@ -13033,7 +13033,7 @@
       </c>
       <c r="I313" s="23"/>
     </row>
-    <row r="314" spans="1:9" ht="43.5" hidden="1">
+    <row r="314" spans="1:9" ht="45" hidden="1">
       <c r="A314" s="21" t="s">
         <v>316</v>
       </c>
@@ -13060,7 +13060,7 @@
       </c>
       <c r="I314" s="23"/>
     </row>
-    <row r="315" spans="1:9" ht="43.5" hidden="1">
+    <row r="315" spans="1:9" ht="45" hidden="1">
       <c r="A315" s="14" t="s">
         <v>317</v>
       </c>
@@ -13087,7 +13087,7 @@
       </c>
       <c r="I315" s="23"/>
     </row>
-    <row r="316" spans="1:9" ht="43.5" hidden="1">
+    <row r="316" spans="1:9" ht="45" hidden="1">
       <c r="A316" s="21" t="s">
         <v>318</v>
       </c>
@@ -13114,7 +13114,7 @@
       </c>
       <c r="I316" s="23"/>
     </row>
-    <row r="317" spans="1:9" ht="29" hidden="1">
+    <row r="317" spans="1:9" ht="30" hidden="1">
       <c r="A317" s="21" t="s">
         <v>319</v>
       </c>
@@ -13141,7 +13141,7 @@
       </c>
       <c r="I317" s="23"/>
     </row>
-    <row r="318" spans="1:9" ht="29" hidden="1">
+    <row r="318" spans="1:9" ht="30" hidden="1">
       <c r="A318" s="21" t="s">
         <v>320</v>
       </c>
@@ -13168,7 +13168,7 @@
       </c>
       <c r="I318" s="23"/>
     </row>
-    <row r="319" spans="1:9" ht="29" hidden="1">
+    <row r="319" spans="1:9" ht="30" hidden="1">
       <c r="A319" s="21" t="s">
         <v>321</v>
       </c>
@@ -13193,7 +13193,7 @@
       </c>
       <c r="I319" s="23"/>
     </row>
-    <row r="320" spans="1:9" ht="29" hidden="1">
+    <row r="320" spans="1:9" ht="30" hidden="1">
       <c r="A320" s="21" t="s">
         <v>322</v>
       </c>
@@ -13243,7 +13243,7 @@
       </c>
       <c r="I321" s="23"/>
     </row>
-    <row r="322" spans="1:9" ht="29" hidden="1">
+    <row r="322" spans="1:9" ht="30" hidden="1">
       <c r="A322" s="21" t="s">
         <v>324</v>
       </c>
@@ -13268,7 +13268,7 @@
       </c>
       <c r="I322" s="23"/>
     </row>
-    <row r="323" spans="1:9" ht="43.5" hidden="1">
+    <row r="323" spans="1:9" ht="30" hidden="1">
       <c r="A323" s="21" t="s">
         <v>325</v>
       </c>
@@ -13318,7 +13318,7 @@
       </c>
       <c r="I324" s="23"/>
     </row>
-    <row r="325" spans="1:9" ht="29" hidden="1">
+    <row r="325" spans="1:9" hidden="1">
       <c r="A325" s="14" t="s">
         <v>327</v>
       </c>
@@ -13345,7 +13345,7 @@
       </c>
       <c r="I325" s="13"/>
     </row>
-    <row r="326" spans="1:9" ht="29" hidden="1">
+    <row r="326" spans="1:9" ht="30" hidden="1">
       <c r="A326" s="21" t="s">
         <v>328</v>
       </c>
@@ -13372,7 +13372,7 @@
       </c>
       <c r="I326" s="23"/>
     </row>
-    <row r="327" spans="1:9" ht="29" hidden="1">
+    <row r="327" spans="1:9" ht="30" hidden="1">
       <c r="A327" s="21" t="s">
         <v>329</v>
       </c>
@@ -13397,7 +13397,7 @@
       </c>
       <c r="I327" s="23"/>
     </row>
-    <row r="328" spans="1:9" ht="29" hidden="1">
+    <row r="328" spans="1:9" ht="30" hidden="1">
       <c r="A328" s="21" t="s">
         <v>330</v>
       </c>
@@ -13422,7 +13422,7 @@
       </c>
       <c r="I328" s="23"/>
     </row>
-    <row r="329" spans="1:9" ht="29" hidden="1">
+    <row r="329" spans="1:9" hidden="1">
       <c r="A329" s="21" t="s">
         <v>331</v>
       </c>
@@ -13449,7 +13449,7 @@
       </c>
       <c r="I329" s="23"/>
     </row>
-    <row r="330" spans="1:9" ht="29" hidden="1">
+    <row r="330" spans="1:9" ht="30" hidden="1">
       <c r="A330" s="21" t="s">
         <v>332</v>
       </c>
@@ -13501,7 +13501,7 @@
       </c>
       <c r="I331" s="13"/>
     </row>
-    <row r="332" spans="1:9" ht="29" hidden="1">
+    <row r="332" spans="1:9" hidden="1">
       <c r="A332" s="14" t="s">
         <v>334</v>
       </c>
@@ -13528,7 +13528,7 @@
       </c>
       <c r="I332" s="23"/>
     </row>
-    <row r="333" spans="1:9" ht="29" hidden="1">
+    <row r="333" spans="1:9" ht="30" hidden="1">
       <c r="A333" s="21" t="s">
         <v>335</v>
       </c>
@@ -13555,7 +13555,7 @@
       </c>
       <c r="I333" s="23"/>
     </row>
-    <row r="334" spans="1:9" ht="29" hidden="1">
+    <row r="334" spans="1:9" ht="30" hidden="1">
       <c r="A334" s="21" t="s">
         <v>336</v>
       </c>
@@ -13580,7 +13580,7 @@
       </c>
       <c r="I334" s="23"/>
     </row>
-    <row r="335" spans="1:9" ht="29" hidden="1">
+    <row r="335" spans="1:9" ht="30" hidden="1">
       <c r="A335" s="14" t="s">
         <v>337</v>
       </c>
@@ -13605,7 +13605,7 @@
       </c>
       <c r="I335" s="23"/>
     </row>
-    <row r="336" spans="1:9" ht="43.5" hidden="1">
+    <row r="336" spans="1:9" ht="45" hidden="1">
       <c r="A336" s="21" t="s">
         <v>338</v>
       </c>
@@ -13632,7 +13632,7 @@
         <v>686</v>
       </c>
     </row>
-    <row r="337" spans="1:9" ht="29" hidden="1">
+    <row r="337" spans="1:9" ht="30" hidden="1">
       <c r="A337" s="21" t="s">
         <v>339</v>
       </c>
@@ -13659,7 +13659,7 @@
       </c>
       <c r="I337" s="23"/>
     </row>
-    <row r="338" spans="1:9" ht="29" hidden="1">
+    <row r="338" spans="1:9" ht="30" hidden="1">
       <c r="A338" s="21" t="s">
         <v>340</v>
       </c>
@@ -13684,7 +13684,7 @@
       </c>
       <c r="I338" s="23"/>
     </row>
-    <row r="339" spans="1:9" ht="29" hidden="1">
+    <row r="339" spans="1:9" ht="30" hidden="1">
       <c r="A339" s="21" t="s">
         <v>341</v>
       </c>
@@ -13734,7 +13734,7 @@
       </c>
       <c r="I340" s="13"/>
     </row>
-    <row r="341" spans="1:9" ht="29" hidden="1">
+    <row r="341" spans="1:9" ht="30" hidden="1">
       <c r="A341" s="14" t="s">
         <v>343</v>
       </c>
@@ -13763,7 +13763,7 @@
         <v>842</v>
       </c>
     </row>
-    <row r="342" spans="1:9" ht="29" hidden="1">
+    <row r="342" spans="1:9" ht="30" hidden="1">
       <c r="A342" s="21" t="s">
         <v>344</v>
       </c>
@@ -13792,7 +13792,7 @@
         <v>842</v>
       </c>
     </row>
-    <row r="343" spans="1:9" ht="29" hidden="1">
+    <row r="343" spans="1:9" ht="30" hidden="1">
       <c r="A343" s="14" t="s">
         <v>900</v>
       </c>
@@ -13817,7 +13817,7 @@
       </c>
       <c r="I343" s="42"/>
     </row>
-    <row r="344" spans="1:9" ht="29" hidden="1">
+    <row r="344" spans="1:9" ht="30" hidden="1">
       <c r="A344" s="14" t="s">
         <v>901</v>
       </c>
@@ -13842,7 +13842,7 @@
       </c>
       <c r="I344" s="42"/>
     </row>
-    <row r="345" spans="1:9" ht="29" hidden="1">
+    <row r="345" spans="1:9" ht="30" hidden="1">
       <c r="A345" s="14" t="s">
         <v>902</v>
       </c>
@@ -13867,7 +13867,7 @@
       </c>
       <c r="I345" s="42"/>
     </row>
-    <row r="346" spans="1:9" ht="43.5" hidden="1">
+    <row r="346" spans="1:9" ht="45" hidden="1">
       <c r="A346" s="21" t="s">
         <v>352</v>
       </c>
@@ -13892,7 +13892,7 @@
       </c>
       <c r="I346" s="23"/>
     </row>
-    <row r="347" spans="1:9" ht="29" hidden="1">
+    <row r="347" spans="1:9" ht="30" hidden="1">
       <c r="A347" s="21" t="s">
         <v>353</v>
       </c>
@@ -13917,7 +13917,7 @@
       </c>
       <c r="I347" s="23"/>
     </row>
-    <row r="348" spans="1:9" ht="29" hidden="1">
+    <row r="348" spans="1:9" ht="30" hidden="1">
       <c r="A348" s="21" t="s">
         <v>354</v>
       </c>
@@ -13942,7 +13942,7 @@
       </c>
       <c r="I348" s="23"/>
     </row>
-    <row r="349" spans="1:9" ht="217.5" hidden="1">
+    <row r="349" spans="1:9" ht="210" hidden="1">
       <c r="A349" s="21" t="s">
         <v>355</v>
       </c>
@@ -13967,7 +13967,7 @@
       </c>
       <c r="I349" s="23"/>
     </row>
-    <row r="350" spans="1:9" ht="203" hidden="1">
+    <row r="350" spans="1:9" ht="210" hidden="1">
       <c r="A350" s="21" t="s">
         <v>356</v>
       </c>
@@ -13992,7 +13992,7 @@
       </c>
       <c r="I350" s="23"/>
     </row>
-    <row r="351" spans="1:9" ht="43.5" hidden="1">
+    <row r="351" spans="1:9" ht="30" hidden="1">
       <c r="A351" s="21" t="s">
         <v>357</v>
       </c>
@@ -14017,7 +14017,7 @@
       </c>
       <c r="I351" s="23"/>
     </row>
-    <row r="352" spans="1:9" ht="29" hidden="1">
+    <row r="352" spans="1:9" ht="30" hidden="1">
       <c r="A352" s="14" t="s">
         <v>358</v>
       </c>
@@ -14042,7 +14042,7 @@
       </c>
       <c r="I352" s="23"/>
     </row>
-    <row r="353" spans="1:9" ht="29" hidden="1">
+    <row r="353" spans="1:9" ht="30" hidden="1">
       <c r="A353" s="21" t="s">
         <v>359</v>
       </c>
@@ -14067,7 +14067,7 @@
       </c>
       <c r="I353" s="23"/>
     </row>
-    <row r="354" spans="1:9" ht="43.5" hidden="1">
+    <row r="354" spans="1:9" ht="45" hidden="1">
       <c r="A354" s="14" t="s">
         <v>360</v>
       </c>
@@ -14092,7 +14092,7 @@
       </c>
       <c r="I354" s="23"/>
     </row>
-    <row r="355" spans="1:9" ht="29" hidden="1">
+    <row r="355" spans="1:9" ht="30" hidden="1">
       <c r="A355" s="21" t="s">
         <v>361</v>
       </c>
@@ -14117,7 +14117,7 @@
       </c>
       <c r="I355" s="23"/>
     </row>
-    <row r="356" spans="1:9" ht="43.5" hidden="1">
+    <row r="356" spans="1:9" ht="45" hidden="1">
       <c r="A356" s="21" t="s">
         <v>362</v>
       </c>
@@ -14146,7 +14146,7 @@
         <v>687</v>
       </c>
     </row>
-    <row r="357" spans="1:9" ht="43.5" hidden="1">
+    <row r="357" spans="1:9" ht="45" hidden="1">
       <c r="A357" s="21" t="s">
         <v>363</v>
       </c>
@@ -14175,7 +14175,7 @@
         <v>687</v>
       </c>
     </row>
-    <row r="358" spans="1:9" ht="43.5" hidden="1">
+    <row r="358" spans="1:9" ht="45" hidden="1">
       <c r="A358" s="21" t="s">
         <v>364</v>
       </c>
@@ -14204,7 +14204,7 @@
         <v>687</v>
       </c>
     </row>
-    <row r="359" spans="1:9" ht="43.5" hidden="1">
+    <row r="359" spans="1:9" ht="30" hidden="1">
       <c r="A359" s="14" t="s">
         <v>832</v>
       </c>
@@ -14231,7 +14231,7 @@
       </c>
       <c r="I359" s="42"/>
     </row>
-    <row r="360" spans="1:9" ht="43.5" hidden="1">
+    <row r="360" spans="1:9" ht="45" hidden="1">
       <c r="A360" s="14" t="s">
         <v>833</v>
       </c>
@@ -14260,7 +14260,7 @@
         <v>687</v>
       </c>
     </row>
-    <row r="361" spans="1:9" ht="29" hidden="1">
+    <row r="361" spans="1:9" ht="30" hidden="1">
       <c r="A361" s="14" t="s">
         <v>834</v>
       </c>
@@ -14287,7 +14287,7 @@
       </c>
       <c r="I361" s="42"/>
     </row>
-    <row r="362" spans="1:9" ht="43.5" hidden="1">
+    <row r="362" spans="1:9" ht="45" hidden="1">
       <c r="A362" s="14" t="s">
         <v>835</v>
       </c>
@@ -14316,7 +14316,7 @@
         <v>687</v>
       </c>
     </row>
-    <row r="363" spans="1:9" ht="43.5" hidden="1">
+    <row r="363" spans="1:9" ht="30" hidden="1">
       <c r="A363" s="14" t="s">
         <v>862</v>
       </c>
@@ -14343,7 +14343,7 @@
       </c>
       <c r="I363" s="42"/>
     </row>
-    <row r="364" spans="1:9" ht="43.5" hidden="1">
+    <row r="364" spans="1:9" ht="45" hidden="1">
       <c r="A364" s="14" t="s">
         <v>863</v>
       </c>
@@ -14372,7 +14372,7 @@
         <v>687</v>
       </c>
     </row>
-    <row r="365" spans="1:9" ht="43.5" hidden="1">
+    <row r="365" spans="1:9" ht="30" hidden="1">
       <c r="A365" s="14" t="s">
         <v>864</v>
       </c>
@@ -14399,7 +14399,7 @@
       </c>
       <c r="I365" s="42"/>
     </row>
-    <row r="366" spans="1:9" ht="43.5" hidden="1">
+    <row r="366" spans="1:9" ht="45" hidden="1">
       <c r="A366" s="14" t="s">
         <v>865</v>
       </c>
@@ -14428,7 +14428,7 @@
         <v>687</v>
       </c>
     </row>
-    <row r="367" spans="1:9" ht="43.5" hidden="1">
+    <row r="367" spans="1:9" ht="30" hidden="1">
       <c r="A367" s="14" t="s">
         <v>836</v>
       </c>
@@ -14455,7 +14455,7 @@
       </c>
       <c r="I367" s="42"/>
     </row>
-    <row r="368" spans="1:9" ht="43.5" hidden="1">
+    <row r="368" spans="1:9" ht="45" hidden="1">
       <c r="A368" s="14" t="s">
         <v>837</v>
       </c>
@@ -14484,7 +14484,7 @@
         <v>687</v>
       </c>
     </row>
-    <row r="369" spans="1:9" ht="29" hidden="1">
+    <row r="369" spans="1:9" ht="30" hidden="1">
       <c r="A369" s="14" t="s">
         <v>838</v>
       </c>
@@ -14511,7 +14511,7 @@
       </c>
       <c r="I369" s="42"/>
     </row>
-    <row r="370" spans="1:9" ht="43.5" hidden="1">
+    <row r="370" spans="1:9" ht="45" hidden="1">
       <c r="A370" s="14" t="s">
         <v>839</v>
       </c>
@@ -14540,7 +14540,7 @@
         <v>687</v>
       </c>
     </row>
-    <row r="371" spans="1:9" ht="72.5" hidden="1">
+    <row r="371" spans="1:9" ht="60" hidden="1">
       <c r="A371" s="21" t="s">
         <v>365</v>
       </c>
@@ -14567,7 +14567,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="372" spans="1:9" ht="58" hidden="1">
+    <row r="372" spans="1:9" ht="45" hidden="1">
       <c r="A372" s="21" t="s">
         <v>366</v>
       </c>
@@ -14594,7 +14594,7 @@
         <v>871</v>
       </c>
     </row>
-    <row r="373" spans="1:9" ht="58" hidden="1">
+    <row r="373" spans="1:9" ht="45" hidden="1">
       <c r="A373" s="21" t="s">
         <v>367</v>
       </c>
@@ -14621,7 +14621,7 @@
         <v>872</v>
       </c>
     </row>
-    <row r="374" spans="1:9" ht="58" hidden="1">
+    <row r="374" spans="1:9" ht="45" hidden="1">
       <c r="A374" s="21" t="s">
         <v>368</v>
       </c>
@@ -14673,7 +14673,7 @@
       </c>
       <c r="I375" s="23"/>
     </row>
-    <row r="376" spans="1:9" ht="29" hidden="1">
+    <row r="376" spans="1:9" ht="30" hidden="1">
       <c r="A376" s="21" t="s">
         <v>370</v>
       </c>
@@ -14698,7 +14698,7 @@
       </c>
       <c r="I376" s="23"/>
     </row>
-    <row r="377" spans="1:9" ht="29" hidden="1">
+    <row r="377" spans="1:9" ht="30" hidden="1">
       <c r="A377" s="21" t="s">
         <v>371</v>
       </c>
@@ -14748,7 +14748,7 @@
       </c>
       <c r="I378" s="23"/>
     </row>
-    <row r="379" spans="1:9" ht="29" hidden="1">
+    <row r="379" spans="1:9" ht="30" hidden="1">
       <c r="A379" s="21" t="s">
         <v>373</v>
       </c>
@@ -14773,7 +14773,7 @@
       </c>
       <c r="I379" s="23"/>
     </row>
-    <row r="380" spans="1:9" ht="130.5" hidden="1">
+    <row r="380" spans="1:9" ht="135" hidden="1">
       <c r="A380" s="21" t="s">
         <v>374</v>
       </c>
@@ -14798,7 +14798,7 @@
       </c>
       <c r="I380" s="23"/>
     </row>
-    <row r="381" spans="1:9" ht="29" hidden="1">
+    <row r="381" spans="1:9" ht="30" hidden="1">
       <c r="A381" s="21" t="s">
         <v>375</v>
       </c>
@@ -14823,7 +14823,7 @@
       </c>
       <c r="I381" s="23"/>
     </row>
-    <row r="382" spans="1:9" ht="246.5" hidden="1">
+    <row r="382" spans="1:9" ht="255" hidden="1">
       <c r="A382" s="21" t="s">
         <v>376</v>
       </c>
@@ -14848,7 +14848,7 @@
       </c>
       <c r="I382" s="23"/>
     </row>
-    <row r="383" spans="1:9" ht="43.5" hidden="1">
+    <row r="383" spans="1:9" ht="45" hidden="1">
       <c r="A383" s="21" t="s">
         <v>377</v>
       </c>
@@ -14875,7 +14875,7 @@
         <v>689</v>
       </c>
     </row>
-    <row r="384" spans="1:9" ht="43.5" hidden="1">
+    <row r="384" spans="1:9" ht="45" hidden="1">
       <c r="A384" s="21" t="s">
         <v>378</v>
       </c>
@@ -14902,7 +14902,7 @@
         <v>698</v>
       </c>
     </row>
-    <row r="385" spans="1:9" ht="29" hidden="1">
+    <row r="385" spans="1:9" ht="30" hidden="1">
       <c r="A385" s="21" t="s">
         <v>379</v>
       </c>
@@ -14929,7 +14929,7 @@
         <v>873</v>
       </c>
     </row>
-    <row r="386" spans="1:9" ht="29" hidden="1">
+    <row r="386" spans="1:9" ht="30" hidden="1">
       <c r="A386" s="21" t="s">
         <v>380</v>
       </c>
@@ -14956,7 +14956,7 @@
         <v>874</v>
       </c>
     </row>
-    <row r="387" spans="1:9" ht="29" hidden="1">
+    <row r="387" spans="1:9" ht="30" hidden="1">
       <c r="A387" s="21" t="s">
         <v>381</v>
       </c>
@@ -14983,7 +14983,7 @@
         <v>690</v>
       </c>
     </row>
-    <row r="388" spans="1:9" ht="43.5" hidden="1">
+    <row r="388" spans="1:9" ht="45" hidden="1">
       <c r="A388" s="21" t="s">
         <v>382</v>
       </c>
@@ -15010,7 +15010,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="389" spans="1:9" ht="58" hidden="1">
+    <row r="389" spans="1:9" ht="45" hidden="1">
       <c r="A389" s="21" t="s">
         <v>383</v>
       </c>
@@ -15087,7 +15087,7 @@
       </c>
       <c r="I391" s="23"/>
     </row>
-    <row r="392" spans="1:9" ht="58" hidden="1">
+    <row r="392" spans="1:9" ht="60" hidden="1">
       <c r="A392" s="21" t="s">
         <v>386</v>
       </c>
@@ -15112,7 +15112,7 @@
       </c>
       <c r="I392" s="23"/>
     </row>
-    <row r="393" spans="1:9" ht="348" hidden="1">
+    <row r="393" spans="1:9" ht="360" hidden="1">
       <c r="A393" s="21" t="s">
         <v>387</v>
       </c>
@@ -15137,7 +15137,7 @@
       </c>
       <c r="I393" s="23"/>
     </row>
-    <row r="394" spans="1:9" ht="43.5" hidden="1">
+    <row r="394" spans="1:9" ht="30" hidden="1">
       <c r="A394" s="21" t="s">
         <v>388</v>
       </c>
@@ -15269,6 +15269,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F2EA47BB262D974097182E2CA8AB13E1" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="74597e8d9e42e7e4fc8eda6d37675aa2">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4aeb20c0e3442673af7ee10786458764">
     <xsd:element name="properties">
@@ -15317,22 +15332,29 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{923F65C5-DEAB-400B-AA1F-124F40EE10AC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6D33261-F3C6-4621-88F1-D76E5ABE1865}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EDB2DE12-5EF6-4CF2-820D-5F9FE329E08E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -15347,28 +15369,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6D33261-F3C6-4621-88F1-D76E5ABE1865}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{923F65C5-DEAB-400B-AA1F-124F40EE10AC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{f42aa342-8706-4288-bd11-ebb85995028c}" enabled="1" method="Privileged" siteId="{72f988bf-86f1-41af-91ab-2d7cd011db47}" removed="0"/>

</xml_diff>